<commit_message>
updated analyses and plots
</commit_message>
<xml_diff>
--- a/Data/Supplemental/Supplemental_Tables.xlsx
+++ b/Data/Supplemental/Supplemental_Tables.xlsx
@@ -40,28 +40,28 @@
     <t xml:space="preserve">SSID</t>
   </si>
   <si>
-    <t xml:space="preserve">288_28</t>
+    <t xml:space="preserve">300_28</t>
   </si>
   <si>
-    <t xml:space="preserve">311_31</t>
+    <t xml:space="preserve">300_31</t>
   </si>
   <si>
-    <t xml:space="preserve">3285_28</t>
+    <t xml:space="preserve">3300_28</t>
   </si>
   <si>
-    <t xml:space="preserve">3309_31</t>
+    <t xml:space="preserve">3300_31</t>
   </si>
   <si>
-    <t xml:space="preserve">405_31</t>
+    <t xml:space="preserve">420_28</t>
   </si>
   <si>
-    <t xml:space="preserve">447_28</t>
+    <t xml:space="preserve">420_31</t>
   </si>
   <si>
-    <t xml:space="preserve">673_28</t>
+    <t xml:space="preserve">680_28</t>
   </si>
   <si>
-    <t xml:space="preserve">701_31</t>
+    <t xml:space="preserve">680_31</t>
   </si>
   <si>
     <t xml:space="preserve">PSTR</t>
@@ -397,7 +397,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
     <col min="1" max="1" width="7.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="9.71" hidden="0" customWidth="1"/>
@@ -437,13 +437,13 @@
         <v>11</v>
       </c>
       <c r="D2" t="n">
-        <v>0.49</v>
+        <v>0.54</v>
       </c>
       <c r="E2" t="n">
-        <v>0.4</v>
+        <v>0.47</v>
       </c>
       <c r="F2" t="n">
-        <v>0.57</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="3">
@@ -457,13 +457,13 @@
         <v>9</v>
       </c>
       <c r="D3" t="n">
-        <v>0.44</v>
+        <v>0.48</v>
       </c>
       <c r="E3" t="n">
-        <v>0.35</v>
+        <v>0.41</v>
       </c>
       <c r="F3" t="n">
-        <v>0.52</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="4">
@@ -477,13 +477,13 @@
         <v>12</v>
       </c>
       <c r="D4" t="n">
-        <v>0.45</v>
+        <v>0.43</v>
       </c>
       <c r="E4" t="n">
         <v>0.37</v>
       </c>
       <c r="F4" t="n">
-        <v>0.53</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="5">
@@ -497,13 +497,13 @@
         <v>12</v>
       </c>
       <c r="D5" t="n">
-        <v>0.39</v>
+        <v>0.38</v>
       </c>
       <c r="E5" t="n">
         <v>0.31</v>
       </c>
       <c r="F5" t="n">
-        <v>0.47</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="6">
@@ -517,13 +517,13 @@
         <v>12</v>
       </c>
       <c r="D6" t="n">
-        <v>0.46</v>
+        <v>0.5</v>
       </c>
       <c r="E6" t="n">
-        <v>0.38</v>
+        <v>0.43</v>
       </c>
       <c r="F6" t="n">
-        <v>0.54</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="7">
@@ -537,13 +537,13 @@
         <v>12</v>
       </c>
       <c r="D7" t="n">
-        <v>0.52</v>
+        <v>0.45</v>
       </c>
       <c r="E7" t="n">
-        <v>0.44</v>
+        <v>0.38</v>
       </c>
       <c r="F7" t="n">
-        <v>0.6</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="8">
@@ -557,13 +557,13 @@
         <v>13</v>
       </c>
       <c r="D8" t="n">
-        <v>0.47</v>
+        <v>0.46</v>
       </c>
       <c r="E8" t="n">
-        <v>0.38</v>
+        <v>0.39</v>
       </c>
       <c r="F8" t="n">
-        <v>0.54</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="9">
@@ -577,13 +577,13 @@
         <v>12</v>
       </c>
       <c r="D9" t="n">
-        <v>0.41</v>
+        <v>0.4</v>
       </c>
       <c r="E9" t="n">
-        <v>0.33</v>
+        <v>0.34</v>
       </c>
       <c r="F9" t="n">
-        <v>0.49</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="10">
@@ -597,13 +597,13 @@
         <v>16</v>
       </c>
       <c r="D10" t="n">
-        <v>0.56</v>
+        <v>0.53</v>
       </c>
       <c r="E10" t="n">
-        <v>0.49</v>
+        <v>0.47</v>
       </c>
       <c r="F10" t="n">
-        <v>0.64</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="11">
@@ -617,13 +617,13 @@
         <v>9</v>
       </c>
       <c r="D11" t="n">
-        <v>0.32</v>
+        <v>0.27</v>
       </c>
       <c r="E11" t="n">
-        <v>0.23</v>
+        <v>0.19</v>
       </c>
       <c r="F11" t="n">
-        <v>0.41</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="12">
@@ -637,13 +637,13 @@
         <v>16</v>
       </c>
       <c r="D12" t="n">
-        <v>0.42</v>
+        <v>0.43</v>
       </c>
       <c r="E12" t="n">
-        <v>0.34</v>
+        <v>0.36</v>
       </c>
       <c r="F12" t="n">
-        <v>0.5</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="13">
@@ -660,10 +660,10 @@
         <v>0.17</v>
       </c>
       <c r="E13" t="n">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="F13" t="n">
-        <v>0.27</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="14">
@@ -674,16 +674,16 @@
         <v>11</v>
       </c>
       <c r="C14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D14" t="n">
-        <v>0.18</v>
+        <v>0.49</v>
       </c>
       <c r="E14" t="n">
-        <v>0.07</v>
+        <v>0.42</v>
       </c>
       <c r="F14" t="n">
-        <v>0.29</v>
+        <v>0.56</v>
       </c>
     </row>
     <row r="15">
@@ -694,16 +694,16 @@
         <v>12</v>
       </c>
       <c r="C15" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D15" t="n">
-        <v>0.42</v>
+        <v>0.23</v>
       </c>
       <c r="E15" t="n">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="F15" t="n">
-        <v>0.54</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="16">
@@ -720,10 +720,10 @@
         <v>0.45</v>
       </c>
       <c r="E16" t="n">
-        <v>0.37</v>
+        <v>0.39</v>
       </c>
       <c r="F16" t="n">
-        <v>0.53</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="17">
@@ -734,16 +734,16 @@
         <v>14</v>
       </c>
       <c r="C17" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D17" t="n">
-        <v>0.21</v>
+        <v>0.19</v>
       </c>
       <c r="E17" t="n">
         <v>0.11</v>
       </c>
       <c r="F17" t="n">
-        <v>0.31</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="18">
@@ -757,13 +757,13 @@
         <v>11</v>
       </c>
       <c r="D18" t="n">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
       <c r="E18" t="n">
-        <v>0.15</v>
+        <v>0.17</v>
       </c>
       <c r="F18" t="n">
-        <v>0.33</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="19">
@@ -780,10 +780,10 @@
         <v>0.19</v>
       </c>
       <c r="E19" t="n">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="F19" t="n">
-        <v>0.29</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="20">
@@ -797,10 +797,10 @@
         <v>12</v>
       </c>
       <c r="D20" t="n">
-        <v>0.11</v>
+        <v>0.13</v>
       </c>
       <c r="E20" t="n">
-        <v>0.02</v>
+        <v>0.06</v>
       </c>
       <c r="F20" t="n">
         <v>0.2</v>
@@ -817,10 +817,10 @@
         <v>4</v>
       </c>
       <c r="D21" t="n">
-        <v>0.06</v>
+        <v>0.08</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.05</v>
+        <v>0</v>
       </c>
       <c r="F21" t="n">
         <v>0.17</v>
@@ -834,16 +834,16 @@
         <v>11</v>
       </c>
       <c r="C22" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D22" t="n">
-        <v>0.16</v>
+        <v>0.2</v>
       </c>
       <c r="E22" t="n">
-        <v>0.07</v>
+        <v>0.13</v>
       </c>
       <c r="F22" t="n">
-        <v>0.27</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="23">
@@ -854,16 +854,16 @@
         <v>12</v>
       </c>
       <c r="C23" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D23" t="n">
-        <v>0.21</v>
+        <v>0.15</v>
       </c>
       <c r="E23" t="n">
-        <v>0.12</v>
+        <v>0.07</v>
       </c>
       <c r="F23" t="n">
-        <v>0.3</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="24">
@@ -877,13 +877,13 @@
         <v>10</v>
       </c>
       <c r="D24" t="n">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="E24" t="n">
-        <v>0.06</v>
+        <v>0.09</v>
       </c>
       <c r="F24" t="n">
-        <v>0.25</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="25">
@@ -900,10 +900,10 @@
         <v>0.11</v>
       </c>
       <c r="E25" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="F25" t="n">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
     </row>
   </sheetData>
@@ -918,7 +918,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
     <col min="1" max="1" width="7.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="9.71" hidden="0" customWidth="1"/>
@@ -958,13 +958,13 @@
         <v>11</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4</v>
+        <v>0.37</v>
       </c>
       <c r="E2" t="n">
-        <v>0.29</v>
+        <v>0.3</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="3">
@@ -978,13 +978,13 @@
         <v>9</v>
       </c>
       <c r="D3" t="n">
-        <v>0.37</v>
+        <v>0.35</v>
       </c>
       <c r="E3" t="n">
-        <v>0.26</v>
+        <v>0.28</v>
       </c>
       <c r="F3" t="n">
-        <v>0.48</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="4">
@@ -1001,10 +1001,10 @@
         <v>0.37</v>
       </c>
       <c r="E4" t="n">
-        <v>0.27</v>
+        <v>0.3</v>
       </c>
       <c r="F4" t="n">
-        <v>0.47</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="5">
@@ -1021,10 +1021,10 @@
         <v>0.35</v>
       </c>
       <c r="E5" t="n">
-        <v>0.25</v>
+        <v>0.28</v>
       </c>
       <c r="F5" t="n">
-        <v>0.45</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="6">
@@ -1038,13 +1038,13 @@
         <v>12</v>
       </c>
       <c r="D6" t="n">
-        <v>0.38</v>
+        <v>0.37</v>
       </c>
       <c r="E6" t="n">
-        <v>0.29</v>
+        <v>0.3</v>
       </c>
       <c r="F6" t="n">
-        <v>0.48</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="7">
@@ -1058,13 +1058,13 @@
         <v>12</v>
       </c>
       <c r="D7" t="n">
-        <v>0.41</v>
+        <v>0.35</v>
       </c>
       <c r="E7" t="n">
-        <v>0.3</v>
+        <v>0.27</v>
       </c>
       <c r="F7" t="n">
-        <v>0.51</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="8">
@@ -1078,13 +1078,13 @@
         <v>13</v>
       </c>
       <c r="D8" t="n">
-        <v>0.33</v>
+        <v>0.38</v>
       </c>
       <c r="E8" t="n">
-        <v>0.23</v>
+        <v>0.31</v>
       </c>
       <c r="F8" t="n">
-        <v>0.43</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="9">
@@ -1098,13 +1098,13 @@
         <v>12</v>
       </c>
       <c r="D9" t="n">
-        <v>0.31</v>
+        <v>0.36</v>
       </c>
       <c r="E9" t="n">
-        <v>0.21</v>
+        <v>0.29</v>
       </c>
       <c r="F9" t="n">
-        <v>0.41</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="10">
@@ -1118,13 +1118,13 @@
         <v>16</v>
       </c>
       <c r="D10" t="n">
-        <v>0.27</v>
+        <v>0.24</v>
       </c>
       <c r="E10" t="n">
-        <v>0.18</v>
+        <v>0.17</v>
       </c>
       <c r="F10" t="n">
-        <v>0.37</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="11">
@@ -1138,13 +1138,13 @@
         <v>9</v>
       </c>
       <c r="D11" t="n">
-        <v>0.14</v>
+        <v>0.11</v>
       </c>
       <c r="E11" t="n">
         <v>0.02</v>
       </c>
       <c r="F11" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="12">
@@ -1158,13 +1158,13 @@
         <v>15</v>
       </c>
       <c r="D12" t="n">
-        <v>0.22</v>
+        <v>0.24</v>
       </c>
       <c r="E12" t="n">
-        <v>0.12</v>
+        <v>0.17</v>
       </c>
       <c r="F12" t="n">
-        <v>0.32</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="13">
@@ -1178,10 +1178,10 @@
         <v>8</v>
       </c>
       <c r="D13" t="n">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.04</v>
+        <v>0.02</v>
       </c>
       <c r="F13" t="n">
         <v>0.19</v>
@@ -1198,13 +1198,13 @@
         <v>5</v>
       </c>
       <c r="D14" t="n">
-        <v>0.12</v>
+        <v>0.24</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.03</v>
+        <v>0.17</v>
       </c>
       <c r="F14" t="n">
-        <v>0.26</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="15">
@@ -1218,13 +1218,13 @@
         <v>5</v>
       </c>
       <c r="D15" t="n">
-        <v>0.26</v>
+        <v>0.11</v>
       </c>
       <c r="E15" t="n">
-        <v>0.11</v>
+        <v>0.02</v>
       </c>
       <c r="F15" t="n">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="16">
@@ -1238,13 +1238,13 @@
         <v>14</v>
       </c>
       <c r="D16" t="n">
-        <v>0.22</v>
+        <v>0.24</v>
       </c>
       <c r="E16" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
       <c r="F16" t="n">
-        <v>0.32</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="17">
@@ -1255,13 +1255,13 @@
         <v>14</v>
       </c>
       <c r="C17" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D17" t="n">
-        <v>0.07</v>
+        <v>0.11</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.04</v>
+        <v>0.02</v>
       </c>
       <c r="F17" t="n">
         <v>0.2</v>
@@ -1278,13 +1278,13 @@
         <v>11</v>
       </c>
       <c r="D18" t="n">
-        <v>0.21</v>
+        <v>0.15</v>
       </c>
       <c r="E18" t="n">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="F18" t="n">
-        <v>0.33</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="19">
@@ -1298,13 +1298,13 @@
         <v>6</v>
       </c>
       <c r="D19" t="n">
-        <v>0.26</v>
+        <v>0.2</v>
       </c>
       <c r="E19" t="n">
-        <v>0.13</v>
+        <v>0.11</v>
       </c>
       <c r="F19" t="n">
-        <v>0.38</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="20">
@@ -1318,13 +1318,13 @@
         <v>12</v>
       </c>
       <c r="D20" t="n">
-        <v>0.13</v>
+        <v>0.16</v>
       </c>
       <c r="E20" t="n">
-        <v>0.01</v>
+        <v>0.08</v>
       </c>
       <c r="F20" t="n">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="21">
@@ -1338,13 +1338,13 @@
         <v>4</v>
       </c>
       <c r="D21" t="n">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
       <c r="E21" t="n">
-        <v>0.07</v>
+        <v>0.14</v>
       </c>
       <c r="F21" t="n">
-        <v>0.33</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="22">
@@ -1355,16 +1355,16 @@
         <v>11</v>
       </c>
       <c r="C22" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D22" t="n">
-        <v>0.22</v>
+        <v>0.16</v>
       </c>
       <c r="E22" t="n">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="F22" t="n">
-        <v>0.34</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="23">
@@ -1375,16 +1375,16 @@
         <v>12</v>
       </c>
       <c r="C23" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D23" t="n">
-        <v>0.17</v>
+        <v>0.2</v>
       </c>
       <c r="E23" t="n">
-        <v>0.06</v>
+        <v>0.11</v>
       </c>
       <c r="F23" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="24">
@@ -1398,10 +1398,10 @@
         <v>10</v>
       </c>
       <c r="D24" t="n">
-        <v>0.11</v>
+        <v>0.16</v>
       </c>
       <c r="E24" t="n">
-        <v>0.01</v>
+        <v>0.08</v>
       </c>
       <c r="F24" t="n">
         <v>0.23</v>
@@ -1418,13 +1418,13 @@
         <v>9</v>
       </c>
       <c r="D25" t="n">
-        <v>0.16</v>
+        <v>0.2</v>
       </c>
       <c r="E25" t="n">
-        <v>0.05</v>
+        <v>0.11</v>
       </c>
       <c r="F25" t="n">
-        <v>0.28</v>
+        <v>0.29</v>
       </c>
     </row>
   </sheetData>
@@ -1439,7 +1439,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
     <col min="1" max="1" width="7.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="9.71" hidden="0" customWidth="1"/>
@@ -1559,13 +1559,13 @@
         <v>12</v>
       </c>
       <c r="D6" t="n">
-        <v>0.75</v>
+        <v>1.08</v>
       </c>
       <c r="E6" t="n">
-        <v>0.57</v>
+        <v>0.9</v>
       </c>
       <c r="F6" t="n">
-        <v>0.94</v>
+        <v>1.26</v>
       </c>
     </row>
     <row r="7">
@@ -1579,13 +1579,13 @@
         <v>12</v>
       </c>
       <c r="D7" t="n">
-        <v>1.08</v>
+        <v>0.75</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9</v>
+        <v>0.57</v>
       </c>
       <c r="F7" t="n">
-        <v>1.26</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="8">
@@ -1716,16 +1716,16 @@
         <v>11</v>
       </c>
       <c r="C14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D14" t="n">
-        <v>0.4</v>
+        <v>0.67</v>
       </c>
       <c r="E14" t="n">
-        <v>0.16</v>
+        <v>0.41</v>
       </c>
       <c r="F14" t="n">
-        <v>0.65</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="15">
@@ -1736,16 +1736,16 @@
         <v>12</v>
       </c>
       <c r="C15" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D15" t="n">
-        <v>0.67</v>
+        <v>0.4</v>
       </c>
       <c r="E15" t="n">
-        <v>0.41</v>
+        <v>0.16</v>
       </c>
       <c r="F15" t="n">
-        <v>0.92</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="16">
@@ -1876,16 +1876,16 @@
         <v>11</v>
       </c>
       <c r="C22" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D22" t="n">
-        <v>0.73</v>
+        <v>0.9</v>
       </c>
       <c r="E22" t="n">
-        <v>0.51</v>
+        <v>0.71</v>
       </c>
       <c r="F22" t="n">
-        <v>0.95</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="23">
@@ -1896,16 +1896,16 @@
         <v>12</v>
       </c>
       <c r="C23" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D23" t="n">
-        <v>0.9</v>
+        <v>0.73</v>
       </c>
       <c r="E23" t="n">
-        <v>0.71</v>
+        <v>0.51</v>
       </c>
       <c r="F23" t="n">
-        <v>1.1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="24">
@@ -1960,7 +1960,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
     <col min="1" max="1" width="7.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="9.71" hidden="0" customWidth="1"/>
@@ -2080,13 +2080,13 @@
         <v>12</v>
       </c>
       <c r="D6" t="n">
-        <v>2.61</v>
+        <v>3.48</v>
       </c>
       <c r="E6" t="n">
-        <v>1.55</v>
+        <v>2.42</v>
       </c>
       <c r="F6" t="n">
-        <v>3.67</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="7">
@@ -2100,13 +2100,13 @@
         <v>12</v>
       </c>
       <c r="D7" t="n">
-        <v>3.48</v>
+        <v>2.61</v>
       </c>
       <c r="E7" t="n">
-        <v>2.42</v>
+        <v>1.55</v>
       </c>
       <c r="F7" t="n">
-        <v>4.5</v>
+        <v>3.67</v>
       </c>
     </row>
     <row r="8">
@@ -2237,16 +2237,16 @@
         <v>11</v>
       </c>
       <c r="C14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D14" t="n">
-        <v>0.45</v>
+        <v>2.16</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.96</v>
+        <v>0.75</v>
       </c>
       <c r="F14" t="n">
-        <v>1.86</v>
+        <v>3.61</v>
       </c>
     </row>
     <row r="15">
@@ -2257,16 +2257,16 @@
         <v>12</v>
       </c>
       <c r="C15" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D15" t="n">
-        <v>2.16</v>
+        <v>0.45</v>
       </c>
       <c r="E15" t="n">
-        <v>0.75</v>
+        <v>-0.96</v>
       </c>
       <c r="F15" t="n">
-        <v>3.61</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="16">
@@ -2397,16 +2397,16 @@
         <v>11</v>
       </c>
       <c r="C22" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D22" t="n">
-        <v>5.51</v>
+        <v>6.43</v>
       </c>
       <c r="E22" t="n">
-        <v>4.22</v>
+        <v>5.28</v>
       </c>
       <c r="F22" t="n">
-        <v>6.83</v>
+        <v>7.57</v>
       </c>
     </row>
     <row r="23">
@@ -2417,16 +2417,16 @@
         <v>12</v>
       </c>
       <c r="C23" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D23" t="n">
-        <v>6.43</v>
+        <v>5.51</v>
       </c>
       <c r="E23" t="n">
-        <v>5.28</v>
+        <v>4.22</v>
       </c>
       <c r="F23" t="n">
-        <v>7.57</v>
+        <v>6.83</v>
       </c>
     </row>
     <row r="24">
@@ -2481,7 +2481,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
     <col min="1" max="1" width="7.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="9.71" hidden="0" customWidth="1"/>
@@ -2521,13 +2521,13 @@
         <v>11</v>
       </c>
       <c r="D2" t="n">
-        <v>111.62</v>
+        <v>112.38</v>
       </c>
       <c r="E2" t="n">
-        <v>79.83</v>
+        <v>81.74</v>
       </c>
       <c r="F2" t="n">
-        <v>142.93</v>
+        <v>143.62</v>
       </c>
     </row>
     <row r="3">
@@ -2541,13 +2541,13 @@
         <v>9</v>
       </c>
       <c r="D3" t="n">
-        <v>105.32</v>
+        <v>105.47</v>
       </c>
       <c r="E3" t="n">
-        <v>71.66</v>
+        <v>71.18</v>
       </c>
       <c r="F3" t="n">
-        <v>138.94</v>
+        <v>140.02</v>
       </c>
     </row>
     <row r="4">
@@ -2561,13 +2561,13 @@
         <v>12</v>
       </c>
       <c r="D4" t="n">
-        <v>48.77</v>
+        <v>48.52</v>
       </c>
       <c r="E4" t="n">
-        <v>17.98</v>
+        <v>17.15</v>
       </c>
       <c r="F4" t="n">
-        <v>79.06</v>
+        <v>79.21</v>
       </c>
     </row>
     <row r="5">
@@ -2581,13 +2581,13 @@
         <v>12</v>
       </c>
       <c r="D5" t="n">
-        <v>32.88</v>
+        <v>32.61</v>
       </c>
       <c r="E5" t="n">
-        <v>2.52</v>
+        <v>3.07</v>
       </c>
       <c r="F5" t="n">
-        <v>62.85</v>
+        <v>63.16</v>
       </c>
     </row>
     <row r="6">
@@ -2601,13 +2601,13 @@
         <v>12</v>
       </c>
       <c r="D6" t="n">
-        <v>78.09</v>
+        <v>155.21</v>
       </c>
       <c r="E6" t="n">
-        <v>46.98</v>
+        <v>122.77</v>
       </c>
       <c r="F6" t="n">
-        <v>108.9</v>
+        <v>186.81</v>
       </c>
     </row>
     <row r="7">
@@ -2621,13 +2621,13 @@
         <v>12</v>
       </c>
       <c r="D7" t="n">
-        <v>155.02</v>
+        <v>77.84</v>
       </c>
       <c r="E7" t="n">
-        <v>123.15</v>
+        <v>46.62</v>
       </c>
       <c r="F7" t="n">
-        <v>185.6</v>
+        <v>108.58</v>
       </c>
     </row>
     <row r="8">
@@ -2641,13 +2641,13 @@
         <v>13</v>
       </c>
       <c r="D8" t="n">
-        <v>83.8</v>
+        <v>83.24</v>
       </c>
       <c r="E8" t="n">
-        <v>54.26</v>
+        <v>53.49</v>
       </c>
       <c r="F8" t="n">
-        <v>112.09</v>
+        <v>114.4</v>
       </c>
     </row>
     <row r="9">
@@ -2661,13 +2661,13 @@
         <v>12</v>
       </c>
       <c r="D9" t="n">
-        <v>82.13</v>
+        <v>82.41</v>
       </c>
       <c r="E9" t="n">
-        <v>52.64</v>
+        <v>51.78</v>
       </c>
       <c r="F9" t="n">
-        <v>112.24</v>
+        <v>113.66</v>
       </c>
     </row>
     <row r="10">
@@ -2681,13 +2681,13 @@
         <v>16</v>
       </c>
       <c r="D10" t="n">
-        <v>186.56</v>
+        <v>185.93</v>
       </c>
       <c r="E10" t="n">
-        <v>157.46</v>
+        <v>157.24</v>
       </c>
       <c r="F10" t="n">
-        <v>214.7</v>
+        <v>214.55</v>
       </c>
     </row>
     <row r="11">
@@ -2701,13 +2701,13 @@
         <v>9</v>
       </c>
       <c r="D11" t="n">
-        <v>120.87</v>
+        <v>120.37</v>
       </c>
       <c r="E11" t="n">
-        <v>86.12</v>
+        <v>85.65</v>
       </c>
       <c r="F11" t="n">
-        <v>156.21</v>
+        <v>154.64</v>
       </c>
     </row>
     <row r="12">
@@ -2721,13 +2721,13 @@
         <v>16</v>
       </c>
       <c r="D12" t="n">
-        <v>78.92</v>
+        <v>78.53</v>
       </c>
       <c r="E12" t="n">
-        <v>50.45</v>
+        <v>51.36</v>
       </c>
       <c r="F12" t="n">
-        <v>107.95</v>
+        <v>106.93</v>
       </c>
     </row>
     <row r="13">
@@ -2741,13 +2741,13 @@
         <v>8</v>
       </c>
       <c r="D13" t="n">
-        <v>-1.6</v>
+        <v>-1.42</v>
       </c>
       <c r="E13" t="n">
-        <v>-37.38</v>
+        <v>-37.11</v>
       </c>
       <c r="F13" t="n">
-        <v>34.54</v>
+        <v>34.23</v>
       </c>
     </row>
     <row r="14">
@@ -2758,16 +2758,16 @@
         <v>11</v>
       </c>
       <c r="C14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D14" t="n">
-        <v>26.31</v>
+        <v>161.17</v>
       </c>
       <c r="E14" t="n">
-        <v>-13.62</v>
+        <v>118.71</v>
       </c>
       <c r="F14" t="n">
-        <v>66.76</v>
+        <v>202.49</v>
       </c>
     </row>
     <row r="15">
@@ -2778,16 +2778,16 @@
         <v>12</v>
       </c>
       <c r="C15" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D15" t="n">
-        <v>161.1</v>
+        <v>26.74</v>
       </c>
       <c r="E15" t="n">
-        <v>118.69</v>
+        <v>-14.58</v>
       </c>
       <c r="F15" t="n">
-        <v>203.66</v>
+        <v>66.79</v>
       </c>
     </row>
     <row r="16">
@@ -2801,13 +2801,13 @@
         <v>14</v>
       </c>
       <c r="D16" t="n">
-        <v>83.7</v>
+        <v>84.1</v>
       </c>
       <c r="E16" t="n">
-        <v>54.83</v>
+        <v>54.62</v>
       </c>
       <c r="F16" t="n">
-        <v>112.5</v>
+        <v>114.41</v>
       </c>
     </row>
     <row r="17">
@@ -2818,16 +2818,16 @@
         <v>14</v>
       </c>
       <c r="C17" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D17" t="n">
-        <v>17.8</v>
+        <v>17.96</v>
       </c>
       <c r="E17" t="n">
-        <v>-17.46</v>
+        <v>-22.3</v>
       </c>
       <c r="F17" t="n">
-        <v>55.99</v>
+        <v>58.03</v>
       </c>
     </row>
     <row r="18">
@@ -2841,13 +2841,13 @@
         <v>11</v>
       </c>
       <c r="D18" t="n">
-        <v>96.99</v>
+        <v>97.02</v>
       </c>
       <c r="E18" t="n">
-        <v>64.84</v>
+        <v>63.84</v>
       </c>
       <c r="F18" t="n">
-        <v>130.13</v>
+        <v>130.54</v>
       </c>
     </row>
     <row r="19">
@@ -2861,13 +2861,13 @@
         <v>6</v>
       </c>
       <c r="D19" t="n">
-        <v>155.8</v>
+        <v>155.01</v>
       </c>
       <c r="E19" t="n">
-        <v>116.69</v>
+        <v>116.85</v>
       </c>
       <c r="F19" t="n">
-        <v>193.74</v>
+        <v>192.29</v>
       </c>
     </row>
     <row r="20">
@@ -2881,13 +2881,13 @@
         <v>12</v>
       </c>
       <c r="D20" t="n">
-        <v>15.6</v>
+        <v>15.56</v>
       </c>
       <c r="E20" t="n">
-        <v>-16.92</v>
+        <v>-18.42</v>
       </c>
       <c r="F20" t="n">
-        <v>47.45</v>
+        <v>45.96</v>
       </c>
     </row>
     <row r="21">
@@ -2901,13 +2901,13 @@
         <v>4</v>
       </c>
       <c r="D21" t="n">
-        <v>61.57</v>
+        <v>61.04</v>
       </c>
       <c r="E21" t="n">
-        <v>19.84</v>
+        <v>19.29</v>
       </c>
       <c r="F21" t="n">
-        <v>101.9</v>
+        <v>101.45</v>
       </c>
     </row>
     <row r="22">
@@ -2918,16 +2918,16 @@
         <v>11</v>
       </c>
       <c r="C22" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D22" t="n">
-        <v>52.42</v>
+        <v>64.66</v>
       </c>
       <c r="E22" t="n">
-        <v>15.21</v>
+        <v>33.23</v>
       </c>
       <c r="F22" t="n">
-        <v>88.19</v>
+        <v>97.25</v>
       </c>
     </row>
     <row r="23">
@@ -2938,16 +2938,16 @@
         <v>12</v>
       </c>
       <c r="C23" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D23" t="n">
-        <v>64.58</v>
+        <v>51.82</v>
       </c>
       <c r="E23" t="n">
-        <v>33.39</v>
+        <v>15.19</v>
       </c>
       <c r="F23" t="n">
-        <v>95.25</v>
+        <v>89.83</v>
       </c>
     </row>
     <row r="24">
@@ -2961,13 +2961,13 @@
         <v>10</v>
       </c>
       <c r="D24" t="n">
-        <v>33.03</v>
+        <v>33.69</v>
       </c>
       <c r="E24" t="n">
-        <v>-0.94</v>
+        <v>1.31</v>
       </c>
       <c r="F24" t="n">
-        <v>66.96</v>
+        <v>67.61</v>
       </c>
     </row>
     <row r="25">
@@ -2981,13 +2981,13 @@
         <v>9</v>
       </c>
       <c r="D25" t="n">
-        <v>95.56</v>
+        <v>96.83</v>
       </c>
       <c r="E25" t="n">
-        <v>61.63</v>
+        <v>62.24</v>
       </c>
       <c r="F25" t="n">
-        <v>129.07</v>
+        <v>133.28</v>
       </c>
     </row>
   </sheetData>
@@ -3002,7 +3002,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
     <col min="1" max="1" width="7.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="9.71" hidden="0" customWidth="1"/>
@@ -3045,10 +3045,10 @@
         <v>2.02</v>
       </c>
       <c r="E2" t="n">
-        <v>1.62</v>
+        <v>1.61</v>
       </c>
       <c r="F2" t="n">
-        <v>2.42</v>
+        <v>2.43</v>
       </c>
     </row>
     <row r="3">
@@ -3068,7 +3068,7 @@
         <v>1.21</v>
       </c>
       <c r="F3" t="n">
-        <v>2.03</v>
+        <v>2.04</v>
       </c>
     </row>
     <row r="4">
@@ -3105,10 +3105,10 @@
         <v>1.53</v>
       </c>
       <c r="E5" t="n">
-        <v>1.18</v>
+        <v>1.17</v>
       </c>
       <c r="F5" t="n">
-        <v>1.88</v>
+        <v>1.89</v>
       </c>
     </row>
     <row r="6">
@@ -3122,13 +3122,13 @@
         <v>12</v>
       </c>
       <c r="D6" t="n">
-        <v>1.58</v>
+        <v>2.02</v>
       </c>
       <c r="E6" t="n">
-        <v>1.21</v>
+        <v>1.65</v>
       </c>
       <c r="F6" t="n">
-        <v>1.95</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="7">
@@ -3142,13 +3142,13 @@
         <v>12</v>
       </c>
       <c r="D7" t="n">
-        <v>2.03</v>
+        <v>1.58</v>
       </c>
       <c r="E7" t="n">
-        <v>1.66</v>
+        <v>1.21</v>
       </c>
       <c r="F7" t="n">
-        <v>2.4</v>
+        <v>1.95</v>
       </c>
     </row>
     <row r="8">
@@ -3165,10 +3165,10 @@
         <v>2.06</v>
       </c>
       <c r="E8" t="n">
-        <v>1.71</v>
+        <v>1.7</v>
       </c>
       <c r="F8" t="n">
-        <v>2.42</v>
+        <v>2.41</v>
       </c>
     </row>
     <row r="9">
@@ -3182,7 +3182,7 @@
         <v>12</v>
       </c>
       <c r="D9" t="n">
-        <v>1.66</v>
+        <v>1.65</v>
       </c>
       <c r="E9" t="n">
         <v>1.29</v>
@@ -3202,13 +3202,13 @@
         <v>16</v>
       </c>
       <c r="D10" t="n">
-        <v>1.59</v>
+        <v>1.6</v>
       </c>
       <c r="E10" t="n">
         <v>1.25</v>
       </c>
       <c r="F10" t="n">
-        <v>1.93</v>
+        <v>1.94</v>
       </c>
     </row>
     <row r="11">
@@ -3228,7 +3228,7 @@
         <v>0.58</v>
       </c>
       <c r="F11" t="n">
-        <v>1.33</v>
+        <v>1.35</v>
       </c>
     </row>
     <row r="12">
@@ -3242,13 +3242,13 @@
         <v>15</v>
       </c>
       <c r="D12" t="n">
-        <v>1.27</v>
+        <v>1.28</v>
       </c>
       <c r="E12" t="n">
-        <v>0.9</v>
+        <v>0.92</v>
       </c>
       <c r="F12" t="n">
-        <v>1.62</v>
+        <v>1.64</v>
       </c>
     </row>
     <row r="13">
@@ -3265,10 +3265,10 @@
         <v>0.6</v>
       </c>
       <c r="E13" t="n">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
       <c r="F13" t="n">
-        <v>0.98</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="14">
@@ -3282,13 +3282,13 @@
         <v>5</v>
       </c>
       <c r="D14" t="n">
-        <v>0.71</v>
+        <v>1.39</v>
       </c>
       <c r="E14" t="n">
-        <v>0.17</v>
+        <v>0.84</v>
       </c>
       <c r="F14" t="n">
-        <v>1.27</v>
+        <v>1.94</v>
       </c>
     </row>
     <row r="15">
@@ -3302,13 +3302,13 @@
         <v>5</v>
       </c>
       <c r="D15" t="n">
-        <v>1.38</v>
+        <v>0.71</v>
       </c>
       <c r="E15" t="n">
-        <v>0.83</v>
+        <v>0.14</v>
       </c>
       <c r="F15" t="n">
-        <v>1.95</v>
+        <v>1.27</v>
       </c>
     </row>
     <row r="16">
@@ -3325,7 +3325,7 @@
         <v>1.23</v>
       </c>
       <c r="E16" t="n">
-        <v>0.86</v>
+        <v>0.82</v>
       </c>
       <c r="F16" t="n">
         <v>1.62</v>
@@ -3339,16 +3339,16 @@
         <v>14</v>
       </c>
       <c r="C17" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D17" t="n">
         <v>0.56</v>
       </c>
       <c r="E17" t="n">
-        <v>0.16</v>
+        <v>0.11</v>
       </c>
       <c r="F17" t="n">
-        <v>0.97</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -3365,10 +3365,10 @@
         <v>1.26</v>
       </c>
       <c r="E18" t="n">
-        <v>0.83</v>
+        <v>0.84</v>
       </c>
       <c r="F18" t="n">
-        <v>1.68</v>
+        <v>1.69</v>
       </c>
     </row>
     <row r="19">
@@ -3385,10 +3385,10 @@
         <v>1.12</v>
       </c>
       <c r="E19" t="n">
-        <v>0.66</v>
+        <v>0.65</v>
       </c>
       <c r="F19" t="n">
-        <v>1.58</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="20">
@@ -3405,10 +3405,10 @@
         <v>0.86</v>
       </c>
       <c r="E20" t="n">
-        <v>0.42</v>
+        <v>0.41</v>
       </c>
       <c r="F20" t="n">
-        <v>1.3</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="21">
@@ -3425,10 +3425,10 @@
         <v>0.56</v>
       </c>
       <c r="E21" t="n">
-        <v>0.14</v>
+        <v>0.13</v>
       </c>
       <c r="F21" t="n">
-        <v>0.97</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="22">
@@ -3439,16 +3439,16 @@
         <v>11</v>
       </c>
       <c r="C22" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D22" t="n">
-        <v>1.13</v>
+        <v>1.26</v>
       </c>
       <c r="E22" t="n">
-        <v>0.71</v>
+        <v>0.86</v>
       </c>
       <c r="F22" t="n">
-        <v>1.56</v>
+        <v>1.66</v>
       </c>
     </row>
     <row r="23">
@@ -3459,16 +3459,16 @@
         <v>12</v>
       </c>
       <c r="C23" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D23" t="n">
-        <v>1.26</v>
+        <v>1.14</v>
       </c>
       <c r="E23" t="n">
-        <v>0.85</v>
+        <v>0.71</v>
       </c>
       <c r="F23" t="n">
-        <v>1.67</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="24">
@@ -3485,10 +3485,10 @@
         <v>0.85</v>
       </c>
       <c r="E24" t="n">
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
       <c r="F24" t="n">
-        <v>1.27</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="25">
@@ -3502,7 +3502,7 @@
         <v>9</v>
       </c>
       <c r="D25" t="n">
-        <v>0.73</v>
+        <v>0.72</v>
       </c>
       <c r="E25" t="n">
         <v>0.31</v>

</xml_diff>

<commit_message>
removed bootstrapping of each phys parameter for now
</commit_message>
<xml_diff>
--- a/Data/Supplemental/Supplemental_Tables.xlsx
+++ b/Data/Supplemental/Supplemental_Tables.xlsx
@@ -18,35 +18,44 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2_Nagelkerke</t>
+  </si>
   <si>
     <t xml:space="preserve">RMSE</t>
   </si>
   <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Model</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AIC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BIC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R2_Nagelkerke</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sigma</t>
   </si>
   <si>
+    <t xml:space="preserve">Performance_Score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">species</t>
+  </si>
+  <si>
     <t xml:space="preserve">ssid_dist_mod2</t>
   </si>
   <si>
     <t xml:space="preserve">glm</t>
   </si>
   <si>
+    <t xml:space="preserve">SSID</t>
+  </si>
+  <si>
     <t xml:space="preserve">ssid_dist_mod5</t>
   </si>
   <si>
@@ -65,6 +74,9 @@
     <t xml:space="preserve">pstr_dist_mod</t>
   </si>
   <si>
+    <t xml:space="preserve">PSTR</t>
+  </si>
+  <si>
     <t xml:space="preserve">pstr_dist_mod3</t>
   </si>
   <si>
@@ -83,6 +95,9 @@
     <t xml:space="preserve">past_dist_mod2</t>
   </si>
   <si>
+    <t xml:space="preserve">PAST</t>
+  </si>
+  <si>
     <t xml:space="preserve">past_dist_mod6</t>
   </si>
   <si>
@@ -116,15 +131,9 @@
     <t xml:space="preserve">P-value</t>
   </si>
   <si>
-    <t xml:space="preserve">species</t>
-  </si>
-  <si>
     <t xml:space="preserve">pCO2</t>
   </si>
   <si>
-    <t xml:space="preserve">SSID</t>
-  </si>
-  <si>
     <t xml:space="preserve">temperature</t>
   </si>
   <si>
@@ -135,12 +144,6 @@
   </si>
   <si>
     <t xml:space="preserve">Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PSTR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAST</t>
   </si>
   <si>
     <t xml:space="preserve">Estimate</t>
@@ -520,12 +523,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="11.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="14.71" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="5.71" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="14.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="5.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="11.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="11.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="11.71" hidden="0" customWidth="1"/>
-    <col min="6" max="6" width="13.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="13.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="11.71" hidden="0" customWidth="1"/>
     <col min="7" max="7" width="11.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
@@ -551,419 +554,533 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="n">
+        <v>254.683422784345</v>
+      </c>
+      <c r="D2" t="n">
+        <v>277.858303919708</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.289881890066827</v>
+      </c>
+      <c r="F2" t="n">
         <v>1.29262470130398</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="n">
-        <v>254.683422784345</v>
-      </c>
-      <c r="E2" t="n">
-        <v>277.858303919708</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.289881890066827</v>
       </c>
       <c r="G2" t="n">
         <v>0.649729578582662</v>
       </c>
+      <c r="H2" t="n">
+        <v>0.854745824353904</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="n">
+        <v>256.413268318287</v>
+      </c>
+      <c r="D3" t="n">
+        <v>281.905637567186</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.292761447492809</v>
+      </c>
+      <c r="F3" t="n">
         <v>1.28997214275863</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="n">
-        <v>256.413268318287</v>
-      </c>
-      <c r="E3" t="n">
-        <v>281.905637567186</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.292761447492809</v>
       </c>
       <c r="G3" t="n">
         <v>0.653598017783624</v>
       </c>
+      <c r="H3" t="n">
+        <v>0.743356910333585</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>1.33685206759309</v>
+      <c r="A4" t="s">
+        <v>13</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
+      <c r="C4" t="n">
+        <v>254.784076277884</v>
       </c>
       <c r="D4" t="n">
-        <v>254.784076277884</v>
+        <v>271.006493072638</v>
       </c>
       <c r="E4" t="n">
-        <v>271.006493072638</v>
+        <v>0.221293865819629</v>
       </c>
       <c r="F4" t="n">
-        <v>0.221293865819629</v>
+        <v>1.33685206759309</v>
       </c>
       <c r="G4" t="n">
         <v>0.660221243481209</v>
       </c>
+      <c r="H4" t="n">
+        <v>0.718856507821234</v>
+      </c>
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="n">
+        <v>256.459685216432</v>
+      </c>
+      <c r="D5" t="n">
+        <v>277.317078238259</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.248251573288632</v>
+      </c>
+      <c r="F5" t="n">
         <v>1.32703239021409</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="n">
-        <v>256.459685216432</v>
-      </c>
-      <c r="E5" t="n">
-        <v>277.317078238259</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.248251573288632</v>
       </c>
       <c r="G5" t="n">
         <v>0.660323946676384</v>
       </c>
+      <c r="H5" t="n">
+        <v>0.646792845479442</v>
+      </c>
+      <c r="I5" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="n">
+        <v>260.350380774684</v>
+      </c>
+      <c r="D6" t="n">
+        <v>295.112702477729</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.334557340572031</v>
+      </c>
+      <c r="F6" t="n">
         <v>1.25915636320845</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="n">
-        <v>260.350380774684</v>
-      </c>
-      <c r="E6" t="n">
-        <v>295.112702477729</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.334557340572031</v>
       </c>
       <c r="G6" t="n">
         <v>0.65765620578295</v>
       </c>
+      <c r="H6" t="n">
+        <v>0.552681343942572</v>
+      </c>
+      <c r="I6" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="n">
+        <v>259.428598143242</v>
+      </c>
+      <c r="D7" t="n">
+        <v>273.33352682446</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.138149690082059</v>
+      </c>
+      <c r="F7" t="n">
         <v>1.41513230209438</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="n">
-        <v>259.428598143242</v>
-      </c>
-      <c r="E7" t="n">
-        <v>273.33352682446</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.138149690082059</v>
       </c>
       <c r="G7" t="n">
         <v>0.683232758346128</v>
       </c>
+      <c r="H7" t="n">
+        <v>0.213225323112274</v>
+      </c>
+      <c r="I7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="n">
+        <v>242.516703895245</v>
+      </c>
+      <c r="D8" t="n">
+        <v>276.666695680486</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.240144603424102</v>
+      </c>
+      <c r="F8" t="n">
         <v>1.20314020794441</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="n">
-        <v>242.516703895245</v>
-      </c>
-      <c r="E8" t="n">
-        <v>276.666695680486</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.240144603424102</v>
       </c>
       <c r="G8" t="n">
         <v>0.610555511910597</v>
       </c>
+      <c r="H8" t="n">
+        <v>0.686224184930279</v>
+      </c>
+      <c r="I8" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="n">
+        <v>239.681804585509</v>
+      </c>
+      <c r="D9" t="n">
+        <v>260.171799656653</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.124866303848032</v>
+      </c>
+      <c r="F9" t="n">
         <v>1.309966507513</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="n">
-        <v>239.681804585509</v>
-      </c>
-      <c r="E9" t="n">
-        <v>260.171799656653</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.124866303848032</v>
       </c>
       <c r="G9" t="n">
         <v>0.617457697907694</v>
       </c>
+      <c r="H9" t="n">
+        <v>0.660564459335823</v>
+      </c>
+      <c r="I9" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="n">
+        <v>240.528409524339</v>
+      </c>
+      <c r="D10" t="n">
+        <v>254.188406238435</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.0263119873581479</v>
+      </c>
+      <c r="F10" t="n">
         <v>1.37956224074052</v>
-      </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" t="n">
-        <v>240.528409524339</v>
-      </c>
-      <c r="E10" t="n">
-        <v>254.188406238435</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.0263119873581479</v>
       </c>
       <c r="G10" t="n">
         <v>0.63120362432392</v>
       </c>
+      <c r="H10" t="n">
+        <v>0.394684562103032</v>
+      </c>
+      <c r="I10" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="n">
+        <v>244.192824641472</v>
+      </c>
+      <c r="D11" t="n">
+        <v>269.236151950649</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.117900592626395</v>
+      </c>
+      <c r="F11" t="n">
         <v>1.29606716762676</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" t="n">
-        <v>244.192824641472</v>
-      </c>
-      <c r="E11" t="n">
-        <v>269.236151950649</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.117900592626395</v>
       </c>
       <c r="G11" t="n">
         <v>0.629449300949665</v>
       </c>
+      <c r="H11" t="n">
+        <v>0.308605020356308</v>
+      </c>
+      <c r="I11" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="n">
+        <v>242.160356976941</v>
+      </c>
+      <c r="D12" t="n">
+        <v>258.097019810054</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.0319087109072532</v>
+      </c>
+      <c r="F12" t="n">
         <v>1.3759561794257</v>
-      </c>
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" t="n">
-        <v>242.160356976941</v>
-      </c>
-      <c r="E12" t="n">
-        <v>258.097019810054</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.0319087109072532</v>
       </c>
       <c r="G12" t="n">
         <v>0.634437089524784</v>
       </c>
+      <c r="H12" t="n">
+        <v>0.276902627614324</v>
+      </c>
+      <c r="I12" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="n">
+        <v>244.66511199227</v>
+      </c>
+      <c r="D13" t="n">
+        <v>267.431773182431</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.0833341437980105</v>
+      </c>
+      <c r="F13" t="n">
         <v>1.3463148269653</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" t="n">
-        <v>244.66511199227</v>
-      </c>
-      <c r="E13" t="n">
-        <v>267.431773182431</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0.0833341437980105</v>
       </c>
       <c r="G13" t="n">
         <v>0.634657737764423</v>
       </c>
+      <c r="H13" t="n">
+        <v>0.1731917080177</v>
+      </c>
+      <c r="I13" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="n">
+        <v>193.318428177883</v>
+      </c>
+      <c r="D14" t="n">
+        <v>213.748940856228</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.111584537214595</v>
+      </c>
+      <c r="F14" t="n">
         <v>1.16377369348989</v>
-      </c>
-      <c r="B14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" t="n">
-        <v>193.318428177883</v>
-      </c>
-      <c r="E14" t="n">
-        <v>213.748940856228</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0.111584537214595</v>
       </c>
       <c r="G14" t="n">
         <v>0.564288808324294</v>
       </c>
+      <c r="H14" t="n">
+        <v>0.621845298710502</v>
+      </c>
+      <c r="I14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="n">
+        <v>186.424963238973</v>
+      </c>
+      <c r="D15" t="n">
+        <v>198.68327084598</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.0925414249759693</v>
+      </c>
+      <c r="F15" t="n">
         <v>1.17632249621167</v>
-      </c>
-      <c r="B15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" t="n">
-        <v>186.424963238973</v>
-      </c>
-      <c r="E15" t="n">
-        <v>198.68327084598</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0.0925414249759693</v>
       </c>
       <c r="G15" t="n">
         <v>0.547211390575651</v>
       </c>
+      <c r="H15" t="n">
+        <v>0.600252768220211</v>
+      </c>
+      <c r="I15" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="n">
+        <v>195.317824385769</v>
+      </c>
+      <c r="D16" t="n">
+        <v>217.791388331949</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.111594810139725</v>
+      </c>
+      <c r="F16" t="n">
         <v>1.16372456501238</v>
-      </c>
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" t="n">
-        <v>195.317824385769</v>
-      </c>
-      <c r="E16" t="n">
-        <v>217.791388331949</v>
-      </c>
-      <c r="F16" t="n">
-        <v>0.111594810139725</v>
       </c>
       <c r="G16" t="n">
         <v>0.570257392773385</v>
       </c>
+      <c r="H16" t="n">
+        <v>0.539344875545181</v>
+      </c>
+      <c r="I16" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" t="n">
+        <v>188.393667538143</v>
+      </c>
+      <c r="D17" t="n">
+        <v>202.695026412985</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.0930860104824456</v>
+      </c>
+      <c r="F17" t="n">
         <v>1.17634434601149</v>
-      </c>
-      <c r="B17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" t="n">
-        <v>188.393667538143</v>
-      </c>
-      <c r="E17" t="n">
-        <v>202.695026412985</v>
-      </c>
-      <c r="F17" t="n">
-        <v>0.0930860104824456</v>
       </c>
       <c r="G17" t="n">
         <v>0.55240505389221</v>
       </c>
+      <c r="H17" t="n">
+        <v>0.525677581296886</v>
+      </c>
+      <c r="I17" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="n">
+        <v>192.025100558009</v>
+      </c>
+      <c r="D18" t="n">
+        <v>210.41256196852</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.099473145045119</v>
+      </c>
+      <c r="F18" t="n">
         <v>1.17065362639906</v>
-      </c>
-      <c r="B18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" t="n">
-        <v>192.025100558009</v>
-      </c>
-      <c r="E18" t="n">
-        <v>210.41256196852</v>
-      </c>
-      <c r="F18" t="n">
-        <v>0.099473145045119</v>
       </c>
       <c r="G18" t="n">
         <v>0.561825067112333</v>
       </c>
+      <c r="H18" t="n">
+        <v>0.496429873061618</v>
+      </c>
+      <c r="I18" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="n">
+        <v>200.974454563788</v>
+      </c>
+      <c r="D19" t="n">
+        <v>229.577172313472</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.117416265544572</v>
+      </c>
+      <c r="F19" t="n">
         <v>1.15905593863403</v>
-      </c>
-      <c r="B19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" t="n">
-        <v>200.974454563788</v>
-      </c>
-      <c r="E19" t="n">
-        <v>229.577172313472</v>
-      </c>
-      <c r="F19" t="n">
-        <v>0.117416265544572</v>
       </c>
       <c r="G19" t="n">
         <v>0.587679914119203</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="I19" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -991,30 +1108,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="G1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -1032,12 +1149,12 @@
         <v>0.00067</v>
       </c>
       <c r="G2" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -1055,12 +1172,12 @@
         <v>0.00533</v>
       </c>
       <c r="G3" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -1078,12 +1195,12 @@
         <v>0.00333</v>
       </c>
       <c r="G4" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B5" t="n">
         <v>80</v>
@@ -1097,12 +1214,12 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B6" t="n">
         <v>85</v>
@@ -1116,12 +1233,12 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B7" t="n">
         <v>1</v>
@@ -1139,12 +1256,12 @@
         <v>0.00067</v>
       </c>
       <c r="G7" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B8" t="n">
         <v>3</v>
@@ -1162,12 +1279,12 @@
         <v>0.002</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B9" t="n">
         <v>1</v>
@@ -1185,12 +1302,12 @@
         <v>0.00067</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B10" t="n">
         <v>71</v>
@@ -1204,12 +1321,12 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B11" t="n">
         <v>76</v>
@@ -1223,12 +1340,12 @@
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B12" t="n">
         <v>1</v>
@@ -1246,12 +1363,12 @@
         <v>0.81945</v>
       </c>
       <c r="G12" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B13" t="n">
         <v>1</v>
@@ -1269,12 +1386,12 @@
         <v>0.00067</v>
       </c>
       <c r="G13" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B14" t="n">
         <v>3</v>
@@ -1292,12 +1409,12 @@
         <v>0.00067</v>
       </c>
       <c r="G14" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B15" t="n">
         <v>62</v>
@@ -1311,12 +1428,12 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B16" t="n">
         <v>67</v>
@@ -1330,7 +1447,7 @@
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1357,27 +1474,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B2" t="n">
         <v>0.754</v>
@@ -1392,12 +1509,12 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B3" t="n">
         <v>-0.204</v>
@@ -1412,12 +1529,12 @@
         <v>0.016</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B4" t="n">
         <v>-0.117</v>
@@ -1432,12 +1549,12 @@
         <v>0.429</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B5" t="n">
         <v>-0.135</v>
@@ -1452,12 +1569,12 @@
         <v>0.458</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B6" t="n">
         <v>-0.128</v>
@@ -1472,12 +1589,12 @@
         <v>0.335</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B7" t="n">
         <v>-0.029</v>
@@ -1492,12 +1609,12 @@
         <v>0.735</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B8" t="n">
         <v>0.302</v>
@@ -1512,12 +1629,12 @@
         <v>0.039</v>
       </c>
       <c r="F8" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B9" t="n">
         <v>-0.243</v>
@@ -1532,12 +1649,12 @@
         <v>0.151</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B10" t="n">
         <v>-0.043</v>
@@ -1552,12 +1669,12 @@
         <v>0.743</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B11" t="n">
         <v>0.844</v>
@@ -1572,12 +1689,12 @@
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B12" t="n">
         <v>0.043</v>
@@ -1592,12 +1709,12 @@
         <v>0.565</v>
       </c>
       <c r="F12" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B13" t="n">
         <v>0.086</v>
@@ -1612,12 +1729,12 @@
         <v>0.508</v>
       </c>
       <c r="F13" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B14" t="n">
         <v>0.071</v>
@@ -1632,12 +1749,12 @@
         <v>0.76</v>
       </c>
       <c r="F14" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B15" t="n">
         <v>-0.11</v>
@@ -1652,12 +1769,12 @@
         <v>0.438</v>
       </c>
       <c r="F15" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B16" t="n">
         <v>-0.035</v>
@@ -1672,12 +1789,12 @@
         <v>0.673</v>
       </c>
       <c r="F16" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B17" t="n">
         <v>0.86</v>
@@ -1692,12 +1809,12 @@
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B18" t="n">
         <v>-0.012</v>
@@ -1712,12 +1829,12 @@
         <v>0.863</v>
       </c>
       <c r="F18" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B19" t="n">
         <v>-0.043</v>
@@ -1732,12 +1849,12 @@
         <v>0.723</v>
       </c>
       <c r="F19" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B20" t="n">
         <v>-0.21</v>
@@ -1752,12 +1869,12 @@
         <v>0.263</v>
       </c>
       <c r="F20" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B21" t="n">
         <v>0.086</v>
@@ -1772,12 +1889,12 @@
         <v>0.463</v>
       </c>
       <c r="F21" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B22" t="n">
         <v>-0.151</v>
@@ -1792,7 +1909,7 @@
         <v>0.061</v>
       </c>
       <c r="F22" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1819,27 +1936,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B2" t="n">
         <v>2.79</v>
@@ -1854,12 +1971,12 @@
         <v>0.02</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B3" t="n">
         <v>4.36</v>
@@ -1874,12 +1991,12 @@
         <v>0.03</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B4" t="n">
         <v>0.05</v>
@@ -1894,12 +2011,12 @@
         <v>0.74</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B5" t="n">
         <v>2.21</v>
@@ -1914,12 +2031,12 @@
         <v>0.2</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B6" t="n">
         <v>30.45</v>
@@ -1930,12 +2047,12 @@
       <c r="D6"/>
       <c r="E6"/>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B7" t="n">
         <v>0.13</v>
@@ -1950,12 +2067,12 @@
         <v>0.57</v>
       </c>
       <c r="F7" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B8" t="n">
         <v>0.48</v>
@@ -1970,12 +2087,12 @@
         <v>0.75</v>
       </c>
       <c r="F8" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B9" t="n">
         <v>0.07</v>
@@ -1990,12 +2107,12 @@
         <v>0.68</v>
       </c>
       <c r="F9" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B10" t="n">
         <v>25.8</v>
@@ -2006,12 +2123,12 @@
       <c r="D10"/>
       <c r="E10"/>
       <c r="F10" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B11" t="n">
         <v>0.01</v>
@@ -2026,12 +2143,12 @@
         <v>0.86</v>
       </c>
       <c r="F11" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B12" t="n">
         <v>0.67</v>
@@ -2046,12 +2163,12 @@
         <v>0.49</v>
       </c>
       <c r="F12" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B13" t="n">
         <v>1.04</v>
@@ -2066,12 +2183,12 @@
         <v>0.06</v>
       </c>
       <c r="F13" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B14" t="n">
         <v>13.9</v>
@@ -2082,7 +2199,7 @@
       <c r="D14"/>
       <c r="E14"/>
       <c r="F14" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -2109,27 +2226,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -2149,7 +2266,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -2169,7 +2286,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -2189,7 +2306,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B5" t="n">
         <v>1</v>
@@ -2209,7 +2326,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B6" t="n">
         <v>37</v>
@@ -2225,7 +2342,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B7" t="n">
         <v>43</v>
@@ -2262,24 +2379,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B2" t="n">
         <v>0.815</v>
@@ -2296,7 +2413,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B3" t="n">
         <v>-0.212</v>
@@ -2313,7 +2430,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B4" t="n">
         <v>0.277</v>
@@ -2330,7 +2447,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B5" t="n">
         <v>-0.332</v>
@@ -2347,7 +2464,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B6" t="n">
         <v>0.034</v>
@@ -2364,7 +2481,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B7" t="n">
         <v>-0.214</v>
@@ -2402,24 +2519,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B2" t="n">
         <v>2.83</v>
@@ -2436,7 +2553,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B3" t="n">
         <v>0.04</v>
@@ -2453,7 +2570,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B4" t="n">
         <v>1.42</v>
@@ -2470,7 +2587,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B5" t="n">
         <v>11.05</v>

</xml_diff>

<commit_message>
new markdown for holobiont phys only manuscript
</commit_message>
<xml_diff>
--- a/Data/Supplemental/Supplemental_Tables.xlsx
+++ b/Data/Supplemental/Supplemental_Tables.xlsx
@@ -10,15 +10,12 @@
     <sheet name="Table S2 - PERMANOVA all" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Table S3 - Plasticity GLM" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Table S4 - Plasticity ANOVA" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Table S5 - SSID PERMANOVA" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Table S6 - SSID plasticity GLM" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Table S7 - SSID plast ANOVA" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -186,12 +183,6 @@
   </si>
   <si>
     <t xml:space="preserve">Residuals</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dominant symbiont</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dominant symbiont (D)</t>
   </si>
 </sst>
 </file>
@@ -2206,400 +2197,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
-  <cols>
-    <col min="1" max="1" width="17.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="3.71" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="14.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="5.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="5.71" hidden="0" customWidth="1"/>
-    <col min="6" max="6" width="7.71" hidden="0" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" t="n">
-        <v>3</v>
-      </c>
-      <c r="C2" t="n">
-        <v>60040</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.261</v>
-      </c>
-      <c r="E2" t="n">
-        <v>7.99</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.00067</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="n">
-        <v>13659</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.059</v>
-      </c>
-      <c r="E3" t="n">
-        <v>5.45</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.00466</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" t="n">
-        <v>18472</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="E4" t="n">
-        <v>7.38</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.002</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="n">
-        <v>44886</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.195</v>
-      </c>
-      <c r="E5" t="n">
-        <v>17.92</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.00067</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" t="n">
-        <v>37</v>
-      </c>
-      <c r="C6" t="n">
-        <v>92656</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.403</v>
-      </c>
-      <c r="E6"/>
-      <c r="F6"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" t="n">
-        <v>43</v>
-      </c>
-      <c r="C7" t="n">
-        <v>229711</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7"/>
-      <c r="F7"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
-  <cols>
-    <col min="1" max="1" width="21.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="8.71" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="14.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="9.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="7.71" hidden="0" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0.815</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.108</v>
-      </c>
-      <c r="D2" t="n">
-        <v>7.58</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" t="n">
-        <v>-0.212</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.162</v>
-      </c>
-      <c r="D3" t="n">
-        <v>-1.3</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.201</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0.277</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.207</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1.34</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.19</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" t="n">
-        <v>-0.332</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.148</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-2.24</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.032</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0.034</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.102</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.34</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.737</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7" t="n">
-        <v>-0.214</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.105</v>
-      </c>
-      <c r="D7" t="n">
-        <v>-2.03</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.05</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
-  <cols>
-    <col min="1" max="1" width="17.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="14.71" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="3.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="8.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="7.71" hidden="0" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" t="n">
-        <v>2.83</v>
-      </c>
-      <c r="C2" t="n">
-        <v>3</v>
-      </c>
-      <c r="D2" t="n">
-        <v>2.9</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.74</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" t="n">
-        <v>1.42</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" t="n">
-        <v>11.05</v>
-      </c>
-      <c r="C5" t="n">
-        <v>34</v>
-      </c>
-      <c r="D5"/>
-      <c r="E5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
final table S2 formatting
</commit_message>
<xml_diff>
--- a/Data/Supplemental/Supplemental_Tables.xlsx
+++ b/Data/Supplemental/Supplemental_Tables.xlsx
@@ -15,9 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
-  <si>
-    <t xml:space="preserve">Name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+  <si>
+    <t xml:space="preserve">Species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model formula</t>
   </si>
   <si>
     <t xml:space="preserve">Model</t>
@@ -29,7 +32,7 @@
     <t xml:space="preserve">BIC</t>
   </si>
   <si>
-    <t xml:space="preserve">R2_Nagelkerke</t>
+    <t xml:space="preserve">Nagelkerke R2</t>
   </si>
   <si>
     <t xml:space="preserve">RMSE</t>
@@ -38,109 +41,82 @@
     <t xml:space="preserve">Sigma</t>
   </si>
   <si>
-    <t xml:space="preserve">Performance_Score</t>
+    <t xml:space="preserve">Performance score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ssid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reef environment * pCO2 + temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">glm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reef environment * (pCO2 + temperature)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reef environment + pCO2 + temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reef environment + pCO2 * temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reef environment * pCO2 * temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pCO2 + temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pstr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">past</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Df</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sum of Squares</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P-value</t>
   </si>
   <si>
     <t xml:space="preserve">species</t>
   </si>
   <si>
-    <t xml:space="preserve">ssid_dist_mod2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">glm</t>
+    <t xml:space="preserve">pCO2</t>
   </si>
   <si>
     <t xml:space="preserve">SSID</t>
   </si>
   <si>
-    <t xml:space="preserve">ssid_dist_mod5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ssid_dist_mod4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ssid_dist_mod3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ssid_dist_mod</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ssid_dist_mod6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pstr_dist_mod</t>
+    <t xml:space="preserve">temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reef environment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total</t>
   </si>
   <si>
     <t xml:space="preserve">PSTR</t>
   </si>
   <si>
-    <t xml:space="preserve">pstr_dist_mod3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pstr_dist_mod6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pstr_dist_mod5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pstr_dist_mod4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pstr_dist_mod2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">past_dist_mod2</t>
-  </si>
-  <si>
     <t xml:space="preserve">PAST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">past_dist_mod6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">past_dist_mod5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">past_dist_mod4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">past_dist_mod3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">past_dist_mod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Df</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sum of Squares</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P-value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pCO2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reef environment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total</t>
   </si>
   <si>
     <t xml:space="preserve">Estimate</t>
@@ -514,12 +490,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="14.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="5.71" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="11.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="11.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="13.71" hidden="0" customWidth="1"/>
-    <col min="6" max="6" width="11.71" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="7.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="39.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="5.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="6.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="6.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="13.71" hidden="0" customWidth="1"/>
     <col min="7" max="7" width="11.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
@@ -559,171 +535,171 @@
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="n">
-        <v>254.683422784345</v>
+      <c r="C2" t="s">
+        <v>11</v>
       </c>
       <c r="D2" t="n">
-        <v>277.858303919708</v>
+        <v>254.68</v>
       </c>
       <c r="E2" t="n">
-        <v>0.289881890066827</v>
+        <v>277.86</v>
       </c>
       <c r="F2" t="n">
+        <v>0.2899</v>
+      </c>
+      <c r="G2" t="n">
         <v>1.29262470130398</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>0.649729578582662</v>
       </c>
-      <c r="H2" t="n">
-        <v>0.854745824353904</v>
-      </c>
-      <c r="I2" t="s">
-        <v>11</v>
+      <c r="I2" t="n">
+        <v>85.5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="n">
-        <v>256.413268318287</v>
+      <c r="C3" t="s">
+        <v>11</v>
       </c>
       <c r="D3" t="n">
-        <v>281.905637567186</v>
+        <v>256.41</v>
       </c>
       <c r="E3" t="n">
-        <v>0.292761447492809</v>
+        <v>281.91</v>
       </c>
       <c r="F3" t="n">
+        <v>0.2928</v>
+      </c>
+      <c r="G3" t="n">
         <v>1.28997214275863</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>0.653598017783624</v>
       </c>
-      <c r="H3" t="n">
-        <v>0.743356910333585</v>
-      </c>
-      <c r="I3" t="s">
-        <v>11</v>
+      <c r="I3" t="n">
+        <v>74.3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="n">
-        <v>254.784076277884</v>
+      <c r="C4" t="s">
+        <v>11</v>
       </c>
       <c r="D4" t="n">
-        <v>271.006493072638</v>
+        <v>254.78</v>
       </c>
       <c r="E4" t="n">
-        <v>0.221293865819629</v>
+        <v>271.01</v>
       </c>
       <c r="F4" t="n">
+        <v>0.2213</v>
+      </c>
+      <c r="G4" t="n">
         <v>1.33685206759309</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>0.660221243481209</v>
       </c>
-      <c r="H4" t="n">
-        <v>0.718856507821234</v>
-      </c>
-      <c r="I4" t="s">
-        <v>11</v>
+      <c r="I4" t="n">
+        <v>71.9</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="n">
-        <v>256.459685216432</v>
+      <c r="C5" t="s">
+        <v>11</v>
       </c>
       <c r="D5" t="n">
-        <v>277.317078238259</v>
+        <v>256.46</v>
       </c>
       <c r="E5" t="n">
-        <v>0.248251573288632</v>
+        <v>277.32</v>
       </c>
       <c r="F5" t="n">
+        <v>0.2483</v>
+      </c>
+      <c r="G5" t="n">
         <v>1.32703239021409</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>0.660323946676384</v>
       </c>
-      <c r="H5" t="n">
-        <v>0.646792845479442</v>
-      </c>
-      <c r="I5" t="s">
-        <v>11</v>
+      <c r="I5" t="n">
+        <v>64.7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="n">
-        <v>260.350380774684</v>
+      <c r="C6" t="s">
+        <v>11</v>
       </c>
       <c r="D6" t="n">
-        <v>295.112702477729</v>
+        <v>260.35</v>
       </c>
       <c r="E6" t="n">
-        <v>0.334557340572031</v>
+        <v>295.11</v>
       </c>
       <c r="F6" t="n">
+        <v>0.3346</v>
+      </c>
+      <c r="G6" t="n">
         <v>1.25915636320845</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>0.65765620578295</v>
       </c>
-      <c r="H6" t="n">
-        <v>0.552681343942572</v>
-      </c>
-      <c r="I6" t="s">
-        <v>11</v>
+      <c r="I6" t="n">
+        <v>55.3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="n">
-        <v>259.428598143242</v>
+      <c r="C7" t="s">
+        <v>11</v>
       </c>
       <c r="D7" t="n">
-        <v>273.33352682446</v>
+        <v>259.43</v>
       </c>
       <c r="E7" t="n">
-        <v>0.138149690082059</v>
+        <v>273.33</v>
       </c>
       <c r="F7" t="n">
+        <v>0.1381</v>
+      </c>
+      <c r="G7" t="n">
         <v>1.41513230209438</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>0.683232758346128</v>
       </c>
-      <c r="H7" t="n">
-        <v>0.213225323112274</v>
-      </c>
-      <c r="I7" t="s">
-        <v>11</v>
+      <c r="I7" t="n">
+        <v>21.3</v>
       </c>
     </row>
     <row r="8">
@@ -731,347 +707,347 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="n">
-        <v>242.516703895245</v>
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
       </c>
       <c r="D8" t="n">
-        <v>276.666695680486</v>
+        <v>242.52</v>
       </c>
       <c r="E8" t="n">
-        <v>0.240144603424102</v>
+        <v>276.67</v>
       </c>
       <c r="F8" t="n">
+        <v>0.2401</v>
+      </c>
+      <c r="G8" t="n">
         <v>1.20314020794441</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>0.610555511910597</v>
       </c>
-      <c r="H8" t="n">
-        <v>0.686224184930279</v>
-      </c>
-      <c r="I8" t="s">
-        <v>18</v>
+      <c r="I8" t="n">
+        <v>68.6</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="n">
-        <v>239.681804585509</v>
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
       </c>
       <c r="D9" t="n">
-        <v>260.171799656653</v>
+        <v>239.68</v>
       </c>
       <c r="E9" t="n">
-        <v>0.124866303848032</v>
+        <v>260.17</v>
       </c>
       <c r="F9" t="n">
+        <v>0.1249</v>
+      </c>
+      <c r="G9" t="n">
         <v>1.309966507513</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>0.617457697907694</v>
       </c>
-      <c r="H9" t="n">
-        <v>0.660564459335823</v>
-      </c>
-      <c r="I9" t="s">
-        <v>18</v>
+      <c r="I9" t="n">
+        <v>66.1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="n">
-        <v>240.528409524339</v>
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
       </c>
       <c r="D10" t="n">
-        <v>254.188406238435</v>
+        <v>240.53</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0263119873581479</v>
+        <v>254.19</v>
       </c>
       <c r="F10" t="n">
+        <v>0.0263</v>
+      </c>
+      <c r="G10" t="n">
         <v>1.37956224074052</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>0.63120362432392</v>
       </c>
-      <c r="H10" t="n">
-        <v>0.394684562103032</v>
-      </c>
-      <c r="I10" t="s">
-        <v>18</v>
+      <c r="I10" t="n">
+        <v>39.5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" t="n">
-        <v>244.192824641472</v>
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
       </c>
       <c r="D11" t="n">
-        <v>269.236151950649</v>
+        <v>244.19</v>
       </c>
       <c r="E11" t="n">
-        <v>0.117900592626395</v>
+        <v>269.24</v>
       </c>
       <c r="F11" t="n">
+        <v>0.1179</v>
+      </c>
+      <c r="G11" t="n">
         <v>1.29606716762676</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>0.629449300949665</v>
       </c>
-      <c r="H11" t="n">
-        <v>0.308605020356308</v>
-      </c>
-      <c r="I11" t="s">
-        <v>18</v>
+      <c r="I11" t="n">
+        <v>30.9</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" t="n">
-        <v>242.160356976941</v>
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
       </c>
       <c r="D12" t="n">
-        <v>258.097019810054</v>
+        <v>242.16</v>
       </c>
       <c r="E12" t="n">
-        <v>0.0319087109072532</v>
+        <v>258.1</v>
       </c>
       <c r="F12" t="n">
+        <v>0.0319</v>
+      </c>
+      <c r="G12" t="n">
         <v>1.3759561794257</v>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>0.634437089524784</v>
       </c>
-      <c r="H12" t="n">
-        <v>0.276902627614324</v>
-      </c>
-      <c r="I12" t="s">
-        <v>18</v>
+      <c r="I12" t="n">
+        <v>27.7</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
-      <c r="C13" t="n">
-        <v>244.66511199227</v>
+      <c r="C13" t="s">
+        <v>11</v>
       </c>
       <c r="D13" t="n">
-        <v>267.431773182431</v>
+        <v>244.67</v>
       </c>
       <c r="E13" t="n">
-        <v>0.0833341437980105</v>
+        <v>267.43</v>
       </c>
       <c r="F13" t="n">
+        <v>0.0833</v>
+      </c>
+      <c r="G13" t="n">
         <v>1.3463148269653</v>
       </c>
-      <c r="G13" t="n">
+      <c r="H13" t="n">
         <v>0.634657737764423</v>
       </c>
-      <c r="H13" t="n">
-        <v>0.1731917080177</v>
-      </c>
-      <c r="I13" t="s">
-        <v>18</v>
+      <c r="I13" t="n">
+        <v>17.3</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
       </c>
-      <c r="C14" t="n">
-        <v>193.318428177883</v>
+      <c r="C14" t="s">
+        <v>11</v>
       </c>
       <c r="D14" t="n">
-        <v>213.748940856228</v>
+        <v>193.32</v>
       </c>
       <c r="E14" t="n">
-        <v>0.111584537214595</v>
+        <v>213.75</v>
       </c>
       <c r="F14" t="n">
+        <v>0.1116</v>
+      </c>
+      <c r="G14" t="n">
         <v>1.16377369348989</v>
       </c>
-      <c r="G14" t="n">
+      <c r="H14" t="n">
         <v>0.564288808324294</v>
       </c>
-      <c r="H14" t="n">
-        <v>0.621845298710502</v>
-      </c>
-      <c r="I14" t="s">
-        <v>25</v>
+      <c r="I14" t="n">
+        <v>62.2</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" t="n">
-        <v>186.424963238973</v>
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
       </c>
       <c r="D15" t="n">
-        <v>198.68327084598</v>
+        <v>186.42</v>
       </c>
       <c r="E15" t="n">
-        <v>0.0925414249759693</v>
+        <v>198.68</v>
       </c>
       <c r="F15" t="n">
+        <v>0.0925</v>
+      </c>
+      <c r="G15" t="n">
         <v>1.17632249621167</v>
       </c>
-      <c r="G15" t="n">
+      <c r="H15" t="n">
         <v>0.547211390575651</v>
       </c>
-      <c r="H15" t="n">
-        <v>0.600252768220211</v>
-      </c>
-      <c r="I15" t="s">
-        <v>25</v>
+      <c r="I15" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" t="n">
-        <v>195.317824385769</v>
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
       </c>
       <c r="D16" t="n">
-        <v>217.791388331949</v>
+        <v>195.32</v>
       </c>
       <c r="E16" t="n">
-        <v>0.111594810139725</v>
+        <v>217.79</v>
       </c>
       <c r="F16" t="n">
+        <v>0.1116</v>
+      </c>
+      <c r="G16" t="n">
         <v>1.16372456501238</v>
       </c>
-      <c r="G16" t="n">
+      <c r="H16" t="n">
         <v>0.570257392773385</v>
       </c>
-      <c r="H16" t="n">
-        <v>0.539344875545181</v>
-      </c>
-      <c r="I16" t="s">
-        <v>25</v>
+      <c r="I16" t="n">
+        <v>53.9</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" t="n">
-        <v>188.393667538143</v>
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
       </c>
       <c r="D17" t="n">
-        <v>202.695026412985</v>
+        <v>188.39</v>
       </c>
       <c r="E17" t="n">
-        <v>0.0930860104824456</v>
+        <v>202.7</v>
       </c>
       <c r="F17" t="n">
+        <v>0.0931</v>
+      </c>
+      <c r="G17" t="n">
         <v>1.17634434601149</v>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>0.55240505389221</v>
       </c>
-      <c r="H17" t="n">
-        <v>0.525677581296886</v>
-      </c>
-      <c r="I17" t="s">
-        <v>25</v>
+      <c r="I17" t="n">
+        <v>52.6</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" t="n">
-        <v>192.025100558009</v>
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
       </c>
       <c r="D18" t="n">
-        <v>210.41256196852</v>
+        <v>192.03</v>
       </c>
       <c r="E18" t="n">
-        <v>0.099473145045119</v>
+        <v>210.41</v>
       </c>
       <c r="F18" t="n">
+        <v>0.0995</v>
+      </c>
+      <c r="G18" t="n">
         <v>1.17065362639906</v>
       </c>
-      <c r="G18" t="n">
+      <c r="H18" t="n">
         <v>0.561825067112333</v>
       </c>
-      <c r="H18" t="n">
-        <v>0.496429873061618</v>
-      </c>
-      <c r="I18" t="s">
-        <v>25</v>
+      <c r="I18" t="n">
+        <v>49.6</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" t="n">
-        <v>200.974454563788</v>
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
       </c>
       <c r="D19" t="n">
-        <v>229.577172313472</v>
+        <v>200.97</v>
       </c>
       <c r="E19" t="n">
-        <v>0.117416265544572</v>
+        <v>229.58</v>
       </c>
       <c r="F19" t="n">
+        <v>0.1174</v>
+      </c>
+      <c r="G19" t="n">
         <v>1.15905593863403</v>
       </c>
-      <c r="G19" t="n">
+      <c r="H19" t="n">
         <v>0.587679914119203</v>
       </c>
-      <c r="H19" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="I19" t="s">
-        <v>25</v>
+      <c r="I19" t="n">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1099,30 +1075,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F1" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="G1" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -1140,12 +1116,12 @@
         <v>0.00067</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -1163,12 +1139,12 @@
         <v>0.00533</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -1186,12 +1162,12 @@
         <v>0.00333</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B5" t="n">
         <v>80</v>
@@ -1205,12 +1181,12 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B6" t="n">
         <v>85</v>
@@ -1224,12 +1200,12 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B7" t="n">
         <v>1</v>
@@ -1247,12 +1223,12 @@
         <v>0.00067</v>
       </c>
       <c r="G7" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B8" t="n">
         <v>3</v>
@@ -1270,12 +1246,12 @@
         <v>0.002</v>
       </c>
       <c r="G8" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B9" t="n">
         <v>1</v>
@@ -1293,12 +1269,12 @@
         <v>0.00067</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B10" t="n">
         <v>71</v>
@@ -1312,12 +1288,12 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B11" t="n">
         <v>76</v>
@@ -1331,12 +1307,12 @@
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B12" t="n">
         <v>1</v>
@@ -1354,12 +1330,12 @@
         <v>0.81945</v>
       </c>
       <c r="G12" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B13" t="n">
         <v>1</v>
@@ -1377,12 +1353,12 @@
         <v>0.00067</v>
       </c>
       <c r="G13" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B14" t="n">
         <v>3</v>
@@ -1400,12 +1376,12 @@
         <v>0.00067</v>
       </c>
       <c r="G14" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B15" t="n">
         <v>62</v>
@@ -1419,12 +1395,12 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B16" t="n">
         <v>67</v>
@@ -1438,7 +1414,7 @@
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1465,27 +1441,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E1" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="F1" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B2" t="n">
         <v>0.754</v>
@@ -1500,12 +1476,12 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B3" t="n">
         <v>-0.204</v>
@@ -1520,12 +1496,12 @@
         <v>0.016</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B4" t="n">
         <v>-0.117</v>
@@ -1540,12 +1516,12 @@
         <v>0.429</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B5" t="n">
         <v>-0.135</v>
@@ -1560,12 +1536,12 @@
         <v>0.458</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B6" t="n">
         <v>-0.128</v>
@@ -1580,12 +1556,12 @@
         <v>0.335</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B7" t="n">
         <v>-0.029</v>
@@ -1600,12 +1576,12 @@
         <v>0.735</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B8" t="n">
         <v>0.302</v>
@@ -1620,12 +1596,12 @@
         <v>0.039</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B9" t="n">
         <v>-0.243</v>
@@ -1640,12 +1616,12 @@
         <v>0.151</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B10" t="n">
         <v>-0.043</v>
@@ -1660,12 +1636,12 @@
         <v>0.743</v>
       </c>
       <c r="F10" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B11" t="n">
         <v>0.844</v>
@@ -1680,12 +1656,12 @@
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B12" t="n">
         <v>0.043</v>
@@ -1700,12 +1676,12 @@
         <v>0.565</v>
       </c>
       <c r="F12" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B13" t="n">
         <v>0.086</v>
@@ -1720,12 +1696,12 @@
         <v>0.508</v>
       </c>
       <c r="F13" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B14" t="n">
         <v>0.071</v>
@@ -1740,12 +1716,12 @@
         <v>0.76</v>
       </c>
       <c r="F14" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B15" t="n">
         <v>-0.11</v>
@@ -1760,12 +1736,12 @@
         <v>0.438</v>
       </c>
       <c r="F15" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B16" t="n">
         <v>-0.035</v>
@@ -1780,12 +1756,12 @@
         <v>0.673</v>
       </c>
       <c r="F16" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B17" t="n">
         <v>0.86</v>
@@ -1800,12 +1776,12 @@
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B18" t="n">
         <v>-0.012</v>
@@ -1820,12 +1796,12 @@
         <v>0.863</v>
       </c>
       <c r="F18" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B19" t="n">
         <v>-0.043</v>
@@ -1840,12 +1816,12 @@
         <v>0.723</v>
       </c>
       <c r="F19" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B20" t="n">
         <v>-0.21</v>
@@ -1860,12 +1836,12 @@
         <v>0.263</v>
       </c>
       <c r="F20" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B21" t="n">
         <v>0.086</v>
@@ -1880,12 +1856,12 @@
         <v>0.463</v>
       </c>
       <c r="F21" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B22" t="n">
         <v>-0.151</v>
@@ -1900,7 +1876,7 @@
         <v>0.061</v>
       </c>
       <c r="F22" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1927,27 +1903,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E1" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="F1" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B2" t="n">
         <v>2.79</v>
@@ -1962,12 +1938,12 @@
         <v>0.02</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B3" t="n">
         <v>4.36</v>
@@ -1982,12 +1958,12 @@
         <v>0.03</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B4" t="n">
         <v>0.05</v>
@@ -2002,12 +1978,12 @@
         <v>0.74</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B5" t="n">
         <v>2.21</v>
@@ -2022,12 +1998,12 @@
         <v>0.2</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B6" t="n">
         <v>30.45</v>
@@ -2038,12 +2014,12 @@
       <c r="D6"/>
       <c r="E6"/>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B7" t="n">
         <v>0.13</v>
@@ -2058,12 +2034,12 @@
         <v>0.57</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B8" t="n">
         <v>0.48</v>
@@ -2078,12 +2054,12 @@
         <v>0.75</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B9" t="n">
         <v>0.07</v>
@@ -2098,12 +2074,12 @@
         <v>0.68</v>
       </c>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B10" t="n">
         <v>25.8</v>
@@ -2114,12 +2090,12 @@
       <c r="D10"/>
       <c r="E10"/>
       <c r="F10" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B11" t="n">
         <v>0.01</v>
@@ -2134,12 +2110,12 @@
         <v>0.86</v>
       </c>
       <c r="F11" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B12" t="n">
         <v>0.67</v>
@@ -2154,12 +2130,12 @@
         <v>0.49</v>
       </c>
       <c r="F12" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B13" t="n">
         <v>1.04</v>
@@ -2174,12 +2150,12 @@
         <v>0.06</v>
       </c>
       <c r="F13" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B14" t="n">
         <v>13.9</v>
@@ -2190,7 +2166,7 @@
       <c r="D14"/>
       <c r="E14"/>
       <c r="F14" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added PCA for species differences
</commit_message>
<xml_diff>
--- a/Data/Supplemental/Supplemental_Tables.xlsx
+++ b/Data/Supplemental/Supplemental_Tables.xlsx
@@ -1136,7 +1136,7 @@
         <v>5.7</v>
       </c>
       <c r="F3" t="n">
-        <v>0.00533</v>
+        <v>0.00733</v>
       </c>
       <c r="G3" t="s">
         <v>27</v>
@@ -1159,7 +1159,7 @@
         <v>6.1</v>
       </c>
       <c r="F4" t="n">
-        <v>0.00333</v>
+        <v>0.00933</v>
       </c>
       <c r="G4" t="s">
         <v>27</v>
@@ -1243,7 +1243,7 @@
         <v>4.42</v>
       </c>
       <c r="F8" t="n">
-        <v>0.002</v>
+        <v>0.00266</v>
       </c>
       <c r="G8" t="s">
         <v>32</v>
@@ -1327,7 +1327,7 @@
         <v>0.17</v>
       </c>
       <c r="F12" t="n">
-        <v>0.81945</v>
+        <v>0.82945</v>
       </c>
       <c r="G12" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
Figures 4 and S4 with  table S5 added
</commit_message>
<xml_diff>
--- a/Data/Supplemental/Supplemental_Tables.xlsx
+++ b/Data/Supplemental/Supplemental_Tables.xlsx
@@ -7,15 +7,16 @@
   </bookViews>
   <sheets>
     <sheet name="Table S1 - Plasticity AIC" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Table S2 - PERMANOVA all" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Table S2 - PERMANOVA" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Table S3 - Plasticity GLM" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Table S4 - Plasticity ANOVA" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Table S5 - Species PERMANOVA" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t xml:space="preserve">Species</t>
   </si>
@@ -159,6 +160,15 @@
   </si>
   <si>
     <t xml:space="preserve">Residuals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">temperature:species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pCO2:species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reef environment:species</t>
   </si>
 </sst>
 </file>
@@ -1136,7 +1146,7 @@
         <v>5.7</v>
       </c>
       <c r="F3" t="n">
-        <v>0.00733</v>
+        <v>0.00533</v>
       </c>
       <c r="G3" t="s">
         <v>27</v>
@@ -1159,7 +1169,7 @@
         <v>6.1</v>
       </c>
       <c r="F4" t="n">
-        <v>0.00933</v>
+        <v>0.00333</v>
       </c>
       <c r="G4" t="s">
         <v>27</v>
@@ -1243,7 +1253,7 @@
         <v>4.42</v>
       </c>
       <c r="F8" t="n">
-        <v>0.00266</v>
+        <v>0.002</v>
       </c>
       <c r="G8" t="s">
         <v>32</v>
@@ -1327,7 +1337,7 @@
         <v>0.17</v>
       </c>
       <c r="F12" t="n">
-        <v>0.82945</v>
+        <v>0.81945</v>
       </c>
       <c r="G12" t="s">
         <v>33</v>
@@ -2173,4 +2183,218 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <cols>
+    <col min="1" max="1" width="24.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="3.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="14.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="5.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="5.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="7.71" hidden="0" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" t="n">
+        <v>441584</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.084</v>
+      </c>
+      <c r="E2" t="n">
+        <v>14.9</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.00067</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>44470</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="E3" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.02398</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>69064</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="E4" t="n">
+        <v>6.99</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.006</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1690024</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="E5" t="n">
+        <v>85.53</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.00067</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" t="n">
+        <v>657172</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.124</v>
+      </c>
+      <c r="E6" t="n">
+        <v>33.26</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.00067</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" t="n">
+        <v>129807</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2.19</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.01999</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" t="n">
+        <v>134579</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="E8" t="n">
+        <v>6.81</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.00067</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="n">
+        <v>214</v>
+      </c>
+      <c r="C9" t="n">
+        <v>2114166</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="E9"/>
+      <c r="F9"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="n">
+        <v>231</v>
+      </c>
+      <c r="C10" t="n">
+        <v>5280867</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10"/>
+      <c r="F10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed some incorrect table labeltable labels
</commit_message>
<xml_diff>
--- a/Data/Supplemental/Supplemental_Tables.xlsx
+++ b/Data/Supplemental/Supplemental_Tables.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t xml:space="preserve">Species</t>
   </si>
@@ -141,6 +141,9 @@
     <t xml:space="preserve">pCO2-EOC</t>
   </si>
   <si>
+    <t xml:space="preserve">pCO2-extreme</t>
+  </si>
+  <si>
     <t xml:space="preserve">temperature (31C)</t>
   </si>
   <si>
@@ -150,7 +153,7 @@
     <t xml:space="preserve">reef environment (offshore):pCO2-EOC</t>
   </si>
   <si>
-    <t xml:space="preserve">reef environment (offshore):pCO2</t>
+    <t xml:space="preserve">reef environment (offshore):pCO2-extreme</t>
   </si>
   <si>
     <t xml:space="preserve">F values</t>
@@ -1551,7 +1554,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="B6" t="n">
         <v>-0.128</v>
@@ -1571,7 +1574,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B7" t="n">
         <v>-0.029</v>
@@ -1591,7 +1594,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B8" t="n">
         <v>0.302</v>
@@ -1611,7 +1614,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B9" t="n">
         <v>-0.243</v>
@@ -1631,7 +1634,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B10" t="n">
         <v>-0.043</v>
@@ -1731,7 +1734,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="B15" t="n">
         <v>-0.11</v>
@@ -1751,7 +1754,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B16" t="n">
         <v>-0.035</v>
@@ -1851,7 +1854,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="B21" t="n">
         <v>0.086</v>
@@ -1871,7 +1874,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B22" t="n">
         <v>-0.151</v>
@@ -1922,7 +1925,7 @@
         <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
         <v>24</v>
@@ -1993,7 +1996,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B5" t="n">
         <v>2.21</v>
@@ -2013,7 +2016,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B6" t="n">
         <v>30.45</v>
@@ -2089,7 +2092,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B10" t="n">
         <v>25.8</v>
@@ -2165,7 +2168,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B14" t="n">
         <v>13.9</v>
@@ -2303,7 +2306,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B6" t="n">
         <v>2</v>
@@ -2323,7 +2326,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B7" t="n">
         <v>6</v>
@@ -2343,7 +2346,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B8" t="n">
         <v>2</v>

</xml_diff>

<commit_message>
added table S6 of the host v symbiont PCAs
</commit_message>
<xml_diff>
--- a/Data/Supplemental/Supplemental_Tables.xlsx
+++ b/Data/Supplemental/Supplemental_Tables.xlsx
@@ -11,12 +11,13 @@
     <sheet name="Table S3 - Plasticity GLM" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Table S4 - Plasticity ANOVA" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Table S5 - Species PERMANOVA" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Table S6 - HostVsymb PERMANOVA" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t xml:space="preserve">Species</t>
   </si>
@@ -172,6 +173,21 @@
   </si>
   <si>
     <t xml:space="preserve">reef environment:species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Df </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sum of Squares </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">F </t>
+  </si>
+  <si>
+    <t xml:space="preserve">P-value </t>
   </si>
 </sst>
 </file>
@@ -2400,4 +2416,592 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <cols>
+    <col min="1" max="1" width="16.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="3.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="14.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="5.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="5.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="7.71" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="3.71" hidden="0" customWidth="1"/>
+    <col min="8" max="8" width="15.71" hidden="0" customWidth="1"/>
+    <col min="9" max="9" width="5.71" hidden="0" customWidth="1"/>
+    <col min="10" max="10" width="5.71" hidden="0" customWidth="1"/>
+    <col min="11" max="11" width="8.71" hidden="0" customWidth="1"/>
+    <col min="12" max="12" width="7.71" hidden="0" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.74883</v>
+      </c>
+      <c r="G2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2" t="n">
+        <v>150227</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.272</v>
+      </c>
+      <c r="J2" t="n">
+        <v>11.45</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.00067</v>
+      </c>
+      <c r="L2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.075</v>
+      </c>
+      <c r="E3" t="n">
+        <v>6.65</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" t="n">
+        <v>24933</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.045</v>
+      </c>
+      <c r="J3" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="L3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.58294</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" t="n">
+        <v>26680</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.048</v>
+      </c>
+      <c r="J4" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="L4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="n">
+        <v>80</v>
+      </c>
+      <c r="C5" t="n">
+        <v>30</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.901</v>
+      </c>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5" t="n">
+        <v>80</v>
+      </c>
+      <c r="H5" t="n">
+        <v>349805</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.634</v>
+      </c>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="n">
+        <v>85</v>
+      </c>
+      <c r="C6" t="n">
+        <v>34</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6" t="n">
+        <v>85</v>
+      </c>
+      <c r="H6" t="n">
+        <v>551646</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.041</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.28714</v>
+      </c>
+      <c r="G7" t="n">
+        <v>3</v>
+      </c>
+      <c r="H7" t="n">
+        <v>196108</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.096</v>
+      </c>
+      <c r="J7" t="n">
+        <v>4.41</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.00333</v>
+      </c>
+      <c r="L7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.147</v>
+      </c>
+      <c r="E8" t="n">
+        <v>13.12</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.00067</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" t="n">
+        <v>619660</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.304</v>
+      </c>
+      <c r="J8" t="n">
+        <v>41.82</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.00067</v>
+      </c>
+      <c r="L8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.15923</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" t="n">
+        <v>167947</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.083</v>
+      </c>
+      <c r="J9" t="n">
+        <v>11.34</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.00133</v>
+      </c>
+      <c r="L9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="n">
+        <v>71</v>
+      </c>
+      <c r="C10" t="n">
+        <v>14</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.793</v>
+      </c>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10" t="n">
+        <v>71</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1051979</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.517</v>
+      </c>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="n">
+        <v>76</v>
+      </c>
+      <c r="C11" t="n">
+        <v>18</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11" t="n">
+        <v>76</v>
+      </c>
+      <c r="H11" t="n">
+        <v>2035695</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="n">
+        <v>3</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.136</v>
+      </c>
+      <c r="E12" t="n">
+        <v>3.48</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.01865</v>
+      </c>
+      <c r="G12" t="n">
+        <v>3</v>
+      </c>
+      <c r="H12" t="n">
+        <v>100597</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.298</v>
+      </c>
+      <c r="J12" t="n">
+        <v>11.23</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.00067</v>
+      </c>
+      <c r="L12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.036</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2.76</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.1006</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" t="n">
+        <v>51174</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.151</v>
+      </c>
+      <c r="J13" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.00067</v>
+      </c>
+      <c r="L13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.021</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1.64</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.20053</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" t="n">
+        <v>969</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.68754</v>
+      </c>
+      <c r="L14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="n">
+        <v>62</v>
+      </c>
+      <c r="C15" t="n">
+        <v>10</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.807</v>
+      </c>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15" t="n">
+        <v>62</v>
+      </c>
+      <c r="H15" t="n">
+        <v>185165</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.548</v>
+      </c>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="n">
+        <v>67</v>
+      </c>
+      <c r="C16" t="n">
+        <v>13</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16" t="n">
+        <v>67</v>
+      </c>
+      <c r="H16" t="n">
+        <v>337905</v>
+      </c>
+      <c r="I16" t="n">
+        <v>1</v>
+      </c>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed chlorophyll a data
</commit_message>
<xml_diff>
--- a/Data/Supplemental/Supplemental_Tables.xlsx
+++ b/Data/Supplemental/Supplemental_Tables.xlsx
@@ -577,10 +577,10 @@
         <v>0.2899</v>
       </c>
       <c r="G2" t="n">
-        <v>1.29262470130398</v>
+        <v>1.2926268490263</v>
       </c>
       <c r="H2" t="n">
-        <v>0.649729578582662</v>
+        <v>0.649718186195778</v>
       </c>
       <c r="I2" t="n">
         <v>85.5</v>
@@ -600,16 +600,16 @@
         <v>256.41</v>
       </c>
       <c r="E3" t="n">
-        <v>281.91</v>
+        <v>281.9</v>
       </c>
       <c r="F3" t="n">
         <v>0.2928</v>
       </c>
       <c r="G3" t="n">
-        <v>1.28997214275863</v>
+        <v>1.2899740213025</v>
       </c>
       <c r="H3" t="n">
-        <v>0.653598017783624</v>
+        <v>0.653586411465873</v>
       </c>
       <c r="I3" t="n">
         <v>74.3</v>
@@ -635,10 +635,10 @@
         <v>0.2213</v>
       </c>
       <c r="G4" t="n">
-        <v>1.33685206759309</v>
+        <v>1.33685374011254</v>
       </c>
       <c r="H4" t="n">
-        <v>0.660221243481209</v>
+        <v>0.660209766997358</v>
       </c>
       <c r="I4" t="n">
         <v>71.9</v>
@@ -664,10 +664,10 @@
         <v>0.2483</v>
       </c>
       <c r="G5" t="n">
-        <v>1.32703239021409</v>
+        <v>1.32703425546414</v>
       </c>
       <c r="H5" t="n">
-        <v>0.660323946676384</v>
+        <v>0.660312676146787</v>
       </c>
       <c r="I5" t="n">
         <v>64.7</v>
@@ -693,10 +693,10 @@
         <v>0.3346</v>
       </c>
       <c r="G6" t="n">
-        <v>1.25915636320845</v>
+        <v>1.25915911436328</v>
       </c>
       <c r="H6" t="n">
-        <v>0.65765620578295</v>
+        <v>0.657644659640462</v>
       </c>
       <c r="I6" t="n">
         <v>55.3</v>
@@ -719,13 +719,13 @@
         <v>273.33</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1381</v>
+        <v>0.1382</v>
       </c>
       <c r="G7" t="n">
-        <v>1.41513230209438</v>
+        <v>1.4151360221094</v>
       </c>
       <c r="H7" t="n">
-        <v>0.683232758346128</v>
+        <v>0.683221885809563</v>
       </c>
       <c r="I7" t="n">
         <v>21.3</v>
@@ -751,10 +751,10 @@
         <v>0.2401</v>
       </c>
       <c r="G8" t="n">
-        <v>1.20314020794441</v>
+        <v>1.20315338344266</v>
       </c>
       <c r="H8" t="n">
-        <v>0.610555511910597</v>
+        <v>0.610559911143328</v>
       </c>
       <c r="I8" t="n">
         <v>68.6</v>
@@ -780,10 +780,10 @@
         <v>0.1249</v>
       </c>
       <c r="G9" t="n">
-        <v>1.309966507513</v>
+        <v>1.30997747698609</v>
       </c>
       <c r="H9" t="n">
-        <v>0.617457697907694</v>
+        <v>0.617460634216792</v>
       </c>
       <c r="I9" t="n">
         <v>66.1</v>
@@ -809,10 +809,10 @@
         <v>0.0263</v>
       </c>
       <c r="G10" t="n">
-        <v>1.37956224074052</v>
+        <v>1.37957299867158</v>
       </c>
       <c r="H10" t="n">
-        <v>0.63120362432392</v>
+        <v>0.631205876260462</v>
       </c>
       <c r="I10" t="n">
         <v>39.5</v>
@@ -838,10 +838,10 @@
         <v>0.1179</v>
       </c>
       <c r="G11" t="n">
-        <v>1.29606716762676</v>
+        <v>1.29607785162445</v>
       </c>
       <c r="H11" t="n">
-        <v>0.629449300949665</v>
+        <v>0.629451678765452</v>
       </c>
       <c r="I11" t="n">
         <v>30.9</v>
@@ -867,10 +867,10 @@
         <v>0.0319</v>
       </c>
       <c r="G12" t="n">
-        <v>1.3759561794257</v>
+        <v>1.37596637996336</v>
       </c>
       <c r="H12" t="n">
-        <v>0.634437089524784</v>
+        <v>0.634439131239188</v>
       </c>
       <c r="I12" t="n">
         <v>27.7</v>
@@ -896,10 +896,10 @@
         <v>0.0833</v>
       </c>
       <c r="G13" t="n">
-        <v>1.3463148269653</v>
+        <v>1.34632437229469</v>
       </c>
       <c r="H13" t="n">
-        <v>0.634657737764423</v>
+        <v>0.634659628138949</v>
       </c>
       <c r="I13" t="n">
         <v>17.3</v>
@@ -925,10 +925,10 @@
         <v>0.1116</v>
       </c>
       <c r="G14" t="n">
-        <v>1.16377369348989</v>
+        <v>1.16376490169629</v>
       </c>
       <c r="H14" t="n">
-        <v>0.564288808324294</v>
+        <v>0.564285238534006</v>
       </c>
       <c r="I14" t="n">
         <v>62.2</v>
@@ -954,10 +954,10 @@
         <v>0.0925</v>
       </c>
       <c r="G15" t="n">
-        <v>1.17632249621167</v>
+        <v>1.17631329356072</v>
       </c>
       <c r="H15" t="n">
-        <v>0.547211390575651</v>
+        <v>0.547207956382125</v>
       </c>
       <c r="I15" t="n">
         <v>60</v>
@@ -983,10 +983,10 @@
         <v>0.1116</v>
       </c>
       <c r="G16" t="n">
-        <v>1.16372456501238</v>
+        <v>1.1637156190192</v>
       </c>
       <c r="H16" t="n">
-        <v>0.570257392773385</v>
+        <v>0.570253769164272</v>
       </c>
       <c r="I16" t="n">
         <v>53.9</v>
@@ -1006,16 +1006,16 @@
         <v>188.39</v>
       </c>
       <c r="E17" t="n">
-        <v>202.7</v>
+        <v>202.69</v>
       </c>
       <c r="F17" t="n">
         <v>0.0931</v>
       </c>
       <c r="G17" t="n">
-        <v>1.17634434601149</v>
+        <v>1.17633511372074</v>
       </c>
       <c r="H17" t="n">
-        <v>0.55240505389221</v>
+        <v>0.552401500246739</v>
       </c>
       <c r="I17" t="n">
         <v>52.6</v>
@@ -1032,7 +1032,7 @@
         <v>11</v>
       </c>
       <c r="D18" t="n">
-        <v>192.03</v>
+        <v>192.02</v>
       </c>
       <c r="E18" t="n">
         <v>210.41</v>
@@ -1041,10 +1041,10 @@
         <v>0.0995</v>
       </c>
       <c r="G18" t="n">
-        <v>1.17065362639906</v>
+        <v>1.17064356267687</v>
       </c>
       <c r="H18" t="n">
-        <v>0.561825067112333</v>
+        <v>0.561821146309639</v>
       </c>
       <c r="I18" t="n">
         <v>49.6</v>
@@ -1070,10 +1070,10 @@
         <v>0.1174</v>
       </c>
       <c r="G19" t="n">
-        <v>1.15905593863403</v>
+        <v>1.15904635034672</v>
       </c>
       <c r="H19" t="n">
-        <v>0.587679914119203</v>
+        <v>0.587675913316996</v>
       </c>
       <c r="I19" t="n">
         <v>40</v>
@@ -1133,13 +1133,13 @@
         <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>150243</v>
+        <v>61072</v>
       </c>
       <c r="D2" t="n">
-        <v>0.272</v>
+        <v>0.208</v>
       </c>
       <c r="E2" t="n">
-        <v>11.45</v>
+        <v>8.15</v>
       </c>
       <c r="F2" t="n">
         <v>0.00067</v>
@@ -1156,16 +1156,16 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>24935</v>
+        <v>7471</v>
       </c>
       <c r="D3" t="n">
-        <v>0.045</v>
+        <v>0.025</v>
       </c>
       <c r="E3" t="n">
-        <v>5.7</v>
+        <v>2.99</v>
       </c>
       <c r="F3" t="n">
-        <v>0.00533</v>
+        <v>0.08728</v>
       </c>
       <c r="G3" t="s">
         <v>27</v>
@@ -1179,16 +1179,16 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>26681</v>
+        <v>24705</v>
       </c>
       <c r="D4" t="n">
-        <v>0.048</v>
+        <v>0.084</v>
       </c>
       <c r="E4" t="n">
-        <v>6.1</v>
+        <v>9.89</v>
       </c>
       <c r="F4" t="n">
-        <v>0.00333</v>
+        <v>0.002</v>
       </c>
       <c r="G4" t="s">
         <v>27</v>
@@ -1202,10 +1202,10 @@
         <v>80</v>
       </c>
       <c r="C5" t="n">
-        <v>349861</v>
+        <v>199740</v>
       </c>
       <c r="D5" t="n">
-        <v>0.634</v>
+        <v>0.682</v>
       </c>
       <c r="E5"/>
       <c r="F5"/>
@@ -1221,7 +1221,7 @@
         <v>85</v>
       </c>
       <c r="C6" t="n">
-        <v>551720</v>
+        <v>292988</v>
       </c>
       <c r="D6" t="n">
         <v>1</v>
@@ -1240,13 +1240,13 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>162037</v>
+        <v>97850</v>
       </c>
       <c r="D7" t="n">
-        <v>0.08</v>
+        <v>0.087</v>
       </c>
       <c r="E7" t="n">
-        <v>10.94</v>
+        <v>14.29</v>
       </c>
       <c r="F7" t="n">
         <v>0.00067</v>
@@ -1263,16 +1263,16 @@
         <v>3</v>
       </c>
       <c r="C8" t="n">
-        <v>196323</v>
+        <v>26676</v>
       </c>
       <c r="D8" t="n">
-        <v>0.096</v>
+        <v>0.024</v>
       </c>
       <c r="E8" t="n">
-        <v>4.42</v>
+        <v>1.3</v>
       </c>
       <c r="F8" t="n">
-        <v>0.002</v>
+        <v>0.31246</v>
       </c>
       <c r="G8" t="s">
         <v>32</v>
@@ -1286,13 +1286,13 @@
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>625389</v>
+        <v>519372</v>
       </c>
       <c r="D9" t="n">
-        <v>0.307</v>
+        <v>0.46</v>
       </c>
       <c r="E9" t="n">
-        <v>42.21</v>
+        <v>75.84</v>
       </c>
       <c r="F9" t="n">
         <v>0.00067</v>
@@ -1309,10 +1309,10 @@
         <v>71</v>
       </c>
       <c r="C10" t="n">
-        <v>1052041</v>
+        <v>486202</v>
       </c>
       <c r="D10" t="n">
-        <v>0.517</v>
+        <v>0.43</v>
       </c>
       <c r="E10"/>
       <c r="F10"/>
@@ -1328,7 +1328,7 @@
         <v>76</v>
       </c>
       <c r="C11" t="n">
-        <v>2035789</v>
+        <v>1130099</v>
       </c>
       <c r="D11" t="n">
         <v>1</v>
@@ -1347,16 +1347,16 @@
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>505</v>
+        <v>157</v>
       </c>
       <c r="D12" t="n">
         <v>0.001</v>
       </c>
       <c r="E12" t="n">
-        <v>0.17</v>
+        <v>0.11</v>
       </c>
       <c r="F12" t="n">
-        <v>0.81945</v>
+        <v>0.76016</v>
       </c>
       <c r="G12" t="s">
         <v>33</v>
@@ -1370,13 +1370,13 @@
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>56228</v>
+        <v>25414</v>
       </c>
       <c r="D13" t="n">
-        <v>0.166</v>
+        <v>0.18</v>
       </c>
       <c r="E13" t="n">
-        <v>18.83</v>
+        <v>18.47</v>
       </c>
       <c r="F13" t="n">
         <v>0.00067</v>
@@ -1393,16 +1393,16 @@
         <v>3</v>
       </c>
       <c r="C14" t="n">
-        <v>96015</v>
+        <v>30537</v>
       </c>
       <c r="D14" t="n">
-        <v>0.284</v>
+        <v>0.216</v>
       </c>
       <c r="E14" t="n">
-        <v>10.72</v>
+        <v>7.4</v>
       </c>
       <c r="F14" t="n">
-        <v>0.00067</v>
+        <v>0.00133</v>
       </c>
       <c r="G14" t="s">
         <v>33</v>
@@ -1416,10 +1416,10 @@
         <v>62</v>
       </c>
       <c r="C15" t="n">
-        <v>185186</v>
+        <v>85309</v>
       </c>
       <c r="D15" t="n">
-        <v>0.548</v>
+        <v>0.603</v>
       </c>
       <c r="E15"/>
       <c r="F15"/>
@@ -1435,7 +1435,7 @@
         <v>67</v>
       </c>
       <c r="C16" t="n">
-        <v>337935</v>
+        <v>141417</v>
       </c>
       <c r="D16" t="n">
         <v>1</v>
@@ -1499,7 +1499,7 @@
         <v>0.084</v>
       </c>
       <c r="D2" t="n">
-        <v>8.94</v>
+        <v>8.95</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -1722,7 +1722,7 @@
         <v>0.67</v>
       </c>
       <c r="E13" t="n">
-        <v>0.508</v>
+        <v>0.507</v>
       </c>
       <c r="F13" t="s">
         <v>32</v>
@@ -1742,7 +1742,7 @@
         <v>0.31</v>
       </c>
       <c r="E14" t="n">
-        <v>0.76</v>
+        <v>0.761</v>
       </c>
       <c r="F14" t="s">
         <v>32</v>
@@ -2216,7 +2216,7 @@
     <col min="2" max="2" width="3.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="14.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="5.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="5.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="6.71" hidden="0" customWidth="1"/>
     <col min="6" max="6" width="7.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2248,13 +2248,13 @@
         <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>441584</v>
+        <v>149393</v>
       </c>
       <c r="D2" t="n">
-        <v>0.084</v>
+        <v>0.038</v>
       </c>
       <c r="E2" t="n">
-        <v>14.9</v>
+        <v>8.24</v>
       </c>
       <c r="F2" t="n">
         <v>0.00067</v>
@@ -2268,16 +2268,16 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>44470</v>
+        <v>17313</v>
       </c>
       <c r="D3" t="n">
-        <v>0.008</v>
+        <v>0.004</v>
       </c>
       <c r="E3" t="n">
-        <v>4.5</v>
+        <v>2.87</v>
       </c>
       <c r="F3" t="n">
-        <v>0.02398</v>
+        <v>0.09194</v>
       </c>
     </row>
     <row r="4">
@@ -2288,16 +2288,16 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>69064</v>
+        <v>58058</v>
       </c>
       <c r="D4" t="n">
-        <v>0.013</v>
+        <v>0.015</v>
       </c>
       <c r="E4" t="n">
-        <v>6.99</v>
+        <v>9.61</v>
       </c>
       <c r="F4" t="n">
-        <v>0.006</v>
+        <v>0.004</v>
       </c>
     </row>
     <row r="5">
@@ -2308,13 +2308,13 @@
         <v>2</v>
       </c>
       <c r="C5" t="n">
-        <v>1690024</v>
+        <v>1642613</v>
       </c>
       <c r="D5" t="n">
-        <v>0.32</v>
+        <v>0.423</v>
       </c>
       <c r="E5" t="n">
-        <v>85.53</v>
+        <v>135.91</v>
       </c>
       <c r="F5" t="n">
         <v>0.00067</v>
@@ -2328,13 +2328,13 @@
         <v>2</v>
       </c>
       <c r="C6" t="n">
-        <v>657172</v>
+        <v>553351</v>
       </c>
       <c r="D6" t="n">
-        <v>0.124</v>
+        <v>0.143</v>
       </c>
       <c r="E6" t="n">
-        <v>33.26</v>
+        <v>45.78</v>
       </c>
       <c r="F6" t="n">
         <v>0.00067</v>
@@ -2348,16 +2348,16 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>129807</v>
+        <v>90865</v>
       </c>
       <c r="D7" t="n">
-        <v>0.025</v>
+        <v>0.023</v>
       </c>
       <c r="E7" t="n">
-        <v>2.19</v>
+        <v>2.51</v>
       </c>
       <c r="F7" t="n">
-        <v>0.01999</v>
+        <v>0.01732</v>
       </c>
     </row>
     <row r="8">
@@ -2368,16 +2368,16 @@
         <v>2</v>
       </c>
       <c r="C8" t="n">
-        <v>134579</v>
+        <v>77259</v>
       </c>
       <c r="D8" t="n">
-        <v>0.025</v>
+        <v>0.02</v>
       </c>
       <c r="E8" t="n">
-        <v>6.81</v>
+        <v>6.39</v>
       </c>
       <c r="F8" t="n">
-        <v>0.00067</v>
+        <v>0.00466</v>
       </c>
     </row>
     <row r="9">
@@ -2388,10 +2388,10 @@
         <v>214</v>
       </c>
       <c r="C9" t="n">
-        <v>2114166</v>
+        <v>1293204</v>
       </c>
       <c r="D9" t="n">
-        <v>0.4</v>
+        <v>0.333</v>
       </c>
       <c r="E9"/>
       <c r="F9"/>
@@ -2404,7 +2404,7 @@
         <v>231</v>
       </c>
       <c r="C10" t="n">
-        <v>5280867</v>
+        <v>3882055</v>
       </c>
       <c r="D10" t="n">
         <v>1</v>
@@ -2501,13 +2501,13 @@
         <v>3</v>
       </c>
       <c r="H2" t="n">
-        <v>150227</v>
+        <v>61056</v>
       </c>
       <c r="I2" t="n">
-        <v>0.272</v>
+        <v>0.208</v>
       </c>
       <c r="J2" t="n">
-        <v>11.45</v>
+        <v>8.15</v>
       </c>
       <c r="K2" t="n">
         <v>0.00067</v>
@@ -2539,16 +2539,16 @@
         <v>1</v>
       </c>
       <c r="H3" t="n">
-        <v>24933</v>
+        <v>7468</v>
       </c>
       <c r="I3" t="n">
-        <v>0.045</v>
+        <v>0.025</v>
       </c>
       <c r="J3" t="n">
-        <v>5.7</v>
+        <v>2.99</v>
       </c>
       <c r="K3" t="n">
-        <v>0.004</v>
+        <v>0.08461</v>
       </c>
       <c r="L3" t="s">
         <v>27</v>
@@ -2577,16 +2577,16 @@
         <v>1</v>
       </c>
       <c r="H4" t="n">
-        <v>26680</v>
+        <v>24705</v>
       </c>
       <c r="I4" t="n">
-        <v>0.048</v>
+        <v>0.084</v>
       </c>
       <c r="J4" t="n">
-        <v>6.1</v>
+        <v>9.9</v>
       </c>
       <c r="K4" t="n">
-        <v>0.004</v>
+        <v>0.002</v>
       </c>
       <c r="L4" t="s">
         <v>27</v>
@@ -2611,10 +2611,10 @@
         <v>80</v>
       </c>
       <c r="H5" t="n">
-        <v>349805</v>
+        <v>199684</v>
       </c>
       <c r="I5" t="n">
-        <v>0.634</v>
+        <v>0.682</v>
       </c>
       <c r="J5"/>
       <c r="K5"/>
@@ -2641,7 +2641,7 @@
         <v>85</v>
       </c>
       <c r="H6" t="n">
-        <v>551646</v>
+        <v>292913</v>
       </c>
       <c r="I6" t="n">
         <v>1</v>
@@ -2675,16 +2675,16 @@
         <v>3</v>
       </c>
       <c r="H7" t="n">
-        <v>196108</v>
+        <v>26899</v>
       </c>
       <c r="I7" t="n">
-        <v>0.096</v>
+        <v>0.024</v>
       </c>
       <c r="J7" t="n">
-        <v>4.41</v>
+        <v>1.31</v>
       </c>
       <c r="K7" t="n">
-        <v>0.00333</v>
+        <v>0.27781</v>
       </c>
       <c r="L7" t="s">
         <v>32</v>
@@ -2713,13 +2713,13 @@
         <v>1</v>
       </c>
       <c r="H8" t="n">
-        <v>619660</v>
+        <v>515173</v>
       </c>
       <c r="I8" t="n">
-        <v>0.304</v>
+        <v>0.456</v>
       </c>
       <c r="J8" t="n">
-        <v>41.82</v>
+        <v>75.24</v>
       </c>
       <c r="K8" t="n">
         <v>0.00067</v>
@@ -2751,16 +2751,16 @@
         <v>1</v>
       </c>
       <c r="H9" t="n">
-        <v>167947</v>
+        <v>101793</v>
       </c>
       <c r="I9" t="n">
-        <v>0.083</v>
+        <v>0.09</v>
       </c>
       <c r="J9" t="n">
-        <v>11.34</v>
+        <v>14.87</v>
       </c>
       <c r="K9" t="n">
-        <v>0.00133</v>
+        <v>0.00067</v>
       </c>
       <c r="L9" t="s">
         <v>32</v>
@@ -2785,10 +2785,10 @@
         <v>71</v>
       </c>
       <c r="H10" t="n">
-        <v>1051979</v>
+        <v>486140</v>
       </c>
       <c r="I10" t="n">
-        <v>0.517</v>
+        <v>0.43</v>
       </c>
       <c r="J10"/>
       <c r="K10"/>
@@ -2815,7 +2815,7 @@
         <v>76</v>
       </c>
       <c r="H11" t="n">
-        <v>2035695</v>
+        <v>1130005</v>
       </c>
       <c r="I11" t="n">
         <v>1</v>
@@ -2849,13 +2849,13 @@
         <v>3</v>
       </c>
       <c r="H12" t="n">
-        <v>100597</v>
+        <v>29037</v>
       </c>
       <c r="I12" t="n">
-        <v>0.298</v>
+        <v>0.205</v>
       </c>
       <c r="J12" t="n">
-        <v>11.23</v>
+        <v>7.04</v>
       </c>
       <c r="K12" t="n">
         <v>0.00067</v>
@@ -2887,13 +2887,13 @@
         <v>1</v>
       </c>
       <c r="H13" t="n">
-        <v>51174</v>
+        <v>26338</v>
       </c>
       <c r="I13" t="n">
-        <v>0.151</v>
+        <v>0.186</v>
       </c>
       <c r="J13" t="n">
-        <v>17.13</v>
+        <v>19.15</v>
       </c>
       <c r="K13" t="n">
         <v>0.00067</v>
@@ -2925,16 +2925,16 @@
         <v>1</v>
       </c>
       <c r="H14" t="n">
-        <v>969</v>
+        <v>724</v>
       </c>
       <c r="I14" t="n">
-        <v>0.003</v>
+        <v>0.005</v>
       </c>
       <c r="J14" t="n">
-        <v>0.32</v>
+        <v>0.53</v>
       </c>
       <c r="K14" t="n">
-        <v>0.68754</v>
+        <v>0.48168</v>
       </c>
       <c r="L14" t="s">
         <v>33</v>
@@ -2959,10 +2959,10 @@
         <v>62</v>
       </c>
       <c r="H15" t="n">
-        <v>185165</v>
+        <v>85288</v>
       </c>
       <c r="I15" t="n">
-        <v>0.548</v>
+        <v>0.603</v>
       </c>
       <c r="J15"/>
       <c r="K15"/>
@@ -2989,7 +2989,7 @@
         <v>67</v>
       </c>
       <c r="H16" t="n">
-        <v>337905</v>
+        <v>141387</v>
       </c>
       <c r="I16" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
playing with GLMM bootstrapping for plasticity
</commit_message>
<xml_diff>
--- a/Data/Supplemental/Supplemental_Tables.xlsx
+++ b/Data/Supplemental/Supplemental_Tables.xlsx
@@ -2277,7 +2277,7 @@
         <v>2.87</v>
       </c>
       <c r="F3" t="n">
-        <v>0.09194</v>
+        <v>0.09327</v>
       </c>
     </row>
     <row r="4">
@@ -2357,7 +2357,7 @@
         <v>2.51</v>
       </c>
       <c r="F7" t="n">
-        <v>0.01732</v>
+        <v>0.01799</v>
       </c>
     </row>
     <row r="8">
@@ -2495,7 +2495,7 @@
         <v>0.55</v>
       </c>
       <c r="F2" t="n">
-        <v>0.74883</v>
+        <v>0.74817</v>
       </c>
       <c r="G2" t="n">
         <v>3</v>
@@ -2548,7 +2548,7 @@
         <v>2.99</v>
       </c>
       <c r="K3" t="n">
-        <v>0.08461</v>
+        <v>0.08261</v>
       </c>
       <c r="L3" t="s">
         <v>27</v>
@@ -2571,7 +2571,7 @@
         <v>0.52</v>
       </c>
       <c r="F4" t="n">
-        <v>0.58294</v>
+        <v>0.58228</v>
       </c>
       <c r="G4" t="n">
         <v>1</v>
@@ -2684,7 +2684,7 @@
         <v>1.31</v>
       </c>
       <c r="K7" t="n">
-        <v>0.27781</v>
+        <v>0.27848</v>
       </c>
       <c r="L7" t="s">
         <v>32</v>
@@ -2881,7 +2881,7 @@
         <v>2.76</v>
       </c>
       <c r="F13" t="n">
-        <v>0.1006</v>
+        <v>0.09993</v>
       </c>
       <c r="G13" t="n">
         <v>1</v>
@@ -2934,7 +2934,7 @@
         <v>0.53</v>
       </c>
       <c r="K14" t="n">
-        <v>0.48168</v>
+        <v>0.48235</v>
       </c>
       <c r="L14" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
fixed tables to work with GLMM
</commit_message>
<xml_diff>
--- a/Data/Supplemental/Supplemental_Tables.xlsx
+++ b/Data/Supplemental/Supplemental_Tables.xlsx
@@ -9,15 +9,14 @@
     <sheet name="Table S1 - Plasticity AIC" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Table S2 - PERMANOVA" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Table S3 - Plasticity GLM" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Table S4 - Plasticity ANOVA" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Table S5 - Species PERMANOVA" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Table S6 - HostVsymb PERMANOVA" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Table S4 - Species PERMANOVA" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Table S5 - HostVsymb PERMANOVA" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t xml:space="preserve">Species</t>
   </si>
@@ -34,7 +33,13 @@
     <t xml:space="preserve">BIC</t>
   </si>
   <si>
-    <t xml:space="preserve">Nagelkerke R2</t>
+    <t xml:space="preserve">Conditional R2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marginal R2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICC</t>
   </si>
   <si>
     <t xml:space="preserve">RMSE</t>
@@ -49,25 +54,25 @@
     <t xml:space="preserve">ssid</t>
   </si>
   <si>
-    <t xml:space="preserve">reef environment * pCO2 + temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">glm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reef environment * (pCO2 + temperature)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reef environment + pCO2 + temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reef environment + pCO2 * temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reef environment * pCO2 * temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pCO2 + temperature</t>
+    <t xml:space="preserve">reef environment * pCO2 + temperature + (1 | colony)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">glmerMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reef environment * pCO2 * temperature + (1 | colony)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reef environment * (pCO2 + temperature) + (1 | colony)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reef environment + pCO2 + temperature + (1 | colony)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pCO2 + temperature + (1 | colony)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reef environment + pCO2 * temperature + (1 | colony)</t>
   </si>
   <si>
     <t xml:space="preserve">pstr</t>
@@ -130,16 +135,10 @@
     <t xml:space="preserve">Statistic</t>
   </si>
   <si>
-    <t xml:space="preserve">(Intercept)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reef environment (offshore)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pCO2-current</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pCO2-EOC</t>
+    <t xml:space="preserve">Intercept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reef environment (offshore) </t>
   </si>
   <si>
     <t xml:space="preserve">pCO2-extreme</t>
@@ -148,22 +147,10 @@
     <t xml:space="preserve">temperature (31C)</t>
   </si>
   <si>
-    <t xml:space="preserve">reef environment (offshore):pCO2-current</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reef environment (offshore):pCO2-EOC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reef environment (offshore):pCO2-extreme</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F values</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reef environment:pCO2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residuals</t>
+    <t xml:space="preserve">reef environment (offshore) pCO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reef environment (offshore) pCO2-extreme</t>
   </si>
   <si>
     <t xml:space="preserve">temperature:species</t>
@@ -520,11 +507,11 @@
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
     <col min="1" max="1" width="7.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="39.71" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="5.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="6.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="6.71" hidden="0" customWidth="1"/>
-    <col min="6" max="6" width="13.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="54.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="8.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="5.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="5.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="14.71" hidden="0" customWidth="1"/>
     <col min="7" max="7" width="11.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
@@ -556,527 +543,571 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D2" t="n">
-        <v>254.68</v>
+        <v>218.8</v>
       </c>
       <c r="E2" t="n">
-        <v>277.86</v>
+        <v>243.5</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2899</v>
+        <v>0.5059</v>
       </c>
       <c r="G2" t="n">
-        <v>1.2926268490263</v>
+        <v>0.3225</v>
       </c>
       <c r="H2" t="n">
-        <v>0.649718186195778</v>
+        <v>0.270712896490855</v>
       </c>
       <c r="I2" t="n">
-        <v>85.5</v>
+        <v>0.88051736116787</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.309990521732364</v>
+      </c>
+      <c r="K2" t="n">
+        <v>70.7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3" t="n">
-        <v>256.41</v>
+        <v>223.2</v>
       </c>
       <c r="E3" t="n">
-        <v>281.9</v>
+        <v>259.2</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2928</v>
+        <v>0.5445</v>
       </c>
       <c r="G3" t="n">
-        <v>1.2899740213025</v>
+        <v>0.3656</v>
       </c>
       <c r="H3" t="n">
-        <v>0.653586411465873</v>
+        <v>0.28206734361165</v>
       </c>
       <c r="I3" t="n">
-        <v>74.3</v>
+        <v>0.855828398376242</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.294010052276531</v>
+      </c>
+      <c r="K3" t="n">
+        <v>69.6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
       <c r="D4" t="n">
-        <v>254.78</v>
+        <v>220.1</v>
       </c>
       <c r="E4" t="n">
-        <v>271.01</v>
+        <v>247.1</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2213</v>
+        <v>0.5115</v>
       </c>
       <c r="G4" t="n">
-        <v>1.33685374011254</v>
+        <v>0.3288</v>
       </c>
       <c r="H4" t="n">
-        <v>0.660209766997358</v>
+        <v>0.272192941547414</v>
       </c>
       <c r="I4" t="n">
-        <v>71.9</v>
+        <v>0.874857104921775</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.307309431789679</v>
+      </c>
+      <c r="K4" t="n">
+        <v>68.6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D5" t="n">
-        <v>256.46</v>
+        <v>221.6</v>
       </c>
       <c r="E5" t="n">
-        <v>277.32</v>
+        <v>239.6</v>
       </c>
       <c r="F5" t="n">
-        <v>0.2483</v>
+        <v>0.4419</v>
       </c>
       <c r="G5" t="n">
-        <v>1.32703425546414</v>
+        <v>0.2535</v>
       </c>
       <c r="H5" t="n">
-        <v>0.660312676146787</v>
+        <v>0.252287908819288</v>
       </c>
       <c r="I5" t="n">
-        <v>64.7</v>
+        <v>0.933847194038125</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.322867004362844</v>
+      </c>
+      <c r="K5" t="n">
+        <v>39.5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D6" t="n">
-        <v>260.35</v>
+        <v>222.1</v>
       </c>
       <c r="E6" t="n">
-        <v>295.11</v>
+        <v>237.8</v>
       </c>
       <c r="F6" t="n">
-        <v>0.3346</v>
+        <v>0.3698</v>
       </c>
       <c r="G6" t="n">
-        <v>1.25915911436328</v>
+        <v>0.0882</v>
       </c>
       <c r="H6" t="n">
-        <v>0.657644659640462</v>
+        <v>0.308813847521209</v>
       </c>
       <c r="I6" t="n">
-        <v>55.3</v>
+        <v>0.936882340613694</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.331059051190965</v>
+      </c>
+      <c r="K6" t="n">
+        <v>35.9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D7" t="n">
-        <v>259.43</v>
+        <v>225.6</v>
       </c>
       <c r="E7" t="n">
-        <v>273.33</v>
+        <v>248.1</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1382</v>
+        <v>0.4421</v>
       </c>
       <c r="G7" t="n">
-        <v>1.4151360221094</v>
+        <v>0.2534</v>
       </c>
       <c r="H7" t="n">
-        <v>0.683221885809563</v>
+        <v>0.252780589487017</v>
       </c>
       <c r="I7" t="n">
-        <v>21.3</v>
+        <v>0.931849391942536</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.323013486807386</v>
+      </c>
+      <c r="K7" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D8" t="n">
-        <v>242.52</v>
+        <v>110.7</v>
       </c>
       <c r="E8" t="n">
-        <v>276.67</v>
+        <v>128.3</v>
       </c>
       <c r="F8" t="n">
-        <v>0.2401</v>
+        <v>0.4274</v>
       </c>
       <c r="G8" t="n">
-        <v>1.20315338344266</v>
+        <v>0.3474</v>
       </c>
       <c r="H8" t="n">
-        <v>0.610559911143328</v>
+        <v>0.122629862821237</v>
       </c>
       <c r="I8" t="n">
-        <v>68.6</v>
+        <v>1.00977436829259</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.335974696337972</v>
+      </c>
+      <c r="K8" t="n">
+        <v>71.4</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D9" t="n">
-        <v>239.68</v>
+        <v>106</v>
       </c>
       <c r="E9" t="n">
-        <v>260.17</v>
+        <v>118.6</v>
       </c>
       <c r="F9" t="n">
-        <v>0.1249</v>
+        <v>0.3408</v>
       </c>
       <c r="G9" t="n">
-        <v>1.30997747698609</v>
+        <v>0.2916</v>
       </c>
       <c r="H9" t="n">
-        <v>0.617460634216792</v>
+        <v>0.0695117570012863</v>
       </c>
       <c r="I9" t="n">
-        <v>66.1</v>
+        <v>1.12393984931601</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.353702872301073</v>
+      </c>
+      <c r="K9" t="n">
+        <v>44.8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D10" t="n">
-        <v>240.53</v>
+        <v>106.9</v>
       </c>
       <c r="E10" t="n">
-        <v>254.19</v>
+        <v>119.5</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0263</v>
+        <v>0.3131</v>
       </c>
       <c r="G10" t="n">
-        <v>1.37957299867158</v>
+        <v>0.2714</v>
       </c>
       <c r="H10" t="n">
-        <v>0.631205876260462</v>
+        <v>0.0572627664145912</v>
       </c>
       <c r="I10" t="n">
-        <v>39.5</v>
+        <v>1.11383231900867</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.352824835250314</v>
+      </c>
+      <c r="K10" t="n">
+        <v>36.3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
         <v>17</v>
       </c>
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D11" t="n">
-        <v>244.19</v>
+        <v>102.8</v>
       </c>
       <c r="E11" t="n">
-        <v>269.24</v>
+        <v>111.6</v>
       </c>
       <c r="F11" t="n">
-        <v>0.1179</v>
+        <v>0.2678</v>
       </c>
       <c r="G11" t="n">
-        <v>1.29607785162445</v>
+        <v>0.2243</v>
       </c>
       <c r="H11" t="n">
-        <v>0.629451678765452</v>
+        <v>0.0560480703765206</v>
       </c>
       <c r="I11" t="n">
-        <v>30.9</v>
+        <v>1.19677569359115</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.364087168175548</v>
+      </c>
+      <c r="K11" t="n">
+        <v>28.6</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
         <v>13</v>
       </c>
-      <c r="C12" t="s">
-        <v>11</v>
-      </c>
       <c r="D12" t="n">
-        <v>242.16</v>
+        <v>145.9</v>
       </c>
       <c r="E12" t="n">
-        <v>258.1</v>
+        <v>167.8</v>
       </c>
       <c r="F12" t="n">
-        <v>0.0319</v>
+        <v>0.5212</v>
       </c>
       <c r="G12" t="n">
-        <v>1.37596637996336</v>
+        <v>0.195</v>
       </c>
       <c r="H12" t="n">
-        <v>0.634439131239188</v>
+        <v>0.405142468828212</v>
       </c>
       <c r="I12" t="n">
-        <v>27.7</v>
+        <v>0.710112914386074</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.231080473857171</v>
+      </c>
+      <c r="K12" t="n">
+        <v>76.2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D13" t="n">
-        <v>244.67</v>
+        <v>147.9</v>
       </c>
       <c r="E13" t="n">
-        <v>267.43</v>
+        <v>171.8</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0833</v>
+        <v>0.5217</v>
       </c>
       <c r="G13" t="n">
-        <v>1.34632437229469</v>
+        <v>0.1952</v>
       </c>
       <c r="H13" t="n">
-        <v>0.634659628138949</v>
+        <v>0.405616901906066</v>
       </c>
       <c r="I13" t="n">
-        <v>17.3</v>
+        <v>0.70994797179576</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.2309514006937</v>
+      </c>
+      <c r="K13" t="n">
+        <v>72.9</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D14" t="n">
-        <v>193.32</v>
+        <v>153.1</v>
       </c>
       <c r="E14" t="n">
-        <v>213.75</v>
+        <v>182.9</v>
       </c>
       <c r="F14" t="n">
-        <v>0.1116</v>
+        <v>0.5273</v>
       </c>
       <c r="G14" t="n">
-        <v>1.16376490169629</v>
+        <v>0.1994</v>
       </c>
       <c r="H14" t="n">
-        <v>0.564285238534006</v>
+        <v>0.409641424663849</v>
       </c>
       <c r="I14" t="n">
-        <v>62.2</v>
+        <v>0.706971647584522</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.229916347449218</v>
+      </c>
+      <c r="K14" t="n">
+        <v>71.4</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D15" t="n">
-        <v>186.42</v>
+        <v>142.3</v>
       </c>
       <c r="E15" t="n">
-        <v>198.68</v>
+        <v>158.2</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0925</v>
+        <v>0.4988</v>
       </c>
       <c r="G15" t="n">
-        <v>1.17631329356072</v>
+        <v>0.1738</v>
       </c>
       <c r="H15" t="n">
-        <v>0.547207956382125</v>
+        <v>0.393286215931064</v>
       </c>
       <c r="I15" t="n">
-        <v>60</v>
+        <v>0.733244393163204</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.237295448325152</v>
+      </c>
+      <c r="K15" t="n">
+        <v>38.4</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D16" t="n">
-        <v>195.32</v>
+        <v>140.4</v>
       </c>
       <c r="E16" t="n">
-        <v>217.79</v>
+        <v>154.4</v>
       </c>
       <c r="F16" t="n">
-        <v>0.1116</v>
+        <v>0.4853</v>
       </c>
       <c r="G16" t="n">
-        <v>1.1637156190192</v>
+        <v>0.1469</v>
       </c>
       <c r="H16" t="n">
-        <v>0.570253769164272</v>
+        <v>0.396708536729162</v>
       </c>
       <c r="I16" t="n">
-        <v>53.9</v>
+        <v>0.732981216119454</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.238221370319828</v>
+      </c>
+      <c r="K16" t="n">
+        <v>32.1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
         <v>18</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>13</v>
       </c>
-      <c r="C17" t="s">
-        <v>11</v>
-      </c>
       <c r="D17" t="n">
-        <v>188.39</v>
+        <v>146.2</v>
       </c>
       <c r="E17" t="n">
-        <v>202.69</v>
+        <v>166.1</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0931</v>
+        <v>0.4995</v>
       </c>
       <c r="G17" t="n">
-        <v>1.17633511372074</v>
+        <v>0.1741</v>
       </c>
       <c r="H17" t="n">
-        <v>0.552401500246739</v>
+        <v>0.394015465922658</v>
       </c>
       <c r="I17" t="n">
-        <v>52.6</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" t="n">
-        <v>192.02</v>
-      </c>
-      <c r="E18" t="n">
-        <v>210.41</v>
-      </c>
-      <c r="F18" t="n">
-        <v>0.0995</v>
-      </c>
-      <c r="G18" t="n">
-        <v>1.17064356267687</v>
-      </c>
-      <c r="H18" t="n">
-        <v>0.561821146309639</v>
-      </c>
-      <c r="I18" t="n">
-        <v>49.6</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" t="n">
-        <v>200.97</v>
-      </c>
-      <c r="E19" t="n">
-        <v>229.58</v>
-      </c>
-      <c r="F19" t="n">
-        <v>0.1174</v>
-      </c>
-      <c r="G19" t="n">
-        <v>1.15904635034672</v>
-      </c>
-      <c r="H19" t="n">
-        <v>0.587675913316996</v>
-      </c>
-      <c r="I19" t="n">
-        <v>40</v>
+        <v>0.734046668651323</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.237351188594544</v>
+      </c>
+      <c r="K17" t="n">
+        <v>30.5</v>
       </c>
     </row>
   </sheetData>
@@ -1104,30 +1135,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -1145,12 +1176,12 @@
         <v>0.00067</v>
       </c>
       <c r="G2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -1168,12 +1199,12 @@
         <v>0.08728</v>
       </c>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -1191,12 +1222,12 @@
         <v>0.002</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B5" t="n">
         <v>80</v>
@@ -1210,12 +1241,12 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B6" t="n">
         <v>85</v>
@@ -1229,12 +1260,12 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B7" t="n">
         <v>1</v>
@@ -1252,12 +1283,12 @@
         <v>0.00067</v>
       </c>
       <c r="G7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B8" t="n">
         <v>3</v>
@@ -1275,12 +1306,12 @@
         <v>0.31246</v>
       </c>
       <c r="G8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B9" t="n">
         <v>1</v>
@@ -1298,12 +1329,12 @@
         <v>0.00067</v>
       </c>
       <c r="G9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B10" t="n">
         <v>71</v>
@@ -1317,12 +1348,12 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B11" t="n">
         <v>76</v>
@@ -1336,12 +1367,12 @@
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B12" t="n">
         <v>1</v>
@@ -1359,12 +1390,12 @@
         <v>0.76016</v>
       </c>
       <c r="G12" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B13" t="n">
         <v>1</v>
@@ -1382,12 +1413,12 @@
         <v>0.00067</v>
       </c>
       <c r="G13" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B14" t="n">
         <v>3</v>
@@ -1405,12 +1436,12 @@
         <v>0.00133</v>
       </c>
       <c r="G14" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B15" t="n">
         <v>62</v>
@@ -1424,12 +1455,12 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B16" t="n">
         <v>67</v>
@@ -1443,7 +1474,7 @@
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1470,102 +1501,102 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B2" t="n">
-        <v>0.754</v>
+        <v>1.085</v>
       </c>
       <c r="C2" t="n">
-        <v>0.084</v>
+        <v>0.172</v>
       </c>
       <c r="D2" t="n">
-        <v>8.95</v>
+        <v>6.3</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.204</v>
+        <v>-0.058</v>
       </c>
       <c r="C3" t="n">
-        <v>0.083</v>
+        <v>0.248</v>
       </c>
       <c r="D3" t="n">
-        <v>-2.47</v>
+        <v>-0.24</v>
       </c>
       <c r="E3" t="n">
-        <v>0.016</v>
+        <v>0.814</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.117</v>
+        <v>0.335</v>
       </c>
       <c r="C4" t="n">
-        <v>0.146</v>
+        <v>0.173</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.8</v>
+        <v>1.94</v>
       </c>
       <c r="E4" t="n">
-        <v>0.429</v>
+        <v>0.053</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.135</v>
+        <v>0.21</v>
       </c>
       <c r="C5" t="n">
-        <v>0.181</v>
+        <v>0.131</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.75</v>
+        <v>1.6</v>
       </c>
       <c r="E5" t="n">
-        <v>0.458</v>
+        <v>0.109</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6">
@@ -1573,19 +1604,19 @@
         <v>41</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.128</v>
+        <v>0.419</v>
       </c>
       <c r="C6" t="n">
         <v>0.132</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.97</v>
+        <v>3.17</v>
       </c>
       <c r="E6" t="n">
-        <v>0.335</v>
+        <v>0.002</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7">
@@ -1593,19 +1624,19 @@
         <v>42</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.029</v>
+        <v>0.003</v>
       </c>
       <c r="C7" t="n">
-        <v>0.086</v>
+        <v>0.076</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.34</v>
+        <v>0.04</v>
       </c>
       <c r="E7" t="n">
-        <v>0.735</v>
+        <v>0.967</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8">
@@ -1613,299 +1644,259 @@
         <v>43</v>
       </c>
       <c r="B8" t="n">
-        <v>0.302</v>
+        <v>-0.704</v>
       </c>
       <c r="C8" t="n">
-        <v>0.143</v>
+        <v>0.239</v>
       </c>
       <c r="D8" t="n">
-        <v>2.11</v>
+        <v>-2.95</v>
       </c>
       <c r="E8" t="n">
-        <v>0.039</v>
+        <v>0.003</v>
       </c>
       <c r="F8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.243</v>
+        <v>-0.409</v>
       </c>
       <c r="C9" t="n">
-        <v>0.167</v>
+        <v>0.197</v>
       </c>
       <c r="D9" t="n">
-        <v>-1.45</v>
+        <v>-2.08</v>
       </c>
       <c r="E9" t="n">
-        <v>0.151</v>
+        <v>0.037</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.043</v>
+        <v>-0.278</v>
       </c>
       <c r="C10" t="n">
-        <v>0.13</v>
+        <v>0.191</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.33</v>
+        <v>-1.45</v>
       </c>
       <c r="E10" t="n">
-        <v>0.743</v>
+        <v>0.146</v>
       </c>
       <c r="F10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B11" t="n">
-        <v>0.844</v>
+        <v>1.279</v>
       </c>
       <c r="C11" t="n">
-        <v>0.092</v>
+        <v>0.145</v>
       </c>
       <c r="D11" t="n">
-        <v>9.2</v>
+        <v>8.8</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B12" t="n">
-        <v>0.043</v>
+        <v>0.194</v>
       </c>
       <c r="C12" t="n">
-        <v>0.075</v>
+        <v>0.418</v>
       </c>
       <c r="D12" t="n">
-        <v>0.58</v>
+        <v>0.46</v>
       </c>
       <c r="E12" t="n">
-        <v>0.565</v>
+        <v>0.643</v>
       </c>
       <c r="F12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B13" t="n">
-        <v>0.086</v>
+        <v>-0.339</v>
       </c>
       <c r="C13" t="n">
-        <v>0.128</v>
+        <v>0.19</v>
       </c>
       <c r="D13" t="n">
-        <v>0.67</v>
+        <v>-1.79</v>
       </c>
       <c r="E13" t="n">
-        <v>0.507</v>
+        <v>0.074</v>
       </c>
       <c r="F13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B14" t="n">
-        <v>0.071</v>
+        <v>-0.06</v>
       </c>
       <c r="C14" t="n">
-        <v>0.233</v>
+        <v>0.184</v>
       </c>
       <c r="D14" t="n">
-        <v>0.31</v>
+        <v>-0.32</v>
       </c>
       <c r="E14" t="n">
-        <v>0.761</v>
+        <v>0.746</v>
       </c>
       <c r="F14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.11</v>
+        <v>0.226</v>
       </c>
       <c r="C15" t="n">
-        <v>0.141</v>
+        <v>0.17</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.78</v>
+        <v>1.33</v>
       </c>
       <c r="E15" t="n">
-        <v>0.438</v>
+        <v>0.183</v>
       </c>
       <c r="F15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.035</v>
+        <v>1.038</v>
       </c>
       <c r="C16" t="n">
-        <v>0.082</v>
+        <v>0.121</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.42</v>
+        <v>8.61</v>
       </c>
       <c r="E16" t="n">
-        <v>0.673</v>
+        <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B17" t="n">
-        <v>0.86</v>
+        <v>-0.047</v>
       </c>
       <c r="C17" t="n">
-        <v>0.077</v>
+        <v>0.11</v>
       </c>
       <c r="D17" t="n">
-        <v>11.12</v>
+        <v>-0.43</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>0.67</v>
       </c>
       <c r="F17" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.012</v>
+        <v>0.032</v>
       </c>
       <c r="C18" t="n">
-        <v>0.072</v>
+        <v>0.075</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.17</v>
+        <v>0.44</v>
       </c>
       <c r="E18" t="n">
-        <v>0.863</v>
+        <v>0.664</v>
       </c>
       <c r="F18" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.043</v>
+        <v>0.122</v>
       </c>
       <c r="C19" t="n">
-        <v>0.121</v>
+        <v>0.078</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.36</v>
+        <v>1.57</v>
       </c>
       <c r="E19" t="n">
-        <v>0.723</v>
+        <v>0.116</v>
       </c>
       <c r="F19" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.21</v>
+        <v>0.264</v>
       </c>
       <c r="C20" t="n">
-        <v>0.185</v>
+        <v>0.065</v>
       </c>
       <c r="D20" t="n">
-        <v>-1.13</v>
+        <v>4.07</v>
       </c>
       <c r="E20" t="n">
-        <v>0.263</v>
+        <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" t="n">
-        <v>0.086</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0.116</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0.74</v>
-      </c>
-      <c r="E21" t="n">
-        <v>0.463</v>
-      </c>
-      <c r="F21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" t="n">
-        <v>-0.151</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0.079</v>
-      </c>
-      <c r="D22" t="n">
-        <v>-1.92</v>
-      </c>
-      <c r="E22" t="n">
-        <v>0.061</v>
-      </c>
-      <c r="F22" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1915,296 +1906,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
-  <cols>
-    <col min="1" max="1" width="21.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="14.71" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="3.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="8.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="7.71" hidden="0" customWidth="1"/>
-    <col min="6" max="6" width="7.71" hidden="0" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" t="n">
-        <v>2.79</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" t="n">
-        <v>6</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="F2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="n">
-        <v>4.36</v>
-      </c>
-      <c r="C3" t="n">
-        <v>3</v>
-      </c>
-      <c r="D3" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.74</v>
-      </c>
-      <c r="F4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" t="n">
-        <v>2.21</v>
-      </c>
-      <c r="C5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="F5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" t="n">
-        <v>30.45</v>
-      </c>
-      <c r="C6" t="n">
-        <v>66</v>
-      </c>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0.13</v>
-      </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.57</v>
-      </c>
-      <c r="F7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" t="n">
-        <v>0.48</v>
-      </c>
-      <c r="C8" t="n">
-        <v>3</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="F8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.68</v>
-      </c>
-      <c r="F9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" t="n">
-        <v>25.8</v>
-      </c>
-      <c r="C10" t="n">
-        <v>66</v>
-      </c>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.86</v>
-      </c>
-      <c r="F11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" t="n">
-        <v>0.67</v>
-      </c>
-      <c r="C12" t="n">
-        <v>3</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.49</v>
-      </c>
-      <c r="F12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" t="n">
-        <v>1.04</v>
-      </c>
-      <c r="C13" t="n">
-        <v>1</v>
-      </c>
-      <c r="D13" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="F13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" t="n">
-        <v>13.9</v>
-      </c>
-      <c r="C14" t="n">
-        <v>51</v>
-      </c>
-      <c r="D14"/>
-      <c r="E14"/>
-      <c r="F14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2222,27 +1923,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -2262,7 +1963,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -2277,12 +1978,12 @@
         <v>2.87</v>
       </c>
       <c r="F3" t="n">
-        <v>0.09327</v>
+        <v>0.09194</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -2302,7 +2003,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B5" t="n">
         <v>2</v>
@@ -2322,7 +2023,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B6" t="n">
         <v>2</v>
@@ -2342,7 +2043,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B7" t="n">
         <v>6</v>
@@ -2357,12 +2058,12 @@
         <v>2.51</v>
       </c>
       <c r="F7" t="n">
-        <v>0.01799</v>
+        <v>0.01732</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B8" t="n">
         <v>2</v>
@@ -2382,7 +2083,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B9" t="n">
         <v>214</v>
@@ -2398,7 +2099,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B10" t="n">
         <v>231</v>
@@ -2418,7 +2119,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2442,45 +2143,45 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" t="s">
         <v>52</v>
       </c>
-      <c r="H1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J1" t="s">
-        <v>55</v>
-      </c>
-      <c r="K1" t="s">
-        <v>56</v>
-      </c>
       <c r="L1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -2495,7 +2196,7 @@
         <v>0.55</v>
       </c>
       <c r="F2" t="n">
-        <v>0.74817</v>
+        <v>0.74883</v>
       </c>
       <c r="G2" t="n">
         <v>3</v>
@@ -2513,12 +2214,12 @@
         <v>0.00067</v>
       </c>
       <c r="L2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -2548,15 +2249,15 @@
         <v>2.99</v>
       </c>
       <c r="K3" t="n">
-        <v>0.08261</v>
+        <v>0.08461</v>
       </c>
       <c r="L3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -2571,7 +2272,7 @@
         <v>0.52</v>
       </c>
       <c r="F4" t="n">
-        <v>0.58228</v>
+        <v>0.58294</v>
       </c>
       <c r="G4" t="n">
         <v>1</v>
@@ -2589,12 +2290,12 @@
         <v>0.002</v>
       </c>
       <c r="L4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B5" t="n">
         <v>80</v>
@@ -2619,12 +2320,12 @@
       <c r="J5"/>
       <c r="K5"/>
       <c r="L5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B6" t="n">
         <v>85</v>
@@ -2649,12 +2350,12 @@
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B7" t="n">
         <v>3</v>
@@ -2684,15 +2385,15 @@
         <v>1.31</v>
       </c>
       <c r="K7" t="n">
-        <v>0.27848</v>
+        <v>0.27781</v>
       </c>
       <c r="L7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B8" t="n">
         <v>1</v>
@@ -2725,12 +2426,12 @@
         <v>0.00067</v>
       </c>
       <c r="L8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B9" t="n">
         <v>1</v>
@@ -2763,12 +2464,12 @@
         <v>0.00067</v>
       </c>
       <c r="L9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B10" t="n">
         <v>71</v>
@@ -2793,12 +2494,12 @@
       <c r="J10"/>
       <c r="K10"/>
       <c r="L10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B11" t="n">
         <v>76</v>
@@ -2823,12 +2524,12 @@
       <c r="J11"/>
       <c r="K11"/>
       <c r="L11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B12" t="n">
         <v>3</v>
@@ -2861,12 +2562,12 @@
         <v>0.00067</v>
       </c>
       <c r="L12" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B13" t="n">
         <v>1</v>
@@ -2881,7 +2582,7 @@
         <v>2.76</v>
       </c>
       <c r="F13" t="n">
-        <v>0.09993</v>
+        <v>0.1006</v>
       </c>
       <c r="G13" t="n">
         <v>1</v>
@@ -2899,12 +2600,12 @@
         <v>0.00067</v>
       </c>
       <c r="L13" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B14" t="n">
         <v>1</v>
@@ -2934,15 +2635,15 @@
         <v>0.53</v>
       </c>
       <c r="K14" t="n">
-        <v>0.48235</v>
+        <v>0.48168</v>
       </c>
       <c r="L14" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B15" t="n">
         <v>62</v>
@@ -2967,12 +2668,12 @@
       <c r="J15"/>
       <c r="K15"/>
       <c r="L15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B16" t="n">
         <v>67</v>
@@ -2997,7 +2698,7 @@
       <c r="J16"/>
       <c r="K16"/>
       <c r="L16" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update to correlation results and fig caption
</commit_message>
<xml_diff>
--- a/Data/Supplemental/Supplemental_Tables.xlsx
+++ b/Data/Supplemental/Supplemental_Tables.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t xml:space="preserve">Species</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t xml:space="preserve">pstr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reef environment * pCO2 * temperature + (1 | colony)7</t>
   </si>
   <si>
     <t xml:space="preserve">past</t>
@@ -800,34 +803,34 @@
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
         <v>13</v>
       </c>
       <c r="D9" t="n">
-        <v>106</v>
+        <v>105.1</v>
       </c>
       <c r="E9" t="n">
-        <v>118.6</v>
+        <v>116.4</v>
       </c>
       <c r="F9" t="n">
-        <v>0.3408</v>
+        <v>0.3271</v>
       </c>
       <c r="G9" t="n">
-        <v>0.2916</v>
+        <v>0.2594</v>
       </c>
       <c r="H9" t="n">
-        <v>0.0695117570012863</v>
+        <v>0.0914015570605844</v>
       </c>
       <c r="I9" t="n">
-        <v>1.12393984931601</v>
+        <v>1.12817097438964</v>
       </c>
       <c r="J9" t="n">
-        <v>0.353702872301073</v>
+        <v>0.354967986837399</v>
       </c>
       <c r="K9" t="n">
-        <v>44.8</v>
+        <v>47.3</v>
       </c>
     </row>
     <row r="10">
@@ -835,34 +838,34 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
       </c>
       <c r="D10" t="n">
-        <v>106.9</v>
+        <v>106</v>
       </c>
       <c r="E10" t="n">
-        <v>119.5</v>
+        <v>118.6</v>
       </c>
       <c r="F10" t="n">
-        <v>0.3131</v>
+        <v>0.3408</v>
       </c>
       <c r="G10" t="n">
-        <v>0.2714</v>
+        <v>0.2916</v>
       </c>
       <c r="H10" t="n">
-        <v>0.0572627664145912</v>
+        <v>0.0695117570012863</v>
       </c>
       <c r="I10" t="n">
-        <v>1.11383231900867</v>
+        <v>1.12393984931601</v>
       </c>
       <c r="J10" t="n">
-        <v>0.352824835250314</v>
+        <v>0.353702872301073</v>
       </c>
       <c r="K10" t="n">
-        <v>36.3</v>
+        <v>44.8</v>
       </c>
     </row>
     <row r="11">
@@ -870,243 +873,278 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
         <v>13</v>
       </c>
       <c r="D11" t="n">
-        <v>102.8</v>
+        <v>106.9</v>
       </c>
       <c r="E11" t="n">
-        <v>111.6</v>
+        <v>119.5</v>
       </c>
       <c r="F11" t="n">
-        <v>0.2678</v>
+        <v>0.3131</v>
       </c>
       <c r="G11" t="n">
-        <v>0.2243</v>
+        <v>0.2714</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0560480703765206</v>
+        <v>0.0572627664145912</v>
       </c>
       <c r="I11" t="n">
-        <v>1.19677569359115</v>
+        <v>1.11383231900867</v>
       </c>
       <c r="J11" t="n">
-        <v>0.364087168175548</v>
+        <v>0.352824835250314</v>
       </c>
       <c r="K11" t="n">
-        <v>28.6</v>
+        <v>36.3</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
         <v>13</v>
       </c>
       <c r="D12" t="n">
-        <v>145.9</v>
+        <v>102.8</v>
       </c>
       <c r="E12" t="n">
-        <v>167.8</v>
+        <v>111.6</v>
       </c>
       <c r="F12" t="n">
-        <v>0.5212</v>
+        <v>0.2678</v>
       </c>
       <c r="G12" t="n">
-        <v>0.195</v>
+        <v>0.2243</v>
       </c>
       <c r="H12" t="n">
-        <v>0.405142468828212</v>
+        <v>0.0560480703765206</v>
       </c>
       <c r="I12" t="n">
-        <v>0.710112914386074</v>
+        <v>1.19677569359115</v>
       </c>
       <c r="J12" t="n">
-        <v>0.231080473857171</v>
+        <v>0.364087168175548</v>
       </c>
       <c r="K12" t="n">
-        <v>76.2</v>
+        <v>28.6</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
         <v>13</v>
       </c>
       <c r="D13" t="n">
-        <v>147.9</v>
+        <v>145.9</v>
       </c>
       <c r="E13" t="n">
-        <v>171.8</v>
+        <v>167.8</v>
       </c>
       <c r="F13" t="n">
-        <v>0.5217</v>
+        <v>0.5212</v>
       </c>
       <c r="G13" t="n">
-        <v>0.1952</v>
+        <v>0.195</v>
       </c>
       <c r="H13" t="n">
-        <v>0.405616901906066</v>
+        <v>0.405142468828212</v>
       </c>
       <c r="I13" t="n">
-        <v>0.70994797179576</v>
+        <v>0.710112914386074</v>
       </c>
       <c r="J13" t="n">
-        <v>0.2309514006937</v>
+        <v>0.231080473857171</v>
       </c>
       <c r="K13" t="n">
-        <v>72.9</v>
+        <v>76.2</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
       </c>
       <c r="D14" t="n">
-        <v>153.1</v>
+        <v>147.9</v>
       </c>
       <c r="E14" t="n">
-        <v>182.9</v>
+        <v>171.8</v>
       </c>
       <c r="F14" t="n">
-        <v>0.5273</v>
+        <v>0.5217</v>
       </c>
       <c r="G14" t="n">
-        <v>0.1994</v>
+        <v>0.1952</v>
       </c>
       <c r="H14" t="n">
-        <v>0.409641424663849</v>
+        <v>0.405616901906066</v>
       </c>
       <c r="I14" t="n">
-        <v>0.706971647584522</v>
+        <v>0.70994797179576</v>
       </c>
       <c r="J14" t="n">
-        <v>0.229916347449218</v>
+        <v>0.2309514006937</v>
       </c>
       <c r="K14" t="n">
-        <v>71.4</v>
+        <v>72.9</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
         <v>13</v>
       </c>
       <c r="D15" t="n">
-        <v>142.3</v>
+        <v>153.1</v>
       </c>
       <c r="E15" t="n">
-        <v>158.2</v>
+        <v>182.9</v>
       </c>
       <c r="F15" t="n">
-        <v>0.4988</v>
+        <v>0.5273</v>
       </c>
       <c r="G15" t="n">
-        <v>0.1738</v>
+        <v>0.1994</v>
       </c>
       <c r="H15" t="n">
-        <v>0.393286215931064</v>
+        <v>0.409641424663849</v>
       </c>
       <c r="I15" t="n">
-        <v>0.733244393163204</v>
+        <v>0.706971647584522</v>
       </c>
       <c r="J15" t="n">
-        <v>0.237295448325152</v>
+        <v>0.229916347449218</v>
       </c>
       <c r="K15" t="n">
-        <v>38.4</v>
+        <v>71.4</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
       </c>
       <c r="D16" t="n">
-        <v>140.4</v>
+        <v>142.3</v>
       </c>
       <c r="E16" t="n">
-        <v>154.4</v>
+        <v>158.2</v>
       </c>
       <c r="F16" t="n">
-        <v>0.4853</v>
+        <v>0.4988</v>
       </c>
       <c r="G16" t="n">
-        <v>0.1469</v>
+        <v>0.1738</v>
       </c>
       <c r="H16" t="n">
-        <v>0.396708536729162</v>
+        <v>0.393286215931064</v>
       </c>
       <c r="I16" t="n">
-        <v>0.732981216119454</v>
+        <v>0.733244393163204</v>
       </c>
       <c r="J16" t="n">
-        <v>0.238221370319828</v>
+        <v>0.237295448325152</v>
       </c>
       <c r="K16" t="n">
-        <v>32.1</v>
+        <v>38.4</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
         <v>13</v>
       </c>
       <c r="D17" t="n">
+        <v>140.4</v>
+      </c>
+      <c r="E17" t="n">
+        <v>154.4</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.4853</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.1469</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.396708536729162</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.732981216119454</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.238221370319828</v>
+      </c>
+      <c r="K17" t="n">
+        <v>32.1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="n">
         <v>146.2</v>
       </c>
-      <c r="E17" t="n">
+      <c r="E18" t="n">
         <v>166.1</v>
       </c>
-      <c r="F17" t="n">
+      <c r="F18" t="n">
         <v>0.4995</v>
       </c>
-      <c r="G17" t="n">
+      <c r="G18" t="n">
         <v>0.1741</v>
       </c>
-      <c r="H17" t="n">
+      <c r="H18" t="n">
         <v>0.394015465922658</v>
       </c>
-      <c r="I17" t="n">
+      <c r="I18" t="n">
         <v>0.734046668651323</v>
       </c>
-      <c r="J17" t="n">
+      <c r="J18" t="n">
         <v>0.237351188594544</v>
       </c>
-      <c r="K17" t="n">
+      <c r="K18" t="n">
         <v>30.5</v>
       </c>
     </row>
@@ -1135,30 +1173,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -1176,12 +1214,12 @@
         <v>0.00067</v>
       </c>
       <c r="G2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -1199,12 +1237,12 @@
         <v>0.08728</v>
       </c>
       <c r="G3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -1222,12 +1260,12 @@
         <v>0.002</v>
       </c>
       <c r="G4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B5" t="n">
         <v>80</v>
@@ -1241,12 +1279,12 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B6" t="n">
         <v>85</v>
@@ -1260,12 +1298,12 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B7" t="n">
         <v>1</v>
@@ -1283,12 +1321,12 @@
         <v>0.00067</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B8" t="n">
         <v>1</v>
@@ -1306,12 +1344,12 @@
         <v>0.00067</v>
       </c>
       <c r="G8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B9" t="n">
         <v>3</v>
@@ -1329,12 +1367,12 @@
         <v>0.25916</v>
       </c>
       <c r="G9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B10" t="n">
         <v>71</v>
@@ -1348,12 +1386,12 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B11" t="n">
         <v>76</v>
@@ -1367,12 +1405,12 @@
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B12" t="n">
         <v>1</v>
@@ -1390,12 +1428,12 @@
         <v>0.76016</v>
       </c>
       <c r="G12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B13" t="n">
         <v>1</v>
@@ -1413,12 +1451,12 @@
         <v>0.00067</v>
       </c>
       <c r="G13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B14" t="n">
         <v>3</v>
@@ -1436,12 +1474,12 @@
         <v>0.00133</v>
       </c>
       <c r="G14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B15" t="n">
         <v>62</v>
@@ -1455,12 +1493,12 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B16" t="n">
         <v>67</v>
@@ -1474,7 +1512,7 @@
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1501,27 +1539,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B2" t="n">
         <v>1.085</v>
@@ -1536,12 +1574,12 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B3" t="n">
         <v>-0.058</v>
@@ -1556,12 +1594,12 @@
         <v>0.814</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B4" t="n">
         <v>0.335</v>
@@ -1576,12 +1614,12 @@
         <v>0.053</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B5" t="n">
         <v>0.21</v>
@@ -1596,12 +1634,12 @@
         <v>0.109</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B6" t="n">
         <v>0.419</v>
@@ -1616,12 +1654,12 @@
         <v>0.002</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B7" t="n">
         <v>0.003</v>
@@ -1636,12 +1674,12 @@
         <v>0.967</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B8" t="n">
         <v>-0.704</v>
@@ -1656,12 +1694,12 @@
         <v>0.003</v>
       </c>
       <c r="F8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B9" t="n">
         <v>-0.409</v>
@@ -1676,12 +1714,12 @@
         <v>0.037</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B10" t="n">
         <v>-0.278</v>
@@ -1696,12 +1734,12 @@
         <v>0.146</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B11" t="n">
         <v>1.279</v>
@@ -1716,12 +1754,12 @@
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B12" t="n">
         <v>0.194</v>
@@ -1736,12 +1774,12 @@
         <v>0.643</v>
       </c>
       <c r="F12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" t="n">
         <v>-0.339</v>
@@ -1756,12 +1794,12 @@
         <v>0.074</v>
       </c>
       <c r="F13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B14" t="n">
         <v>-0.06</v>
@@ -1776,12 +1814,12 @@
         <v>0.746</v>
       </c>
       <c r="F14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B15" t="n">
         <v>0.226</v>
@@ -1796,12 +1834,12 @@
         <v>0.183</v>
       </c>
       <c r="F15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B16" t="n">
         <v>1.038</v>
@@ -1816,12 +1854,12 @@
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B17" t="n">
         <v>-0.047</v>
@@ -1836,12 +1874,12 @@
         <v>0.67</v>
       </c>
       <c r="F17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B18" t="n">
         <v>0.032</v>
@@ -1856,12 +1894,12 @@
         <v>0.664</v>
       </c>
       <c r="F18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B19" t="n">
         <v>0.122</v>
@@ -1876,12 +1914,12 @@
         <v>0.116</v>
       </c>
       <c r="F19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B20" t="n">
         <v>0.264</v>
@@ -1896,7 +1934,7 @@
         <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1923,27 +1961,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -1963,7 +2001,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -1983,7 +2021,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -2003,7 +2041,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B5" t="n">
         <v>2</v>
@@ -2023,7 +2061,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B6" t="n">
         <v>2</v>
@@ -2043,7 +2081,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B7" t="n">
         <v>6</v>
@@ -2063,7 +2101,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B8" t="n">
         <v>2</v>
@@ -2083,7 +2121,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B9" t="n">
         <v>214</v>
@@ -2099,7 +2137,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B10" t="n">
         <v>231</v>
@@ -2143,45 +2181,45 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -2214,12 +2252,12 @@
         <v>0.00067</v>
       </c>
       <c r="L2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -2252,12 +2290,12 @@
         <v>0.08461</v>
       </c>
       <c r="L3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -2290,12 +2328,12 @@
         <v>0.002</v>
       </c>
       <c r="L4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B5" t="n">
         <v>80</v>
@@ -2320,12 +2358,12 @@
       <c r="J5"/>
       <c r="K5"/>
       <c r="L5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B6" t="n">
         <v>85</v>
@@ -2350,12 +2388,12 @@
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B7" t="n">
         <v>3</v>
@@ -2388,12 +2426,12 @@
         <v>0.27781</v>
       </c>
       <c r="L7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B8" t="n">
         <v>1</v>
@@ -2426,12 +2464,12 @@
         <v>0.00067</v>
       </c>
       <c r="L8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B9" t="n">
         <v>1</v>
@@ -2464,12 +2502,12 @@
         <v>0.00067</v>
       </c>
       <c r="L9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B10" t="n">
         <v>71</v>
@@ -2494,12 +2532,12 @@
       <c r="J10"/>
       <c r="K10"/>
       <c r="L10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B11" t="n">
         <v>76</v>
@@ -2524,12 +2562,12 @@
       <c r="J11"/>
       <c r="K11"/>
       <c r="L11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B12" t="n">
         <v>3</v>
@@ -2562,12 +2600,12 @@
         <v>0.00067</v>
       </c>
       <c r="L12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B13" t="n">
         <v>1</v>
@@ -2600,12 +2638,12 @@
         <v>0.00067</v>
       </c>
       <c r="L13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B14" t="n">
         <v>1</v>
@@ -2638,12 +2676,12 @@
         <v>0.48168</v>
       </c>
       <c r="L14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B15" t="n">
         <v>62</v>
@@ -2668,12 +2706,12 @@
       <c r="J15"/>
       <c r="K15"/>
       <c r="L15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B16" t="n">
         <v>67</v>
@@ -2698,7 +2736,7 @@
       <c r="J16"/>
       <c r="K16"/>
       <c r="L16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated boot for SSID and PSTR
</commit_message>
<xml_diff>
--- a/Data/Supplemental/Supplemental_Tables.xlsx
+++ b/Data/Supplemental/Supplemental_Tables.xlsx
@@ -774,25 +774,25 @@
         <v>13</v>
       </c>
       <c r="D8" t="n">
-        <v>110.7</v>
+        <v>105.6</v>
       </c>
       <c r="E8" t="n">
-        <v>128.3</v>
+        <v>121.5</v>
       </c>
       <c r="F8" t="n">
-        <v>0.4274</v>
+        <v>0.3969</v>
       </c>
       <c r="G8" t="n">
-        <v>0.3474</v>
+        <v>0.317</v>
       </c>
       <c r="H8" t="n">
-        <v>0.122629862821237</v>
+        <v>0.117033435887396</v>
       </c>
       <c r="I8" t="n">
-        <v>1.00977436829259</v>
+        <v>1.02875627247403</v>
       </c>
       <c r="J8" t="n">
-        <v>0.335974696337972</v>
+        <v>0.342860527251939</v>
       </c>
       <c r="K8" t="n">
         <v>71.4</v>
@@ -809,28 +809,28 @@
         <v>13</v>
       </c>
       <c r="D9" t="n">
-        <v>105.1</v>
+        <v>99.8</v>
       </c>
       <c r="E9" t="n">
-        <v>116.4</v>
+        <v>109.6</v>
       </c>
       <c r="F9" t="n">
-        <v>0.3271</v>
+        <v>0.2918</v>
       </c>
       <c r="G9" t="n">
-        <v>0.2594</v>
+        <v>0.2233</v>
       </c>
       <c r="H9" t="n">
-        <v>0.0914015570605844</v>
+        <v>0.0882187502302896</v>
       </c>
       <c r="I9" t="n">
-        <v>1.12817097438964</v>
+        <v>1.15145387403649</v>
       </c>
       <c r="J9" t="n">
-        <v>0.354967986837399</v>
+        <v>0.362141524711882</v>
       </c>
       <c r="K9" t="n">
-        <v>47.3</v>
+        <v>47.1</v>
       </c>
     </row>
     <row r="10">
@@ -844,28 +844,28 @@
         <v>13</v>
       </c>
       <c r="D10" t="n">
-        <v>106</v>
+        <v>100.8</v>
       </c>
       <c r="E10" t="n">
-        <v>118.6</v>
+        <v>111.8</v>
       </c>
       <c r="F10" t="n">
-        <v>0.3408</v>
+        <v>0.3093</v>
       </c>
       <c r="G10" t="n">
-        <v>0.2916</v>
+        <v>0.2614</v>
       </c>
       <c r="H10" t="n">
-        <v>0.0695117570012863</v>
+        <v>0.0648056876434838</v>
       </c>
       <c r="I10" t="n">
-        <v>1.12393984931601</v>
+        <v>1.14657450978296</v>
       </c>
       <c r="J10" t="n">
-        <v>0.353702872301073</v>
+        <v>0.36062662799942</v>
       </c>
       <c r="K10" t="n">
-        <v>44.8</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11">
@@ -879,28 +879,28 @@
         <v>13</v>
       </c>
       <c r="D11" t="n">
-        <v>106.9</v>
+        <v>101.6</v>
       </c>
       <c r="E11" t="n">
-        <v>119.5</v>
+        <v>112.6</v>
       </c>
       <c r="F11" t="n">
-        <v>0.3131</v>
+        <v>0.2784</v>
       </c>
       <c r="G11" t="n">
-        <v>0.2714</v>
+        <v>0.2378</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0572627664145912</v>
+        <v>0.0533714820211562</v>
       </c>
       <c r="I11" t="n">
-        <v>1.11383231900867</v>
+        <v>1.13665595795787</v>
       </c>
       <c r="J11" t="n">
-        <v>0.352824835250314</v>
+        <v>0.359834556845443</v>
       </c>
       <c r="K11" t="n">
-        <v>36.3</v>
+        <v>36.2</v>
       </c>
     </row>
     <row r="12">
@@ -914,28 +914,28 @@
         <v>13</v>
       </c>
       <c r="D12" t="n">
-        <v>102.8</v>
+        <v>97.5</v>
       </c>
       <c r="E12" t="n">
-        <v>111.6</v>
+        <v>104.8</v>
       </c>
       <c r="F12" t="n">
-        <v>0.2678</v>
+        <v>0.232</v>
       </c>
       <c r="G12" t="n">
-        <v>0.2243</v>
+        <v>0.188</v>
       </c>
       <c r="H12" t="n">
-        <v>0.0560480703765206</v>
+        <v>0.0541808464958402</v>
       </c>
       <c r="I12" t="n">
-        <v>1.19677569359115</v>
+        <v>1.22142050234447</v>
       </c>
       <c r="J12" t="n">
-        <v>0.364087168175548</v>
+        <v>0.371319943278335</v>
       </c>
       <c r="K12" t="n">
-        <v>28.6</v>
+        <v>28.8</v>
       </c>
     </row>
     <row r="13">
@@ -1745,10 +1745,10 @@
         <v>1.279</v>
       </c>
       <c r="C11" t="n">
-        <v>0.145</v>
+        <v>0.148</v>
       </c>
       <c r="D11" t="n">
-        <v>8.8</v>
+        <v>8.66</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -1762,16 +1762,16 @@
         <v>29</v>
       </c>
       <c r="B12" t="n">
-        <v>0.194</v>
+        <v>-0.338</v>
       </c>
       <c r="C12" t="n">
-        <v>0.418</v>
+        <v>0.193</v>
       </c>
       <c r="D12" t="n">
-        <v>0.46</v>
+        <v>-1.75</v>
       </c>
       <c r="E12" t="n">
-        <v>0.643</v>
+        <v>0.08</v>
       </c>
       <c r="F12" t="s">
         <v>35</v>
@@ -1779,19 +1779,19 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.339</v>
+        <v>-0.059</v>
       </c>
       <c r="C13" t="n">
-        <v>0.19</v>
+        <v>0.187</v>
       </c>
       <c r="D13" t="n">
-        <v>-1.79</v>
+        <v>-0.31</v>
       </c>
       <c r="E13" t="n">
-        <v>0.074</v>
+        <v>0.753</v>
       </c>
       <c r="F13" t="s">
         <v>35</v>
@@ -1799,19 +1799,19 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.06</v>
+        <v>0.227</v>
       </c>
       <c r="C14" t="n">
-        <v>0.184</v>
+        <v>0.173</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.32</v>
+        <v>1.31</v>
       </c>
       <c r="E14" t="n">
-        <v>0.746</v>
+        <v>0.19</v>
       </c>
       <c r="F14" t="s">
         <v>35</v>
@@ -1819,39 +1819,39 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B15" t="n">
-        <v>0.226</v>
+        <v>1.038</v>
       </c>
       <c r="C15" t="n">
-        <v>0.17</v>
+        <v>0.121</v>
       </c>
       <c r="D15" t="n">
-        <v>1.33</v>
+        <v>8.61</v>
       </c>
       <c r="E15" t="n">
-        <v>0.183</v>
+        <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B16" t="n">
-        <v>1.038</v>
+        <v>-0.047</v>
       </c>
       <c r="C16" t="n">
-        <v>0.121</v>
+        <v>0.11</v>
       </c>
       <c r="D16" t="n">
-        <v>8.61</v>
+        <v>-0.43</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>0.67</v>
       </c>
       <c r="F16" t="s">
         <v>36</v>
@@ -1862,16 +1862,16 @@
         <v>29</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.047</v>
+        <v>0.032</v>
       </c>
       <c r="C17" t="n">
-        <v>0.11</v>
+        <v>0.075</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.43</v>
+        <v>0.44</v>
       </c>
       <c r="E17" t="n">
-        <v>0.67</v>
+        <v>0.664</v>
       </c>
       <c r="F17" t="s">
         <v>36</v>
@@ -1879,19 +1879,19 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B18" t="n">
-        <v>0.032</v>
+        <v>0.122</v>
       </c>
       <c r="C18" t="n">
-        <v>0.075</v>
+        <v>0.078</v>
       </c>
       <c r="D18" t="n">
-        <v>0.44</v>
+        <v>1.57</v>
       </c>
       <c r="E18" t="n">
-        <v>0.664</v>
+        <v>0.116</v>
       </c>
       <c r="F18" t="s">
         <v>36</v>
@@ -1899,41 +1899,21 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B19" t="n">
-        <v>0.122</v>
+        <v>0.264</v>
       </c>
       <c r="C19" t="n">
-        <v>0.078</v>
+        <v>0.065</v>
       </c>
       <c r="D19" t="n">
-        <v>1.57</v>
+        <v>4.07</v>
       </c>
       <c r="E19" t="n">
-        <v>0.116</v>
+        <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" t="n">
-        <v>0.264</v>
-      </c>
-      <c r="C20" t="n">
-        <v>0.065</v>
-      </c>
-      <c r="D20" t="n">
-        <v>4.07</v>
-      </c>
-      <c r="E20" t="n">
-        <v>0</v>
-      </c>
-      <c r="F20" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
boot plasticity of all species
</commit_message>
<xml_diff>
--- a/Data/Supplemental/Supplemental_Tables.xlsx
+++ b/Data/Supplemental/Supplemental_Tables.xlsx
@@ -1234,7 +1234,7 @@
         <v>2.99</v>
       </c>
       <c r="F3" t="n">
-        <v>0.08728</v>
+        <v>0.09127</v>
       </c>
       <c r="G3" t="s">
         <v>30</v>
@@ -1257,7 +1257,7 @@
         <v>9.89</v>
       </c>
       <c r="F4" t="n">
-        <v>0.002</v>
+        <v>0.00133</v>
       </c>
       <c r="G4" t="s">
         <v>30</v>
@@ -1364,7 +1364,7 @@
         <v>1.48</v>
       </c>
       <c r="F9" t="n">
-        <v>0.25916</v>
+        <v>0.23651</v>
       </c>
       <c r="G9" t="s">
         <v>35</v>
@@ -1425,7 +1425,7 @@
         <v>0.11</v>
       </c>
       <c r="F12" t="n">
-        <v>0.76016</v>
+        <v>0.74151</v>
       </c>
       <c r="G12" t="s">
         <v>36</v>
@@ -1471,7 +1471,7 @@
         <v>7.4</v>
       </c>
       <c r="F14" t="n">
-        <v>0.00133</v>
+        <v>0.00067</v>
       </c>
       <c r="G14" t="s">
         <v>36</v>
@@ -1996,7 +1996,7 @@
         <v>2.87</v>
       </c>
       <c r="F3" t="n">
-        <v>0.09194</v>
+        <v>0.09327</v>
       </c>
     </row>
     <row r="4">
@@ -2016,7 +2016,7 @@
         <v>9.61</v>
       </c>
       <c r="F4" t="n">
-        <v>0.004</v>
+        <v>0.00466</v>
       </c>
     </row>
     <row r="5">
@@ -2076,7 +2076,7 @@
         <v>2.51</v>
       </c>
       <c r="F7" t="n">
-        <v>0.01732</v>
+        <v>0.02398</v>
       </c>
     </row>
     <row r="8">
@@ -2096,7 +2096,7 @@
         <v>6.39</v>
       </c>
       <c r="F8" t="n">
-        <v>0.00466</v>
+        <v>0.004</v>
       </c>
     </row>
     <row r="9">
@@ -2214,7 +2214,7 @@
         <v>0.55</v>
       </c>
       <c r="F2" t="n">
-        <v>0.74883</v>
+        <v>0.74284</v>
       </c>
       <c r="G2" t="n">
         <v>3</v>
@@ -2252,7 +2252,7 @@
         <v>6.65</v>
       </c>
       <c r="F3" t="n">
-        <v>0.004</v>
+        <v>0.00333</v>
       </c>
       <c r="G3" t="n">
         <v>1</v>
@@ -2267,7 +2267,7 @@
         <v>2.99</v>
       </c>
       <c r="K3" t="n">
-        <v>0.08461</v>
+        <v>0.09927</v>
       </c>
       <c r="L3" t="s">
         <v>30</v>
@@ -2290,7 +2290,7 @@
         <v>0.52</v>
       </c>
       <c r="F4" t="n">
-        <v>0.58294</v>
+        <v>0.56829</v>
       </c>
       <c r="G4" t="n">
         <v>1</v>
@@ -2388,7 +2388,7 @@
         <v>1.23</v>
       </c>
       <c r="F7" t="n">
-        <v>0.28714</v>
+        <v>0.30513</v>
       </c>
       <c r="G7" t="n">
         <v>3</v>
@@ -2403,7 +2403,7 @@
         <v>1.31</v>
       </c>
       <c r="K7" t="n">
-        <v>0.27781</v>
+        <v>0.27981</v>
       </c>
       <c r="L7" t="s">
         <v>35</v>
@@ -2464,7 +2464,7 @@
         <v>1.75</v>
       </c>
       <c r="F9" t="n">
-        <v>0.15923</v>
+        <v>0.15656</v>
       </c>
       <c r="G9" t="n">
         <v>1</v>
@@ -2562,7 +2562,7 @@
         <v>3.48</v>
       </c>
       <c r="F12" t="n">
-        <v>0.01865</v>
+        <v>0.01532</v>
       </c>
       <c r="G12" t="n">
         <v>3</v>
@@ -2577,7 +2577,7 @@
         <v>7.04</v>
       </c>
       <c r="K12" t="n">
-        <v>0.00067</v>
+        <v>0.00133</v>
       </c>
       <c r="L12" t="s">
         <v>36</v>
@@ -2600,7 +2600,7 @@
         <v>2.76</v>
       </c>
       <c r="F13" t="n">
-        <v>0.1006</v>
+        <v>0.08195</v>
       </c>
       <c r="G13" t="n">
         <v>1</v>
@@ -2638,7 +2638,7 @@
         <v>1.64</v>
       </c>
       <c r="F14" t="n">
-        <v>0.20053</v>
+        <v>0.17988</v>
       </c>
       <c r="G14" t="n">
         <v>1</v>
@@ -2653,7 +2653,7 @@
         <v>0.53</v>
       </c>
       <c r="K14" t="n">
-        <v>0.48168</v>
+        <v>0.47901</v>
       </c>
       <c r="L14" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
update to plasticity AIC table
</commit_message>
<xml_diff>
--- a/Data/Supplemental/Supplemental_Tables.xlsx
+++ b/Data/Supplemental/Supplemental_Tables.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t xml:space="preserve">Species</t>
   </si>
@@ -76,9 +76,6 @@
   </si>
   <si>
     <t xml:space="preserve">pstr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reef environment * pCO2 * temperature + (1 | colony)7</t>
   </si>
   <si>
     <t xml:space="preserve">past</t>
@@ -570,10 +567,10 @@
         <v>243.5</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5059</v>
+        <v>0.506</v>
       </c>
       <c r="G2" t="n">
-        <v>0.3225</v>
+        <v>0.322</v>
       </c>
       <c r="H2" t="n">
         <v>0.270712896490855</v>
@@ -605,10 +602,10 @@
         <v>259.2</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5445</v>
+        <v>0.545</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3656</v>
+        <v>0.366</v>
       </c>
       <c r="H3" t="n">
         <v>0.28206734361165</v>
@@ -640,10 +637,10 @@
         <v>247.1</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5115</v>
+        <v>0.512</v>
       </c>
       <c r="G4" t="n">
-        <v>0.3288</v>
+        <v>0.329</v>
       </c>
       <c r="H4" t="n">
         <v>0.272192941547414</v>
@@ -675,10 +672,10 @@
         <v>239.6</v>
       </c>
       <c r="F5" t="n">
-        <v>0.4419</v>
+        <v>0.442</v>
       </c>
       <c r="G5" t="n">
-        <v>0.2535</v>
+        <v>0.254</v>
       </c>
       <c r="H5" t="n">
         <v>0.252287908819288</v>
@@ -710,10 +707,10 @@
         <v>237.8</v>
       </c>
       <c r="F6" t="n">
-        <v>0.3698</v>
+        <v>0.37</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0882</v>
+        <v>0.088</v>
       </c>
       <c r="H6" t="n">
         <v>0.308813847521209</v>
@@ -745,10 +742,10 @@
         <v>248.1</v>
       </c>
       <c r="F7" t="n">
-        <v>0.4421</v>
+        <v>0.442</v>
       </c>
       <c r="G7" t="n">
-        <v>0.2534</v>
+        <v>0.253</v>
       </c>
       <c r="H7" t="n">
         <v>0.252780589487017</v>
@@ -780,7 +777,7 @@
         <v>121.5</v>
       </c>
       <c r="F8" t="n">
-        <v>0.3969</v>
+        <v>0.397</v>
       </c>
       <c r="G8" t="n">
         <v>0.317</v>
@@ -803,34 +800,34 @@
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
         <v>13</v>
       </c>
       <c r="D9" t="n">
-        <v>99.8</v>
+        <v>100.8</v>
       </c>
       <c r="E9" t="n">
-        <v>109.6</v>
+        <v>111.8</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2918</v>
+        <v>0.309</v>
       </c>
       <c r="G9" t="n">
-        <v>0.2233</v>
+        <v>0.261</v>
       </c>
       <c r="H9" t="n">
-        <v>0.0882187502302896</v>
+        <v>0.0648056876434838</v>
       </c>
       <c r="I9" t="n">
-        <v>1.15145387403649</v>
+        <v>1.14657450978296</v>
       </c>
       <c r="J9" t="n">
-        <v>0.362141524711882</v>
+        <v>0.36062662799942</v>
       </c>
       <c r="K9" t="n">
-        <v>47.1</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10">
@@ -838,34 +835,34 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
       </c>
       <c r="D10" t="n">
-        <v>100.8</v>
+        <v>101.6</v>
       </c>
       <c r="E10" t="n">
-        <v>111.8</v>
+        <v>112.6</v>
       </c>
       <c r="F10" t="n">
-        <v>0.3093</v>
+        <v>0.278</v>
       </c>
       <c r="G10" t="n">
-        <v>0.2614</v>
+        <v>0.238</v>
       </c>
       <c r="H10" t="n">
-        <v>0.0648056876434838</v>
+        <v>0.0533714820211562</v>
       </c>
       <c r="I10" t="n">
-        <v>1.14657450978296</v>
+        <v>1.13665595795787</v>
       </c>
       <c r="J10" t="n">
-        <v>0.36062662799942</v>
+        <v>0.359834556845443</v>
       </c>
       <c r="K10" t="n">
-        <v>45</v>
+        <v>36.2</v>
       </c>
     </row>
     <row r="11">
@@ -873,278 +870,243 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
         <v>13</v>
       </c>
       <c r="D11" t="n">
-        <v>101.6</v>
+        <v>97.5</v>
       </c>
       <c r="E11" t="n">
-        <v>112.6</v>
+        <v>104.8</v>
       </c>
       <c r="F11" t="n">
-        <v>0.2784</v>
+        <v>0.232</v>
       </c>
       <c r="G11" t="n">
-        <v>0.2378</v>
+        <v>0.188</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0533714820211562</v>
+        <v>0.0541808464958402</v>
       </c>
       <c r="I11" t="n">
-        <v>1.13665595795787</v>
+        <v>1.22142050234447</v>
       </c>
       <c r="J11" t="n">
-        <v>0.359834556845443</v>
+        <v>0.371319943278335</v>
       </c>
       <c r="K11" t="n">
-        <v>36.2</v>
+        <v>28.8</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
         <v>13</v>
       </c>
       <c r="D12" t="n">
-        <v>97.5</v>
+        <v>145.9</v>
       </c>
       <c r="E12" t="n">
-        <v>104.8</v>
+        <v>167.8</v>
       </c>
       <c r="F12" t="n">
-        <v>0.232</v>
+        <v>0.521</v>
       </c>
       <c r="G12" t="n">
-        <v>0.188</v>
+        <v>0.195</v>
       </c>
       <c r="H12" t="n">
-        <v>0.0541808464958402</v>
+        <v>0.405142468828212</v>
       </c>
       <c r="I12" t="n">
-        <v>1.22142050234447</v>
+        <v>0.710112914386074</v>
       </c>
       <c r="J12" t="n">
-        <v>0.371319943278335</v>
+        <v>0.231080473857171</v>
       </c>
       <c r="K12" t="n">
-        <v>28.8</v>
+        <v>76.2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
         <v>13</v>
       </c>
       <c r="D13" t="n">
-        <v>145.9</v>
+        <v>147.9</v>
       </c>
       <c r="E13" t="n">
-        <v>167.8</v>
+        <v>171.8</v>
       </c>
       <c r="F13" t="n">
-        <v>0.5212</v>
+        <v>0.522</v>
       </c>
       <c r="G13" t="n">
         <v>0.195</v>
       </c>
       <c r="H13" t="n">
-        <v>0.405142468828212</v>
+        <v>0.405616901906066</v>
       </c>
       <c r="I13" t="n">
-        <v>0.710112914386074</v>
+        <v>0.70994797179576</v>
       </c>
       <c r="J13" t="n">
-        <v>0.231080473857171</v>
+        <v>0.2309514006937</v>
       </c>
       <c r="K13" t="n">
-        <v>76.2</v>
+        <v>72.9</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
       </c>
       <c r="D14" t="n">
-        <v>147.9</v>
+        <v>153.1</v>
       </c>
       <c r="E14" t="n">
-        <v>171.8</v>
+        <v>182.9</v>
       </c>
       <c r="F14" t="n">
-        <v>0.5217</v>
+        <v>0.527</v>
       </c>
       <c r="G14" t="n">
-        <v>0.1952</v>
+        <v>0.199</v>
       </c>
       <c r="H14" t="n">
-        <v>0.405616901906066</v>
+        <v>0.409641424663849</v>
       </c>
       <c r="I14" t="n">
-        <v>0.70994797179576</v>
+        <v>0.706971647584522</v>
       </c>
       <c r="J14" t="n">
-        <v>0.2309514006937</v>
+        <v>0.229916347449218</v>
       </c>
       <c r="K14" t="n">
-        <v>72.9</v>
+        <v>71.4</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
         <v>13</v>
       </c>
       <c r="D15" t="n">
-        <v>153.1</v>
+        <v>142.3</v>
       </c>
       <c r="E15" t="n">
-        <v>182.9</v>
+        <v>158.2</v>
       </c>
       <c r="F15" t="n">
-        <v>0.5273</v>
+        <v>0.499</v>
       </c>
       <c r="G15" t="n">
-        <v>0.1994</v>
+        <v>0.174</v>
       </c>
       <c r="H15" t="n">
-        <v>0.409641424663849</v>
+        <v>0.393286215931064</v>
       </c>
       <c r="I15" t="n">
-        <v>0.706971647584522</v>
+        <v>0.733244393163204</v>
       </c>
       <c r="J15" t="n">
-        <v>0.229916347449218</v>
+        <v>0.237295448325152</v>
       </c>
       <c r="K15" t="n">
-        <v>71.4</v>
+        <v>38.4</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
       </c>
       <c r="D16" t="n">
-        <v>142.3</v>
+        <v>140.4</v>
       </c>
       <c r="E16" t="n">
-        <v>158.2</v>
+        <v>154.4</v>
       </c>
       <c r="F16" t="n">
-        <v>0.4988</v>
+        <v>0.485</v>
       </c>
       <c r="G16" t="n">
-        <v>0.1738</v>
+        <v>0.147</v>
       </c>
       <c r="H16" t="n">
-        <v>0.393286215931064</v>
+        <v>0.396708536729162</v>
       </c>
       <c r="I16" t="n">
-        <v>0.733244393163204</v>
+        <v>0.732981216119454</v>
       </c>
       <c r="J16" t="n">
-        <v>0.237295448325152</v>
+        <v>0.238221370319828</v>
       </c>
       <c r="K16" t="n">
-        <v>38.4</v>
+        <v>32.1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
         <v>13</v>
       </c>
       <c r="D17" t="n">
-        <v>140.4</v>
+        <v>146.2</v>
       </c>
       <c r="E17" t="n">
-        <v>154.4</v>
+        <v>166.1</v>
       </c>
       <c r="F17" t="n">
-        <v>0.4853</v>
+        <v>0.5</v>
       </c>
       <c r="G17" t="n">
-        <v>0.1469</v>
+        <v>0.174</v>
       </c>
       <c r="H17" t="n">
-        <v>0.396708536729162</v>
+        <v>0.394015465922658</v>
       </c>
       <c r="I17" t="n">
-        <v>0.732981216119454</v>
+        <v>0.734046668651323</v>
       </c>
       <c r="J17" t="n">
-        <v>0.238221370319828</v>
+        <v>0.237351188594544</v>
       </c>
       <c r="K17" t="n">
-        <v>32.1</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" t="n">
-        <v>146.2</v>
-      </c>
-      <c r="E18" t="n">
-        <v>166.1</v>
-      </c>
-      <c r="F18" t="n">
-        <v>0.4995</v>
-      </c>
-      <c r="G18" t="n">
-        <v>0.1741</v>
-      </c>
-      <c r="H18" t="n">
-        <v>0.394015465922658</v>
-      </c>
-      <c r="I18" t="n">
-        <v>0.734046668651323</v>
-      </c>
-      <c r="J18" t="n">
-        <v>0.237351188594544</v>
-      </c>
-      <c r="K18" t="n">
         <v>30.5</v>
       </c>
     </row>
@@ -1173,30 +1135,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>26</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>27</v>
-      </c>
-      <c r="G1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -1214,12 +1176,12 @@
         <v>0.00067</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -1237,12 +1199,12 @@
         <v>0.09127</v>
       </c>
       <c r="G3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -1260,12 +1222,12 @@
         <v>0.00133</v>
       </c>
       <c r="G4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" t="n">
         <v>80</v>
@@ -1279,12 +1241,12 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" t="n">
         <v>85</v>
@@ -1298,12 +1260,12 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" t="n">
         <v>1</v>
@@ -1321,12 +1283,12 @@
         <v>0.00067</v>
       </c>
       <c r="G7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" t="n">
         <v>1</v>
@@ -1344,12 +1306,12 @@
         <v>0.00067</v>
       </c>
       <c r="G8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" t="n">
         <v>3</v>
@@ -1367,12 +1329,12 @@
         <v>0.23651</v>
       </c>
       <c r="G9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" t="n">
         <v>71</v>
@@ -1386,12 +1348,12 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" t="n">
         <v>76</v>
@@ -1405,12 +1367,12 @@
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" t="n">
         <v>1</v>
@@ -1428,12 +1390,12 @@
         <v>0.74151</v>
       </c>
       <c r="G12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" t="n">
         <v>1</v>
@@ -1451,12 +1413,12 @@
         <v>0.00067</v>
       </c>
       <c r="G13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" t="n">
         <v>3</v>
@@ -1474,12 +1436,12 @@
         <v>0.00067</v>
       </c>
       <c r="G14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" t="n">
         <v>62</v>
@@ -1493,12 +1455,12 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16" t="n">
         <v>67</v>
@@ -1512,7 +1474,7 @@
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1539,27 +1501,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" t="s">
-        <v>39</v>
-      </c>
       <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
         <v>27</v>
-      </c>
-      <c r="F1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" t="n">
         <v>1.085</v>
@@ -1574,12 +1536,12 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" t="n">
         <v>-0.058</v>
@@ -1594,12 +1556,12 @@
         <v>0.814</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" t="n">
         <v>0.335</v>
@@ -1614,12 +1576,12 @@
         <v>0.053</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" t="n">
         <v>0.21</v>
@@ -1634,12 +1596,12 @@
         <v>0.109</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" t="n">
         <v>0.419</v>
@@ -1654,12 +1616,12 @@
         <v>0.002</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" t="n">
         <v>0.003</v>
@@ -1674,12 +1636,12 @@
         <v>0.967</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" t="n">
         <v>-0.704</v>
@@ -1694,12 +1656,12 @@
         <v>0.003</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" t="n">
         <v>-0.409</v>
@@ -1714,12 +1676,12 @@
         <v>0.037</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" t="n">
         <v>-0.278</v>
@@ -1734,12 +1696,12 @@
         <v>0.146</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" t="n">
         <v>1.279</v>
@@ -1754,12 +1716,12 @@
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" t="n">
         <v>-0.338</v>
@@ -1774,12 +1736,12 @@
         <v>0.08</v>
       </c>
       <c r="F12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13" t="n">
         <v>-0.059</v>
@@ -1794,12 +1756,12 @@
         <v>0.753</v>
       </c>
       <c r="F13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" t="n">
         <v>0.227</v>
@@ -1814,12 +1776,12 @@
         <v>0.19</v>
       </c>
       <c r="F14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" t="n">
         <v>1.038</v>
@@ -1834,12 +1796,12 @@
         <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" t="n">
         <v>-0.047</v>
@@ -1854,12 +1816,12 @@
         <v>0.67</v>
       </c>
       <c r="F16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" t="n">
         <v>0.032</v>
@@ -1874,12 +1836,12 @@
         <v>0.664</v>
       </c>
       <c r="F17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" t="n">
         <v>0.122</v>
@@ -1894,12 +1856,12 @@
         <v>0.116</v>
       </c>
       <c r="F18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" t="n">
         <v>0.264</v>
@@ -1914,7 +1876,7 @@
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1941,27 +1903,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>26</v>
-      </c>
-      <c r="F1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -1981,7 +1943,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -2001,7 +1963,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -2021,7 +1983,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" t="n">
         <v>2</v>
@@ -2041,7 +2003,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" t="n">
         <v>2</v>
@@ -2061,7 +2023,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" t="n">
         <v>6</v>
@@ -2081,7 +2043,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" t="n">
         <v>2</v>
@@ -2101,7 +2063,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" t="n">
         <v>214</v>
@@ -2117,7 +2079,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" t="n">
         <v>231</v>
@@ -2161,45 +2123,45 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>26</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" t="s">
         <v>27</v>
-      </c>
-      <c r="G1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J1" t="s">
-        <v>52</v>
-      </c>
-      <c r="K1" t="s">
-        <v>53</v>
-      </c>
-      <c r="L1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -2214,7 +2176,7 @@
         <v>0.55</v>
       </c>
       <c r="F2" t="n">
-        <v>0.74284</v>
+        <v>0.74217</v>
       </c>
       <c r="G2" t="n">
         <v>3</v>
@@ -2232,12 +2194,12 @@
         <v>0.00067</v>
       </c>
       <c r="L2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -2270,12 +2232,12 @@
         <v>0.09927</v>
       </c>
       <c r="L3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -2290,7 +2252,7 @@
         <v>0.52</v>
       </c>
       <c r="F4" t="n">
-        <v>0.56829</v>
+        <v>0.56762</v>
       </c>
       <c r="G4" t="n">
         <v>1</v>
@@ -2308,12 +2270,12 @@
         <v>0.002</v>
       </c>
       <c r="L4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" t="n">
         <v>80</v>
@@ -2338,12 +2300,12 @@
       <c r="J5"/>
       <c r="K5"/>
       <c r="L5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" t="n">
         <v>85</v>
@@ -2368,12 +2330,12 @@
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" t="n">
         <v>3</v>
@@ -2406,12 +2368,12 @@
         <v>0.27981</v>
       </c>
       <c r="L7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" t="n">
         <v>1</v>
@@ -2444,12 +2406,12 @@
         <v>0.00067</v>
       </c>
       <c r="L8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" t="n">
         <v>1</v>
@@ -2482,12 +2444,12 @@
         <v>0.00067</v>
       </c>
       <c r="L9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" t="n">
         <v>71</v>
@@ -2512,12 +2474,12 @@
       <c r="J10"/>
       <c r="K10"/>
       <c r="L10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" t="n">
         <v>76</v>
@@ -2542,12 +2504,12 @@
       <c r="J11"/>
       <c r="K11"/>
       <c r="L11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" t="n">
         <v>3</v>
@@ -2580,12 +2542,12 @@
         <v>0.00133</v>
       </c>
       <c r="L12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" t="n">
         <v>1</v>
@@ -2618,12 +2580,12 @@
         <v>0.00067</v>
       </c>
       <c r="L13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" t="n">
         <v>1</v>
@@ -2656,12 +2618,12 @@
         <v>0.47901</v>
       </c>
       <c r="L14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" t="n">
         <v>62</v>
@@ -2686,12 +2648,12 @@
       <c r="J15"/>
       <c r="K15"/>
       <c r="L15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16" t="n">
         <v>67</v>
@@ -2716,7 +2678,7 @@
       <c r="J16"/>
       <c r="K16"/>
       <c r="L16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bootstrapped symb v host plasticity
</commit_message>
<xml_diff>
--- a/Data/Supplemental/Supplemental_Tables.xlsx
+++ b/Data/Supplemental/Supplemental_Tables.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t xml:space="preserve">Species</t>
   </si>
@@ -135,10 +135,16 @@
     <t xml:space="preserve">Statistic</t>
   </si>
   <si>
-    <t xml:space="preserve">Intercept</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reef environment (offshore) </t>
+    <t xml:space="preserve">(Intercept)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reef environment (offshore)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pCO2-current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pCO2-EOC</t>
   </si>
   <si>
     <t xml:space="preserve">pCO2-extreme</t>
@@ -147,10 +153,13 @@
     <t xml:space="preserve">temperature (31C)</t>
   </si>
   <si>
-    <t xml:space="preserve">reef environment (offshore) pCO2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reef environment (offshore) pCO2-extreme</t>
+    <t xml:space="preserve">reef environment (offshore):pCO2-current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reef environment (offshore):pCO2-EOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reef environment (offshore):pCO2-extreme</t>
   </si>
   <si>
     <t xml:space="preserve">temperature:species</t>
@@ -1561,7 +1570,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="B4" t="n">
         <v>0.335</v>
@@ -1581,7 +1590,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B5" t="n">
         <v>0.21</v>
@@ -1601,7 +1610,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B6" t="n">
         <v>0.419</v>
@@ -1621,7 +1630,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B7" t="n">
         <v>0.003</v>
@@ -1641,7 +1650,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B8" t="n">
         <v>-0.704</v>
@@ -1661,7 +1670,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B9" t="n">
         <v>-0.409</v>
@@ -1681,7 +1690,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B10" t="n">
         <v>-0.278</v>
@@ -1701,59 +1710,47 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="B11" t="n">
-        <v>1.279</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.148</v>
-      </c>
-      <c r="D11" t="n">
-        <v>8.66</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
+        <v>0.506</v>
+      </c>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
       <c r="F11" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.338</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0.193</v>
-      </c>
-      <c r="D12" t="n">
-        <v>-1.75</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.08</v>
-      </c>
+        <v>0.322</v>
+      </c>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
       <c r="F12" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.059</v>
+        <v>1.279</v>
       </c>
       <c r="C13" t="n">
-        <v>0.187</v>
+        <v>0.148</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.31</v>
+        <v>8.66</v>
       </c>
       <c r="E13" t="n">
-        <v>0.753</v>
+        <v>0</v>
       </c>
       <c r="F13" t="s">
         <v>34</v>
@@ -1764,16 +1761,16 @@
         <v>42</v>
       </c>
       <c r="B14" t="n">
-        <v>0.227</v>
+        <v>-0.338</v>
       </c>
       <c r="C14" t="n">
-        <v>0.173</v>
+        <v>0.193</v>
       </c>
       <c r="D14" t="n">
-        <v>1.31</v>
+        <v>-1.75</v>
       </c>
       <c r="E14" t="n">
-        <v>0.19</v>
+        <v>0.08</v>
       </c>
       <c r="F14" t="s">
         <v>34</v>
@@ -1781,101 +1778,197 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B15" t="n">
-        <v>1.038</v>
+        <v>-0.059</v>
       </c>
       <c r="C15" t="n">
-        <v>0.121</v>
+        <v>0.187</v>
       </c>
       <c r="D15" t="n">
-        <v>8.61</v>
+        <v>-0.31</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>0.753</v>
       </c>
       <c r="F15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.047</v>
+        <v>0.227</v>
       </c>
       <c r="C16" t="n">
-        <v>0.11</v>
+        <v>0.173</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.43</v>
+        <v>1.31</v>
       </c>
       <c r="E16" t="n">
-        <v>0.67</v>
+        <v>0.19</v>
       </c>
       <c r="F16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="B17" t="n">
-        <v>0.032</v>
-      </c>
-      <c r="C17" t="n">
-        <v>0.075</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0.664</v>
-      </c>
+        <v>0.232</v>
+      </c>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
       <c r="F17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="B18" t="n">
-        <v>0.122</v>
-      </c>
-      <c r="C18" t="n">
-        <v>0.078</v>
-      </c>
-      <c r="D18" t="n">
-        <v>1.57</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0.116</v>
-      </c>
+        <v>0.188</v>
+      </c>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
       <c r="F18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B19" t="n">
-        <v>0.264</v>
+        <v>1.038</v>
       </c>
       <c r="C19" t="n">
-        <v>0.065</v>
+        <v>0.121</v>
       </c>
       <c r="D19" t="n">
-        <v>4.07</v>
+        <v>8.61</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
       </c>
       <c r="F19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" t="n">
+        <v>-0.047</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="D20" t="n">
+        <v>-0.43</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="F20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0.032</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.075</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.664</v>
+      </c>
+      <c r="F21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0.122</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.078</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.116</v>
+      </c>
+      <c r="F22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0.264</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.065</v>
+      </c>
+      <c r="D23" t="n">
+        <v>4.07</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0.485</v>
+      </c>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0.147</v>
+      </c>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2003,7 +2096,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B6" t="n">
         <v>2</v>
@@ -2023,7 +2116,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B7" t="n">
         <v>6</v>
@@ -2043,7 +2136,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B8" t="n">
         <v>2</v>
@@ -2141,19 +2234,19 @@
         <v>26</v>
       </c>
       <c r="G1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="H1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="I1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="J1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="K1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="L1" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
added symb v host plasticity tables
</commit_message>
<xml_diff>
--- a/Data/Supplemental/Supplemental_Tables.xlsx
+++ b/Data/Supplemental/Supplemental_Tables.xlsx
@@ -11,6 +11,8 @@
     <sheet name="Table S3 - Plasticity GLM" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Table S4 - Species PERMANOVA" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Table S5 - HostVsymb PERMANOVA" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Table S6 - HostVsymb Plast AIC" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Table S7 - HostVsymb Plast GLM" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
 </workbook>
 </file>
@@ -2778,4 +2780,1169 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <cols>
+    <col min="1" max="1" width="16.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="3.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="14.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="5.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="5.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="7.71" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="3.71" hidden="0" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.74217</v>
+      </c>
+      <c r="G2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2" t="n">
+        <v>61056</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.208</v>
+      </c>
+      <c r="J2" t="n">
+        <v>8.15</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.00067</v>
+      </c>
+      <c r="L2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.075</v>
+      </c>
+      <c r="E3" t="n">
+        <v>6.65</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.00333</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" t="n">
+        <v>7468</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="J3" t="n">
+        <v>2.99</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.09927</v>
+      </c>
+      <c r="L3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.56762</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" t="n">
+        <v>24705</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.084</v>
+      </c>
+      <c r="J4" t="n">
+        <v>9.9</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="L4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="n">
+        <v>80</v>
+      </c>
+      <c r="C5" t="n">
+        <v>30</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.901</v>
+      </c>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5" t="n">
+        <v>80</v>
+      </c>
+      <c r="H5" t="n">
+        <v>199684</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.682</v>
+      </c>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="n">
+        <v>85</v>
+      </c>
+      <c r="C6" t="n">
+        <v>34</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6" t="n">
+        <v>85</v>
+      </c>
+      <c r="H6" t="n">
+        <v>292913</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.041</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.30513</v>
+      </c>
+      <c r="G7" t="n">
+        <v>3</v>
+      </c>
+      <c r="H7" t="n">
+        <v>26899</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.024</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1.31</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.27981</v>
+      </c>
+      <c r="L7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.147</v>
+      </c>
+      <c r="E8" t="n">
+        <v>13.12</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.00067</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" t="n">
+        <v>515173</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.456</v>
+      </c>
+      <c r="J8" t="n">
+        <v>75.24</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.00067</v>
+      </c>
+      <c r="L8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.15656</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" t="n">
+        <v>101793</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="J9" t="n">
+        <v>14.87</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.00067</v>
+      </c>
+      <c r="L9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="n">
+        <v>71</v>
+      </c>
+      <c r="C10" t="n">
+        <v>14</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.793</v>
+      </c>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10" t="n">
+        <v>71</v>
+      </c>
+      <c r="H10" t="n">
+        <v>486140</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="n">
+        <v>76</v>
+      </c>
+      <c r="C11" t="n">
+        <v>18</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11" t="n">
+        <v>76</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1130005</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="n">
+        <v>3</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.136</v>
+      </c>
+      <c r="E12" t="n">
+        <v>3.48</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.01532</v>
+      </c>
+      <c r="G12" t="n">
+        <v>3</v>
+      </c>
+      <c r="H12" t="n">
+        <v>29037</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.205</v>
+      </c>
+      <c r="J12" t="n">
+        <v>7.04</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.00133</v>
+      </c>
+      <c r="L12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.036</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2.76</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.08195</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" t="n">
+        <v>26338</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.186</v>
+      </c>
+      <c r="J13" t="n">
+        <v>19.15</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.00067</v>
+      </c>
+      <c r="L13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.021</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1.64</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.17988</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" t="n">
+        <v>724</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.47901</v>
+      </c>
+      <c r="L14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="n">
+        <v>62</v>
+      </c>
+      <c r="C15" t="n">
+        <v>10</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.807</v>
+      </c>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15" t="n">
+        <v>62</v>
+      </c>
+      <c r="H15" t="n">
+        <v>85288</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.603</v>
+      </c>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="n">
+        <v>67</v>
+      </c>
+      <c r="C16" t="n">
+        <v>13</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16" t="n">
+        <v>67</v>
+      </c>
+      <c r="H16" t="n">
+        <v>141387</v>
+      </c>
+      <c r="I16" t="n">
+        <v>1</v>
+      </c>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <cols>
+    <col min="1" max="1" width="16.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="3.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="14.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="5.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="5.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="7.71" hidden="0" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.74217</v>
+      </c>
+      <c r="G2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2" t="n">
+        <v>61056</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.208</v>
+      </c>
+      <c r="J2" t="n">
+        <v>8.15</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.00067</v>
+      </c>
+      <c r="L2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.075</v>
+      </c>
+      <c r="E3" t="n">
+        <v>6.65</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.00333</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" t="n">
+        <v>7468</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="J3" t="n">
+        <v>2.99</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.09927</v>
+      </c>
+      <c r="L3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.56762</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" t="n">
+        <v>24705</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.084</v>
+      </c>
+      <c r="J4" t="n">
+        <v>9.9</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="L4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="n">
+        <v>80</v>
+      </c>
+      <c r="C5" t="n">
+        <v>30</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.901</v>
+      </c>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5" t="n">
+        <v>80</v>
+      </c>
+      <c r="H5" t="n">
+        <v>199684</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.682</v>
+      </c>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="n">
+        <v>85</v>
+      </c>
+      <c r="C6" t="n">
+        <v>34</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6" t="n">
+        <v>85</v>
+      </c>
+      <c r="H6" t="n">
+        <v>292913</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.041</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.30513</v>
+      </c>
+      <c r="G7" t="n">
+        <v>3</v>
+      </c>
+      <c r="H7" t="n">
+        <v>26899</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.024</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1.31</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.27981</v>
+      </c>
+      <c r="L7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.147</v>
+      </c>
+      <c r="E8" t="n">
+        <v>13.12</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.00067</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" t="n">
+        <v>515173</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.456</v>
+      </c>
+      <c r="J8" t="n">
+        <v>75.24</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.00067</v>
+      </c>
+      <c r="L8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.15656</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" t="n">
+        <v>101793</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="J9" t="n">
+        <v>14.87</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.00067</v>
+      </c>
+      <c r="L9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="n">
+        <v>71</v>
+      </c>
+      <c r="C10" t="n">
+        <v>14</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.793</v>
+      </c>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10" t="n">
+        <v>71</v>
+      </c>
+      <c r="H10" t="n">
+        <v>486140</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="n">
+        <v>76</v>
+      </c>
+      <c r="C11" t="n">
+        <v>18</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11" t="n">
+        <v>76</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1130005</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="n">
+        <v>3</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.136</v>
+      </c>
+      <c r="E12" t="n">
+        <v>3.48</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.01532</v>
+      </c>
+      <c r="G12" t="n">
+        <v>3</v>
+      </c>
+      <c r="H12" t="n">
+        <v>29037</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.205</v>
+      </c>
+      <c r="J12" t="n">
+        <v>7.04</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.00133</v>
+      </c>
+      <c r="L12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.036</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2.76</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.08195</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" t="n">
+        <v>26338</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.186</v>
+      </c>
+      <c r="J13" t="n">
+        <v>19.15</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.00067</v>
+      </c>
+      <c r="L13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.021</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1.64</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.17988</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" t="n">
+        <v>724</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.47901</v>
+      </c>
+      <c r="L14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="n">
+        <v>62</v>
+      </c>
+      <c r="C15" t="n">
+        <v>10</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.807</v>
+      </c>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15" t="n">
+        <v>62</v>
+      </c>
+      <c r="H15" t="n">
+        <v>85288</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.603</v>
+      </c>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="n">
+        <v>67</v>
+      </c>
+      <c r="C16" t="n">
+        <v>13</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16" t="n">
+        <v>67</v>
+      </c>
+      <c r="H16" t="n">
+        <v>141387</v>
+      </c>
+      <c r="I16" t="n">
+        <v>1</v>
+      </c>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed supplemental table spreadsheet
</commit_message>
<xml_diff>
--- a/Data/Supplemental/Supplemental_Tables.xlsx
+++ b/Data/Supplemental/Supplemental_Tables.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
   <si>
     <t xml:space="preserve">Species</t>
   </si>
@@ -186,6 +186,105 @@
   </si>
   <si>
     <t xml:space="preserve">P-value </t>
+  </si>
+  <si>
+    <t xml:space="preserve">species * part * reef environment * pCO2 * temperature + (1 | colony)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">species * part * reef environment * (pCO2 + temperature) + (1 | colony)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reef environment * species * part * (pCO2 + temperature) + (1 | colony)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">species * part * (pCO2 + temperature + reef environment) + (1 | colony)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">species * part * (pCO2 + temperature) + (1 | colony)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">species * part * (pCO2 + temperature) + reef environment + (1 | colony)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">species * part * reef environment * pCO2 + temperature + (1 | colony)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">species * part * pCO2 + temperature + (1 | colony)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">species * reef environment + part + pCO2 + temperature + (1 | colony)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">species * part * reef environment + pCO2 * temperature + (1 | colony)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">symbionts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSTR:symbionts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAST:symbionts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSTR:pCO2-current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAST:pCO2-current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSTR:pCO2-EOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAST:pCO2-EOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSTR:pCO2-extreme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAST:pCO2-extreme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSTR:temperature (31C)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAST:temperature (31C)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">symbionts:pCO2-current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">symbionts:pCO2-EOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">symbionts:pCO2-extreme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">symbionts:temperature (31C)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSTR:symbionts:pCO2-current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAST:symbionts:pCO2-current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSTR:symbionts:pCO2-EOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAST:symbionts:pCO2-EOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSTR:symbionts:pCO2-extreme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAST:symbionts:pCO2-extreme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSTR:symbionts:temperature (31C)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAST:symbionts:temperature (31C)</t>
   </si>
 </sst>
 </file>
@@ -2271,7 +2370,7 @@
         <v>0.55</v>
       </c>
       <c r="F2" t="n">
-        <v>0.74217</v>
+        <v>0.74883</v>
       </c>
       <c r="G2" t="n">
         <v>3</v>
@@ -2324,7 +2423,7 @@
         <v>2.99</v>
       </c>
       <c r="K3" t="n">
-        <v>0.09927</v>
+        <v>0.10127</v>
       </c>
       <c r="L3" t="s">
         <v>29</v>
@@ -2347,7 +2446,7 @@
         <v>0.52</v>
       </c>
       <c r="F4" t="n">
-        <v>0.56762</v>
+        <v>0.57295</v>
       </c>
       <c r="G4" t="n">
         <v>1</v>
@@ -2362,7 +2461,7 @@
         <v>9.9</v>
       </c>
       <c r="K4" t="n">
-        <v>0.002</v>
+        <v>0.00266</v>
       </c>
       <c r="L4" t="s">
         <v>29</v>
@@ -2445,7 +2544,7 @@
         <v>1.23</v>
       </c>
       <c r="F7" t="n">
-        <v>0.30513</v>
+        <v>0.3058</v>
       </c>
       <c r="G7" t="n">
         <v>3</v>
@@ -2460,7 +2559,7 @@
         <v>1.31</v>
       </c>
       <c r="K7" t="n">
-        <v>0.27981</v>
+        <v>0.28181</v>
       </c>
       <c r="L7" t="s">
         <v>34</v>
@@ -2657,7 +2756,7 @@
         <v>2.76</v>
       </c>
       <c r="F13" t="n">
-        <v>0.08195</v>
+        <v>0.08328</v>
       </c>
       <c r="G13" t="n">
         <v>1</v>
@@ -2695,7 +2794,7 @@
         <v>1.64</v>
       </c>
       <c r="F14" t="n">
-        <v>0.17988</v>
+        <v>0.18121</v>
       </c>
       <c r="G14" t="n">
         <v>1</v>
@@ -2710,7 +2809,7 @@
         <v>0.53</v>
       </c>
       <c r="K14" t="n">
-        <v>0.47901</v>
+        <v>0.47768</v>
       </c>
       <c r="L14" t="s">
         <v>35</v>
@@ -2790,573 +2889,397 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="16.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="3.71" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="14.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="5.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="5.71" hidden="0" customWidth="1"/>
-    <col min="6" max="6" width="7.71" hidden="0" customWidth="1"/>
-    <col min="7" max="7" width="3.71" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="71.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="8.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="5.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="6.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="14.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="11.71" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="11.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="J1" t="s">
-        <v>54</v>
-      </c>
-      <c r="K1" t="s">
-        <v>55</v>
-      </c>
-      <c r="L1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" t="n">
-        <v>3</v>
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>923.1</v>
       </c>
       <c r="D2" t="n">
-        <v>0.019</v>
+        <v>1219.4</v>
       </c>
       <c r="E2" t="n">
-        <v>0.55</v>
+        <v>0.43</v>
       </c>
       <c r="F2" t="n">
-        <v>0.74217</v>
+        <v>0.318</v>
       </c>
       <c r="G2" t="n">
-        <v>3</v>
+        <v>0.163808918863028</v>
       </c>
       <c r="H2" t="n">
-        <v>61056</v>
+        <v>0.884761957168762</v>
       </c>
       <c r="I2" t="n">
-        <v>0.208</v>
+        <v>0.445413568049554</v>
       </c>
       <c r="J2" t="n">
-        <v>8.15</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.00067</v>
-      </c>
-      <c r="L2" t="s">
-        <v>29</v>
+        <v>71.4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" t="n">
-        <v>1</v>
+        <v>57</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>902.1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.075</v>
+        <v>1124.3</v>
       </c>
       <c r="E3" t="n">
-        <v>6.65</v>
+        <v>0.391</v>
       </c>
       <c r="F3" t="n">
-        <v>0.00333</v>
+        <v>0.279</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>0.155601596236983</v>
       </c>
       <c r="H3" t="n">
-        <v>7468</v>
+        <v>0.913117790532205</v>
       </c>
       <c r="I3" t="n">
-        <v>0.025</v>
+        <v>0.459316964023187</v>
       </c>
       <c r="J3" t="n">
-        <v>2.99</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.09927</v>
-      </c>
-      <c r="L3" t="s">
-        <v>29</v>
+        <v>69.6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" t="n">
-        <v>1</v>
+        <v>58</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>902.1</v>
       </c>
       <c r="D4" t="n">
-        <v>0.006</v>
+        <v>1124.3</v>
       </c>
       <c r="E4" t="n">
-        <v>0.52</v>
+        <v>0.391</v>
       </c>
       <c r="F4" t="n">
-        <v>0.56762</v>
+        <v>0.279</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>0.15560159623606</v>
       </c>
       <c r="H4" t="n">
-        <v>24705</v>
+        <v>0.913117790532225</v>
       </c>
       <c r="I4" t="n">
-        <v>0.084</v>
+        <v>0.45931696402331</v>
       </c>
       <c r="J4" t="n">
-        <v>9.9</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="L4" t="s">
-        <v>29</v>
+        <v>69.6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" t="n">
-        <v>80</v>
+        <v>58</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
       </c>
       <c r="C5" t="n">
-        <v>30</v>
+        <v>902.1</v>
       </c>
       <c r="D5" t="n">
-        <v>0.901</v>
-      </c>
-      <c r="E5"/>
-      <c r="F5"/>
+        <v>1124.3</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.391</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.279</v>
+      </c>
       <c r="G5" t="n">
-        <v>80</v>
+        <v>0.15560159623606</v>
       </c>
       <c r="H5" t="n">
-        <v>199684</v>
+        <v>0.913117790532225</v>
       </c>
       <c r="I5" t="n">
-        <v>0.682</v>
-      </c>
-      <c r="J5"/>
-      <c r="K5"/>
-      <c r="L5" t="s">
-        <v>29</v>
+        <v>0.45931696402331</v>
+      </c>
+      <c r="J5" t="n">
+        <v>69.6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" t="n">
-        <v>85</v>
+        <v>59</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
       </c>
       <c r="C6" t="n">
-        <v>34</v>
+        <v>883.9</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6"/>
-      <c r="F6"/>
+        <v>1024.7</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.323</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.213</v>
+      </c>
       <c r="G6" t="n">
-        <v>85</v>
+        <v>0.140299887725969</v>
       </c>
       <c r="H6" t="n">
-        <v>292913</v>
+        <v>0.935545346998836</v>
       </c>
       <c r="I6" t="n">
-        <v>1</v>
-      </c>
-      <c r="J6"/>
-      <c r="K6"/>
-      <c r="L6" t="s">
-        <v>29</v>
+        <v>0.476813006415758</v>
+      </c>
+      <c r="J6" t="n">
+        <v>60.8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" t="n">
-        <v>3</v>
+        <v>60</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>882</v>
       </c>
       <c r="D7" t="n">
-        <v>0.041</v>
+        <v>1000.5</v>
       </c>
       <c r="E7" t="n">
-        <v>1.23</v>
+        <v>0.28</v>
       </c>
       <c r="F7" t="n">
-        <v>0.30513</v>
+        <v>0.139</v>
       </c>
       <c r="G7" t="n">
-        <v>3</v>
+        <v>0.163557385601623</v>
       </c>
       <c r="H7" t="n">
-        <v>26899</v>
+        <v>0.950478505425775</v>
       </c>
       <c r="I7" t="n">
-        <v>0.024</v>
+        <v>0.488720975684716</v>
       </c>
       <c r="J7" t="n">
-        <v>1.31</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.27981</v>
-      </c>
-      <c r="L7" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" t="n">
-        <v>1</v>
+        <v>61</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
       </c>
       <c r="C8" t="n">
-        <v>3</v>
+        <v>883.5</v>
       </c>
       <c r="D8" t="n">
-        <v>0.147</v>
+        <v>1005.7</v>
       </c>
       <c r="E8" t="n">
-        <v>13.12</v>
+        <v>0.282</v>
       </c>
       <c r="F8" t="n">
-        <v>0.00067</v>
+        <v>0.144</v>
       </c>
       <c r="G8" t="n">
-        <v>1</v>
+        <v>0.161404588840658</v>
       </c>
       <c r="H8" t="n">
-        <v>515173</v>
+        <v>0.950207028249464</v>
       </c>
       <c r="I8" t="n">
-        <v>0.456</v>
+        <v>0.488554386711269</v>
       </c>
       <c r="J8" t="n">
-        <v>75.24</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.00067</v>
-      </c>
-      <c r="L8" t="s">
-        <v>34</v>
+        <v>58.1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" t="n">
-        <v>1</v>
+        <v>62</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>904.6</v>
       </c>
       <c r="D9" t="n">
-        <v>0.02</v>
+        <v>1086.1</v>
       </c>
       <c r="E9" t="n">
-        <v>1.75</v>
+        <v>0.338</v>
       </c>
       <c r="F9" t="n">
-        <v>0.15656</v>
+        <v>0.225</v>
       </c>
       <c r="G9" t="n">
-        <v>1</v>
+        <v>0.144855151671333</v>
       </c>
       <c r="H9" t="n">
-        <v>101793</v>
+        <v>0.948918411064145</v>
       </c>
       <c r="I9" t="n">
-        <v>0.09</v>
+        <v>0.477396911101414</v>
       </c>
       <c r="J9" t="n">
-        <v>14.87</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0.00067</v>
-      </c>
-      <c r="L9" t="s">
-        <v>34</v>
+        <v>52.4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" t="n">
-        <v>71</v>
+        <v>63</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
       </c>
       <c r="C10" t="n">
-        <v>14</v>
+        <v>890.2</v>
       </c>
       <c r="D10" t="n">
-        <v>0.793</v>
-      </c>
-      <c r="E10"/>
-      <c r="F10"/>
+        <v>990.2</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.235</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.093</v>
+      </c>
       <c r="G10" t="n">
-        <v>71</v>
+        <v>0.15714351271921</v>
       </c>
       <c r="H10" t="n">
-        <v>486140</v>
+        <v>0.982507593773722</v>
       </c>
       <c r="I10" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="J10"/>
-      <c r="K10"/>
-      <c r="L10" t="s">
-        <v>34</v>
+        <v>0.505803686210093</v>
+      </c>
+      <c r="J10" t="n">
+        <v>41.7</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" t="n">
-        <v>76</v>
+        <v>64</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
       </c>
       <c r="C11" t="n">
-        <v>18</v>
+        <v>881.2</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
-      </c>
-      <c r="E11"/>
-      <c r="F11"/>
+        <v>929.4</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.205</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.095</v>
+      </c>
       <c r="G11" t="n">
-        <v>76</v>
+        <v>0.121607431578392</v>
       </c>
       <c r="H11" t="n">
-        <v>1130005</v>
+        <v>1.01492820576266</v>
       </c>
       <c r="I11" t="n">
-        <v>1</v>
-      </c>
-      <c r="J11"/>
-      <c r="K11"/>
-      <c r="L11" t="s">
-        <v>34</v>
+        <v>0.513921291795915</v>
+      </c>
+      <c r="J11" t="n">
+        <v>28.7</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" t="n">
-        <v>3</v>
+        <v>65</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
       </c>
       <c r="C12" t="n">
-        <v>2</v>
+        <v>890.2</v>
       </c>
       <c r="D12" t="n">
-        <v>0.136</v>
+        <v>964.2</v>
       </c>
       <c r="E12" t="n">
-        <v>3.48</v>
+        <v>0.222</v>
       </c>
       <c r="F12" t="n">
-        <v>0.01532</v>
+        <v>0.113</v>
       </c>
       <c r="G12" t="n">
-        <v>3</v>
+        <v>0.122648787498884</v>
       </c>
       <c r="H12" t="n">
-        <v>29037</v>
+        <v>1.00853413549591</v>
       </c>
       <c r="I12" t="n">
-        <v>0.205</v>
+        <v>0.508488836427211</v>
       </c>
       <c r="J12" t="n">
-        <v>7.04</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0.00133</v>
-      </c>
-      <c r="L12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.036</v>
-      </c>
-      <c r="E13" t="n">
-        <v>2.76</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0.08195</v>
-      </c>
-      <c r="G13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H13" t="n">
-        <v>26338</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0.186</v>
-      </c>
-      <c r="J13" t="n">
-        <v>19.15</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0.00067</v>
-      </c>
-      <c r="L13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0.021</v>
-      </c>
-      <c r="E14" t="n">
-        <v>1.64</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0.17988</v>
-      </c>
-      <c r="G14" t="n">
-        <v>1</v>
-      </c>
-      <c r="H14" t="n">
-        <v>724</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0.005</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0.53</v>
-      </c>
-      <c r="K14" t="n">
-        <v>0.47901</v>
-      </c>
-      <c r="L14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" t="n">
-        <v>62</v>
-      </c>
-      <c r="C15" t="n">
-        <v>10</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0.807</v>
-      </c>
-      <c r="E15"/>
-      <c r="F15"/>
-      <c r="G15" t="n">
-        <v>62</v>
-      </c>
-      <c r="H15" t="n">
-        <v>85288</v>
-      </c>
-      <c r="I15" t="n">
-        <v>0.603</v>
-      </c>
-      <c r="J15"/>
-      <c r="K15"/>
-      <c r="L15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" t="n">
-        <v>67</v>
-      </c>
-      <c r="C16" t="n">
-        <v>13</v>
-      </c>
-      <c r="D16" t="n">
-        <v>1</v>
-      </c>
-      <c r="E16"/>
-      <c r="F16"/>
-      <c r="G16" t="n">
-        <v>67</v>
-      </c>
-      <c r="H16" t="n">
-        <v>141387</v>
-      </c>
-      <c r="I16" t="n">
-        <v>1</v>
-      </c>
-      <c r="J16"/>
-      <c r="K16"/>
-      <c r="L16" t="s">
-        <v>35</v>
+        <v>28.3</v>
       </c>
     </row>
   </sheetData>
@@ -3373,12 +3296,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="16.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="3.71" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="32.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="8.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="14.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="5.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="5.71" hidden="0" customWidth="1"/>
-    <col min="6" max="6" width="7.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="9.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="7.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="9.15" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3386,560 +3309,549 @@
         <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" t="s">
         <v>26</v>
-      </c>
-      <c r="G1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J1" t="s">
-        <v>54</v>
-      </c>
-      <c r="K1" t="s">
-        <v>55</v>
-      </c>
-      <c r="L1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>0.8</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0.172</v>
       </c>
       <c r="D2" t="n">
-        <v>0.019</v>
+        <v>4.66</v>
       </c>
       <c r="E2" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.74217</v>
-      </c>
-      <c r="G2" t="n">
-        <v>3</v>
-      </c>
-      <c r="H2" t="n">
-        <v>61056</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.208</v>
-      </c>
-      <c r="J2" t="n">
-        <v>8.15</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.00067</v>
-      </c>
-      <c r="L2" t="s">
-        <v>29</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>0.29</v>
       </c>
       <c r="D3" t="n">
-        <v>0.075</v>
+        <v>0.69</v>
       </c>
       <c r="E3" t="n">
-        <v>6.65</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.00333</v>
-      </c>
-      <c r="G3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" t="n">
-        <v>7468</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.025</v>
-      </c>
-      <c r="J3" t="n">
-        <v>2.99</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.09927</v>
-      </c>
-      <c r="L3" t="s">
-        <v>29</v>
+        <v>0.491</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>-0.357</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>0.244</v>
       </c>
       <c r="D4" t="n">
-        <v>0.006</v>
+        <v>-1.47</v>
       </c>
       <c r="E4" t="n">
-        <v>0.52</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.56762</v>
-      </c>
-      <c r="G4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" t="n">
-        <v>24705</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.084</v>
-      </c>
-      <c r="J4" t="n">
-        <v>9.9</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="L4" t="s">
-        <v>29</v>
+        <v>0.143</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="B5" t="n">
-        <v>80</v>
+        <v>-0.515</v>
       </c>
       <c r="C5" t="n">
-        <v>30</v>
+        <v>0.185</v>
       </c>
       <c r="D5" t="n">
-        <v>0.901</v>
-      </c>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5" t="n">
-        <v>80</v>
-      </c>
-      <c r="H5" t="n">
-        <v>199684</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.682</v>
-      </c>
-      <c r="J5"/>
-      <c r="K5"/>
-      <c r="L5" t="s">
-        <v>29</v>
+        <v>-2.78</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.005</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B6" t="n">
-        <v>85</v>
+        <v>0.235</v>
       </c>
       <c r="C6" t="n">
-        <v>34</v>
+        <v>0.214</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6" t="n">
-        <v>85</v>
-      </c>
-      <c r="H6" t="n">
-        <v>292913</v>
-      </c>
-      <c r="I6" t="n">
-        <v>1</v>
-      </c>
-      <c r="J6"/>
-      <c r="K6"/>
-      <c r="L6" t="s">
-        <v>29</v>
+        <v>1.1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.272</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B7" t="n">
-        <v>3</v>
+        <v>0.006</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>0.164</v>
       </c>
       <c r="D7" t="n">
-        <v>0.041</v>
+        <v>0.03</v>
       </c>
       <c r="E7" t="n">
-        <v>1.23</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.30513</v>
-      </c>
-      <c r="G7" t="n">
-        <v>3</v>
-      </c>
-      <c r="H7" t="n">
-        <v>26899</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.024</v>
-      </c>
-      <c r="J7" t="n">
-        <v>1.31</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.27981</v>
-      </c>
-      <c r="L7" t="s">
-        <v>34</v>
+        <v>0.972</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>-0.021</v>
       </c>
       <c r="C8" t="n">
-        <v>3</v>
+        <v>0.161</v>
       </c>
       <c r="D8" t="n">
-        <v>0.147</v>
+        <v>-0.13</v>
       </c>
       <c r="E8" t="n">
-        <v>13.12</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.00067</v>
-      </c>
-      <c r="G8" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" t="n">
-        <v>515173</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.456</v>
-      </c>
-      <c r="J8" t="n">
-        <v>75.24</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.00067</v>
-      </c>
-      <c r="L8" t="s">
-        <v>34</v>
+        <v>0.896</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>-0.252</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>0.128</v>
       </c>
       <c r="D9" t="n">
-        <v>0.02</v>
+        <v>-1.97</v>
       </c>
       <c r="E9" t="n">
-        <v>1.75</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.15656</v>
-      </c>
-      <c r="G9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" t="n">
-        <v>101793</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="J9" t="n">
-        <v>14.87</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0.00067</v>
-      </c>
-      <c r="L9" t="s">
-        <v>34</v>
+        <v>0.049</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="B10" t="n">
-        <v>71</v>
+        <v>0.222</v>
       </c>
       <c r="C10" t="n">
-        <v>14</v>
+        <v>0.308</v>
       </c>
       <c r="D10" t="n">
-        <v>0.793</v>
-      </c>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10" t="n">
-        <v>71</v>
-      </c>
-      <c r="H10" t="n">
-        <v>486140</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="J10"/>
-      <c r="K10"/>
-      <c r="L10" t="s">
-        <v>34</v>
+        <v>0.72</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.472</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="B11" t="n">
-        <v>76</v>
+        <v>0.685</v>
       </c>
       <c r="C11" t="n">
-        <v>18</v>
+        <v>0.27</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
-      </c>
-      <c r="E11"/>
-      <c r="F11"/>
-      <c r="G11" t="n">
-        <v>76</v>
-      </c>
-      <c r="H11" t="n">
-        <v>1130005</v>
-      </c>
-      <c r="I11" t="n">
-        <v>1</v>
-      </c>
-      <c r="J11"/>
-      <c r="K11"/>
-      <c r="L11" t="s">
-        <v>34</v>
+        <v>2.54</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.011</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="B12" t="n">
-        <v>3</v>
+        <v>-0.088</v>
       </c>
       <c r="C12" t="n">
-        <v>2</v>
+        <v>0.592</v>
       </c>
       <c r="D12" t="n">
-        <v>0.136</v>
+        <v>-0.15</v>
       </c>
       <c r="E12" t="n">
-        <v>3.48</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.01532</v>
-      </c>
-      <c r="G12" t="n">
-        <v>3</v>
-      </c>
-      <c r="H12" t="n">
-        <v>29037</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0.205</v>
-      </c>
-      <c r="J12" t="n">
-        <v>7.04</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0.00133</v>
-      </c>
-      <c r="L12" t="s">
-        <v>35</v>
+        <v>0.882</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>-0.569</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>0.339</v>
       </c>
       <c r="D13" t="n">
-        <v>0.036</v>
+        <v>-1.68</v>
       </c>
       <c r="E13" t="n">
-        <v>2.76</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0.08195</v>
-      </c>
-      <c r="G13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H13" t="n">
-        <v>26338</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0.186</v>
-      </c>
-      <c r="J13" t="n">
-        <v>19.15</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0.00067</v>
-      </c>
-      <c r="L13" t="s">
-        <v>35</v>
+        <v>0.093</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>-0.451</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>0.298</v>
       </c>
       <c r="D14" t="n">
-        <v>0.021</v>
+        <v>-1.51</v>
       </c>
       <c r="E14" t="n">
-        <v>1.64</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0.17988</v>
-      </c>
-      <c r="G14" t="n">
-        <v>1</v>
-      </c>
-      <c r="H14" t="n">
-        <v>724</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0.005</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0.53</v>
-      </c>
-      <c r="K14" t="n">
-        <v>0.47901</v>
-      </c>
-      <c r="L14" t="s">
-        <v>35</v>
+        <v>0.131</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="B15" t="n">
-        <v>62</v>
+        <v>0.05</v>
       </c>
       <c r="C15" t="n">
-        <v>10</v>
+        <v>0.24</v>
       </c>
       <c r="D15" t="n">
-        <v>0.807</v>
-      </c>
-      <c r="E15"/>
-      <c r="F15"/>
-      <c r="G15" t="n">
-        <v>62</v>
-      </c>
-      <c r="H15" t="n">
-        <v>85288</v>
-      </c>
-      <c r="I15" t="n">
-        <v>0.603</v>
-      </c>
-      <c r="J15"/>
-      <c r="K15"/>
-      <c r="L15" t="s">
-        <v>35</v>
+        <v>0.21</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.835</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="B16" t="n">
-        <v>67</v>
+        <v>-0.154</v>
       </c>
       <c r="C16" t="n">
-        <v>13</v>
+        <v>0.288</v>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
-      </c>
-      <c r="E16"/>
-      <c r="F16"/>
-      <c r="G16" t="n">
-        <v>67</v>
-      </c>
-      <c r="H16" t="n">
-        <v>141387</v>
-      </c>
-      <c r="I16" t="n">
-        <v>1</v>
-      </c>
-      <c r="J16"/>
-      <c r="K16"/>
-      <c r="L16" t="s">
-        <v>35</v>
-      </c>
+        <v>-0.54</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.592</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.236</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.245</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.336</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0.071</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.775</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0.608</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="D19" t="n">
+        <v>3.04</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.002</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" t="n">
+        <v>-0.299</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.298</v>
+      </c>
+      <c r="D20" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.316</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0.134</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.227</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.556</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0.564</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.226</v>
+      </c>
+      <c r="D22" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.013</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0.524</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.181</v>
+      </c>
+      <c r="D23" t="n">
+        <v>2.89</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.004</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0.362</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.818</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.658</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0.673</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.473</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.155</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" t="n">
+        <v>-0.177</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.418</v>
+      </c>
+      <c r="D26" t="n">
+        <v>-0.42</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.672</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" t="n">
+        <v>-0.181</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.335</v>
+      </c>
+      <c r="D27" t="n">
+        <v>-0.54</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" t="n">
+        <v>-0.482</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.401</v>
+      </c>
+      <c r="D28" t="n">
+        <v>-1.2</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.229</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" t="n">
+        <v>-0.891</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.341</v>
+      </c>
+      <c r="D29" t="n">
+        <v>-2.61</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.009</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>87</v>
+      </c>
+      <c r="B30" t="n">
+        <v>0.191</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.586</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" t="n">
+        <v>-0.606</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.281</v>
+      </c>
+      <c r="D31" t="n">
+        <v>-2.16</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.031</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" t="n">
+        <v>0.139</v>
+      </c>
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="E33"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated Fig 1 with plot labels and checked random effect of tanks in plasticity
</commit_message>
<xml_diff>
--- a/Data/Supplemental/Supplemental_Tables.xlsx
+++ b/Data/Supplemental/Supplemental_Tables.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr date1904="false"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
   <si>
     <t xml:space="preserve">Species</t>
   </si>
@@ -56,18 +56,21 @@
     <t xml:space="preserve">ssid</t>
   </si>
   <si>
+    <t xml:space="preserve">reef environment * pCO2 + temperature + (1 | colony)b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">glmerMod</t>
+  </si>
+  <si>
     <t xml:space="preserve">reef environment * pCO2 + temperature + (1 | colony)</t>
   </si>
   <si>
-    <t xml:space="preserve">glmerMod</t>
+    <t xml:space="preserve">reef environment * (pCO2 + temperature) + (1 | colony)</t>
   </si>
   <si>
     <t xml:space="preserve">reef environment * pCO2 * temperature + (1 | colony)</t>
   </si>
   <si>
-    <t xml:space="preserve">reef environment * (pCO2 + temperature) + (1 | colony)</t>
-  </si>
-  <si>
     <t xml:space="preserve">reef environment + pCO2 + temperature + (1 | colony)</t>
   </si>
   <si>
@@ -81,6 +84,9 @@
   </si>
   <si>
     <t xml:space="preserve">past</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pCO2 + temperature + (1 | colony)b</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -290,7 +296,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="1">
     <font>
@@ -609,10 +615,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
@@ -671,28 +677,28 @@
         <v>13</v>
       </c>
       <c r="D2" t="n">
-        <v>218.8</v>
+        <v>218.4</v>
       </c>
       <c r="E2" t="n">
-        <v>243.5</v>
+        <v>245.4</v>
       </c>
       <c r="F2" t="n">
-        <v>0.506</v>
+        <v>0.542</v>
       </c>
       <c r="G2" t="n">
-        <v>0.322</v>
+        <v>0.307</v>
       </c>
       <c r="H2" t="n">
-        <v>0.270712896490855</v>
+        <v>0.339978050295066</v>
       </c>
       <c r="I2" t="n">
-        <v>0.88051736116787</v>
+        <v>0.824533279005936</v>
       </c>
       <c r="J2" t="n">
-        <v>0.309990521732364</v>
+        <v>0.297768433607305</v>
       </c>
       <c r="K2" t="n">
-        <v>70.7</v>
+        <v>90.3</v>
       </c>
     </row>
     <row r="3">
@@ -706,28 +712,28 @@
         <v>13</v>
       </c>
       <c r="D3" t="n">
-        <v>223.2</v>
+        <v>218.8</v>
       </c>
       <c r="E3" t="n">
-        <v>259.2</v>
+        <v>243.5</v>
       </c>
       <c r="F3" t="n">
-        <v>0.545</v>
+        <v>0.506</v>
       </c>
       <c r="G3" t="n">
-        <v>0.366</v>
+        <v>0.322</v>
       </c>
       <c r="H3" t="n">
-        <v>0.28206734361165</v>
+        <v>0.270712896490855</v>
       </c>
       <c r="I3" t="n">
-        <v>0.855828398376242</v>
+        <v>0.88051736116787</v>
       </c>
       <c r="J3" t="n">
-        <v>0.294010052276531</v>
+        <v>0.309990521732364</v>
       </c>
       <c r="K3" t="n">
-        <v>69.6</v>
+        <v>65.6</v>
       </c>
     </row>
     <row r="4">
@@ -762,7 +768,7 @@
         <v>0.307309431789679</v>
       </c>
       <c r="K4" t="n">
-        <v>68.6</v>
+        <v>63.3</v>
       </c>
     </row>
     <row r="5">
@@ -776,28 +782,28 @@
         <v>13</v>
       </c>
       <c r="D5" t="n">
-        <v>221.6</v>
+        <v>223.2</v>
       </c>
       <c r="E5" t="n">
-        <v>239.6</v>
+        <v>259.2</v>
       </c>
       <c r="F5" t="n">
-        <v>0.442</v>
+        <v>0.545</v>
       </c>
       <c r="G5" t="n">
-        <v>0.254</v>
+        <v>0.366</v>
       </c>
       <c r="H5" t="n">
-        <v>0.252287908819288</v>
+        <v>0.28206734361165</v>
       </c>
       <c r="I5" t="n">
-        <v>0.933847194038125</v>
+        <v>0.855828398376242</v>
       </c>
       <c r="J5" t="n">
-        <v>0.322867004362844</v>
+        <v>0.294010052276531</v>
       </c>
       <c r="K5" t="n">
-        <v>39.5</v>
+        <v>62.8</v>
       </c>
     </row>
     <row r="6">
@@ -811,28 +817,28 @@
         <v>13</v>
       </c>
       <c r="D6" t="n">
-        <v>222.1</v>
+        <v>221.6</v>
       </c>
       <c r="E6" t="n">
-        <v>237.8</v>
+        <v>239.6</v>
       </c>
       <c r="F6" t="n">
-        <v>0.37</v>
+        <v>0.442</v>
       </c>
       <c r="G6" t="n">
-        <v>0.088</v>
+        <v>0.254</v>
       </c>
       <c r="H6" t="n">
-        <v>0.308813847521209</v>
+        <v>0.252287908819288</v>
       </c>
       <c r="I6" t="n">
-        <v>0.936882340613694</v>
+        <v>0.933847194038125</v>
       </c>
       <c r="J6" t="n">
-        <v>0.331059051190965</v>
+        <v>0.322867004362844</v>
       </c>
       <c r="K6" t="n">
-        <v>35.9</v>
+        <v>38.9</v>
       </c>
     </row>
     <row r="7">
@@ -846,168 +852,168 @@
         <v>13</v>
       </c>
       <c r="D7" t="n">
-        <v>225.6</v>
+        <v>222.1</v>
       </c>
       <c r="E7" t="n">
-        <v>248.1</v>
+        <v>237.8</v>
       </c>
       <c r="F7" t="n">
-        <v>0.442</v>
+        <v>0.37</v>
       </c>
       <c r="G7" t="n">
-        <v>0.253</v>
+        <v>0.088</v>
       </c>
       <c r="H7" t="n">
-        <v>0.252780589487017</v>
+        <v>0.308813847521209</v>
       </c>
       <c r="I7" t="n">
-        <v>0.931849391942536</v>
+        <v>0.936882340613694</v>
       </c>
       <c r="J7" t="n">
-        <v>0.323013486807386</v>
+        <v>0.331059051190965</v>
       </c>
       <c r="K7" t="n">
-        <v>26</v>
+        <v>30.5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
         <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
       </c>
       <c r="D8" t="n">
-        <v>105.6</v>
+        <v>225.6</v>
       </c>
       <c r="E8" t="n">
-        <v>121.5</v>
+        <v>248.1</v>
       </c>
       <c r="F8" t="n">
-        <v>0.397</v>
+        <v>0.442</v>
       </c>
       <c r="G8" t="n">
-        <v>0.317</v>
+        <v>0.253</v>
       </c>
       <c r="H8" t="n">
-        <v>0.117033435887396</v>
+        <v>0.252780589487017</v>
       </c>
       <c r="I8" t="n">
-        <v>1.02875627247403</v>
+        <v>0.931849391942536</v>
       </c>
       <c r="J8" t="n">
-        <v>0.342860527251939</v>
+        <v>0.323013486807386</v>
       </c>
       <c r="K8" t="n">
-        <v>71.4</v>
+        <v>25.7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
         <v>13</v>
       </c>
       <c r="D9" t="n">
-        <v>100.8</v>
+        <v>105.6</v>
       </c>
       <c r="E9" t="n">
-        <v>111.8</v>
+        <v>121.5</v>
       </c>
       <c r="F9" t="n">
-        <v>0.309</v>
+        <v>0.397</v>
       </c>
       <c r="G9" t="n">
-        <v>0.261</v>
+        <v>0.317</v>
       </c>
       <c r="H9" t="n">
-        <v>0.0648056876434838</v>
+        <v>0.117033435887396</v>
       </c>
       <c r="I9" t="n">
-        <v>1.14657450978296</v>
+        <v>1.02875627247403</v>
       </c>
       <c r="J9" t="n">
-        <v>0.36062662799942</v>
+        <v>0.342860527251939</v>
       </c>
       <c r="K9" t="n">
-        <v>45</v>
+        <v>71.4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
       </c>
       <c r="D10" t="n">
-        <v>101.6</v>
+        <v>100.8</v>
       </c>
       <c r="E10" t="n">
-        <v>112.6</v>
+        <v>111.8</v>
       </c>
       <c r="F10" t="n">
-        <v>0.278</v>
+        <v>0.309</v>
       </c>
       <c r="G10" t="n">
-        <v>0.238</v>
+        <v>0.261</v>
       </c>
       <c r="H10" t="n">
-        <v>0.0533714820211562</v>
+        <v>0.0648056876434838</v>
       </c>
       <c r="I10" t="n">
-        <v>1.13665595795787</v>
+        <v>1.14657450978296</v>
       </c>
       <c r="J10" t="n">
-        <v>0.359834556845443</v>
+        <v>0.36062662799942</v>
       </c>
       <c r="K10" t="n">
-        <v>36.2</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
         <v>19</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
       </c>
       <c r="C11" t="s">
         <v>13</v>
       </c>
       <c r="D11" t="n">
-        <v>97.5</v>
+        <v>101.6</v>
       </c>
       <c r="E11" t="n">
-        <v>104.8</v>
+        <v>112.6</v>
       </c>
       <c r="F11" t="n">
-        <v>0.232</v>
+        <v>0.278</v>
       </c>
       <c r="G11" t="n">
-        <v>0.188</v>
+        <v>0.238</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0541808464958402</v>
+        <v>0.0533714820211562</v>
       </c>
       <c r="I11" t="n">
-        <v>1.22142050234447</v>
+        <v>1.13665595795787</v>
       </c>
       <c r="J11" t="n">
-        <v>0.371319943278335</v>
+        <v>0.359834556845443</v>
       </c>
       <c r="K11" t="n">
-        <v>28.8</v>
+        <v>36.2</v>
       </c>
     </row>
     <row r="12">
@@ -1015,109 +1021,109 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
         <v>13</v>
       </c>
       <c r="D12" t="n">
-        <v>145.9</v>
+        <v>97.5</v>
       </c>
       <c r="E12" t="n">
-        <v>167.8</v>
+        <v>104.8</v>
       </c>
       <c r="F12" t="n">
-        <v>0.521</v>
+        <v>0.232</v>
       </c>
       <c r="G12" t="n">
-        <v>0.195</v>
+        <v>0.188</v>
       </c>
       <c r="H12" t="n">
-        <v>0.405142468828212</v>
+        <v>0.0541808464958402</v>
       </c>
       <c r="I12" t="n">
-        <v>0.710112914386074</v>
+        <v>1.22142050234447</v>
       </c>
       <c r="J12" t="n">
-        <v>0.231080473857171</v>
+        <v>0.371319943278335</v>
       </c>
       <c r="K12" t="n">
-        <v>76.2</v>
+        <v>28.8</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
         <v>13</v>
       </c>
       <c r="D13" t="n">
-        <v>147.9</v>
+        <v>145.9</v>
       </c>
       <c r="E13" t="n">
-        <v>171.8</v>
+        <v>167.8</v>
       </c>
       <c r="F13" t="n">
-        <v>0.522</v>
+        <v>0.521</v>
       </c>
       <c r="G13" t="n">
         <v>0.195</v>
       </c>
       <c r="H13" t="n">
-        <v>0.405616901906066</v>
+        <v>0.405142468828212</v>
       </c>
       <c r="I13" t="n">
-        <v>0.70994797179576</v>
+        <v>0.710112914386074</v>
       </c>
       <c r="J13" t="n">
-        <v>0.2309514006937</v>
+        <v>0.231080473857171</v>
       </c>
       <c r="K13" t="n">
-        <v>72.9</v>
+        <v>76.2</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
       </c>
       <c r="D14" t="n">
-        <v>153.1</v>
+        <v>147.9</v>
       </c>
       <c r="E14" t="n">
-        <v>182.9</v>
+        <v>171.8</v>
       </c>
       <c r="F14" t="n">
-        <v>0.527</v>
+        <v>0.522</v>
       </c>
       <c r="G14" t="n">
-        <v>0.199</v>
+        <v>0.195</v>
       </c>
       <c r="H14" t="n">
-        <v>0.409641424663849</v>
+        <v>0.405616901906066</v>
       </c>
       <c r="I14" t="n">
-        <v>0.706971647584522</v>
+        <v>0.70994797179576</v>
       </c>
       <c r="J14" t="n">
-        <v>0.229916347449218</v>
+        <v>0.2309514006937</v>
       </c>
       <c r="K14" t="n">
-        <v>71.4</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
@@ -1126,98 +1132,168 @@
         <v>13</v>
       </c>
       <c r="D15" t="n">
-        <v>142.3</v>
+        <v>153.1</v>
       </c>
       <c r="E15" t="n">
-        <v>158.2</v>
+        <v>182.9</v>
       </c>
       <c r="F15" t="n">
-        <v>0.499</v>
+        <v>0.527</v>
       </c>
       <c r="G15" t="n">
-        <v>0.174</v>
+        <v>0.199</v>
       </c>
       <c r="H15" t="n">
-        <v>0.393286215931064</v>
+        <v>0.409641424663849</v>
       </c>
       <c r="I15" t="n">
-        <v>0.733244393163204</v>
+        <v>0.706971647584522</v>
       </c>
       <c r="J15" t="n">
-        <v>0.237295448325152</v>
+        <v>0.229916347449218</v>
       </c>
       <c r="K15" t="n">
-        <v>38.4</v>
+        <v>71.4</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
       </c>
       <c r="D16" t="n">
-        <v>140.4</v>
+        <v>142.4</v>
       </c>
       <c r="E16" t="n">
-        <v>154.4</v>
+        <v>158.3</v>
       </c>
       <c r="F16" t="n">
-        <v>0.485</v>
+        <v>0.493</v>
       </c>
       <c r="G16" t="n">
-        <v>0.147</v>
+        <v>0.145</v>
       </c>
       <c r="H16" t="n">
-        <v>0.396708536729162</v>
+        <v>0.407604756872208</v>
       </c>
       <c r="I16" t="n">
-        <v>0.732981216119454</v>
+        <v>0.727645800628731</v>
       </c>
       <c r="J16" t="n">
-        <v>0.238221370319828</v>
+        <v>0.236973047639022</v>
       </c>
       <c r="K16" t="n">
-        <v>32.1</v>
+        <v>45.1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
         <v>13</v>
       </c>
       <c r="D17" t="n">
-        <v>146.2</v>
+        <v>142.3</v>
       </c>
       <c r="E17" t="n">
-        <v>166.1</v>
+        <v>158.2</v>
       </c>
       <c r="F17" t="n">
-        <v>0.5</v>
+        <v>0.499</v>
       </c>
       <c r="G17" t="n">
         <v>0.174</v>
       </c>
       <c r="H17" t="n">
+        <v>0.393286215931064</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.733244393163204</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.237295448325152</v>
+      </c>
+      <c r="K17" t="n">
+        <v>38.7</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="n">
+        <v>140.4</v>
+      </c>
+      <c r="E18" t="n">
+        <v>154.4</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.485</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.147</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.396708536729162</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.732981216119454</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.238221370319828</v>
+      </c>
+      <c r="K18" t="n">
+        <v>32.7</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="n">
+        <v>146.2</v>
+      </c>
+      <c r="E19" t="n">
+        <v>166.1</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.174</v>
+      </c>
+      <c r="H19" t="n">
         <v>0.394015465922658</v>
       </c>
-      <c r="I17" t="n">
+      <c r="I19" t="n">
         <v>0.734046668651323</v>
       </c>
-      <c r="J17" t="n">
+      <c r="J19" t="n">
         <v>0.237351188594544</v>
       </c>
-      <c r="K17" t="n">
-        <v>30.5</v>
+      <c r="K19" t="n">
+        <v>30.8</v>
       </c>
     </row>
   </sheetData>
@@ -1227,10 +1303,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
@@ -1245,30 +1321,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -1286,12 +1362,12 @@
         <v>0.00067</v>
       </c>
       <c r="G2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -1309,12 +1385,12 @@
         <v>0.09127</v>
       </c>
       <c r="G3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -1332,12 +1408,12 @@
         <v>0.00133</v>
       </c>
       <c r="G4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B5" t="n">
         <v>80</v>
@@ -1351,12 +1427,12 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B6" t="n">
         <v>85</v>
@@ -1370,12 +1446,12 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B7" t="n">
         <v>1</v>
@@ -1393,12 +1469,12 @@
         <v>0.00067</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B8" t="n">
         <v>1</v>
@@ -1416,12 +1492,12 @@
         <v>0.00067</v>
       </c>
       <c r="G8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B9" t="n">
         <v>3</v>
@@ -1439,12 +1515,12 @@
         <v>0.23651</v>
       </c>
       <c r="G9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B10" t="n">
         <v>71</v>
@@ -1458,12 +1534,12 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B11" t="n">
         <v>76</v>
@@ -1477,12 +1553,12 @@
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B12" t="n">
         <v>1</v>
@@ -1500,12 +1576,12 @@
         <v>0.74151</v>
       </c>
       <c r="G12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B13" t="n">
         <v>1</v>
@@ -1523,12 +1599,12 @@
         <v>0.00067</v>
       </c>
       <c r="G13" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B14" t="n">
         <v>3</v>
@@ -1546,12 +1622,12 @@
         <v>0.00067</v>
       </c>
       <c r="G14" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B15" t="n">
         <v>62</v>
@@ -1565,12 +1641,12 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B16" t="n">
         <v>67</v>
@@ -1584,7 +1660,7 @@
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1594,10 +1670,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
@@ -1611,202 +1687,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B2" t="n">
-        <v>1.085</v>
+        <v>1.05</v>
       </c>
       <c r="C2" t="n">
-        <v>0.172</v>
+        <v>0.006</v>
       </c>
       <c r="D2" t="n">
-        <v>6.3</v>
+        <v>187.16</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.058</v>
+        <v>0.01</v>
       </c>
       <c r="C3" t="n">
-        <v>0.248</v>
+        <v>0.006</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.24</v>
+        <v>1.73</v>
       </c>
       <c r="E3" t="n">
-        <v>0.814</v>
+        <v>0.084</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B4" t="n">
-        <v>0.335</v>
+        <v>0.378</v>
       </c>
       <c r="C4" t="n">
-        <v>0.173</v>
+        <v>0.006</v>
       </c>
       <c r="D4" t="n">
-        <v>1.94</v>
+        <v>67.01</v>
       </c>
       <c r="E4" t="n">
-        <v>0.053</v>
+        <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B5" t="n">
-        <v>0.21</v>
+        <v>0.223</v>
       </c>
       <c r="C5" t="n">
-        <v>0.131</v>
+        <v>0.006</v>
       </c>
       <c r="D5" t="n">
-        <v>1.6</v>
+        <v>39.36</v>
       </c>
       <c r="E5" t="n">
-        <v>0.109</v>
+        <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B6" t="n">
-        <v>0.419</v>
+        <v>0.444</v>
       </c>
       <c r="C6" t="n">
-        <v>0.132</v>
+        <v>0.006</v>
       </c>
       <c r="D6" t="n">
-        <v>3.17</v>
+        <v>78.84</v>
       </c>
       <c r="E6" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B7" t="n">
-        <v>0.003</v>
+        <v>0.002</v>
       </c>
       <c r="C7" t="n">
-        <v>0.076</v>
+        <v>0.006</v>
       </c>
       <c r="D7" t="n">
-        <v>0.04</v>
+        <v>0.32</v>
       </c>
       <c r="E7" t="n">
-        <v>0.967</v>
+        <v>0.748</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.704</v>
+        <v>-0.771</v>
       </c>
       <c r="C8" t="n">
-        <v>0.239</v>
+        <v>0.006</v>
       </c>
       <c r="D8" t="n">
-        <v>-2.95</v>
+        <v>-136.94</v>
       </c>
       <c r="E8" t="n">
-        <v>0.003</v>
+        <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.409</v>
+        <v>-0.446</v>
       </c>
       <c r="C9" t="n">
-        <v>0.197</v>
+        <v>0.006</v>
       </c>
       <c r="D9" t="n">
-        <v>-2.08</v>
+        <v>-79.4</v>
       </c>
       <c r="E9" t="n">
-        <v>0.037</v>
+        <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.278</v>
+        <v>-0.33</v>
       </c>
       <c r="C10" t="n">
-        <v>0.191</v>
+        <v>0.006</v>
       </c>
       <c r="D10" t="n">
-        <v>-1.45</v>
+        <v>-58.53</v>
       </c>
       <c r="E10" t="n">
-        <v>0.146</v>
+        <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11">
@@ -1814,13 +1890,13 @@
         <v>5</v>
       </c>
       <c r="B11" t="n">
-        <v>0.506</v>
+        <v>0.542</v>
       </c>
       <c r="C11"/>
       <c r="D11"/>
       <c r="E11"/>
       <c r="F11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12">
@@ -1828,18 +1904,18 @@
         <v>6</v>
       </c>
       <c r="B12" t="n">
-        <v>0.322</v>
+        <v>0.307</v>
       </c>
       <c r="C12"/>
       <c r="D12"/>
       <c r="E12"/>
       <c r="F12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B13" t="n">
         <v>1.279</v>
@@ -1854,12 +1930,12 @@
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B14" t="n">
         <v>-0.338</v>
@@ -1874,12 +1950,12 @@
         <v>0.08</v>
       </c>
       <c r="F14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B15" t="n">
         <v>-0.059</v>
@@ -1894,12 +1970,12 @@
         <v>0.753</v>
       </c>
       <c r="F15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B16" t="n">
         <v>0.227</v>
@@ -1914,7 +1990,7 @@
         <v>0.19</v>
       </c>
       <c r="F16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17">
@@ -1928,7 +2004,7 @@
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18">
@@ -1942,12 +2018,12 @@
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B19" t="n">
         <v>1.038</v>
@@ -1962,12 +2038,12 @@
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B20" t="n">
         <v>-0.047</v>
@@ -1982,12 +2058,12 @@
         <v>0.67</v>
       </c>
       <c r="F20" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B21" t="n">
         <v>0.032</v>
@@ -2002,12 +2078,12 @@
         <v>0.664</v>
       </c>
       <c r="F21" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B22" t="n">
         <v>0.122</v>
@@ -2022,12 +2098,12 @@
         <v>0.116</v>
       </c>
       <c r="F22" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B23" t="n">
         <v>0.264</v>
@@ -2042,7 +2118,7 @@
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24">
@@ -2056,7 +2132,7 @@
       <c r="D24"/>
       <c r="E24"/>
       <c r="F24" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25">
@@ -2070,7 +2146,7 @@
       <c r="D25"/>
       <c r="E25"/>
       <c r="F25" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2080,10 +2156,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
@@ -2097,27 +2173,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -2137,7 +2213,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -2157,7 +2233,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -2177,7 +2253,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B5" t="n">
         <v>2</v>
@@ -2197,7 +2273,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B6" t="n">
         <v>2</v>
@@ -2217,7 +2293,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B7" t="n">
         <v>6</v>
@@ -2237,7 +2313,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B8" t="n">
         <v>2</v>
@@ -2257,7 +2333,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B9" t="n">
         <v>214</v>
@@ -2273,7 +2349,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B10" t="n">
         <v>231</v>
@@ -2294,10 +2370,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
@@ -2317,45 +2393,45 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="J1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="K1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="L1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -2370,7 +2446,7 @@
         <v>0.55</v>
       </c>
       <c r="F2" t="n">
-        <v>0.74883</v>
+        <v>0.74217</v>
       </c>
       <c r="G2" t="n">
         <v>3</v>
@@ -2388,12 +2464,12 @@
         <v>0.00067</v>
       </c>
       <c r="L2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -2423,15 +2499,15 @@
         <v>2.99</v>
       </c>
       <c r="K3" t="n">
-        <v>0.10127</v>
+        <v>0.09927</v>
       </c>
       <c r="L3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -2446,7 +2522,7 @@
         <v>0.52</v>
       </c>
       <c r="F4" t="n">
-        <v>0.57295</v>
+        <v>0.56762</v>
       </c>
       <c r="G4" t="n">
         <v>1</v>
@@ -2461,15 +2537,15 @@
         <v>9.9</v>
       </c>
       <c r="K4" t="n">
-        <v>0.00266</v>
+        <v>0.002</v>
       </c>
       <c r="L4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B5" t="n">
         <v>80</v>
@@ -2494,12 +2570,12 @@
       <c r="J5"/>
       <c r="K5"/>
       <c r="L5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B6" t="n">
         <v>85</v>
@@ -2524,12 +2600,12 @@
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B7" t="n">
         <v>3</v>
@@ -2544,7 +2620,7 @@
         <v>1.23</v>
       </c>
       <c r="F7" t="n">
-        <v>0.3058</v>
+        <v>0.30513</v>
       </c>
       <c r="G7" t="n">
         <v>3</v>
@@ -2559,15 +2635,15 @@
         <v>1.31</v>
       </c>
       <c r="K7" t="n">
-        <v>0.28181</v>
+        <v>0.27981</v>
       </c>
       <c r="L7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B8" t="n">
         <v>1</v>
@@ -2600,12 +2676,12 @@
         <v>0.00067</v>
       </c>
       <c r="L8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B9" t="n">
         <v>1</v>
@@ -2638,12 +2714,12 @@
         <v>0.00067</v>
       </c>
       <c r="L9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B10" t="n">
         <v>71</v>
@@ -2668,12 +2744,12 @@
       <c r="J10"/>
       <c r="K10"/>
       <c r="L10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B11" t="n">
         <v>76</v>
@@ -2698,12 +2774,12 @@
       <c r="J11"/>
       <c r="K11"/>
       <c r="L11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B12" t="n">
         <v>3</v>
@@ -2736,12 +2812,12 @@
         <v>0.00133</v>
       </c>
       <c r="L12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B13" t="n">
         <v>1</v>
@@ -2756,7 +2832,7 @@
         <v>2.76</v>
       </c>
       <c r="F13" t="n">
-        <v>0.08328</v>
+        <v>0.08195</v>
       </c>
       <c r="G13" t="n">
         <v>1</v>
@@ -2774,12 +2850,12 @@
         <v>0.00067</v>
       </c>
       <c r="L13" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B14" t="n">
         <v>1</v>
@@ -2794,7 +2870,7 @@
         <v>1.64</v>
       </c>
       <c r="F14" t="n">
-        <v>0.18121</v>
+        <v>0.17988</v>
       </c>
       <c r="G14" t="n">
         <v>1</v>
@@ -2809,15 +2885,15 @@
         <v>0.53</v>
       </c>
       <c r="K14" t="n">
-        <v>0.47768</v>
+        <v>0.47901</v>
       </c>
       <c r="L14" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B15" t="n">
         <v>62</v>
@@ -2842,12 +2918,12 @@
       <c r="J15"/>
       <c r="K15"/>
       <c r="L15" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B16" t="n">
         <v>67</v>
@@ -2872,7 +2948,7 @@
       <c r="J16"/>
       <c r="K16"/>
       <c r="L16" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2882,10 +2958,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
@@ -2932,7 +3008,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
@@ -2964,7 +3040,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
@@ -2996,7 +3072,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -3028,7 +3104,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
@@ -3060,7 +3136,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
@@ -3092,7 +3168,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
@@ -3124,7 +3200,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
@@ -3156,7 +3232,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
@@ -3188,7 +3264,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
@@ -3220,7 +3296,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
@@ -3252,7 +3328,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
@@ -3289,10 +3365,10 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
@@ -3306,24 +3382,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B2" t="n">
         <v>0.8</v>
@@ -3340,7 +3416,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B3" t="n">
         <v>0.2</v>
@@ -3357,7 +3433,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B4" t="n">
         <v>-0.357</v>
@@ -3374,7 +3450,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B5" t="n">
         <v>-0.515</v>
@@ -3391,7 +3467,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B6" t="n">
         <v>0.235</v>
@@ -3408,7 +3484,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B7" t="n">
         <v>0.006</v>
@@ -3425,7 +3501,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B8" t="n">
         <v>-0.021</v>
@@ -3442,7 +3518,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B9" t="n">
         <v>-0.252</v>
@@ -3459,7 +3535,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B10" t="n">
         <v>0.222</v>
@@ -3476,7 +3552,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B11" t="n">
         <v>0.685</v>
@@ -3493,7 +3569,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B12" t="n">
         <v>-0.088</v>
@@ -3510,7 +3586,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B13" t="n">
         <v>-0.569</v>
@@ -3527,7 +3603,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B14" t="n">
         <v>-0.451</v>
@@ -3544,7 +3620,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B15" t="n">
         <v>0.05</v>
@@ -3561,7 +3637,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B16" t="n">
         <v>-0.154</v>
@@ -3578,7 +3654,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B17" t="n">
         <v>0.236</v>
@@ -3595,7 +3671,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B18" t="n">
         <v>0.071</v>
@@ -3612,7 +3688,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B19" t="n">
         <v>0.608</v>
@@ -3629,7 +3705,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B20" t="n">
         <v>-0.299</v>
@@ -3646,7 +3722,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B21" t="n">
         <v>0.134</v>
@@ -3663,7 +3739,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B22" t="n">
         <v>0.564</v>
@@ -3680,7 +3756,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B23" t="n">
         <v>0.524</v>
@@ -3697,7 +3773,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B24" t="n">
         <v>0.362</v>
@@ -3714,7 +3790,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B25" t="n">
         <v>0.673</v>
@@ -3731,7 +3807,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B26" t="n">
         <v>-0.177</v>
@@ -3748,7 +3824,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B27" t="n">
         <v>-0.181</v>
@@ -3765,7 +3841,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B28" t="n">
         <v>-0.482</v>
@@ -3782,7 +3858,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B29" t="n">
         <v>-0.891</v>
@@ -3799,7 +3875,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B30" t="n">
         <v>0.191</v>
@@ -3816,7 +3892,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B31" t="n">
         <v>-0.606</v>

</xml_diff>

<commit_message>
update to PCAs and new knit
</commit_message>
<xml_diff>
--- a/Data/Supplemental/Supplemental_Tables.xlsx
+++ b/Data/Supplemental/Supplemental_Tables.xlsx
@@ -2446,7 +2446,7 @@
         <v>0.55</v>
       </c>
       <c r="F2" t="n">
-        <v>0.74217</v>
+        <v>0.73751</v>
       </c>
       <c r="G2" t="n">
         <v>3</v>
@@ -2484,7 +2484,7 @@
         <v>6.65</v>
       </c>
       <c r="F3" t="n">
-        <v>0.00333</v>
+        <v>0.004</v>
       </c>
       <c r="G3" t="n">
         <v>1</v>
@@ -2499,7 +2499,7 @@
         <v>2.99</v>
       </c>
       <c r="K3" t="n">
-        <v>0.09927</v>
+        <v>0.09394</v>
       </c>
       <c r="L3" t="s">
         <v>31</v>
@@ -2522,7 +2522,7 @@
         <v>0.52</v>
       </c>
       <c r="F4" t="n">
-        <v>0.56762</v>
+        <v>0.58961</v>
       </c>
       <c r="G4" t="n">
         <v>1</v>
@@ -2537,7 +2537,7 @@
         <v>9.9</v>
       </c>
       <c r="K4" t="n">
-        <v>0.002</v>
+        <v>0.00133</v>
       </c>
       <c r="L4" t="s">
         <v>31</v>
@@ -2620,7 +2620,7 @@
         <v>1.23</v>
       </c>
       <c r="F7" t="n">
-        <v>0.30513</v>
+        <v>0.30446</v>
       </c>
       <c r="G7" t="n">
         <v>3</v>
@@ -2635,7 +2635,7 @@
         <v>1.31</v>
       </c>
       <c r="K7" t="n">
-        <v>0.27981</v>
+        <v>0.27382</v>
       </c>
       <c r="L7" t="s">
         <v>36</v>
@@ -2696,7 +2696,7 @@
         <v>1.75</v>
       </c>
       <c r="F9" t="n">
-        <v>0.15656</v>
+        <v>0.17522</v>
       </c>
       <c r="G9" t="n">
         <v>1</v>
@@ -2794,7 +2794,7 @@
         <v>3.48</v>
       </c>
       <c r="F12" t="n">
-        <v>0.01532</v>
+        <v>0.01799</v>
       </c>
       <c r="G12" t="n">
         <v>3</v>
@@ -2809,7 +2809,7 @@
         <v>7.04</v>
       </c>
       <c r="K12" t="n">
-        <v>0.00133</v>
+        <v>0.002</v>
       </c>
       <c r="L12" t="s">
         <v>37</v>
@@ -2832,7 +2832,7 @@
         <v>2.76</v>
       </c>
       <c r="F13" t="n">
-        <v>0.08195</v>
+        <v>0.08994</v>
       </c>
       <c r="G13" t="n">
         <v>1</v>
@@ -2870,7 +2870,7 @@
         <v>1.64</v>
       </c>
       <c r="F14" t="n">
-        <v>0.17988</v>
+        <v>0.18787</v>
       </c>
       <c r="G14" t="n">
         <v>1</v>
@@ -2885,7 +2885,7 @@
         <v>0.53</v>
       </c>
       <c r="K14" t="n">
-        <v>0.47901</v>
+        <v>0.48368</v>
       </c>
       <c r="L14" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
update PCAs by treatment and plascticity labels
</commit_message>
<xml_diff>
--- a/Data/Supplemental/Supplemental_Tables.xlsx
+++ b/Data/Supplemental/Supplemental_Tables.xlsx
@@ -1573,7 +1573,7 @@
         <v>0.11</v>
       </c>
       <c r="F12" t="n">
-        <v>0.74151</v>
+        <v>0.74284</v>
       </c>
       <c r="G12" t="s">
         <v>37</v>
@@ -2228,7 +2228,7 @@
         <v>2.87</v>
       </c>
       <c r="F3" t="n">
-        <v>0.09327</v>
+        <v>0.09127</v>
       </c>
     </row>
     <row r="4">
@@ -2248,7 +2248,7 @@
         <v>9.61</v>
       </c>
       <c r="F4" t="n">
-        <v>0.00466</v>
+        <v>0.00533</v>
       </c>
     </row>
     <row r="5">
@@ -2308,7 +2308,7 @@
         <v>2.51</v>
       </c>
       <c r="F7" t="n">
-        <v>0.02398</v>
+        <v>0.02265</v>
       </c>
     </row>
     <row r="8">
@@ -2446,7 +2446,7 @@
         <v>0.55</v>
       </c>
       <c r="F2" t="n">
-        <v>0.73751</v>
+        <v>0.74017</v>
       </c>
       <c r="G2" t="n">
         <v>3</v>
@@ -2499,7 +2499,7 @@
         <v>2.99</v>
       </c>
       <c r="K3" t="n">
-        <v>0.09394</v>
+        <v>0.0946</v>
       </c>
       <c r="L3" t="s">
         <v>31</v>
@@ -2522,7 +2522,7 @@
         <v>0.52</v>
       </c>
       <c r="F4" t="n">
-        <v>0.58961</v>
+        <v>0.58628</v>
       </c>
       <c r="G4" t="n">
         <v>1</v>
@@ -2620,7 +2620,7 @@
         <v>1.23</v>
       </c>
       <c r="F7" t="n">
-        <v>0.30446</v>
+        <v>0.30513</v>
       </c>
       <c r="G7" t="n">
         <v>3</v>
@@ -2696,7 +2696,7 @@
         <v>1.75</v>
       </c>
       <c r="F9" t="n">
-        <v>0.17522</v>
+        <v>0.17655</v>
       </c>
       <c r="G9" t="n">
         <v>1</v>
@@ -2794,7 +2794,7 @@
         <v>3.48</v>
       </c>
       <c r="F12" t="n">
-        <v>0.01799</v>
+        <v>0.01732</v>
       </c>
       <c r="G12" t="n">
         <v>3</v>
@@ -2832,7 +2832,7 @@
         <v>2.76</v>
       </c>
       <c r="F13" t="n">
-        <v>0.08994</v>
+        <v>0.08861</v>
       </c>
       <c r="G13" t="n">
         <v>1</v>
@@ -2870,7 +2870,7 @@
         <v>1.64</v>
       </c>
       <c r="F14" t="n">
-        <v>0.18787</v>
+        <v>0.18654</v>
       </c>
       <c r="G14" t="n">
         <v>1</v>
@@ -2885,7 +2885,7 @@
         <v>0.53</v>
       </c>
       <c r="K14" t="n">
-        <v>0.48368</v>
+        <v>0.48301</v>
       </c>
       <c r="L14" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
update to supplemental tables
</commit_message>
<xml_diff>
--- a/Data/Supplemental/Supplemental_Tables.xlsx
+++ b/Data/Supplemental/Supplemental_Tables.xlsx
@@ -56,7 +56,7 @@
     <t xml:space="preserve">ssid</t>
   </si>
   <si>
-    <t xml:space="preserve">reef environment * pCO2 + temperature + (1 | colony)b</t>
+    <t xml:space="preserve">reef environment * pCO2 + temperature + (1 | colony) + (1 | tank)</t>
   </si>
   <si>
     <t xml:space="preserve">glmerMod</t>
@@ -86,7 +86,7 @@
     <t xml:space="preserve">past</t>
   </si>
   <si>
-    <t xml:space="preserve">pCO2 + temperature + (1 | colony)b</t>
+    <t xml:space="preserve">pCO2 + temperature + (1 | colony) + (1 | tank)</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -623,7 +623,7 @@
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
     <col min="1" max="1" width="7.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="54.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="65.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="8.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="5.71" hidden="0" customWidth="1"/>
     <col min="5" max="5" width="5.71" hidden="0" customWidth="1"/>
@@ -1350,13 +1350,13 @@
         <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>61072</v>
+        <v>59423</v>
       </c>
       <c r="D2" t="n">
-        <v>0.208</v>
+        <v>0.203</v>
       </c>
       <c r="E2" t="n">
-        <v>8.15</v>
+        <v>7.93</v>
       </c>
       <c r="F2" t="n">
         <v>0.00067</v>
@@ -1373,16 +1373,16 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>7471</v>
+        <v>9320</v>
       </c>
       <c r="D3" t="n">
-        <v>0.025</v>
+        <v>0.032</v>
       </c>
       <c r="E3" t="n">
-        <v>2.99</v>
+        <v>3.73</v>
       </c>
       <c r="F3" t="n">
-        <v>0.09127</v>
+        <v>0.06529</v>
       </c>
       <c r="G3" t="s">
         <v>31</v>
@@ -1457,13 +1457,13 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>97850</v>
+        <v>101796</v>
       </c>
       <c r="D7" t="n">
-        <v>0.087</v>
+        <v>0.09</v>
       </c>
       <c r="E7" t="n">
-        <v>14.29</v>
+        <v>14.87</v>
       </c>
       <c r="F7" t="n">
         <v>0.00067</v>
@@ -1480,13 +1480,13 @@
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>515604</v>
+        <v>519372</v>
       </c>
       <c r="D8" t="n">
-        <v>0.456</v>
+        <v>0.46</v>
       </c>
       <c r="E8" t="n">
-        <v>75.29</v>
+        <v>75.84</v>
       </c>
       <c r="F8" t="n">
         <v>0.00067</v>
@@ -1564,16 +1564,16 @@
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>157</v>
+        <v>724</v>
       </c>
       <c r="D12" t="n">
-        <v>0.001</v>
+        <v>0.005</v>
       </c>
       <c r="E12" t="n">
-        <v>0.11</v>
+        <v>0.53</v>
       </c>
       <c r="F12" t="n">
-        <v>0.74284</v>
+        <v>0.45237</v>
       </c>
       <c r="G12" t="s">
         <v>37</v>
@@ -1587,13 +1587,13 @@
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>25414</v>
+        <v>27051</v>
       </c>
       <c r="D13" t="n">
-        <v>0.18</v>
+        <v>0.191</v>
       </c>
       <c r="E13" t="n">
-        <v>18.47</v>
+        <v>19.66</v>
       </c>
       <c r="F13" t="n">
         <v>0.00067</v>
@@ -2228,7 +2228,7 @@
         <v>2.87</v>
       </c>
       <c r="F3" t="n">
-        <v>0.09127</v>
+        <v>0.09327</v>
       </c>
     </row>
     <row r="4">
@@ -2248,7 +2248,7 @@
         <v>9.61</v>
       </c>
       <c r="F4" t="n">
-        <v>0.00533</v>
+        <v>0.00466</v>
       </c>
     </row>
     <row r="5">
@@ -2308,7 +2308,7 @@
         <v>2.51</v>
       </c>
       <c r="F7" t="n">
-        <v>0.02265</v>
+        <v>0.02398</v>
       </c>
     </row>
     <row r="8">
@@ -2446,7 +2446,7 @@
         <v>0.55</v>
       </c>
       <c r="F2" t="n">
-        <v>0.74017</v>
+        <v>0.74883</v>
       </c>
       <c r="G2" t="n">
         <v>3</v>
@@ -2484,7 +2484,7 @@
         <v>6.65</v>
       </c>
       <c r="F3" t="n">
-        <v>0.004</v>
+        <v>0.00333</v>
       </c>
       <c r="G3" t="n">
         <v>1</v>
@@ -2499,7 +2499,7 @@
         <v>2.99</v>
       </c>
       <c r="K3" t="n">
-        <v>0.0946</v>
+        <v>0.09927</v>
       </c>
       <c r="L3" t="s">
         <v>31</v>
@@ -2522,7 +2522,7 @@
         <v>0.52</v>
       </c>
       <c r="F4" t="n">
-        <v>0.58628</v>
+        <v>0.57295</v>
       </c>
       <c r="G4" t="n">
         <v>1</v>
@@ -2537,7 +2537,7 @@
         <v>9.9</v>
       </c>
       <c r="K4" t="n">
-        <v>0.00133</v>
+        <v>0.002</v>
       </c>
       <c r="L4" t="s">
         <v>31</v>
@@ -2620,7 +2620,7 @@
         <v>1.23</v>
       </c>
       <c r="F7" t="n">
-        <v>0.30513</v>
+        <v>0.30713</v>
       </c>
       <c r="G7" t="n">
         <v>3</v>
@@ -2635,7 +2635,7 @@
         <v>1.31</v>
       </c>
       <c r="K7" t="n">
-        <v>0.27382</v>
+        <v>0.27981</v>
       </c>
       <c r="L7" t="s">
         <v>36</v>
@@ -2696,7 +2696,7 @@
         <v>1.75</v>
       </c>
       <c r="F9" t="n">
-        <v>0.17655</v>
+        <v>0.15723</v>
       </c>
       <c r="G9" t="n">
         <v>1</v>
@@ -2794,7 +2794,7 @@
         <v>3.48</v>
       </c>
       <c r="F12" t="n">
-        <v>0.01732</v>
+        <v>0.01599</v>
       </c>
       <c r="G12" t="n">
         <v>3</v>
@@ -2809,7 +2809,7 @@
         <v>7.04</v>
       </c>
       <c r="K12" t="n">
-        <v>0.002</v>
+        <v>0.00133</v>
       </c>
       <c r="L12" t="s">
         <v>37</v>
@@ -2832,7 +2832,7 @@
         <v>2.76</v>
       </c>
       <c r="F13" t="n">
-        <v>0.08861</v>
+        <v>0.08328</v>
       </c>
       <c r="G13" t="n">
         <v>1</v>
@@ -2870,7 +2870,7 @@
         <v>1.64</v>
       </c>
       <c r="F14" t="n">
-        <v>0.18654</v>
+        <v>0.18055</v>
       </c>
       <c r="G14" t="n">
         <v>1</v>
@@ -2885,7 +2885,7 @@
         <v>0.53</v>
       </c>
       <c r="K14" t="n">
-        <v>0.48301</v>
+        <v>0.47901</v>
       </c>
       <c r="L14" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
update to all plasticity models and figures
</commit_message>
<xml_diff>
--- a/Data/Supplemental/Supplemental_Tables.xlsx
+++ b/Data/Supplemental/Supplemental_Tables.xlsx
@@ -689,13 +689,13 @@
         <v>0.307</v>
       </c>
       <c r="H2" t="n">
-        <v>0.339978050295066</v>
+        <v>0.339921366849096</v>
       </c>
       <c r="I2" t="n">
-        <v>0.824533279005936</v>
+        <v>0.824553438127845</v>
       </c>
       <c r="J2" t="n">
-        <v>0.297768433607305</v>
+        <v>0.29777176529434</v>
       </c>
       <c r="K2" t="n">
         <v>90.3</v>
@@ -724,13 +724,13 @@
         <v>0.322</v>
       </c>
       <c r="H3" t="n">
-        <v>0.270712896490855</v>
+        <v>0.270712906666334</v>
       </c>
       <c r="I3" t="n">
-        <v>0.88051736116787</v>
+        <v>0.880517357628651</v>
       </c>
       <c r="J3" t="n">
-        <v>0.309990521732364</v>
+        <v>0.309990520594351</v>
       </c>
       <c r="K3" t="n">
         <v>65.6</v>
@@ -753,19 +753,19 @@
         <v>247.1</v>
       </c>
       <c r="F4" t="n">
-        <v>0.512</v>
+        <v>0.511</v>
       </c>
       <c r="G4" t="n">
         <v>0.329</v>
       </c>
       <c r="H4" t="n">
-        <v>0.272192941547414</v>
+        <v>0.272155096268899</v>
       </c>
       <c r="I4" t="n">
-        <v>0.874857104921775</v>
+        <v>0.874876231377499</v>
       </c>
       <c r="J4" t="n">
-        <v>0.307309431789679</v>
+        <v>0.307314521780736</v>
       </c>
       <c r="K4" t="n">
         <v>63.3</v>
@@ -794,13 +794,13 @@
         <v>0.366</v>
       </c>
       <c r="H5" t="n">
-        <v>0.28206734361165</v>
+        <v>0.282067343982829</v>
       </c>
       <c r="I5" t="n">
-        <v>0.855828398376242</v>
+        <v>0.855828398264632</v>
       </c>
       <c r="J5" t="n">
-        <v>0.294010052276531</v>
+        <v>0.294010052236142</v>
       </c>
       <c r="K5" t="n">
         <v>62.8</v>
@@ -829,13 +829,13 @@
         <v>0.254</v>
       </c>
       <c r="H6" t="n">
-        <v>0.252287908819288</v>
+        <v>0.252287909332907</v>
       </c>
       <c r="I6" t="n">
-        <v>0.933847194038125</v>
+        <v>0.933847193844437</v>
       </c>
       <c r="J6" t="n">
-        <v>0.322867004362844</v>
+        <v>0.322867004307088</v>
       </c>
       <c r="K6" t="n">
         <v>38.9</v>
@@ -864,13 +864,13 @@
         <v>0.088</v>
       </c>
       <c r="H7" t="n">
-        <v>0.308813847521209</v>
+        <v>0.308813845572371</v>
       </c>
       <c r="I7" t="n">
-        <v>0.936882340613694</v>
+        <v>0.936882341333349</v>
       </c>
       <c r="J7" t="n">
-        <v>0.331059051190965</v>
+        <v>0.331059051431514</v>
       </c>
       <c r="K7" t="n">
         <v>30.5</v>
@@ -899,13 +899,13 @@
         <v>0.253</v>
       </c>
       <c r="H8" t="n">
-        <v>0.252780589487017</v>
+        <v>0.252780623700835</v>
       </c>
       <c r="I8" t="n">
-        <v>0.931849391942536</v>
+        <v>0.931849378942401</v>
       </c>
       <c r="J8" t="n">
-        <v>0.323013486807386</v>
+        <v>0.323013483263546</v>
       </c>
       <c r="K8" t="n">
         <v>25.7</v>
@@ -922,25 +922,25 @@
         <v>13</v>
       </c>
       <c r="D9" t="n">
-        <v>105.6</v>
+        <v>110.7</v>
       </c>
       <c r="E9" t="n">
-        <v>121.5</v>
+        <v>128.3</v>
       </c>
       <c r="F9" t="n">
-        <v>0.397</v>
+        <v>0.427</v>
       </c>
       <c r="G9" t="n">
-        <v>0.317</v>
+        <v>0.347</v>
       </c>
       <c r="H9" t="n">
-        <v>0.117033435887396</v>
+        <v>0.12264193082729</v>
       </c>
       <c r="I9" t="n">
-        <v>1.02875627247403</v>
+        <v>1.00977970615862</v>
       </c>
       <c r="J9" t="n">
-        <v>0.342860527251939</v>
+        <v>0.335976868226673</v>
       </c>
       <c r="K9" t="n">
         <v>71.4</v>
@@ -957,28 +957,28 @@
         <v>13</v>
       </c>
       <c r="D10" t="n">
-        <v>100.8</v>
+        <v>106</v>
       </c>
       <c r="E10" t="n">
-        <v>111.8</v>
+        <v>118.6</v>
       </c>
       <c r="F10" t="n">
-        <v>0.309</v>
+        <v>0.341</v>
       </c>
       <c r="G10" t="n">
-        <v>0.261</v>
+        <v>0.292</v>
       </c>
       <c r="H10" t="n">
-        <v>0.0648056876434838</v>
+        <v>0.069512358021633</v>
       </c>
       <c r="I10" t="n">
-        <v>1.14657450978296</v>
+        <v>1.12393872070358</v>
       </c>
       <c r="J10" t="n">
-        <v>0.36062662799942</v>
+        <v>0.353702412571083</v>
       </c>
       <c r="K10" t="n">
-        <v>45</v>
+        <v>44.8</v>
       </c>
     </row>
     <row r="11">
@@ -992,28 +992,28 @@
         <v>13</v>
       </c>
       <c r="D11" t="n">
-        <v>101.6</v>
+        <v>106.9</v>
       </c>
       <c r="E11" t="n">
-        <v>112.6</v>
+        <v>119.5</v>
       </c>
       <c r="F11" t="n">
-        <v>0.278</v>
+        <v>0.313</v>
       </c>
       <c r="G11" t="n">
-        <v>0.238</v>
+        <v>0.271</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0533714820211562</v>
+        <v>0.0572627646077092</v>
       </c>
       <c r="I11" t="n">
-        <v>1.13665595795787</v>
+        <v>1.11383231952833</v>
       </c>
       <c r="J11" t="n">
-        <v>0.359834556845443</v>
+        <v>0.352824835342725</v>
       </c>
       <c r="K11" t="n">
-        <v>36.2</v>
+        <v>36.3</v>
       </c>
     </row>
     <row r="12">
@@ -1027,28 +1027,28 @@
         <v>13</v>
       </c>
       <c r="D12" t="n">
-        <v>97.5</v>
+        <v>102.8</v>
       </c>
       <c r="E12" t="n">
-        <v>104.8</v>
+        <v>111.6</v>
       </c>
       <c r="F12" t="n">
-        <v>0.232</v>
+        <v>0.268</v>
       </c>
       <c r="G12" t="n">
-        <v>0.188</v>
+        <v>0.224</v>
       </c>
       <c r="H12" t="n">
-        <v>0.0541808464958402</v>
+        <v>0.056048071109652</v>
       </c>
       <c r="I12" t="n">
-        <v>1.22142050234447</v>
+        <v>1.19677569320301</v>
       </c>
       <c r="J12" t="n">
-        <v>0.371319943278335</v>
+        <v>0.36408716814135</v>
       </c>
       <c r="K12" t="n">
-        <v>28.8</v>
+        <v>28.6</v>
       </c>
     </row>
     <row r="13">
@@ -1074,13 +1074,13 @@
         <v>0.195</v>
       </c>
       <c r="H13" t="n">
-        <v>0.405142468828212</v>
+        <v>0.405142466313655</v>
       </c>
       <c r="I13" t="n">
-        <v>0.710112914386074</v>
+        <v>0.710112914902594</v>
       </c>
       <c r="J13" t="n">
-        <v>0.231080473857171</v>
+        <v>0.231080474175141</v>
       </c>
       <c r="K13" t="n">
         <v>76.2</v>
@@ -1109,13 +1109,13 @@
         <v>0.195</v>
       </c>
       <c r="H14" t="n">
-        <v>0.405616901906066</v>
+        <v>0.405616901269354</v>
       </c>
       <c r="I14" t="n">
-        <v>0.70994797179576</v>
+        <v>0.709947971925215</v>
       </c>
       <c r="J14" t="n">
-        <v>0.2309514006937</v>
+        <v>0.230951400774421</v>
       </c>
       <c r="K14" t="n">
         <v>73</v>
@@ -1144,13 +1144,13 @@
         <v>0.199</v>
       </c>
       <c r="H15" t="n">
-        <v>0.409641424663849</v>
+        <v>0.409641426216089</v>
       </c>
       <c r="I15" t="n">
-        <v>0.706971647584522</v>
+        <v>0.70697164728988</v>
       </c>
       <c r="J15" t="n">
-        <v>0.229916347449218</v>
+        <v>0.229916347254973</v>
       </c>
       <c r="K15" t="n">
         <v>71.4</v>
@@ -1179,13 +1179,13 @@
         <v>0.145</v>
       </c>
       <c r="H16" t="n">
-        <v>0.407604756872208</v>
+        <v>0.40760856417087</v>
       </c>
       <c r="I16" t="n">
-        <v>0.727645800628731</v>
+        <v>0.727645208726944</v>
       </c>
       <c r="J16" t="n">
-        <v>0.236973047639022</v>
+        <v>0.236972613071863</v>
       </c>
       <c r="K16" t="n">
         <v>45.1</v>
@@ -1214,13 +1214,13 @@
         <v>0.174</v>
       </c>
       <c r="H17" t="n">
-        <v>0.393286215931064</v>
+        <v>0.393286214699538</v>
       </c>
       <c r="I17" t="n">
-        <v>0.733244393163204</v>
+        <v>0.73324439340205</v>
       </c>
       <c r="J17" t="n">
-        <v>0.237295448325152</v>
+        <v>0.237295448480225</v>
       </c>
       <c r="K17" t="n">
         <v>38.7</v>
@@ -1249,13 +1249,13 @@
         <v>0.147</v>
       </c>
       <c r="H18" t="n">
-        <v>0.396708536729162</v>
+        <v>0.396708536396551</v>
       </c>
       <c r="I18" t="n">
-        <v>0.732981216119454</v>
+        <v>0.732981216183524</v>
       </c>
       <c r="J18" t="n">
-        <v>0.238221370319828</v>
+        <v>0.238221370362628</v>
       </c>
       <c r="K18" t="n">
         <v>32.7</v>
@@ -1284,13 +1284,13 @@
         <v>0.174</v>
       </c>
       <c r="H19" t="n">
-        <v>0.394015465922658</v>
+        <v>0.394017895328747</v>
       </c>
       <c r="I19" t="n">
-        <v>0.734046668651323</v>
+        <v>0.734044282144376</v>
       </c>
       <c r="J19" t="n">
-        <v>0.237351188594544</v>
+        <v>0.23735001040535</v>
       </c>
       <c r="K19" t="n">
         <v>30.8</v>
@@ -1382,7 +1382,7 @@
         <v>3.73</v>
       </c>
       <c r="F3" t="n">
-        <v>0.06529</v>
+        <v>0.05929</v>
       </c>
       <c r="G3" t="s">
         <v>31</v>
@@ -1512,7 +1512,7 @@
         <v>1.48</v>
       </c>
       <c r="F9" t="n">
-        <v>0.23651</v>
+        <v>0.22785</v>
       </c>
       <c r="G9" t="s">
         <v>36</v>
@@ -1573,7 +1573,7 @@
         <v>0.53</v>
       </c>
       <c r="F12" t="n">
-        <v>0.45237</v>
+        <v>0.46036</v>
       </c>
       <c r="G12" t="s">
         <v>37</v>
@@ -1596,7 +1596,7 @@
         <v>19.66</v>
       </c>
       <c r="F13" t="n">
-        <v>0.00067</v>
+        <v>0.00133</v>
       </c>
       <c r="G13" t="s">
         <v>37</v>
@@ -1716,7 +1716,7 @@
         <v>0.006</v>
       </c>
       <c r="D2" t="n">
-        <v>187.16</v>
+        <v>187.01</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -1736,10 +1736,10 @@
         <v>0.006</v>
       </c>
       <c r="D3" t="n">
-        <v>1.73</v>
+        <v>1.72</v>
       </c>
       <c r="E3" t="n">
-        <v>0.084</v>
+        <v>0.085</v>
       </c>
       <c r="F3" t="s">
         <v>31</v>
@@ -1756,7 +1756,7 @@
         <v>0.006</v>
       </c>
       <c r="D4" t="n">
-        <v>67.01</v>
+        <v>66.95</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -1776,7 +1776,7 @@
         <v>0.006</v>
       </c>
       <c r="D5" t="n">
-        <v>39.36</v>
+        <v>39.32</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -1796,7 +1796,7 @@
         <v>0.006</v>
       </c>
       <c r="D6" t="n">
-        <v>78.84</v>
+        <v>78.75</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -1816,10 +1816,10 @@
         <v>0.006</v>
       </c>
       <c r="D7" t="n">
-        <v>0.32</v>
+        <v>0.31</v>
       </c>
       <c r="E7" t="n">
-        <v>0.748</v>
+        <v>0.753</v>
       </c>
       <c r="F7" t="s">
         <v>31</v>
@@ -1836,7 +1836,7 @@
         <v>0.006</v>
       </c>
       <c r="D8" t="n">
-        <v>-136.94</v>
+        <v>-136.81</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -1856,7 +1856,7 @@
         <v>0.006</v>
       </c>
       <c r="D9" t="n">
-        <v>-79.4</v>
+        <v>-79.33</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -1876,7 +1876,7 @@
         <v>0.006</v>
       </c>
       <c r="D10" t="n">
-        <v>-58.53</v>
+        <v>-58.48</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -2026,13 +2026,13 @@
         <v>41</v>
       </c>
       <c r="B19" t="n">
-        <v>1.038</v>
+        <v>1.033</v>
       </c>
       <c r="C19" t="n">
-        <v>0.121</v>
+        <v>0.125</v>
       </c>
       <c r="D19" t="n">
-        <v>8.61</v>
+        <v>8.25</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
@@ -2046,16 +2046,16 @@
         <v>43</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.047</v>
+        <v>-0.045</v>
       </c>
       <c r="C20" t="n">
-        <v>0.11</v>
+        <v>0.115</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.43</v>
+        <v>-0.39</v>
       </c>
       <c r="E20" t="n">
-        <v>0.67</v>
+        <v>0.694</v>
       </c>
       <c r="F20" t="s">
         <v>37</v>
@@ -2066,16 +2066,16 @@
         <v>44</v>
       </c>
       <c r="B21" t="n">
-        <v>0.032</v>
+        <v>0.033</v>
       </c>
       <c r="C21" t="n">
-        <v>0.075</v>
+        <v>0.079</v>
       </c>
       <c r="D21" t="n">
-        <v>0.44</v>
+        <v>0.42</v>
       </c>
       <c r="E21" t="n">
-        <v>0.664</v>
+        <v>0.676</v>
       </c>
       <c r="F21" t="s">
         <v>37</v>
@@ -2086,16 +2086,16 @@
         <v>45</v>
       </c>
       <c r="B22" t="n">
-        <v>0.122</v>
+        <v>0.124</v>
       </c>
       <c r="C22" t="n">
-        <v>0.078</v>
+        <v>0.082</v>
       </c>
       <c r="D22" t="n">
-        <v>1.57</v>
+        <v>1.51</v>
       </c>
       <c r="E22" t="n">
-        <v>0.116</v>
+        <v>0.131</v>
       </c>
       <c r="F22" t="s">
         <v>37</v>
@@ -2106,13 +2106,13 @@
         <v>46</v>
       </c>
       <c r="B23" t="n">
-        <v>0.264</v>
+        <v>0.262</v>
       </c>
       <c r="C23" t="n">
-        <v>0.065</v>
+        <v>0.069</v>
       </c>
       <c r="D23" t="n">
-        <v>4.07</v>
+        <v>3.82</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
@@ -2126,7 +2126,7 @@
         <v>5</v>
       </c>
       <c r="B24" t="n">
-        <v>0.485</v>
+        <v>0.493</v>
       </c>
       <c r="C24"/>
       <c r="D24"/>
@@ -2140,7 +2140,7 @@
         <v>6</v>
       </c>
       <c r="B25" t="n">
-        <v>0.147</v>
+        <v>0.145</v>
       </c>
       <c r="C25"/>
       <c r="D25"/>
@@ -2228,7 +2228,7 @@
         <v>2.87</v>
       </c>
       <c r="F3" t="n">
-        <v>0.09327</v>
+        <v>0.0986</v>
       </c>
     </row>
     <row r="4">
@@ -2248,7 +2248,7 @@
         <v>9.61</v>
       </c>
       <c r="F4" t="n">
-        <v>0.00466</v>
+        <v>0.004</v>
       </c>
     </row>
     <row r="5">
@@ -2308,7 +2308,7 @@
         <v>2.51</v>
       </c>
       <c r="F7" t="n">
-        <v>0.02398</v>
+        <v>0.01865</v>
       </c>
     </row>
     <row r="8">
@@ -2328,7 +2328,7 @@
         <v>6.39</v>
       </c>
       <c r="F8" t="n">
-        <v>0.004</v>
+        <v>0.00533</v>
       </c>
     </row>
     <row r="9">
@@ -2484,7 +2484,7 @@
         <v>6.65</v>
       </c>
       <c r="F3" t="n">
-        <v>0.00333</v>
+        <v>0.00666</v>
       </c>
       <c r="G3" t="n">
         <v>1</v>
@@ -2499,7 +2499,7 @@
         <v>2.99</v>
       </c>
       <c r="K3" t="n">
-        <v>0.09927</v>
+        <v>0.0966</v>
       </c>
       <c r="L3" t="s">
         <v>31</v>
@@ -2522,7 +2522,7 @@
         <v>0.52</v>
       </c>
       <c r="F4" t="n">
-        <v>0.57295</v>
+        <v>0.56762</v>
       </c>
       <c r="G4" t="n">
         <v>1</v>
@@ -2537,7 +2537,7 @@
         <v>9.9</v>
       </c>
       <c r="K4" t="n">
-        <v>0.002</v>
+        <v>0.00266</v>
       </c>
       <c r="L4" t="s">
         <v>31</v>
@@ -2620,7 +2620,7 @@
         <v>1.23</v>
       </c>
       <c r="F7" t="n">
-        <v>0.30713</v>
+        <v>0.27515</v>
       </c>
       <c r="G7" t="n">
         <v>3</v>
@@ -2635,7 +2635,7 @@
         <v>1.31</v>
       </c>
       <c r="K7" t="n">
-        <v>0.27981</v>
+        <v>0.28115</v>
       </c>
       <c r="L7" t="s">
         <v>36</v>
@@ -2696,7 +2696,7 @@
         <v>1.75</v>
       </c>
       <c r="F9" t="n">
-        <v>0.15723</v>
+        <v>0.16855</v>
       </c>
       <c r="G9" t="n">
         <v>1</v>
@@ -2711,7 +2711,7 @@
         <v>14.87</v>
       </c>
       <c r="K9" t="n">
-        <v>0.00067</v>
+        <v>0.00133</v>
       </c>
       <c r="L9" t="s">
         <v>36</v>
@@ -2794,7 +2794,7 @@
         <v>3.48</v>
       </c>
       <c r="F12" t="n">
-        <v>0.01599</v>
+        <v>0.01332</v>
       </c>
       <c r="G12" t="n">
         <v>3</v>
@@ -2809,7 +2809,7 @@
         <v>7.04</v>
       </c>
       <c r="K12" t="n">
-        <v>0.00133</v>
+        <v>0.00067</v>
       </c>
       <c r="L12" t="s">
         <v>37</v>
@@ -2832,7 +2832,7 @@
         <v>2.76</v>
       </c>
       <c r="F13" t="n">
-        <v>0.08328</v>
+        <v>0.09127</v>
       </c>
       <c r="G13" t="n">
         <v>1</v>
@@ -2870,7 +2870,7 @@
         <v>1.64</v>
       </c>
       <c r="F14" t="n">
-        <v>0.18055</v>
+        <v>0.20253</v>
       </c>
       <c r="G14" t="n">
         <v>1</v>
@@ -2885,7 +2885,7 @@
         <v>0.53</v>
       </c>
       <c r="K14" t="n">
-        <v>0.47901</v>
+        <v>0.46636</v>
       </c>
       <c r="L14" t="s">
         <v>37</v>
@@ -3026,13 +3026,13 @@
         <v>0.318</v>
       </c>
       <c r="G2" t="n">
-        <v>0.163808918863028</v>
+        <v>0.163808918846475</v>
       </c>
       <c r="H2" t="n">
-        <v>0.884761957168762</v>
+        <v>0.884761957169536</v>
       </c>
       <c r="I2" t="n">
-        <v>0.445413568049554</v>
+        <v>0.445413568051623</v>
       </c>
       <c r="J2" t="n">
         <v>71.4</v>
@@ -3058,13 +3058,13 @@
         <v>0.279</v>
       </c>
       <c r="G3" t="n">
-        <v>0.155601596236983</v>
+        <v>0.155601596236995</v>
       </c>
       <c r="H3" t="n">
-        <v>0.913117790532205</v>
+        <v>0.913117790532039</v>
       </c>
       <c r="I3" t="n">
-        <v>0.459316964023187</v>
+        <v>0.45931696402324</v>
       </c>
       <c r="J3" t="n">
         <v>69.6</v>
@@ -3090,13 +3090,13 @@
         <v>0.279</v>
       </c>
       <c r="G4" t="n">
-        <v>0.15560159623606</v>
+        <v>0.155601596236034</v>
       </c>
       <c r="H4" t="n">
-        <v>0.913117790532225</v>
+        <v>0.913117790532143</v>
       </c>
       <c r="I4" t="n">
-        <v>0.45931696402331</v>
+        <v>0.459316964023365</v>
       </c>
       <c r="J4" t="n">
         <v>69.6</v>
@@ -3122,13 +3122,13 @@
         <v>0.279</v>
       </c>
       <c r="G5" t="n">
-        <v>0.15560159623606</v>
+        <v>0.155601596236034</v>
       </c>
       <c r="H5" t="n">
-        <v>0.913117790532225</v>
+        <v>0.913117790532143</v>
       </c>
       <c r="I5" t="n">
-        <v>0.45931696402331</v>
+        <v>0.459316964023365</v>
       </c>
       <c r="J5" t="n">
         <v>69.6</v>
@@ -3151,16 +3151,16 @@
         <v>0.323</v>
       </c>
       <c r="F6" t="n">
-        <v>0.213</v>
+        <v>0.212</v>
       </c>
       <c r="G6" t="n">
-        <v>0.140299887725969</v>
+        <v>0.140275722020262</v>
       </c>
       <c r="H6" t="n">
-        <v>0.935545346998836</v>
+        <v>0.935551604873005</v>
       </c>
       <c r="I6" t="n">
-        <v>0.476813006415758</v>
+        <v>0.476818047697685</v>
       </c>
       <c r="J6" t="n">
         <v>60.8</v>
@@ -3186,16 +3186,16 @@
         <v>0.139</v>
       </c>
       <c r="G7" t="n">
-        <v>0.163557385601623</v>
+        <v>0.163720683028945</v>
       </c>
       <c r="H7" t="n">
-        <v>0.950478505425775</v>
+        <v>0.950425796937665</v>
       </c>
       <c r="I7" t="n">
-        <v>0.488720975684716</v>
+        <v>0.488694314791684</v>
       </c>
       <c r="J7" t="n">
-        <v>59</v>
+        <v>59.1</v>
       </c>
     </row>
     <row r="8">
@@ -3218,13 +3218,13 @@
         <v>0.144</v>
       </c>
       <c r="G8" t="n">
-        <v>0.161404588840658</v>
+        <v>0.161404588856711</v>
       </c>
       <c r="H8" t="n">
-        <v>0.950207028249464</v>
+        <v>0.950207028246836</v>
       </c>
       <c r="I8" t="n">
-        <v>0.488554386711269</v>
+        <v>0.488554386709045</v>
       </c>
       <c r="J8" t="n">
         <v>58.1</v>
@@ -3250,13 +3250,13 @@
         <v>0.225</v>
       </c>
       <c r="G9" t="n">
-        <v>0.144855151671333</v>
+        <v>0.144860307744428</v>
       </c>
       <c r="H9" t="n">
-        <v>0.948918411064145</v>
+        <v>0.948916968928776</v>
       </c>
       <c r="I9" t="n">
-        <v>0.477396911101414</v>
+        <v>0.477395026003451</v>
       </c>
       <c r="J9" t="n">
         <v>52.4</v>
@@ -3282,13 +3282,13 @@
         <v>0.093</v>
       </c>
       <c r="G10" t="n">
-        <v>0.15714351271921</v>
+        <v>0.157143513626403</v>
       </c>
       <c r="H10" t="n">
-        <v>0.982507593773722</v>
+        <v>0.982507593585701</v>
       </c>
       <c r="I10" t="n">
-        <v>0.505803686210093</v>
+        <v>0.505803686093402</v>
       </c>
       <c r="J10" t="n">
         <v>41.7</v>
@@ -3314,13 +3314,13 @@
         <v>0.095</v>
       </c>
       <c r="G11" t="n">
-        <v>0.121607431578392</v>
+        <v>0.121607431312658</v>
       </c>
       <c r="H11" t="n">
-        <v>1.01492820576266</v>
+        <v>1.01492820585159</v>
       </c>
       <c r="I11" t="n">
-        <v>0.513921291795915</v>
+        <v>0.513921291826242</v>
       </c>
       <c r="J11" t="n">
         <v>28.7</v>
@@ -3346,13 +3346,13 @@
         <v>0.113</v>
       </c>
       <c r="G12" t="n">
-        <v>0.122648787498884</v>
+        <v>0.122648785796666</v>
       </c>
       <c r="H12" t="n">
-        <v>1.00853413549591</v>
+        <v>1.00853413602528</v>
       </c>
       <c r="I12" t="n">
-        <v>0.508488836427211</v>
+        <v>0.508488836608921</v>
       </c>
       <c r="J12" t="n">
         <v>28.3</v>
@@ -3419,7 +3419,7 @@
         <v>36</v>
       </c>
       <c r="B3" t="n">
-        <v>0.2</v>
+        <v>0.199</v>
       </c>
       <c r="C3" t="n">
         <v>0.29</v>
@@ -3428,7 +3428,7 @@
         <v>0.69</v>
       </c>
       <c r="E3" t="n">
-        <v>0.491</v>
+        <v>0.492</v>
       </c>
     </row>
     <row r="4">
@@ -3442,7 +3442,7 @@
         <v>0.244</v>
       </c>
       <c r="D4" t="n">
-        <v>-1.47</v>
+        <v>-1.46</v>
       </c>
       <c r="E4" t="n">
         <v>0.143</v>
@@ -3470,7 +3470,7 @@
         <v>43</v>
       </c>
       <c r="B6" t="n">
-        <v>0.235</v>
+        <v>0.234</v>
       </c>
       <c r="C6" t="n">
         <v>0.214</v>
@@ -3479,7 +3479,7 @@
         <v>1.1</v>
       </c>
       <c r="E6" t="n">
-        <v>0.272</v>
+        <v>0.273</v>
       </c>
     </row>
     <row r="7">
@@ -3487,7 +3487,7 @@
         <v>44</v>
       </c>
       <c r="B7" t="n">
-        <v>0.006</v>
+        <v>0.005</v>
       </c>
       <c r="C7" t="n">
         <v>0.164</v>
@@ -3496,7 +3496,7 @@
         <v>0.03</v>
       </c>
       <c r="E7" t="n">
-        <v>0.972</v>
+        <v>0.974</v>
       </c>
     </row>
     <row r="8">
@@ -3513,7 +3513,7 @@
         <v>-0.13</v>
       </c>
       <c r="E8" t="n">
-        <v>0.896</v>
+        <v>0.895</v>
       </c>
     </row>
     <row r="9">
@@ -3527,10 +3527,10 @@
         <v>0.128</v>
       </c>
       <c r="D9" t="n">
-        <v>-1.97</v>
+        <v>-1.96</v>
       </c>
       <c r="E9" t="n">
-        <v>0.049</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="10">
@@ -3538,7 +3538,7 @@
         <v>69</v>
       </c>
       <c r="B10" t="n">
-        <v>0.222</v>
+        <v>0.223</v>
       </c>
       <c r="C10" t="n">
         <v>0.308</v>
@@ -3547,7 +3547,7 @@
         <v>0.72</v>
       </c>
       <c r="E10" t="n">
-        <v>0.472</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="11">
@@ -3561,7 +3561,7 @@
         <v>0.27</v>
       </c>
       <c r="D11" t="n">
-        <v>2.54</v>
+        <v>2.53</v>
       </c>
       <c r="E11" t="n">
         <v>0.011</v>
@@ -3589,7 +3589,7 @@
         <v>72</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.569</v>
+        <v>-0.568</v>
       </c>
       <c r="C13" t="n">
         <v>0.339</v>
@@ -3598,7 +3598,7 @@
         <v>-1.68</v>
       </c>
       <c r="E13" t="n">
-        <v>0.093</v>
+        <v>0.094</v>
       </c>
     </row>
     <row r="14">
@@ -3606,7 +3606,7 @@
         <v>73</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.451</v>
+        <v>-0.45</v>
       </c>
       <c r="C14" t="n">
         <v>0.298</v>
@@ -3623,7 +3623,7 @@
         <v>74</v>
       </c>
       <c r="B15" t="n">
-        <v>0.05</v>
+        <v>0.051</v>
       </c>
       <c r="C15" t="n">
         <v>0.24</v>
@@ -3632,7 +3632,7 @@
         <v>0.21</v>
       </c>
       <c r="E15" t="n">
-        <v>0.835</v>
+        <v>0.833</v>
       </c>
     </row>
     <row r="16">
@@ -3646,10 +3646,10 @@
         <v>0.288</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.54</v>
+        <v>-0.53</v>
       </c>
       <c r="E16" t="n">
-        <v>0.592</v>
+        <v>0.593</v>
       </c>
     </row>
     <row r="17">
@@ -3666,7 +3666,7 @@
         <v>0.96</v>
       </c>
       <c r="E17" t="n">
-        <v>0.336</v>
+        <v>0.335</v>
       </c>
     </row>
     <row r="18">
@@ -3674,7 +3674,7 @@
         <v>77</v>
       </c>
       <c r="B18" t="n">
-        <v>0.071</v>
+        <v>0.072</v>
       </c>
       <c r="C18" t="n">
         <v>0.25</v>
@@ -3683,7 +3683,7 @@
         <v>0.29</v>
       </c>
       <c r="E18" t="n">
-        <v>0.775</v>
+        <v>0.774</v>
       </c>
     </row>
     <row r="19">
@@ -3734,7 +3734,7 @@
         <v>0.59</v>
       </c>
       <c r="E21" t="n">
-        <v>0.556</v>
+        <v>0.555</v>
       </c>
     </row>
     <row r="22">
@@ -3785,7 +3785,7 @@
         <v>0.44</v>
       </c>
       <c r="E24" t="n">
-        <v>0.658</v>
+        <v>0.659</v>
       </c>
     </row>
     <row r="25">
@@ -3802,7 +3802,7 @@
         <v>1.42</v>
       </c>
       <c r="E25" t="n">
-        <v>0.155</v>
+        <v>0.154</v>
       </c>
     </row>
     <row r="26">
@@ -3810,16 +3810,16 @@
         <v>85</v>
       </c>
       <c r="B26" t="n">
-        <v>-0.177</v>
+        <v>-0.179</v>
       </c>
       <c r="C26" t="n">
         <v>0.418</v>
       </c>
       <c r="D26" t="n">
-        <v>-0.42</v>
+        <v>-0.43</v>
       </c>
       <c r="E26" t="n">
-        <v>0.672</v>
+        <v>0.669</v>
       </c>
     </row>
     <row r="27">
@@ -3827,7 +3827,7 @@
         <v>86</v>
       </c>
       <c r="B27" t="n">
-        <v>-0.181</v>
+        <v>-0.18</v>
       </c>
       <c r="C27" t="n">
         <v>0.335</v>
@@ -3861,7 +3861,7 @@
         <v>88</v>
       </c>
       <c r="B29" t="n">
-        <v>-0.891</v>
+        <v>-0.89</v>
       </c>
       <c r="C29" t="n">
         <v>0.341</v>
@@ -3878,7 +3878,7 @@
         <v>89</v>
       </c>
       <c r="B30" t="n">
-        <v>0.191</v>
+        <v>0.189</v>
       </c>
       <c r="C30" t="n">
         <v>0.35</v>
@@ -3887,7 +3887,7 @@
         <v>0.54</v>
       </c>
       <c r="E30" t="n">
-        <v>0.586</v>
+        <v>0.589</v>
       </c>
     </row>
     <row r="31">
@@ -3895,7 +3895,7 @@
         <v>90</v>
       </c>
       <c r="B31" t="n">
-        <v>-0.606</v>
+        <v>-0.607</v>
       </c>
       <c r="C31" t="n">
         <v>0.281</v>

</xml_diff>

<commit_message>
added tables and figs at request of reviewers
</commit_message>
<xml_diff>
--- a/Data/Supplemental/Supplemental_Tables.xlsx
+++ b/Data/Supplemental/Supplemental_Tables.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="false"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
@@ -296,7 +296,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
   <fonts count="1">
     <font>
@@ -615,10 +615,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
@@ -1303,10 +1303,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
@@ -1670,10 +1670,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
@@ -2156,10 +2156,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
@@ -2370,10 +2370,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
@@ -2446,7 +2446,7 @@
         <v>0.55</v>
       </c>
       <c r="F2" t="n">
-        <v>0.74883</v>
+        <v>0.74817</v>
       </c>
       <c r="G2" t="n">
         <v>3</v>
@@ -2522,7 +2522,7 @@
         <v>0.52</v>
       </c>
       <c r="F4" t="n">
-        <v>0.56762</v>
+        <v>0.56829</v>
       </c>
       <c r="G4" t="n">
         <v>1</v>
@@ -2696,7 +2696,7 @@
         <v>1.75</v>
       </c>
       <c r="F9" t="n">
-        <v>0.16855</v>
+        <v>0.16589</v>
       </c>
       <c r="G9" t="n">
         <v>1</v>
@@ -2870,7 +2870,7 @@
         <v>1.64</v>
       </c>
       <c r="F14" t="n">
-        <v>0.20253</v>
+        <v>0.20386</v>
       </c>
       <c r="G14" t="n">
         <v>1</v>
@@ -2885,7 +2885,7 @@
         <v>0.53</v>
       </c>
       <c r="K14" t="n">
-        <v>0.46636</v>
+        <v>0.46569</v>
       </c>
       <c r="L14" t="s">
         <v>37</v>
@@ -2958,10 +2958,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
@@ -3365,10 +3365,10 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>

</xml_diff>

<commit_message>
updated supplemental tables to add one for sample size
</commit_message>
<xml_diff>
--- a/Data/Supplemental/Supplemental_Tables.xlsx
+++ b/Data/Supplemental/Supplemental_Tables.xlsx
@@ -1,28 +1,158 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr date1904="false"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Table S1 - Plasticity AIC" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Table S2 - PERMANOVA" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Table S3 - Plasticity GLM" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Table S4 - Species PERMANOVA" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Table S5 - HostVsymb PERMANOVA" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Table S6 - HostVsymb Plast AIC" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Table S7 - HostVsymb Plast GLM" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Table S1 - Sample Size" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Table S2 - Plasticity AIC" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Table S3 - PERMANOVA" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Table S4 - Plasticity GLM" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Table S5 - Species PERMANOVA" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Table S6 - HostVsymb PERMANOVA" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Table S7 - HostVsymb Plast AIC" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Table S8 - HostVsymb Plast GLM" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="134">
+  <si>
+    <t xml:space="preserve">group</t>
+  </si>
   <si>
     <t xml:space="preserve">Species</t>
   </si>
   <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Treatment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offshore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inshore</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Treatment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Offshore</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Inshore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A_current day (uatm)_28C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">current day (uatm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A_current day (uatm)_31C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A_end-of-century (uatm)_28C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end-of-century (uatm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A_end-of-century (uatm)_31C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A_extreme (uatm)_28C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extreme (uatm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A_extreme (uatm)_31C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A_pre industrial (uatm)_28C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pre industrial (uatm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A_pre industrial (uatm)_31C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P_current day (uatm)_28C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P_current day (uatm)_31C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P_end-of-century (uatm)_28C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P_end-of-century (uatm)_31C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P_extreme (uatm)_28C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P_extreme (uatm)_31C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P_pre industrial (uatm)_28C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P_pre industrial (uatm)_31C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S_current day (uatm)_28C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S_current day (uatm)_31C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S_end-of-century (uatm)_28C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S_end-of-century (uatm)_31C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S_extreme (uatm)_28C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S_extreme (uatm)_31C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S_pre industrial (uatm)_28C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S_pre industrial (uatm)_31C</t>
+  </si>
+  <si>
     <t xml:space="preserve">Model formula</t>
   </si>
   <si>
@@ -32,9 +162,15 @@
     <t xml:space="preserve">AIC</t>
   </si>
   <si>
+    <t xml:space="preserve">AIC_wt</t>
+  </si>
+  <si>
     <t xml:space="preserve">BIC</t>
   </si>
   <si>
+    <t xml:space="preserve">BIC_wt</t>
+  </si>
+  <si>
     <t xml:space="preserve">Conditional R2</t>
   </si>
   <si>
@@ -50,36 +186,33 @@
     <t xml:space="preserve">Sigma</t>
   </si>
   <si>
-    <t xml:space="preserve">Performance score</t>
-  </si>
-  <si>
     <t xml:space="preserve">ssid</t>
   </si>
   <si>
+    <t xml:space="preserve">reef environment * pCO2 * temperature + (1 | colony)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">glmerMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reef environment * pCO2 + temperature + (1 | colony)</t>
+  </si>
+  <si>
     <t xml:space="preserve">reef environment * pCO2 + temperature + (1 | colony) + (1 | tank)</t>
   </si>
   <si>
-    <t xml:space="preserve">glmerMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reef environment * pCO2 + temperature + (1 | colony)</t>
+    <t xml:space="preserve">reef environment + pCO2 * temperature + (1 | colony)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reef environment + pCO2 + temperature + (1 | colony)</t>
   </si>
   <si>
     <t xml:space="preserve">reef environment * (pCO2 + temperature) + (1 | colony)</t>
   </si>
   <si>
-    <t xml:space="preserve">reef environment * pCO2 * temperature + (1 | colony)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reef environment + pCO2 + temperature + (1 | colony)</t>
-  </si>
-  <si>
     <t xml:space="preserve">pCO2 + temperature + (1 | colony)</t>
   </si>
   <si>
-    <t xml:space="preserve">reef environment + pCO2 * temperature + (1 | colony)</t>
-  </si>
-  <si>
     <t xml:space="preserve">pstr</t>
   </si>
   <si>
@@ -89,9 +222,6 @@
     <t xml:space="preserve">pCO2 + temperature + (1 | colony) + (1 | tank)</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t xml:space="preserve">Df</t>
   </si>
   <si>
@@ -197,31 +327,31 @@
     <t xml:space="preserve">species * part * reef environment * pCO2 * temperature + (1 | colony)</t>
   </si>
   <si>
+    <t xml:space="preserve">species * part * reef environment * pCO2 + temperature + (1 | colony)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">species * part * reef environment + pCO2 * temperature + (1 | colony)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">species * reef environment + part + pCO2 + temperature + (1 | colony)</t>
+  </si>
+  <si>
     <t xml:space="preserve">species * part * reef environment * (pCO2 + temperature) + (1 | colony)</t>
   </si>
   <si>
+    <t xml:space="preserve">species * part * pCO2 + temperature + (1 | colony)</t>
+  </si>
+  <si>
     <t xml:space="preserve">reef environment * species * part * (pCO2 + temperature) + (1 | colony)</t>
   </si>
   <si>
+    <t xml:space="preserve">species * part * (pCO2 + temperature) + (1 | colony)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">species * part * (pCO2 + temperature) + reef environment + (1 | colony)</t>
+  </si>
+  <si>
     <t xml:space="preserve">species * part * (pCO2 + temperature + reef environment) + (1 | colony)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">species * part * (pCO2 + temperature) + (1 | colony)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">species * part * (pCO2 + temperature) + reef environment + (1 | colony)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">species * part * reef environment * pCO2 + temperature + (1 | colony)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">species * part * pCO2 + temperature + (1 | colony)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">species * reef environment + part + pCO2 + temperature + (1 | colony)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">species * part * reef environment + pCO2 * temperature + (1 | colony)</t>
   </si>
   <si>
     <t xml:space="preserve">symbionts</t>
@@ -296,7 +426,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="1">
     <font>
@@ -615,10 +745,882 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <cols>
+    <col min="1" max="1" width="27.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="7.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="21.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="9.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="8.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="7.71" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="8.71" hidden="0" customWidth="1"/>
+    <col min="8" max="8" width="21.71" hidden="0" customWidth="1"/>
+    <col min="9" max="9" width="10.71" hidden="0" customWidth="1"/>
+    <col min="10" max="10" width="9.71" hidden="0" customWidth="1"/>
+    <col min="11" max="11" width="8.71" hidden="0" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="n">
+        <v>6</v>
+      </c>
+      <c r="F2" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="n">
+        <v>2</v>
+      </c>
+      <c r="K3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="n">
+        <v>6</v>
+      </c>
+      <c r="F4" t="n">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" t="n">
+        <v>5</v>
+      </c>
+      <c r="K4" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F6" t="n">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" t="n">
+        <v>5</v>
+      </c>
+      <c r="K6" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3</v>
+      </c>
+      <c r="F7" t="n">
+        <v>5</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" t="n">
+        <v>3</v>
+      </c>
+      <c r="K7" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="n">
+        <v>6</v>
+      </c>
+      <c r="F8" t="n">
+        <v>5</v>
+      </c>
+      <c r="G8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" t="n">
+        <v>5</v>
+      </c>
+      <c r="K8" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3</v>
+      </c>
+      <c r="F9" t="n">
+        <v>3</v>
+      </c>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" t="n">
+        <v>2</v>
+      </c>
+      <c r="K9" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="n">
+        <v>3</v>
+      </c>
+      <c r="F10" t="n">
+        <v>2</v>
+      </c>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" t="n">
+        <v>3</v>
+      </c>
+      <c r="F11" t="n">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" t="n">
+        <v>9</v>
+      </c>
+      <c r="F12" t="n">
+        <v>6</v>
+      </c>
+      <c r="G12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" t="n">
+        <v>4</v>
+      </c>
+      <c r="K12" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" t="n">
+        <v>5</v>
+      </c>
+      <c r="F13" t="n">
+        <v>3</v>
+      </c>
+      <c r="G13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" t="n">
+        <v>2</v>
+      </c>
+      <c r="K13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" t="n">
+        <v>8</v>
+      </c>
+      <c r="F14" t="n">
+        <v>6</v>
+      </c>
+      <c r="G14" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" t="n">
+        <v>3</v>
+      </c>
+      <c r="K14" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" t="n">
+        <v>3</v>
+      </c>
+      <c r="F15" t="n">
+        <v>2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J15" t="n">
+        <v>2</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" t="n">
+        <v>10</v>
+      </c>
+      <c r="F16" t="n">
+        <v>6</v>
+      </c>
+      <c r="G16" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" t="n">
+        <v>4</v>
+      </c>
+      <c r="K16" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" t="n">
+        <v>5</v>
+      </c>
+      <c r="F17" t="n">
+        <v>4</v>
+      </c>
+      <c r="G17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H17" t="s">
+        <v>24</v>
+      </c>
+      <c r="I17" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" t="n">
+        <v>2</v>
+      </c>
+      <c r="K17" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" t="n">
+        <v>6</v>
+      </c>
+      <c r="F18" t="n">
+        <v>5</v>
+      </c>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" t="n">
+        <v>5</v>
+      </c>
+      <c r="F19" t="n">
+        <v>6</v>
+      </c>
+      <c r="G19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H19" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" t="s">
+        <v>16</v>
+      </c>
+      <c r="J19" t="n">
+        <v>5</v>
+      </c>
+      <c r="K19" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" t="n">
+        <v>6</v>
+      </c>
+      <c r="F20" t="n">
+        <v>6</v>
+      </c>
+      <c r="G20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H20" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" t="n">
+        <v>6</v>
+      </c>
+      <c r="K20" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" t="n">
+        <v>6</v>
+      </c>
+      <c r="F21" t="n">
+        <v>6</v>
+      </c>
+      <c r="G21" t="s">
+        <v>36</v>
+      </c>
+      <c r="H21" t="s">
+        <v>18</v>
+      </c>
+      <c r="I21" t="s">
+        <v>16</v>
+      </c>
+      <c r="J21" t="n">
+        <v>6</v>
+      </c>
+      <c r="K21" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" t="n">
+        <v>7</v>
+      </c>
+      <c r="F22" t="n">
+        <v>5</v>
+      </c>
+      <c r="G22" t="s">
+        <v>36</v>
+      </c>
+      <c r="H22" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" t="n">
+        <v>7</v>
+      </c>
+      <c r="K22" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" t="n">
+        <v>6</v>
+      </c>
+      <c r="F23" t="n">
+        <v>5</v>
+      </c>
+      <c r="G23" t="s">
+        <v>36</v>
+      </c>
+      <c r="H23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J23" t="n">
+        <v>6</v>
+      </c>
+      <c r="K23" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" t="n">
+        <v>6</v>
+      </c>
+      <c r="F24" t="n">
+        <v>4</v>
+      </c>
+      <c r="G24" t="s">
+        <v>36</v>
+      </c>
+      <c r="H24" t="s">
+        <v>24</v>
+      </c>
+      <c r="I24" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24" t="n">
+        <v>6</v>
+      </c>
+      <c r="K24" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" t="n">
+        <v>3</v>
+      </c>
+      <c r="F25" t="n">
+        <v>4</v>
+      </c>
+      <c r="G25" t="s">
+        <v>36</v>
+      </c>
+      <c r="H25" t="s">
+        <v>24</v>
+      </c>
+      <c r="I25" t="s">
+        <v>16</v>
+      </c>
+      <c r="J25" t="n">
+        <v>3</v>
+      </c>
+      <c r="K25" t="n">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
@@ -626,674 +1628,731 @@
     <col min="2" max="2" width="65.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="8.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="5.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="5.71" hidden="0" customWidth="1"/>
-    <col min="6" max="6" width="14.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="11.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="5.71" hidden="0" customWidth="1"/>
     <col min="7" max="7" width="11.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>53</v>
+      </c>
+      <c r="L1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="D2" t="n">
-        <v>218.4</v>
+        <v>223.2</v>
       </c>
       <c r="E2" t="n">
-        <v>245.4</v>
+        <v>0.0332206990579833</v>
       </c>
       <c r="F2" t="n">
-        <v>0.542</v>
+        <v>259.2</v>
       </c>
       <c r="G2" t="n">
-        <v>0.307</v>
+        <v>0.0000152578956652519</v>
       </c>
       <c r="H2" t="n">
-        <v>0.339921366849096</v>
+        <v>0.545</v>
       </c>
       <c r="I2" t="n">
-        <v>0.824553438127845</v>
+        <v>0.366</v>
       </c>
       <c r="J2" t="n">
-        <v>0.29777176529434</v>
+        <v>0.282067343982829</v>
       </c>
       <c r="K2" t="n">
-        <v>90.3</v>
+        <v>0.855828398264632</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.294010052236142</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="D3" t="n">
         <v>218.8</v>
       </c>
       <c r="E3" t="n">
+        <v>0.306747214704836</v>
+      </c>
+      <c r="F3" t="n">
         <v>243.5</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
+        <v>0.0389169854792176</v>
+      </c>
+      <c r="H3" t="n">
         <v>0.506</v>
       </c>
-      <c r="G3" t="n">
+      <c r="I3" t="n">
         <v>0.322</v>
       </c>
-      <c r="H3" t="n">
+      <c r="J3" t="n">
         <v>0.270712906666334</v>
       </c>
-      <c r="I3" t="n">
+      <c r="K3" t="n">
         <v>0.880517357628651</v>
       </c>
-      <c r="J3" t="n">
+      <c r="L3" t="n">
         <v>0.309990520594351</v>
-      </c>
-      <c r="K3" t="n">
-        <v>65.6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="D4" t="n">
-        <v>220.1</v>
+        <v>218.4</v>
       </c>
       <c r="E4" t="n">
-        <v>247.1</v>
+        <v>0.362269389200314</v>
       </c>
       <c r="F4" t="n">
-        <v>0.511</v>
+        <v>245.4</v>
       </c>
       <c r="G4" t="n">
-        <v>0.329</v>
+        <v>0.0149326080218231</v>
       </c>
       <c r="H4" t="n">
-        <v>0.272155096268899</v>
+        <v>0.542</v>
       </c>
       <c r="I4" t="n">
-        <v>0.874876231377499</v>
+        <v>0.307</v>
       </c>
       <c r="J4" t="n">
-        <v>0.307314521780736</v>
+        <v>0.339921366849096</v>
       </c>
       <c r="K4" t="n">
-        <v>63.3</v>
+        <v>0.824553438127845</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.29777176529434</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="D5" t="n">
-        <v>223.2</v>
+        <v>225.6</v>
       </c>
       <c r="E5" t="n">
-        <v>259.2</v>
+        <v>0.0101114805243965</v>
       </c>
       <c r="F5" t="n">
-        <v>0.545</v>
+        <v>248.1</v>
       </c>
       <c r="G5" t="n">
-        <v>0.366</v>
+        <v>0.00394846099478588</v>
       </c>
       <c r="H5" t="n">
-        <v>0.282067343982829</v>
+        <v>0.442</v>
       </c>
       <c r="I5" t="n">
-        <v>0.855828398264632</v>
+        <v>0.253</v>
       </c>
       <c r="J5" t="n">
-        <v>0.294010052236142</v>
+        <v>0.252780623700835</v>
       </c>
       <c r="K5" t="n">
-        <v>62.8</v>
+        <v>0.931849378942401</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.323013483263546</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="D6" t="n">
         <v>221.6</v>
       </c>
       <c r="E6" t="n">
+        <v>0.0730842900050484</v>
+      </c>
+      <c r="F6" t="n">
         <v>239.6</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
+        <v>0.270362348894944</v>
+      </c>
+      <c r="H6" t="n">
         <v>0.442</v>
       </c>
-      <c r="G6" t="n">
+      <c r="I6" t="n">
         <v>0.254</v>
       </c>
-      <c r="H6" t="n">
+      <c r="J6" t="n">
         <v>0.252287909332907</v>
       </c>
-      <c r="I6" t="n">
+      <c r="K6" t="n">
         <v>0.933847193844437</v>
       </c>
-      <c r="J6" t="n">
+      <c r="L6" t="n">
         <v>0.322867004307088</v>
-      </c>
-      <c r="K6" t="n">
-        <v>38.9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="D7" t="n">
-        <v>222.1</v>
+        <v>220.1</v>
       </c>
       <c r="E7" t="n">
-        <v>237.8</v>
+        <v>0.156128467145257</v>
       </c>
       <c r="F7" t="n">
-        <v>0.37</v>
+        <v>247.1</v>
       </c>
       <c r="G7" t="n">
-        <v>0.088</v>
+        <v>0.00643555671671473</v>
       </c>
       <c r="H7" t="n">
-        <v>0.308813845572371</v>
+        <v>0.511</v>
       </c>
       <c r="I7" t="n">
-        <v>0.936882341333349</v>
+        <v>0.329</v>
       </c>
       <c r="J7" t="n">
-        <v>0.331059051431514</v>
+        <v>0.272155096268899</v>
       </c>
       <c r="K7" t="n">
-        <v>30.5</v>
+        <v>0.874876231377499</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.307314521780736</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="D8" t="n">
-        <v>225.6</v>
+        <v>222.1</v>
       </c>
       <c r="E8" t="n">
-        <v>248.1</v>
+        <v>0.0584384593621647</v>
       </c>
       <c r="F8" t="n">
-        <v>0.442</v>
+        <v>237.8</v>
       </c>
       <c r="G8" t="n">
-        <v>0.253</v>
+        <v>0.665388781996849</v>
       </c>
       <c r="H8" t="n">
-        <v>0.252780623700835</v>
+        <v>0.37</v>
       </c>
       <c r="I8" t="n">
-        <v>0.931849378942401</v>
+        <v>0.088</v>
       </c>
       <c r="J8" t="n">
-        <v>0.323013483263546</v>
+        <v>0.308813845572371</v>
       </c>
       <c r="K8" t="n">
-        <v>25.7</v>
+        <v>0.936882341333349</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.331059051431514</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="D9" t="n">
         <v>110.7</v>
       </c>
       <c r="E9" t="n">
+        <v>0.0142713175128634</v>
+      </c>
+      <c r="F9" t="n">
         <v>128.3</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
+        <v>0.000223987725579265</v>
+      </c>
+      <c r="H9" t="n">
         <v>0.427</v>
       </c>
-      <c r="G9" t="n">
+      <c r="I9" t="n">
         <v>0.347</v>
       </c>
-      <c r="H9" t="n">
+      <c r="J9" t="n">
         <v>0.12264193082729</v>
       </c>
-      <c r="I9" t="n">
+      <c r="K9" t="n">
         <v>1.00977970615862</v>
       </c>
-      <c r="J9" t="n">
+      <c r="L9" t="n">
         <v>0.335976868226673</v>
-      </c>
-      <c r="K9" t="n">
-        <v>71.4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="D10" t="n">
         <v>106</v>
       </c>
       <c r="E10" t="n">
+        <v>0.147046341763083</v>
+      </c>
+      <c r="F10" t="n">
         <v>118.6</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
+        <v>0.0285747963670422</v>
+      </c>
+      <c r="H10" t="n">
         <v>0.341</v>
       </c>
-      <c r="G10" t="n">
+      <c r="I10" t="n">
         <v>0.292</v>
       </c>
-      <c r="H10" t="n">
+      <c r="J10" t="n">
         <v>0.069512358021633</v>
       </c>
-      <c r="I10" t="n">
+      <c r="K10" t="n">
         <v>1.12393872070358</v>
       </c>
-      <c r="J10" t="n">
+      <c r="L10" t="n">
         <v>0.353702412571083</v>
-      </c>
-      <c r="K10" t="n">
-        <v>44.8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="D11" t="n">
         <v>106.9</v>
       </c>
       <c r="E11" t="n">
+        <v>0.0960456146502793</v>
+      </c>
+      <c r="F11" t="n">
         <v>119.5</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
+        <v>0.0186640745201331</v>
+      </c>
+      <c r="H11" t="n">
         <v>0.313</v>
       </c>
-      <c r="G11" t="n">
+      <c r="I11" t="n">
         <v>0.271</v>
       </c>
-      <c r="H11" t="n">
+      <c r="J11" t="n">
         <v>0.0572627646077092</v>
       </c>
-      <c r="I11" t="n">
+      <c r="K11" t="n">
         <v>1.11383231952833</v>
       </c>
-      <c r="J11" t="n">
+      <c r="L11" t="n">
         <v>0.352824835342725</v>
-      </c>
-      <c r="K11" t="n">
-        <v>36.3</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="D12" t="n">
         <v>102.8</v>
       </c>
       <c r="E12" t="n">
+        <v>0.742636726073774</v>
+      </c>
+      <c r="F12" t="n">
         <v>111.6</v>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
+        <v>0.952537141387246</v>
+      </c>
+      <c r="H12" t="n">
         <v>0.268</v>
       </c>
-      <c r="G12" t="n">
+      <c r="I12" t="n">
         <v>0.224</v>
       </c>
-      <c r="H12" t="n">
+      <c r="J12" t="n">
         <v>0.056048071109652</v>
       </c>
-      <c r="I12" t="n">
+      <c r="K12" t="n">
         <v>1.19677569320301</v>
       </c>
-      <c r="J12" t="n">
+      <c r="L12" t="n">
         <v>0.36408716814135</v>
-      </c>
-      <c r="K12" t="n">
-        <v>28.6</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="D13" t="n">
-        <v>145.9</v>
+        <v>153.1</v>
       </c>
       <c r="E13" t="n">
-        <v>167.8</v>
+        <v>0.000942088337633318</v>
       </c>
       <c r="F13" t="n">
-        <v>0.521</v>
+        <v>182.9</v>
       </c>
       <c r="G13" t="n">
-        <v>0.195</v>
+        <v>0.000000490675746961884</v>
       </c>
       <c r="H13" t="n">
-        <v>0.405142466313655</v>
+        <v>0.527</v>
       </c>
       <c r="I13" t="n">
-        <v>0.710112914902594</v>
+        <v>0.199</v>
       </c>
       <c r="J13" t="n">
-        <v>0.231080474175141</v>
+        <v>0.409641426216089</v>
       </c>
       <c r="K13" t="n">
-        <v>76.2</v>
+        <v>0.70697164728988</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.229916347254973</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="D14" t="n">
-        <v>147.9</v>
+        <v>145.9</v>
       </c>
       <c r="E14" t="n">
-        <v>171.8</v>
+        <v>0.0336921939959352</v>
       </c>
       <c r="F14" t="n">
-        <v>0.522</v>
+        <v>167.8</v>
       </c>
       <c r="G14" t="n">
+        <v>0.000937220650941962</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.521</v>
+      </c>
+      <c r="I14" t="n">
         <v>0.195</v>
       </c>
-      <c r="H14" t="n">
-        <v>0.405616901269354</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0.709947971925215</v>
-      </c>
       <c r="J14" t="n">
-        <v>0.230951400774421</v>
+        <v>0.405142466313655</v>
       </c>
       <c r="K14" t="n">
-        <v>73</v>
+        <v>0.710112914902594</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.231080474175141</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="D15" t="n">
-        <v>153.1</v>
+        <v>146.2</v>
       </c>
       <c r="E15" t="n">
-        <v>182.9</v>
+        <v>0.0289917494562144</v>
       </c>
       <c r="F15" t="n">
-        <v>0.527</v>
+        <v>166.1</v>
       </c>
       <c r="G15" t="n">
-        <v>0.199</v>
+        <v>0.00218016507203759</v>
       </c>
       <c r="H15" t="n">
-        <v>0.409641426216089</v>
+        <v>0.5</v>
       </c>
       <c r="I15" t="n">
-        <v>0.70697164728988</v>
+        <v>0.174</v>
       </c>
       <c r="J15" t="n">
-        <v>0.229916347254973</v>
+        <v>0.394017895328747</v>
       </c>
       <c r="K15" t="n">
-        <v>71.4</v>
+        <v>0.734044282144376</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.23735001040535</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="D16" t="n">
-        <v>142.4</v>
+        <v>142.3</v>
       </c>
       <c r="E16" t="n">
-        <v>158.3</v>
+        <v>0.204393622665867</v>
       </c>
       <c r="F16" t="n">
-        <v>0.493</v>
+        <v>158.2</v>
       </c>
       <c r="G16" t="n">
-        <v>0.145</v>
+        <v>0.112327758313534</v>
       </c>
       <c r="H16" t="n">
-        <v>0.40760856417087</v>
+        <v>0.499</v>
       </c>
       <c r="I16" t="n">
-        <v>0.727645208726944</v>
+        <v>0.174</v>
       </c>
       <c r="J16" t="n">
-        <v>0.236972613071863</v>
+        <v>0.393286214699538</v>
       </c>
       <c r="K16" t="n">
-        <v>45.1</v>
+        <v>0.73324439340205</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.237295448480225</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="D17" t="n">
-        <v>142.3</v>
+        <v>147.9</v>
       </c>
       <c r="E17" t="n">
-        <v>158.2</v>
+        <v>0.0125689310659239</v>
       </c>
       <c r="F17" t="n">
-        <v>0.499</v>
+        <v>171.8</v>
       </c>
       <c r="G17" t="n">
-        <v>0.174</v>
+        <v>0.00012933274732436</v>
       </c>
       <c r="H17" t="n">
-        <v>0.393286214699538</v>
+        <v>0.522</v>
       </c>
       <c r="I17" t="n">
-        <v>0.73324439340205</v>
+        <v>0.195</v>
       </c>
       <c r="J17" t="n">
-        <v>0.237295448480225</v>
+        <v>0.405616901269354</v>
       </c>
       <c r="K17" t="n">
-        <v>38.7</v>
+        <v>0.709947971925215</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.230951400774421</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="D18" t="n">
         <v>140.4</v>
       </c>
       <c r="E18" t="n">
+        <v>0.522443416391658</v>
+      </c>
+      <c r="F18" t="n">
         <v>154.4</v>
       </c>
-      <c r="F18" t="n">
+      <c r="G18" t="n">
+        <v>0.776178144031763</v>
+      </c>
+      <c r="H18" t="n">
         <v>0.485</v>
       </c>
-      <c r="G18" t="n">
+      <c r="I18" t="n">
         <v>0.147</v>
       </c>
-      <c r="H18" t="n">
+      <c r="J18" t="n">
         <v>0.396708536396551</v>
       </c>
-      <c r="I18" t="n">
+      <c r="K18" t="n">
         <v>0.732981216183524</v>
       </c>
-      <c r="J18" t="n">
+      <c r="L18" t="n">
         <v>0.238221370362628</v>
-      </c>
-      <c r="K18" t="n">
-        <v>32.7</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="D19" t="n">
-        <v>146.2</v>
+        <v>142.4</v>
       </c>
       <c r="E19" t="n">
-        <v>166.1</v>
+        <v>0.196967998086768</v>
       </c>
       <c r="F19" t="n">
-        <v>0.5</v>
+        <v>158.3</v>
       </c>
       <c r="G19" t="n">
-        <v>0.174</v>
+        <v>0.108246888508652</v>
       </c>
       <c r="H19" t="n">
-        <v>0.394017895328747</v>
+        <v>0.493</v>
       </c>
       <c r="I19" t="n">
-        <v>0.734044282144376</v>
+        <v>0.145</v>
       </c>
       <c r="J19" t="n">
-        <v>0.23735001040535</v>
+        <v>0.40760856417087</v>
       </c>
       <c r="K19" t="n">
-        <v>30.8</v>
+        <v>0.727645208726944</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.236972613071863</v>
       </c>
     </row>
   </sheetData>
@@ -1302,11 +2361,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
@@ -1321,30 +2380,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="E1" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="G1" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -1362,12 +2421,12 @@
         <v>0.00067</v>
       </c>
       <c r="G2" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -1385,12 +2444,12 @@
         <v>0.05929</v>
       </c>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -1408,12 +2467,12 @@
         <v>0.00133</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="B5" t="n">
         <v>80</v>
@@ -1427,12 +2486,12 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="B6" t="n">
         <v>85</v>
@@ -1446,12 +2505,12 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="B7" t="n">
         <v>1</v>
@@ -1469,12 +2528,12 @@
         <v>0.00067</v>
       </c>
       <c r="G7" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="B8" t="n">
         <v>1</v>
@@ -1492,12 +2551,12 @@
         <v>0.00067</v>
       </c>
       <c r="G8" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="B9" t="n">
         <v>3</v>
@@ -1515,12 +2574,12 @@
         <v>0.22785</v>
       </c>
       <c r="G9" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="B10" t="n">
         <v>71</v>
@@ -1534,12 +2593,12 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="B11" t="n">
         <v>76</v>
@@ -1553,12 +2612,12 @@
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="B12" t="n">
         <v>1</v>
@@ -1576,12 +2635,12 @@
         <v>0.46036</v>
       </c>
       <c r="G12" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="B13" t="n">
         <v>1</v>
@@ -1599,12 +2658,12 @@
         <v>0.00133</v>
       </c>
       <c r="G13" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="B14" t="n">
         <v>3</v>
@@ -1622,12 +2681,12 @@
         <v>0.00067</v>
       </c>
       <c r="G14" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="B15" t="n">
         <v>62</v>
@@ -1641,12 +2700,12 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="B16" t="n">
         <v>67</v>
@@ -1660,7 +2719,7 @@
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1669,11 +2728,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
@@ -1687,27 +2746,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>81</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>83</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="F1" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="B2" t="n">
         <v>1.05</v>
@@ -1722,12 +2781,12 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="B3" t="n">
         <v>0.01</v>
@@ -1742,12 +2801,12 @@
         <v>0.085</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="B4" t="n">
         <v>0.378</v>
@@ -1762,12 +2821,12 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
       <c r="B5" t="n">
         <v>0.223</v>
@@ -1782,12 +2841,12 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="B6" t="n">
         <v>0.444</v>
@@ -1802,12 +2861,12 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="B7" t="n">
         <v>0.002</v>
@@ -1822,12 +2881,12 @@
         <v>0.753</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>90</v>
       </c>
       <c r="B8" t="n">
         <v>-0.771</v>
@@ -1842,12 +2901,12 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
       <c r="B9" t="n">
         <v>-0.446</v>
@@ -1862,12 +2921,12 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="B10" t="n">
         <v>-0.33</v>
@@ -1882,12 +2941,12 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B11" t="n">
         <v>0.542</v>
@@ -1896,12 +2955,12 @@
       <c r="D11"/>
       <c r="E11"/>
       <c r="F11" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B12" t="n">
         <v>0.307</v>
@@ -1910,12 +2969,12 @@
       <c r="D12"/>
       <c r="E12"/>
       <c r="F12" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="B13" t="n">
         <v>1.279</v>
@@ -1930,12 +2989,12 @@
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
       <c r="B14" t="n">
         <v>-0.338</v>
@@ -1950,12 +3009,12 @@
         <v>0.08</v>
       </c>
       <c r="F14" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="B15" t="n">
         <v>-0.059</v>
@@ -1970,12 +3029,12 @@
         <v>0.753</v>
       </c>
       <c r="F15" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="B16" t="n">
         <v>0.227</v>
@@ -1990,12 +3049,12 @@
         <v>0.19</v>
       </c>
       <c r="F16" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B17" t="n">
         <v>0.232</v>
@@ -2004,12 +3063,12 @@
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B18" t="n">
         <v>0.188</v>
@@ -2018,12 +3077,12 @@
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="B19" t="n">
         <v>1.033</v>
@@ -2038,12 +3097,12 @@
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="B20" t="n">
         <v>-0.045</v>
@@ -2058,12 +3117,12 @@
         <v>0.694</v>
       </c>
       <c r="F20" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
       <c r="B21" t="n">
         <v>0.033</v>
@@ -2078,12 +3137,12 @@
         <v>0.676</v>
       </c>
       <c r="F21" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="B22" t="n">
         <v>0.124</v>
@@ -2098,12 +3157,12 @@
         <v>0.131</v>
       </c>
       <c r="F22" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="B23" t="n">
         <v>0.262</v>
@@ -2118,12 +3177,12 @@
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B24" t="n">
         <v>0.493</v>
@@ -2132,12 +3191,12 @@
       <c r="D24"/>
       <c r="E24"/>
       <c r="F24" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B25" t="n">
         <v>0.145</v>
@@ -2146,7 +3205,7 @@
       <c r="D25"/>
       <c r="E25"/>
       <c r="F25" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2155,11 +3214,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
@@ -2173,27 +3232,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="E1" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -2213,7 +3272,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -2233,7 +3292,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -2253,7 +3312,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
       <c r="B5" t="n">
         <v>2</v>
@@ -2273,7 +3332,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>93</v>
       </c>
       <c r="B6" t="n">
         <v>2</v>
@@ -2293,7 +3352,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>94</v>
       </c>
       <c r="B7" t="n">
         <v>6</v>
@@ -2313,7 +3372,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>95</v>
       </c>
       <c r="B8" t="n">
         <v>2</v>
@@ -2333,7 +3392,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="B9" t="n">
         <v>214</v>
@@ -2349,7 +3408,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="B10" t="n">
         <v>231</v>
@@ -2369,11 +3428,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
@@ -2393,45 +3452,45 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="E1" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="G1" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="H1" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="I1" t="s">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="J1" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="K1" t="s">
-        <v>57</v>
+        <v>100</v>
       </c>
       <c r="L1" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -2446,7 +3505,7 @@
         <v>0.55</v>
       </c>
       <c r="F2" t="n">
-        <v>0.74817</v>
+        <v>0.74883</v>
       </c>
       <c r="G2" t="n">
         <v>3</v>
@@ -2464,12 +3523,12 @@
         <v>0.00067</v>
       </c>
       <c r="L2" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -2502,12 +3561,12 @@
         <v>0.0966</v>
       </c>
       <c r="L3" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -2522,7 +3581,7 @@
         <v>0.52</v>
       </c>
       <c r="F4" t="n">
-        <v>0.56829</v>
+        <v>0.56762</v>
       </c>
       <c r="G4" t="n">
         <v>1</v>
@@ -2540,12 +3599,12 @@
         <v>0.00266</v>
       </c>
       <c r="L4" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="B5" t="n">
         <v>80</v>
@@ -2570,12 +3629,12 @@
       <c r="J5"/>
       <c r="K5"/>
       <c r="L5" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="B6" t="n">
         <v>85</v>
@@ -2600,12 +3659,12 @@
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="B7" t="n">
         <v>3</v>
@@ -2638,12 +3697,12 @@
         <v>0.28115</v>
       </c>
       <c r="L7" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="B8" t="n">
         <v>1</v>
@@ -2676,12 +3735,12 @@
         <v>0.00067</v>
       </c>
       <c r="L8" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="B9" t="n">
         <v>1</v>
@@ -2696,7 +3755,7 @@
         <v>1.75</v>
       </c>
       <c r="F9" t="n">
-        <v>0.16589</v>
+        <v>0.16855</v>
       </c>
       <c r="G9" t="n">
         <v>1</v>
@@ -2714,12 +3773,12 @@
         <v>0.00133</v>
       </c>
       <c r="L9" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="B10" t="n">
         <v>71</v>
@@ -2744,12 +3803,12 @@
       <c r="J10"/>
       <c r="K10"/>
       <c r="L10" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="B11" t="n">
         <v>76</v>
@@ -2774,12 +3833,12 @@
       <c r="J11"/>
       <c r="K11"/>
       <c r="L11" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="B12" t="n">
         <v>3</v>
@@ -2812,12 +3871,12 @@
         <v>0.00067</v>
       </c>
       <c r="L12" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="B13" t="n">
         <v>1</v>
@@ -2850,12 +3909,12 @@
         <v>0.00067</v>
       </c>
       <c r="L13" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="B14" t="n">
         <v>1</v>
@@ -2870,7 +3929,7 @@
         <v>1.64</v>
       </c>
       <c r="F14" t="n">
-        <v>0.20386</v>
+        <v>0.20253</v>
       </c>
       <c r="G14" t="n">
         <v>1</v>
@@ -2885,15 +3944,15 @@
         <v>0.53</v>
       </c>
       <c r="K14" t="n">
-        <v>0.46569</v>
+        <v>0.46636</v>
       </c>
       <c r="L14" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="B15" t="n">
         <v>62</v>
@@ -2918,12 +3977,12 @@
       <c r="J15"/>
       <c r="K15"/>
       <c r="L15" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="B16" t="n">
         <v>67</v>
@@ -2948,414 +4007,7 @@
       <c r="J16"/>
       <c r="K16"/>
       <c r="L16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
-  <cols>
-    <col min="1" max="1" width="71.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="8.71" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="5.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="6.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="14.71" hidden="0" customWidth="1"/>
-    <col min="6" max="6" width="11.71" hidden="0" customWidth="1"/>
-    <col min="7" max="7" width="11.71" hidden="0" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="n">
-        <v>923.1</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1219.4</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.318</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.163808918846475</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.884761957169536</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.445413568051623</v>
-      </c>
-      <c r="J2" t="n">
-        <v>71.4</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="n">
-        <v>902.1</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1124.3</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.391</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.279</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.155601596236995</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.913117790532039</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.45931696402324</v>
-      </c>
-      <c r="J3" t="n">
-        <v>69.6</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="n">
-        <v>902.1</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1124.3</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.391</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.279</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.155601596236034</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.913117790532143</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.459316964023365</v>
-      </c>
-      <c r="J4" t="n">
-        <v>69.6</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="n">
-        <v>902.1</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1124.3</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.391</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.279</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.155601596236034</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.913117790532143</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.459316964023365</v>
-      </c>
-      <c r="J5" t="n">
-        <v>69.6</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="n">
-        <v>883.9</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1024.7</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.323</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.212</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.140275722020262</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.935551604873005</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.476818047697685</v>
-      </c>
-      <c r="J6" t="n">
-        <v>60.8</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="n">
-        <v>882</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1000.5</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.139</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.163720683028945</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.950425796937665</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.488694314791684</v>
-      </c>
-      <c r="J7" t="n">
-        <v>59.1</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="n">
-        <v>883.5</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1005.7</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.282</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.144</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.161404588856711</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.950207028246836</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.488554386709045</v>
-      </c>
-      <c r="J8" t="n">
-        <v>58.1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="n">
-        <v>904.6</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1086.1</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.338</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.225</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.144860307744428</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.948916968928776</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0.477395026003451</v>
-      </c>
-      <c r="J9" t="n">
-        <v>52.4</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>65</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="n">
-        <v>890.2</v>
-      </c>
-      <c r="D10" t="n">
-        <v>990.2</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.235</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.093</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0.157143513626403</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.982507593585701</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0.505803686093402</v>
-      </c>
-      <c r="J10" t="n">
-        <v>41.7</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" t="n">
-        <v>881.2</v>
-      </c>
-      <c r="D11" t="n">
-        <v>929.4</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.205</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.095</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0.121607431312658</v>
-      </c>
-      <c r="H11" t="n">
-        <v>1.01492820585159</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0.513921291826242</v>
-      </c>
-      <c r="J11" t="n">
-        <v>28.7</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" t="n">
-        <v>890.2</v>
-      </c>
-      <c r="D12" t="n">
-        <v>964.2</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.222</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.113</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0.122648785796666</v>
-      </c>
-      <c r="H12" t="n">
-        <v>1.00853413602528</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0.508488836608921</v>
-      </c>
-      <c r="J12" t="n">
-        <v>28.3</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -3365,10 +4017,453 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <cols>
+    <col min="1" max="1" width="71.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="8.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="5.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="11.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="6.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="11.71" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="14.71" hidden="0" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="n">
+        <v>923.1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.000000000356173661287928</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1219.4</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.00000000000000000000000000000000000000000000000000000000000000106026935087453</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.318</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.163808918846475</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.884761957169536</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.445413568051623</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" t="n">
+        <v>904.6</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.00000356476632034088</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1086.1</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.0000000000000000000000000000000000907895747647671</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.338</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.225</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.144860307744428</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.948916968928776</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.477395026003451</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" t="n">
+        <v>890.2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.0049751824323713</v>
+      </c>
+      <c r="E4" t="n">
+        <v>964.2</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.0000000267012839066756</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.222</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.113</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.122648785796666</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1.00853413602528</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.508488836608921</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" t="n">
+        <v>881.2</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.436931983172524</v>
+      </c>
+      <c r="E5" t="n">
+        <v>929.4</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.999999973298655</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.205</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.095</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.121607431312658</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1.01492820585159</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.513921291826242</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" t="n">
+        <v>902.1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.000012830993710202</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1124.3</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.000000000000000000000000000000000000000000464876516436139</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.391</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.279</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.155601596236995</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.913117790532039</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.45931696402324</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" t="n">
+        <v>890.2</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.00479961344622744</v>
+      </c>
+      <c r="E7" t="n">
+        <v>990.2</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.0000000000000604040943674256</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.235</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.093</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.157143513626403</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.982507593585701</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.505803686093402</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" t="n">
+        <v>902.1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0000128309937101984</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1124.3</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.000000000000000000000000000000000000000000464876516436033</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.391</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.279</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.155601596236034</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.913117790532143</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.459316964023365</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" t="n">
+        <v>902.1</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0000128309937101984</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1124.3</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.000000000000000000000000000000000000000000464876516436033</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.391</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.279</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.155601596236034</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.913117790532143</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.459316964023365</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" t="n">
+        <v>882</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.302098653514401</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1000.5</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.000000000000000361974667895156</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.139</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.163720683028945</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.950425796937665</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.488694314791684</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" t="n">
+        <v>883.5</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.138174298373614</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1005.7</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.0000000000000000259830728679035</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.282</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.144</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.161404588856711</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.950207028246836</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.488554386709045</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" t="n">
+        <v>883.9</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.112978210957238</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1024.7</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.00000000000000000000202268013528013</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.323</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.212</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.140275722020262</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.935551604873005</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.476818047697685</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
@@ -3382,24 +4477,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>81</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>83</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="B2" t="n">
         <v>0.8</v>
@@ -3416,7 +4511,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
       <c r="B3" t="n">
         <v>0.199</v>
@@ -3433,7 +4528,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
       <c r="B4" t="n">
         <v>-0.357</v>
@@ -3450,7 +4545,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>111</v>
       </c>
       <c r="B5" t="n">
         <v>-0.515</v>
@@ -3467,7 +4562,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="B6" t="n">
         <v>0.234</v>
@@ -3484,7 +4579,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
       <c r="B7" t="n">
         <v>0.005</v>
@@ -3501,7 +4596,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="B8" t="n">
         <v>-0.021</v>
@@ -3518,7 +4613,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="B9" t="n">
         <v>-0.252</v>
@@ -3535,7 +4630,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>112</v>
       </c>
       <c r="B10" t="n">
         <v>0.223</v>
@@ -3552,7 +4647,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>113</v>
       </c>
       <c r="B11" t="n">
         <v>0.685</v>
@@ -3569,7 +4664,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>114</v>
       </c>
       <c r="B12" t="n">
         <v>-0.088</v>
@@ -3586,7 +4681,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>115</v>
       </c>
       <c r="B13" t="n">
         <v>-0.568</v>
@@ -3603,7 +4698,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>116</v>
       </c>
       <c r="B14" t="n">
         <v>-0.45</v>
@@ -3620,7 +4715,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="B15" t="n">
         <v>0.051</v>
@@ -3637,7 +4732,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>118</v>
       </c>
       <c r="B16" t="n">
         <v>-0.154</v>
@@ -3654,7 +4749,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="B17" t="n">
         <v>0.236</v>
@@ -3671,7 +4766,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>77</v>
+        <v>120</v>
       </c>
       <c r="B18" t="n">
         <v>0.072</v>
@@ -3688,7 +4783,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>121</v>
       </c>
       <c r="B19" t="n">
         <v>0.608</v>
@@ -3705,7 +4800,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>79</v>
+        <v>122</v>
       </c>
       <c r="B20" t="n">
         <v>-0.299</v>
@@ -3722,7 +4817,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>123</v>
       </c>
       <c r="B21" t="n">
         <v>0.134</v>
@@ -3739,7 +4834,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>81</v>
+        <v>124</v>
       </c>
       <c r="B22" t="n">
         <v>0.564</v>
@@ -3756,7 +4851,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>82</v>
+        <v>125</v>
       </c>
       <c r="B23" t="n">
         <v>0.524</v>
@@ -3773,7 +4868,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>83</v>
+        <v>126</v>
       </c>
       <c r="B24" t="n">
         <v>0.362</v>
@@ -3790,7 +4885,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>84</v>
+        <v>127</v>
       </c>
       <c r="B25" t="n">
         <v>0.673</v>
@@ -3807,7 +4902,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>85</v>
+        <v>128</v>
       </c>
       <c r="B26" t="n">
         <v>-0.179</v>
@@ -3824,7 +4919,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>86</v>
+        <v>129</v>
       </c>
       <c r="B27" t="n">
         <v>-0.18</v>
@@ -3841,7 +4936,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>87</v>
+        <v>130</v>
       </c>
       <c r="B28" t="n">
         <v>-0.482</v>
@@ -3858,7 +4953,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>88</v>
+        <v>131</v>
       </c>
       <c r="B29" t="n">
         <v>-0.89</v>
@@ -3875,7 +4970,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>89</v>
+        <v>132</v>
       </c>
       <c r="B30" t="n">
         <v>0.189</v>
@@ -3892,7 +4987,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>90</v>
+        <v>133</v>
       </c>
       <c r="B31" t="n">
         <v>-0.607</v>
@@ -3909,7 +5004,7 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B32" t="n">
         <v>0.28</v>
@@ -3920,7 +5015,7 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B33" t="n">
         <v>0.139</v>

</xml_diff>

<commit_message>
fix supp fig/table numbering
</commit_message>
<xml_diff>
--- a/Data/Supplemental/Supplemental_Tables.xlsx
+++ b/Data/Supplemental/Supplemental_Tables.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
   <si>
     <t xml:space="preserve">group</t>
   </si>
@@ -162,13 +162,7 @@
     <t xml:space="preserve">AIC</t>
   </si>
   <si>
-    <t xml:space="preserve">AIC_wt</t>
-  </si>
-  <si>
     <t xml:space="preserve">BIC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BIC_wt</t>
   </si>
   <si>
     <t xml:space="preserve">Conditional R2</t>
@@ -1628,8 +1622,8 @@
     <col min="2" max="2" width="65.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="8.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="5.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="11.71" hidden="0" customWidth="1"/>
-    <col min="6" max="6" width="5.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="5.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="14.71" hidden="0" customWidth="1"/>
     <col min="7" max="7" width="11.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1664,694 +1658,580 @@
       <c r="J1" t="s">
         <v>52</v>
       </c>
-      <c r="K1" t="s">
-        <v>53</v>
-      </c>
-      <c r="L1" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
         <v>55</v>
-      </c>
-      <c r="B2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" t="s">
-        <v>57</v>
       </c>
       <c r="D2" t="n">
         <v>223.2</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0332206990579833</v>
+        <v>259.2</v>
       </c>
       <c r="F2" t="n">
-        <v>259.2</v>
+        <v>0.545</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0000152578956652519</v>
+        <v>0.366</v>
       </c>
       <c r="H2" t="n">
-        <v>0.545</v>
+        <v>0.282067343982829</v>
       </c>
       <c r="I2" t="n">
-        <v>0.366</v>
+        <v>0.855828398264632</v>
       </c>
       <c r="J2" t="n">
-        <v>0.282067343982829</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.855828398264632</v>
-      </c>
-      <c r="L2" t="n">
         <v>0.294010052236142</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
         <v>55</v>
-      </c>
-      <c r="B3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" t="s">
-        <v>57</v>
       </c>
       <c r="D3" t="n">
         <v>218.8</v>
       </c>
       <c r="E3" t="n">
-        <v>0.306747214704836</v>
+        <v>243.5</v>
       </c>
       <c r="F3" t="n">
-        <v>243.5</v>
+        <v>0.506</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0389169854792176</v>
+        <v>0.322</v>
       </c>
       <c r="H3" t="n">
-        <v>0.506</v>
+        <v>0.270712906666334</v>
       </c>
       <c r="I3" t="n">
-        <v>0.322</v>
+        <v>0.880517357628651</v>
       </c>
       <c r="J3" t="n">
-        <v>0.270712906666334</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.880517357628651</v>
-      </c>
-      <c r="L3" t="n">
         <v>0.309990520594351</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" t="s">
         <v>55</v>
-      </c>
-      <c r="B4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" t="s">
-        <v>57</v>
       </c>
       <c r="D4" t="n">
         <v>218.4</v>
       </c>
       <c r="E4" t="n">
-        <v>0.362269389200314</v>
+        <v>245.4</v>
       </c>
       <c r="F4" t="n">
-        <v>245.4</v>
+        <v>0.542</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0149326080218231</v>
+        <v>0.307</v>
       </c>
       <c r="H4" t="n">
-        <v>0.542</v>
+        <v>0.339921366849096</v>
       </c>
       <c r="I4" t="n">
-        <v>0.307</v>
+        <v>0.824553438127845</v>
       </c>
       <c r="J4" t="n">
-        <v>0.339921366849096</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.824553438127845</v>
-      </c>
-      <c r="L4" t="n">
         <v>0.29777176529434</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" t="s">
         <v>55</v>
-      </c>
-      <c r="B5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" t="s">
-        <v>57</v>
       </c>
       <c r="D5" t="n">
         <v>225.6</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0101114805243965</v>
+        <v>248.1</v>
       </c>
       <c r="F5" t="n">
-        <v>248.1</v>
+        <v>0.442</v>
       </c>
       <c r="G5" t="n">
-        <v>0.00394846099478588</v>
+        <v>0.253</v>
       </c>
       <c r="H5" t="n">
-        <v>0.442</v>
+        <v>0.252780623700835</v>
       </c>
       <c r="I5" t="n">
-        <v>0.253</v>
+        <v>0.931849378942401</v>
       </c>
       <c r="J5" t="n">
-        <v>0.252780623700835</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0.931849378942401</v>
-      </c>
-      <c r="L5" t="n">
         <v>0.323013483263546</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" t="s">
         <v>55</v>
-      </c>
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" t="s">
-        <v>57</v>
       </c>
       <c r="D6" t="n">
         <v>221.6</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0730842900050484</v>
+        <v>239.6</v>
       </c>
       <c r="F6" t="n">
-        <v>239.6</v>
+        <v>0.442</v>
       </c>
       <c r="G6" t="n">
-        <v>0.270362348894944</v>
+        <v>0.254</v>
       </c>
       <c r="H6" t="n">
-        <v>0.442</v>
+        <v>0.252287909332907</v>
       </c>
       <c r="I6" t="n">
-        <v>0.254</v>
+        <v>0.933847193844437</v>
       </c>
       <c r="J6" t="n">
-        <v>0.252287909332907</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0.933847193844437</v>
-      </c>
-      <c r="L6" t="n">
         <v>0.322867004307088</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" t="s">
         <v>55</v>
-      </c>
-      <c r="B7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" t="s">
-        <v>57</v>
       </c>
       <c r="D7" t="n">
         <v>220.1</v>
       </c>
       <c r="E7" t="n">
-        <v>0.156128467145257</v>
+        <v>247.1</v>
       </c>
       <c r="F7" t="n">
-        <v>247.1</v>
+        <v>0.511</v>
       </c>
       <c r="G7" t="n">
-        <v>0.00643555671671473</v>
+        <v>0.329</v>
       </c>
       <c r="H7" t="n">
-        <v>0.511</v>
+        <v>0.272155096268899</v>
       </c>
       <c r="I7" t="n">
-        <v>0.329</v>
+        <v>0.874876231377499</v>
       </c>
       <c r="J7" t="n">
-        <v>0.272155096268899</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.874876231377499</v>
-      </c>
-      <c r="L7" t="n">
         <v>0.307314521780736</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" t="s">
         <v>55</v>
-      </c>
-      <c r="B8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" t="s">
-        <v>57</v>
       </c>
       <c r="D8" t="n">
         <v>222.1</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0584384593621647</v>
+        <v>237.8</v>
       </c>
       <c r="F8" t="n">
-        <v>237.8</v>
+        <v>0.37</v>
       </c>
       <c r="G8" t="n">
-        <v>0.665388781996849</v>
+        <v>0.088</v>
       </c>
       <c r="H8" t="n">
-        <v>0.37</v>
+        <v>0.308813845572371</v>
       </c>
       <c r="I8" t="n">
-        <v>0.088</v>
+        <v>0.936882341333349</v>
       </c>
       <c r="J8" t="n">
-        <v>0.308813845572371</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.936882341333349</v>
-      </c>
-      <c r="L8" t="n">
         <v>0.331059051431514</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D9" t="n">
         <v>110.7</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0142713175128634</v>
+        <v>128.3</v>
       </c>
       <c r="F9" t="n">
-        <v>128.3</v>
+        <v>0.427</v>
       </c>
       <c r="G9" t="n">
-        <v>0.000223987725579265</v>
+        <v>0.347</v>
       </c>
       <c r="H9" t="n">
-        <v>0.427</v>
+        <v>0.12264193082729</v>
       </c>
       <c r="I9" t="n">
-        <v>0.347</v>
+        <v>1.00977970615862</v>
       </c>
       <c r="J9" t="n">
-        <v>0.12264193082729</v>
-      </c>
-      <c r="K9" t="n">
-        <v>1.00977970615862</v>
-      </c>
-      <c r="L9" t="n">
         <v>0.335976868226673</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D10" t="n">
         <v>106</v>
       </c>
       <c r="E10" t="n">
-        <v>0.147046341763083</v>
+        <v>118.6</v>
       </c>
       <c r="F10" t="n">
-        <v>118.6</v>
+        <v>0.341</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0285747963670422</v>
+        <v>0.292</v>
       </c>
       <c r="H10" t="n">
-        <v>0.341</v>
+        <v>0.069512358021633</v>
       </c>
       <c r="I10" t="n">
-        <v>0.292</v>
+        <v>1.12393872070358</v>
       </c>
       <c r="J10" t="n">
-        <v>0.069512358021633</v>
-      </c>
-      <c r="K10" t="n">
-        <v>1.12393872070358</v>
-      </c>
-      <c r="L10" t="n">
         <v>0.353702412571083</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D11" t="n">
         <v>106.9</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0960456146502793</v>
+        <v>119.5</v>
       </c>
       <c r="F11" t="n">
-        <v>119.5</v>
+        <v>0.313</v>
       </c>
       <c r="G11" t="n">
-        <v>0.0186640745201331</v>
+        <v>0.271</v>
       </c>
       <c r="H11" t="n">
-        <v>0.313</v>
+        <v>0.0572627646077092</v>
       </c>
       <c r="I11" t="n">
-        <v>0.271</v>
+        <v>1.11383231952833</v>
       </c>
       <c r="J11" t="n">
-        <v>0.0572627646077092</v>
-      </c>
-      <c r="K11" t="n">
-        <v>1.11383231952833</v>
-      </c>
-      <c r="L11" t="n">
         <v>0.352824835342725</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D12" t="n">
         <v>102.8</v>
       </c>
       <c r="E12" t="n">
-        <v>0.742636726073774</v>
+        <v>111.6</v>
       </c>
       <c r="F12" t="n">
-        <v>111.6</v>
+        <v>0.268</v>
       </c>
       <c r="G12" t="n">
-        <v>0.952537141387246</v>
+        <v>0.224</v>
       </c>
       <c r="H12" t="n">
-        <v>0.268</v>
+        <v>0.056048071109652</v>
       </c>
       <c r="I12" t="n">
-        <v>0.224</v>
+        <v>1.19677569320301</v>
       </c>
       <c r="J12" t="n">
-        <v>0.056048071109652</v>
-      </c>
-      <c r="K12" t="n">
-        <v>1.19677569320301</v>
-      </c>
-      <c r="L12" t="n">
         <v>0.36408716814135</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D13" t="n">
         <v>153.1</v>
       </c>
       <c r="E13" t="n">
-        <v>0.000942088337633318</v>
+        <v>182.9</v>
       </c>
       <c r="F13" t="n">
-        <v>182.9</v>
+        <v>0.527</v>
       </c>
       <c r="G13" t="n">
-        <v>0.000000490675746961884</v>
+        <v>0.199</v>
       </c>
       <c r="H13" t="n">
-        <v>0.527</v>
+        <v>0.409641426216089</v>
       </c>
       <c r="I13" t="n">
-        <v>0.199</v>
+        <v>0.70697164728988</v>
       </c>
       <c r="J13" t="n">
-        <v>0.409641426216089</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0.70697164728988</v>
-      </c>
-      <c r="L13" t="n">
         <v>0.229916347254973</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D14" t="n">
         <v>145.9</v>
       </c>
       <c r="E14" t="n">
-        <v>0.0336921939959352</v>
+        <v>167.8</v>
       </c>
       <c r="F14" t="n">
-        <v>167.8</v>
+        <v>0.521</v>
       </c>
       <c r="G14" t="n">
-        <v>0.000937220650941962</v>
+        <v>0.195</v>
       </c>
       <c r="H14" t="n">
-        <v>0.521</v>
+        <v>0.405142466313655</v>
       </c>
       <c r="I14" t="n">
-        <v>0.195</v>
+        <v>0.710112914902594</v>
       </c>
       <c r="J14" t="n">
-        <v>0.405142466313655</v>
-      </c>
-      <c r="K14" t="n">
-        <v>0.710112914902594</v>
-      </c>
-      <c r="L14" t="n">
         <v>0.231080474175141</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D15" t="n">
         <v>146.2</v>
       </c>
       <c r="E15" t="n">
-        <v>0.0289917494562144</v>
+        <v>166.1</v>
       </c>
       <c r="F15" t="n">
-        <v>166.1</v>
+        <v>0.5</v>
       </c>
       <c r="G15" t="n">
-        <v>0.00218016507203759</v>
+        <v>0.174</v>
       </c>
       <c r="H15" t="n">
-        <v>0.5</v>
+        <v>0.394017895328747</v>
       </c>
       <c r="I15" t="n">
-        <v>0.174</v>
+        <v>0.734044282144376</v>
       </c>
       <c r="J15" t="n">
-        <v>0.394017895328747</v>
-      </c>
-      <c r="K15" t="n">
-        <v>0.734044282144376</v>
-      </c>
-      <c r="L15" t="n">
         <v>0.23735001040535</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D16" t="n">
         <v>142.3</v>
       </c>
       <c r="E16" t="n">
-        <v>0.204393622665867</v>
+        <v>158.2</v>
       </c>
       <c r="F16" t="n">
-        <v>158.2</v>
+        <v>0.499</v>
       </c>
       <c r="G16" t="n">
-        <v>0.112327758313534</v>
+        <v>0.174</v>
       </c>
       <c r="H16" t="n">
-        <v>0.499</v>
+        <v>0.393286214699538</v>
       </c>
       <c r="I16" t="n">
-        <v>0.174</v>
+        <v>0.73324439340205</v>
       </c>
       <c r="J16" t="n">
-        <v>0.393286214699538</v>
-      </c>
-      <c r="K16" t="n">
-        <v>0.73324439340205</v>
-      </c>
-      <c r="L16" t="n">
         <v>0.237295448480225</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D17" t="n">
         <v>147.9</v>
       </c>
       <c r="E17" t="n">
-        <v>0.0125689310659239</v>
+        <v>171.8</v>
       </c>
       <c r="F17" t="n">
-        <v>171.8</v>
+        <v>0.522</v>
       </c>
       <c r="G17" t="n">
-        <v>0.00012933274732436</v>
+        <v>0.195</v>
       </c>
       <c r="H17" t="n">
-        <v>0.522</v>
+        <v>0.405616901269354</v>
       </c>
       <c r="I17" t="n">
-        <v>0.195</v>
+        <v>0.709947971925215</v>
       </c>
       <c r="J17" t="n">
-        <v>0.405616901269354</v>
-      </c>
-      <c r="K17" t="n">
-        <v>0.709947971925215</v>
-      </c>
-      <c r="L17" t="n">
         <v>0.230951400774421</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D18" t="n">
         <v>140.4</v>
       </c>
       <c r="E18" t="n">
-        <v>0.522443416391658</v>
+        <v>154.4</v>
       </c>
       <c r="F18" t="n">
-        <v>154.4</v>
+        <v>0.485</v>
       </c>
       <c r="G18" t="n">
-        <v>0.776178144031763</v>
+        <v>0.147</v>
       </c>
       <c r="H18" t="n">
-        <v>0.485</v>
+        <v>0.396708536396551</v>
       </c>
       <c r="I18" t="n">
-        <v>0.147</v>
+        <v>0.732981216183524</v>
       </c>
       <c r="J18" t="n">
-        <v>0.396708536396551</v>
-      </c>
-      <c r="K18" t="n">
-        <v>0.732981216183524</v>
-      </c>
-      <c r="L18" t="n">
         <v>0.238221370362628</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D19" t="n">
         <v>142.4</v>
       </c>
       <c r="E19" t="n">
-        <v>0.196967998086768</v>
+        <v>158.3</v>
       </c>
       <c r="F19" t="n">
-        <v>158.3</v>
+        <v>0.493</v>
       </c>
       <c r="G19" t="n">
-        <v>0.108246888508652</v>
+        <v>0.145</v>
       </c>
       <c r="H19" t="n">
-        <v>0.493</v>
+        <v>0.40760856417087</v>
       </c>
       <c r="I19" t="n">
-        <v>0.145</v>
+        <v>0.727645208726944</v>
       </c>
       <c r="J19" t="n">
-        <v>0.40760856417087</v>
-      </c>
-      <c r="K19" t="n">
-        <v>0.727645208726944</v>
-      </c>
-      <c r="L19" t="n">
         <v>0.236972613071863</v>
       </c>
     </row>
@@ -2383,27 +2263,27 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
         <v>67</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>68</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>69</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>70</v>
-      </c>
-      <c r="F1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -2421,12 +2301,12 @@
         <v>0.00067</v>
       </c>
       <c r="G2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -2444,12 +2324,12 @@
         <v>0.05929</v>
       </c>
       <c r="G3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -2467,12 +2347,12 @@
         <v>0.00133</v>
       </c>
       <c r="G4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B5" t="n">
         <v>80</v>
@@ -2486,12 +2366,12 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B6" t="n">
         <v>85</v>
@@ -2505,12 +2385,12 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B7" t="n">
         <v>1</v>
@@ -2528,12 +2408,12 @@
         <v>0.00067</v>
       </c>
       <c r="G7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B8" t="n">
         <v>1</v>
@@ -2551,12 +2431,12 @@
         <v>0.00067</v>
       </c>
       <c r="G8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B9" t="n">
         <v>3</v>
@@ -2574,12 +2454,12 @@
         <v>0.22785</v>
       </c>
       <c r="G9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B10" t="n">
         <v>71</v>
@@ -2593,12 +2473,12 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B11" t="n">
         <v>76</v>
@@ -2612,12 +2492,12 @@
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B12" t="n">
         <v>1</v>
@@ -2635,12 +2515,12 @@
         <v>0.46036</v>
       </c>
       <c r="G12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B13" t="n">
         <v>1</v>
@@ -2658,12 +2538,12 @@
         <v>0.00133</v>
       </c>
       <c r="G13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B14" t="n">
         <v>3</v>
@@ -2681,12 +2561,12 @@
         <v>0.00067</v>
       </c>
       <c r="G14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B15" t="n">
         <v>62</v>
@@ -2700,12 +2580,12 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B16" t="n">
         <v>67</v>
@@ -2719,7 +2599,7 @@
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2749,24 +2629,24 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" t="s">
         <v>81</v>
       </c>
-      <c r="C1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" t="s">
-        <v>83</v>
-      </c>
       <c r="E1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B2" t="n">
         <v>1.05</v>
@@ -2781,12 +2661,12 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B3" t="n">
         <v>0.01</v>
@@ -2801,12 +2681,12 @@
         <v>0.085</v>
       </c>
       <c r="F3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B4" t="n">
         <v>0.378</v>
@@ -2821,12 +2701,12 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B5" t="n">
         <v>0.223</v>
@@ -2841,12 +2721,12 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B6" t="n">
         <v>0.444</v>
@@ -2861,12 +2741,12 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B7" t="n">
         <v>0.002</v>
@@ -2881,12 +2761,12 @@
         <v>0.753</v>
       </c>
       <c r="F7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B8" t="n">
         <v>-0.771</v>
@@ -2901,12 +2781,12 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B9" t="n">
         <v>-0.446</v>
@@ -2921,12 +2801,12 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B10" t="n">
         <v>-0.33</v>
@@ -2941,12 +2821,12 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B11" t="n">
         <v>0.542</v>
@@ -2955,12 +2835,12 @@
       <c r="D11"/>
       <c r="E11"/>
       <c r="F11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B12" t="n">
         <v>0.307</v>
@@ -2969,12 +2849,12 @@
       <c r="D12"/>
       <c r="E12"/>
       <c r="F12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B13" t="n">
         <v>1.279</v>
@@ -2989,12 +2869,12 @@
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B14" t="n">
         <v>-0.338</v>
@@ -3009,12 +2889,12 @@
         <v>0.08</v>
       </c>
       <c r="F14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B15" t="n">
         <v>-0.059</v>
@@ -3029,12 +2909,12 @@
         <v>0.753</v>
       </c>
       <c r="F15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B16" t="n">
         <v>0.227</v>
@@ -3049,12 +2929,12 @@
         <v>0.19</v>
       </c>
       <c r="F16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B17" t="n">
         <v>0.232</v>
@@ -3063,12 +2943,12 @@
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B18" t="n">
         <v>0.188</v>
@@ -3077,12 +2957,12 @@
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B19" t="n">
         <v>1.033</v>
@@ -3097,12 +2977,12 @@
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B20" t="n">
         <v>-0.045</v>
@@ -3117,12 +2997,12 @@
         <v>0.694</v>
       </c>
       <c r="F20" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B21" t="n">
         <v>0.033</v>
@@ -3137,12 +3017,12 @@
         <v>0.676</v>
       </c>
       <c r="F21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B22" t="n">
         <v>0.124</v>
@@ -3157,12 +3037,12 @@
         <v>0.131</v>
       </c>
       <c r="F22" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B23" t="n">
         <v>0.262</v>
@@ -3177,12 +3057,12 @@
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B24" t="n">
         <v>0.493</v>
@@ -3191,12 +3071,12 @@
       <c r="D24"/>
       <c r="E24"/>
       <c r="F24" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B25" t="n">
         <v>0.145</v>
@@ -3205,7 +3085,7 @@
       <c r="D25"/>
       <c r="E25"/>
       <c r="F25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -3235,24 +3115,24 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
         <v>67</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>68</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>69</v>
-      </c>
-      <c r="E1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -3272,7 +3152,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -3292,7 +3172,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -3312,7 +3192,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B5" t="n">
         <v>2</v>
@@ -3332,7 +3212,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B6" t="n">
         <v>2</v>
@@ -3352,7 +3232,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B7" t="n">
         <v>6</v>
@@ -3372,7 +3252,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B8" t="n">
         <v>2</v>
@@ -3392,7 +3272,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B9" t="n">
         <v>214</v>
@@ -3408,7 +3288,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B10" t="n">
         <v>231</v>
@@ -3455,42 +3335,42 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
         <v>67</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>68</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>69</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1" t="s">
+        <v>97</v>
+      </c>
+      <c r="K1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L1" t="s">
         <v>70</v>
-      </c>
-      <c r="F1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H1" t="s">
-        <v>97</v>
-      </c>
-      <c r="I1" t="s">
-        <v>98</v>
-      </c>
-      <c r="J1" t="s">
-        <v>99</v>
-      </c>
-      <c r="K1" t="s">
-        <v>100</v>
-      </c>
-      <c r="L1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -3523,12 +3403,12 @@
         <v>0.00067</v>
       </c>
       <c r="L2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -3561,12 +3441,12 @@
         <v>0.0966</v>
       </c>
       <c r="L3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -3599,12 +3479,12 @@
         <v>0.00266</v>
       </c>
       <c r="L4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B5" t="n">
         <v>80</v>
@@ -3629,12 +3509,12 @@
       <c r="J5"/>
       <c r="K5"/>
       <c r="L5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B6" t="n">
         <v>85</v>
@@ -3659,12 +3539,12 @@
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B7" t="n">
         <v>3</v>
@@ -3697,12 +3577,12 @@
         <v>0.28115</v>
       </c>
       <c r="L7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B8" t="n">
         <v>1</v>
@@ -3735,12 +3615,12 @@
         <v>0.00067</v>
       </c>
       <c r="L8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B9" t="n">
         <v>1</v>
@@ -3773,12 +3653,12 @@
         <v>0.00133</v>
       </c>
       <c r="L9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B10" t="n">
         <v>71</v>
@@ -3803,12 +3683,12 @@
       <c r="J10"/>
       <c r="K10"/>
       <c r="L10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B11" t="n">
         <v>76</v>
@@ -3833,12 +3713,12 @@
       <c r="J11"/>
       <c r="K11"/>
       <c r="L11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B12" t="n">
         <v>3</v>
@@ -3871,12 +3751,12 @@
         <v>0.00067</v>
       </c>
       <c r="L12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B13" t="n">
         <v>1</v>
@@ -3909,12 +3789,12 @@
         <v>0.00067</v>
       </c>
       <c r="L13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B14" t="n">
         <v>1</v>
@@ -3947,12 +3827,12 @@
         <v>0.46636</v>
       </c>
       <c r="L14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B15" t="n">
         <v>62</v>
@@ -3977,12 +3857,12 @@
       <c r="J15"/>
       <c r="K15"/>
       <c r="L15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B16" t="n">
         <v>67</v>
@@ -4007,7 +3887,7 @@
       <c r="J16"/>
       <c r="K16"/>
       <c r="L16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -4027,10 +3907,10 @@
     <col min="1" max="1" width="71.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="8.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="5.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="11.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="6.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="6.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="14.71" hidden="0" customWidth="1"/>
     <col min="6" max="6" width="11.71" hidden="0" customWidth="1"/>
-    <col min="7" max="7" width="14.71" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="11.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4061,395 +3941,323 @@
       <c r="I1" t="s">
         <v>52</v>
       </c>
-      <c r="J1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K1" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C2" t="n">
         <v>923.1</v>
       </c>
       <c r="D2" t="n">
-        <v>0.000000000356173661287928</v>
+        <v>1219.4</v>
       </c>
       <c r="E2" t="n">
-        <v>1219.4</v>
+        <v>0.43</v>
       </c>
       <c r="F2" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000106026935087453</v>
+        <v>0.318</v>
       </c>
       <c r="G2" t="n">
-        <v>0.43</v>
+        <v>0.163808918846475</v>
       </c>
       <c r="H2" t="n">
-        <v>0.318</v>
+        <v>0.884761957169536</v>
       </c>
       <c r="I2" t="n">
-        <v>0.163808918846475</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0.884761957169536</v>
-      </c>
-      <c r="K2" t="n">
         <v>0.445413568051623</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C3" t="n">
         <v>904.6</v>
       </c>
       <c r="D3" t="n">
-        <v>0.00000356476632034088</v>
+        <v>1086.1</v>
       </c>
       <c r="E3" t="n">
-        <v>1086.1</v>
+        <v>0.338</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0000000000000000000000000000000000907895747647671</v>
+        <v>0.225</v>
       </c>
       <c r="G3" t="n">
-        <v>0.338</v>
+        <v>0.144860307744428</v>
       </c>
       <c r="H3" t="n">
-        <v>0.225</v>
+        <v>0.948916968928776</v>
       </c>
       <c r="I3" t="n">
-        <v>0.144860307744428</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.948916968928776</v>
-      </c>
-      <c r="K3" t="n">
         <v>0.477395026003451</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C4" t="n">
         <v>890.2</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0049751824323713</v>
+        <v>964.2</v>
       </c>
       <c r="E4" t="n">
-        <v>964.2</v>
+        <v>0.222</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0000000267012839066756</v>
+        <v>0.113</v>
       </c>
       <c r="G4" t="n">
-        <v>0.222</v>
+        <v>0.122648785796666</v>
       </c>
       <c r="H4" t="n">
-        <v>0.113</v>
+        <v>1.00853413602528</v>
       </c>
       <c r="I4" t="n">
-        <v>0.122648785796666</v>
-      </c>
-      <c r="J4" t="n">
-        <v>1.00853413602528</v>
-      </c>
-      <c r="K4" t="n">
         <v>0.508488836608921</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C5" t="n">
         <v>881.2</v>
       </c>
       <c r="D5" t="n">
-        <v>0.436931983172524</v>
+        <v>929.4</v>
       </c>
       <c r="E5" t="n">
-        <v>929.4</v>
+        <v>0.205</v>
       </c>
       <c r="F5" t="n">
-        <v>0.999999973298655</v>
+        <v>0.095</v>
       </c>
       <c r="G5" t="n">
-        <v>0.205</v>
+        <v>0.121607431312658</v>
       </c>
       <c r="H5" t="n">
-        <v>0.095</v>
+        <v>1.01492820585159</v>
       </c>
       <c r="I5" t="n">
-        <v>0.121607431312658</v>
-      </c>
-      <c r="J5" t="n">
-        <v>1.01492820585159</v>
-      </c>
-      <c r="K5" t="n">
         <v>0.513921291826242</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C6" t="n">
         <v>902.1</v>
       </c>
       <c r="D6" t="n">
-        <v>0.000012830993710202</v>
+        <v>1124.3</v>
       </c>
       <c r="E6" t="n">
-        <v>1124.3</v>
+        <v>0.391</v>
       </c>
       <c r="F6" t="n">
-        <v>0.000000000000000000000000000000000000000000464876516436139</v>
+        <v>0.279</v>
       </c>
       <c r="G6" t="n">
-        <v>0.391</v>
+        <v>0.155601596236995</v>
       </c>
       <c r="H6" t="n">
-        <v>0.279</v>
+        <v>0.913117790532039</v>
       </c>
       <c r="I6" t="n">
-        <v>0.155601596236995</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.913117790532039</v>
-      </c>
-      <c r="K6" t="n">
         <v>0.45931696402324</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C7" t="n">
         <v>890.2</v>
       </c>
       <c r="D7" t="n">
-        <v>0.00479961344622744</v>
+        <v>990.2</v>
       </c>
       <c r="E7" t="n">
-        <v>990.2</v>
+        <v>0.235</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0000000000000604040943674256</v>
+        <v>0.093</v>
       </c>
       <c r="G7" t="n">
-        <v>0.235</v>
+        <v>0.157143513626403</v>
       </c>
       <c r="H7" t="n">
-        <v>0.093</v>
+        <v>0.982507593585701</v>
       </c>
       <c r="I7" t="n">
-        <v>0.157143513626403</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.982507593585701</v>
-      </c>
-      <c r="K7" t="n">
         <v>0.505803686093402</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C8" t="n">
         <v>902.1</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0000128309937101984</v>
+        <v>1124.3</v>
       </c>
       <c r="E8" t="n">
-        <v>1124.3</v>
+        <v>0.391</v>
       </c>
       <c r="F8" t="n">
-        <v>0.000000000000000000000000000000000000000000464876516436033</v>
+        <v>0.279</v>
       </c>
       <c r="G8" t="n">
-        <v>0.391</v>
+        <v>0.155601596236034</v>
       </c>
       <c r="H8" t="n">
-        <v>0.279</v>
+        <v>0.913117790532143</v>
       </c>
       <c r="I8" t="n">
-        <v>0.155601596236034</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.913117790532143</v>
-      </c>
-      <c r="K8" t="n">
         <v>0.459316964023365</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C9" t="n">
         <v>902.1</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0000128309937101984</v>
+        <v>1124.3</v>
       </c>
       <c r="E9" t="n">
-        <v>1124.3</v>
+        <v>0.391</v>
       </c>
       <c r="F9" t="n">
-        <v>0.000000000000000000000000000000000000000000464876516436033</v>
+        <v>0.279</v>
       </c>
       <c r="G9" t="n">
-        <v>0.391</v>
+        <v>0.155601596236034</v>
       </c>
       <c r="H9" t="n">
-        <v>0.279</v>
+        <v>0.913117790532143</v>
       </c>
       <c r="I9" t="n">
-        <v>0.155601596236034</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0.913117790532143</v>
-      </c>
-      <c r="K9" t="n">
         <v>0.459316964023365</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C10" t="n">
         <v>882</v>
       </c>
       <c r="D10" t="n">
-        <v>0.302098653514401</v>
+        <v>1000.5</v>
       </c>
       <c r="E10" t="n">
-        <v>1000.5</v>
+        <v>0.28</v>
       </c>
       <c r="F10" t="n">
-        <v>0.000000000000000361974667895156</v>
+        <v>0.139</v>
       </c>
       <c r="G10" t="n">
-        <v>0.28</v>
+        <v>0.163720683028945</v>
       </c>
       <c r="H10" t="n">
-        <v>0.139</v>
+        <v>0.950425796937665</v>
       </c>
       <c r="I10" t="n">
-        <v>0.163720683028945</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0.950425796937665</v>
-      </c>
-      <c r="K10" t="n">
         <v>0.488694314791684</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C11" t="n">
         <v>883.5</v>
       </c>
       <c r="D11" t="n">
-        <v>0.138174298373614</v>
+        <v>1005.7</v>
       </c>
       <c r="E11" t="n">
-        <v>1005.7</v>
+        <v>0.282</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0000000000000000259830728679035</v>
+        <v>0.144</v>
       </c>
       <c r="G11" t="n">
-        <v>0.282</v>
+        <v>0.161404588856711</v>
       </c>
       <c r="H11" t="n">
-        <v>0.144</v>
+        <v>0.950207028246836</v>
       </c>
       <c r="I11" t="n">
-        <v>0.161404588856711</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0.950207028246836</v>
-      </c>
-      <c r="K11" t="n">
         <v>0.488554386709045</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C12" t="n">
         <v>883.9</v>
       </c>
       <c r="D12" t="n">
-        <v>0.112978210957238</v>
+        <v>1024.7</v>
       </c>
       <c r="E12" t="n">
-        <v>1024.7</v>
+        <v>0.323</v>
       </c>
       <c r="F12" t="n">
-        <v>0.00000000000000000000202268013528013</v>
+        <v>0.212</v>
       </c>
       <c r="G12" t="n">
-        <v>0.323</v>
+        <v>0.140275722020262</v>
       </c>
       <c r="H12" t="n">
-        <v>0.212</v>
+        <v>0.935551604873005</v>
       </c>
       <c r="I12" t="n">
-        <v>0.140275722020262</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0.935551604873005</v>
-      </c>
-      <c r="K12" t="n">
         <v>0.476818047697685</v>
       </c>
     </row>
@@ -4480,21 +4288,21 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" t="s">
         <v>81</v>
       </c>
-      <c r="C1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" t="s">
-        <v>83</v>
-      </c>
       <c r="E1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B2" t="n">
         <v>0.8</v>
@@ -4511,7 +4319,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B3" t="n">
         <v>0.199</v>
@@ -4528,7 +4336,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B4" t="n">
         <v>-0.357</v>
@@ -4545,7 +4353,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B5" t="n">
         <v>-0.515</v>
@@ -4562,7 +4370,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B6" t="n">
         <v>0.234</v>
@@ -4579,7 +4387,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B7" t="n">
         <v>0.005</v>
@@ -4596,7 +4404,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B8" t="n">
         <v>-0.021</v>
@@ -4613,7 +4421,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B9" t="n">
         <v>-0.252</v>
@@ -4630,7 +4438,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B10" t="n">
         <v>0.223</v>
@@ -4647,7 +4455,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B11" t="n">
         <v>0.685</v>
@@ -4664,7 +4472,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B12" t="n">
         <v>-0.088</v>
@@ -4681,7 +4489,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B13" t="n">
         <v>-0.568</v>
@@ -4698,7 +4506,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B14" t="n">
         <v>-0.45</v>
@@ -4715,7 +4523,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B15" t="n">
         <v>0.051</v>
@@ -4732,7 +4540,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B16" t="n">
         <v>-0.154</v>
@@ -4749,7 +4557,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B17" t="n">
         <v>0.236</v>
@@ -4766,7 +4574,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B18" t="n">
         <v>0.072</v>
@@ -4783,7 +4591,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B19" t="n">
         <v>0.608</v>
@@ -4800,7 +4608,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B20" t="n">
         <v>-0.299</v>
@@ -4817,7 +4625,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B21" t="n">
         <v>0.134</v>
@@ -4834,7 +4642,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B22" t="n">
         <v>0.564</v>
@@ -4851,7 +4659,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B23" t="n">
         <v>0.524</v>
@@ -4868,7 +4676,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B24" t="n">
         <v>0.362</v>
@@ -4885,7 +4693,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B25" t="n">
         <v>0.673</v>
@@ -4902,7 +4710,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B26" t="n">
         <v>-0.179</v>
@@ -4919,7 +4727,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B27" t="n">
         <v>-0.18</v>
@@ -4936,7 +4744,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B28" t="n">
         <v>-0.482</v>
@@ -4953,7 +4761,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B29" t="n">
         <v>-0.89</v>
@@ -4970,7 +4778,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B30" t="n">
         <v>0.189</v>
@@ -4987,7 +4795,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B31" t="n">
         <v>-0.607</v>
@@ -5004,7 +4812,7 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B32" t="n">
         <v>0.28</v>
@@ -5015,7 +4823,7 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B33" t="n">
         <v>0.139</v>

</xml_diff>

<commit_message>
add table of PCA AIC values
</commit_message>
<xml_diff>
--- a/Data/Supplemental/Supplemental_Tables.xlsx
+++ b/Data/Supplemental/Supplemental_Tables.xlsx
@@ -7,19 +7,20 @@
   </bookViews>
   <sheets>
     <sheet name="Table S1 - Sample Size" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Table S2 - Plasticity AIC" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Table S3 - PERMANOVA" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Table S4 - Plasticity GLM" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Table S5 - Species PERMANOVA" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Table S6 - HostVsymb PERMANOVA" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Table S7 - HostVsymb Plast AIC" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Table S8 - HostVsymb Plast GLM" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Table S2 - PERMANOVA AIC" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Table S3 - Plasticity AIC" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Table S4 - PERMANOVA" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Table S5 - Plasticity GLM" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Table S6 - Species PERMANOVA" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Table S7 - HostVsymb PERMANOVA" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Table S8 - HostVsymb Plast AIC" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Table S9 - HostVsymb Plast GLM" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="137">
   <si>
     <t xml:space="preserve">group</t>
   </si>
@@ -151,6 +152,21 @@
   </si>
   <si>
     <t xml:space="preserve">S_pre industrial (uatm)_31C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full interactive model AIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Best fit (additive) model AIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S. siderea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P. strigosa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P. astreoides</t>
   </si>
   <si>
     <t xml:space="preserve">Model formula</t>
@@ -1618,6 +1634,69 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
+    <col min="1" max="1" width="13.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="26.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="29.71" hidden="0" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="n">
+        <v>692.3</v>
+      </c>
+      <c r="C2" t="n">
+        <v>678.5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="n">
+        <v>696.9</v>
+      </c>
+      <c r="C3" t="n">
+        <v>685.8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" t="n">
+        <v>500.5</v>
+      </c>
+      <c r="C4" t="n">
+        <v>497.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <cols>
     <col min="1" max="1" width="7.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="65.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="8.71" hidden="0" customWidth="1"/>
@@ -1632,42 +1711,42 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="F1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="G1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="H1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="I1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="J1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D2" t="n">
         <v>223.2</v>
@@ -1693,13 +1772,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D3" t="n">
         <v>218.8</v>
@@ -1725,13 +1804,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D4" t="n">
         <v>218.4</v>
@@ -1757,13 +1836,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D5" t="n">
         <v>225.6</v>
@@ -1789,13 +1868,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D6" t="n">
         <v>221.6</v>
@@ -1821,13 +1900,13 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" t="s">
         <v>60</v>
-      </c>
-      <c r="C7" t="s">
-        <v>55</v>
       </c>
       <c r="D7" t="n">
         <v>220.1</v>
@@ -1853,13 +1932,13 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D8" t="n">
         <v>222.1</v>
@@ -1885,13 +1964,13 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D9" t="n">
         <v>110.7</v>
@@ -1917,13 +1996,13 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D10" t="n">
         <v>106</v>
@@ -1949,13 +2028,13 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D11" t="n">
         <v>106.9</v>
@@ -1981,13 +2060,13 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D12" t="n">
         <v>102.8</v>
@@ -2013,13 +2092,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D13" t="n">
         <v>153.1</v>
@@ -2045,13 +2124,13 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D14" t="n">
         <v>145.9</v>
@@ -2077,13 +2156,13 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" t="s">
         <v>63</v>
       </c>
-      <c r="B15" t="s">
-        <v>58</v>
-      </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D15" t="n">
         <v>146.2</v>
@@ -2109,13 +2188,13 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D16" t="n">
         <v>142.3</v>
@@ -2141,13 +2220,13 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" t="s">
         <v>60</v>
-      </c>
-      <c r="C17" t="s">
-        <v>55</v>
       </c>
       <c r="D17" t="n">
         <v>147.9</v>
@@ -2173,13 +2252,13 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B18" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D18" t="n">
         <v>140.4</v>
@@ -2205,13 +2284,13 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B19" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D19" t="n">
         <v>142.4</v>
@@ -2241,7 +2320,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2263,27 +2342,27 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="F1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="G1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -2301,12 +2380,12 @@
         <v>0.00067</v>
       </c>
       <c r="G2" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -2321,15 +2400,15 @@
         <v>3.73</v>
       </c>
       <c r="F3" t="n">
-        <v>0.05929</v>
+        <v>0.05463</v>
       </c>
       <c r="G3" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -2347,12 +2426,12 @@
         <v>0.00133</v>
       </c>
       <c r="G4" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B5" t="n">
         <v>80</v>
@@ -2366,12 +2445,12 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B6" t="n">
         <v>85</v>
@@ -2385,12 +2464,12 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B7" t="n">
         <v>1</v>
@@ -2408,12 +2487,12 @@
         <v>0.00067</v>
       </c>
       <c r="G7" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B8" t="n">
         <v>1</v>
@@ -2431,12 +2510,12 @@
         <v>0.00067</v>
       </c>
       <c r="G8" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B9" t="n">
         <v>3</v>
@@ -2451,15 +2530,15 @@
         <v>1.48</v>
       </c>
       <c r="F9" t="n">
-        <v>0.22785</v>
+        <v>0.22252</v>
       </c>
       <c r="G9" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B10" t="n">
         <v>71</v>
@@ -2473,12 +2552,12 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B11" t="n">
         <v>76</v>
@@ -2492,12 +2571,12 @@
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B12" t="n">
         <v>1</v>
@@ -2512,15 +2591,15 @@
         <v>0.53</v>
       </c>
       <c r="F12" t="n">
-        <v>0.46036</v>
+        <v>0.48568</v>
       </c>
       <c r="G12" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B13" t="n">
         <v>1</v>
@@ -2538,12 +2617,12 @@
         <v>0.00133</v>
       </c>
       <c r="G13" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B14" t="n">
         <v>3</v>
@@ -2561,12 +2640,12 @@
         <v>0.00067</v>
       </c>
       <c r="G14" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B15" t="n">
         <v>62</v>
@@ -2580,12 +2659,12 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B16" t="n">
         <v>67</v>
@@ -2599,7 +2678,7 @@
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2608,7 +2687,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2629,24 +2708,24 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="F1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B2" t="n">
         <v>1.05</v>
@@ -2661,12 +2740,12 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B3" t="n">
         <v>0.01</v>
@@ -2681,12 +2760,12 @@
         <v>0.085</v>
       </c>
       <c r="F3" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B4" t="n">
         <v>0.378</v>
@@ -2701,12 +2780,12 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B5" t="n">
         <v>0.223</v>
@@ -2721,12 +2800,12 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B6" t="n">
         <v>0.444</v>
@@ -2741,12 +2820,12 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B7" t="n">
         <v>0.002</v>
@@ -2761,12 +2840,12 @@
         <v>0.753</v>
       </c>
       <c r="F7" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="B8" t="n">
         <v>-0.771</v>
@@ -2781,12 +2860,12 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B9" t="n">
         <v>-0.446</v>
@@ -2801,12 +2880,12 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B10" t="n">
         <v>-0.33</v>
@@ -2821,12 +2900,12 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B11" t="n">
         <v>0.542</v>
@@ -2835,12 +2914,12 @@
       <c r="D11"/>
       <c r="E11"/>
       <c r="F11" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B12" t="n">
         <v>0.307</v>
@@ -2849,12 +2928,12 @@
       <c r="D12"/>
       <c r="E12"/>
       <c r="F12" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B13" t="n">
         <v>1.279</v>
@@ -2869,12 +2948,12 @@
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B14" t="n">
         <v>-0.338</v>
@@ -2889,12 +2968,12 @@
         <v>0.08</v>
       </c>
       <c r="F14" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B15" t="n">
         <v>-0.059</v>
@@ -2909,12 +2988,12 @@
         <v>0.753</v>
       </c>
       <c r="F15" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B16" t="n">
         <v>0.227</v>
@@ -2929,12 +3008,12 @@
         <v>0.19</v>
       </c>
       <c r="F16" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B17" t="n">
         <v>0.232</v>
@@ -2943,12 +3022,12 @@
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B18" t="n">
         <v>0.188</v>
@@ -2957,12 +3036,12 @@
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B19" t="n">
         <v>1.033</v>
@@ -2977,12 +3056,12 @@
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B20" t="n">
         <v>-0.045</v>
@@ -2997,12 +3076,12 @@
         <v>0.694</v>
       </c>
       <c r="F20" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B21" t="n">
         <v>0.033</v>
@@ -3017,12 +3096,12 @@
         <v>0.676</v>
       </c>
       <c r="F21" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B22" t="n">
         <v>0.124</v>
@@ -3037,12 +3116,12 @@
         <v>0.131</v>
       </c>
       <c r="F22" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B23" t="n">
         <v>0.262</v>
@@ -3057,12 +3136,12 @@
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B24" t="n">
         <v>0.493</v>
@@ -3071,12 +3150,12 @@
       <c r="D24"/>
       <c r="E24"/>
       <c r="F24" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B25" t="n">
         <v>0.145</v>
@@ -3085,7 +3164,7 @@
       <c r="D25"/>
       <c r="E25"/>
       <c r="F25" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -3094,7 +3173,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3115,24 +3194,24 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="F1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -3152,7 +3231,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -3167,12 +3246,12 @@
         <v>2.87</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0986</v>
+        <v>0.0966</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -3187,12 +3266,12 @@
         <v>9.61</v>
       </c>
       <c r="F4" t="n">
-        <v>0.004</v>
+        <v>0.00133</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B5" t="n">
         <v>2</v>
@@ -3212,7 +3291,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B6" t="n">
         <v>2</v>
@@ -3232,7 +3311,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B7" t="n">
         <v>6</v>
@@ -3247,12 +3326,12 @@
         <v>2.51</v>
       </c>
       <c r="F7" t="n">
-        <v>0.01865</v>
+        <v>0.02065</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B8" t="n">
         <v>2</v>
@@ -3267,12 +3346,12 @@
         <v>6.39</v>
       </c>
       <c r="F8" t="n">
-        <v>0.00533</v>
+        <v>0.00266</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B9" t="n">
         <v>214</v>
@@ -3288,7 +3367,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B10" t="n">
         <v>231</v>
@@ -3308,7 +3387,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3335,42 +3414,42 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="F1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="G1" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="H1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="I1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="J1" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="K1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="L1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -3385,7 +3464,7 @@
         <v>0.55</v>
       </c>
       <c r="F2" t="n">
-        <v>0.74883</v>
+        <v>0.77615</v>
       </c>
       <c r="G2" t="n">
         <v>3</v>
@@ -3403,12 +3482,12 @@
         <v>0.00067</v>
       </c>
       <c r="L2" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -3423,7 +3502,7 @@
         <v>6.65</v>
       </c>
       <c r="F3" t="n">
-        <v>0.00666</v>
+        <v>0.002</v>
       </c>
       <c r="G3" t="n">
         <v>1</v>
@@ -3438,15 +3517,15 @@
         <v>2.99</v>
       </c>
       <c r="K3" t="n">
-        <v>0.0966</v>
+        <v>0.09061</v>
       </c>
       <c r="L3" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -3461,7 +3540,7 @@
         <v>0.52</v>
       </c>
       <c r="F4" t="n">
-        <v>0.56762</v>
+        <v>0.58894</v>
       </c>
       <c r="G4" t="n">
         <v>1</v>
@@ -3479,12 +3558,12 @@
         <v>0.00266</v>
       </c>
       <c r="L4" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B5" t="n">
         <v>80</v>
@@ -3509,12 +3588,12 @@
       <c r="J5"/>
       <c r="K5"/>
       <c r="L5" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B6" t="n">
         <v>85</v>
@@ -3539,12 +3618,12 @@
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B7" t="n">
         <v>3</v>
@@ -3559,7 +3638,7 @@
         <v>1.23</v>
       </c>
       <c r="F7" t="n">
-        <v>0.27515</v>
+        <v>0.26382</v>
       </c>
       <c r="G7" t="n">
         <v>3</v>
@@ -3574,15 +3653,15 @@
         <v>1.31</v>
       </c>
       <c r="K7" t="n">
-        <v>0.28115</v>
+        <v>0.27848</v>
       </c>
       <c r="L7" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B8" t="n">
         <v>1</v>
@@ -3615,12 +3694,12 @@
         <v>0.00067</v>
       </c>
       <c r="L8" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B9" t="n">
         <v>1</v>
@@ -3635,7 +3714,7 @@
         <v>1.75</v>
       </c>
       <c r="F9" t="n">
-        <v>0.16855</v>
+        <v>0.17255</v>
       </c>
       <c r="G9" t="n">
         <v>1</v>
@@ -3650,15 +3729,15 @@
         <v>14.87</v>
       </c>
       <c r="K9" t="n">
-        <v>0.00133</v>
+        <v>0.002</v>
       </c>
       <c r="L9" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B10" t="n">
         <v>71</v>
@@ -3683,12 +3762,12 @@
       <c r="J10"/>
       <c r="K10"/>
       <c r="L10" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B11" t="n">
         <v>76</v>
@@ -3713,12 +3792,12 @@
       <c r="J11"/>
       <c r="K11"/>
       <c r="L11" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B12" t="n">
         <v>3</v>
@@ -3733,7 +3812,7 @@
         <v>3.48</v>
       </c>
       <c r="F12" t="n">
-        <v>0.01332</v>
+        <v>0.01666</v>
       </c>
       <c r="G12" t="n">
         <v>3</v>
@@ -3751,12 +3830,12 @@
         <v>0.00067</v>
       </c>
       <c r="L12" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B13" t="n">
         <v>1</v>
@@ -3771,7 +3850,7 @@
         <v>2.76</v>
       </c>
       <c r="F13" t="n">
-        <v>0.09127</v>
+        <v>0.10193</v>
       </c>
       <c r="G13" t="n">
         <v>1</v>
@@ -3789,12 +3868,12 @@
         <v>0.00067</v>
       </c>
       <c r="L13" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B14" t="n">
         <v>1</v>
@@ -3809,7 +3888,7 @@
         <v>1.64</v>
       </c>
       <c r="F14" t="n">
-        <v>0.20253</v>
+        <v>0.1992</v>
       </c>
       <c r="G14" t="n">
         <v>1</v>
@@ -3824,15 +3903,15 @@
         <v>0.53</v>
       </c>
       <c r="K14" t="n">
-        <v>0.46636</v>
+        <v>0.48168</v>
       </c>
       <c r="L14" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B15" t="n">
         <v>62</v>
@@ -3857,12 +3936,12 @@
       <c r="J15"/>
       <c r="K15"/>
       <c r="L15" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B16" t="n">
         <v>67</v>
@@ -3887,7 +3966,7 @@
       <c r="J16"/>
       <c r="K16"/>
       <c r="L16" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -3896,7 +3975,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3915,39 +3994,39 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="F1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="G1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="H1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="I1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C2" t="n">
         <v>923.1</v>
@@ -3973,10 +4052,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C3" t="n">
         <v>904.6</v>
@@ -4002,10 +4081,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C4" t="n">
         <v>890.2</v>
@@ -4031,10 +4110,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C5" t="n">
         <v>881.2</v>
@@ -4060,10 +4139,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C6" t="n">
         <v>902.1</v>
@@ -4089,10 +4168,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C7" t="n">
         <v>890.2</v>
@@ -4118,10 +4197,10 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C8" t="n">
         <v>902.1</v>
@@ -4147,10 +4226,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C9" t="n">
         <v>902.1</v>
@@ -4176,10 +4255,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C10" t="n">
         <v>882</v>
@@ -4205,10 +4284,10 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C11" t="n">
         <v>883.5</v>
@@ -4234,10 +4313,10 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C12" t="n">
         <v>883.9</v>
@@ -4267,7 +4346,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
@@ -4288,21 +4367,21 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B2" t="n">
         <v>0.8</v>
@@ -4319,7 +4398,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B3" t="n">
         <v>0.199</v>
@@ -4336,7 +4415,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B4" t="n">
         <v>-0.357</v>
@@ -4353,7 +4432,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B5" t="n">
         <v>-0.515</v>
@@ -4370,7 +4449,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B6" t="n">
         <v>0.234</v>
@@ -4387,7 +4466,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B7" t="n">
         <v>0.005</v>
@@ -4404,7 +4483,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B8" t="n">
         <v>-0.021</v>
@@ -4421,7 +4500,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B9" t="n">
         <v>-0.252</v>
@@ -4438,7 +4517,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="B10" t="n">
         <v>0.223</v>
@@ -4455,7 +4534,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B11" t="n">
         <v>0.685</v>
@@ -4472,7 +4551,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="B12" t="n">
         <v>-0.088</v>
@@ -4489,7 +4568,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B13" t="n">
         <v>-0.568</v>
@@ -4506,7 +4585,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B14" t="n">
         <v>-0.45</v>
@@ -4523,7 +4602,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="B15" t="n">
         <v>0.051</v>
@@ -4540,7 +4619,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="B16" t="n">
         <v>-0.154</v>
@@ -4557,7 +4636,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B17" t="n">
         <v>0.236</v>
@@ -4574,7 +4653,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B18" t="n">
         <v>0.072</v>
@@ -4591,7 +4670,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="B19" t="n">
         <v>0.608</v>
@@ -4608,7 +4687,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B20" t="n">
         <v>-0.299</v>
@@ -4625,7 +4704,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B21" t="n">
         <v>0.134</v>
@@ -4642,7 +4721,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B22" t="n">
         <v>0.564</v>
@@ -4659,7 +4738,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B23" t="n">
         <v>0.524</v>
@@ -4676,7 +4755,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="B24" t="n">
         <v>0.362</v>
@@ -4693,7 +4772,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B25" t="n">
         <v>0.673</v>
@@ -4710,7 +4789,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="B26" t="n">
         <v>-0.179</v>
@@ -4727,7 +4806,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B27" t="n">
         <v>-0.18</v>
@@ -4744,7 +4823,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B28" t="n">
         <v>-0.482</v>
@@ -4761,7 +4840,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="B29" t="n">
         <v>-0.89</v>
@@ -4778,7 +4857,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="B30" t="n">
         <v>0.189</v>
@@ -4795,7 +4874,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="B31" t="n">
         <v>-0.607</v>
@@ -4812,7 +4891,7 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B32" t="n">
         <v>0.28</v>
@@ -4823,7 +4902,7 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B33" t="n">
         <v>0.139</v>

</xml_diff>

<commit_message>
update to document text
</commit_message>
<xml_diff>
--- a/Data/Supplemental/Supplemental_Tables.xlsx
+++ b/Data/Supplemental/Supplemental_Tables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="139">
   <si>
     <t xml:space="preserve">group</t>
   </si>
@@ -178,7 +178,13 @@
     <t xml:space="preserve">AIC</t>
   </si>
   <si>
+    <t xml:space="preserve">AIC_wt</t>
+  </si>
+  <si>
     <t xml:space="preserve">BIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BIC_wt</t>
   </si>
   <si>
     <t xml:space="preserve">Conditional R2</t>
@@ -1701,8 +1707,8 @@
     <col min="2" max="2" width="65.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="8.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="5.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="5.71" hidden="0" customWidth="1"/>
-    <col min="6" max="6" width="14.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="11.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="5.71" hidden="0" customWidth="1"/>
     <col min="7" max="7" width="11.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1737,580 +1743,694 @@
       <c r="J1" t="s">
         <v>57</v>
       </c>
+      <c r="K1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D2" t="n">
         <v>223.2</v>
       </c>
       <c r="E2" t="n">
+        <v>0.0332206990579833</v>
+      </c>
+      <c r="F2" t="n">
         <v>259.2</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
+        <v>0.0000152578956652519</v>
+      </c>
+      <c r="H2" t="n">
         <v>0.545</v>
       </c>
-      <c r="G2" t="n">
+      <c r="I2" t="n">
         <v>0.366</v>
       </c>
-      <c r="H2" t="n">
+      <c r="J2" t="n">
         <v>0.282067343982829</v>
       </c>
-      <c r="I2" t="n">
+      <c r="K2" t="n">
         <v>0.855828398264632</v>
       </c>
-      <c r="J2" t="n">
+      <c r="L2" t="n">
         <v>0.294010052236142</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D3" t="n">
         <v>218.8</v>
       </c>
       <c r="E3" t="n">
+        <v>0.306747214704836</v>
+      </c>
+      <c r="F3" t="n">
         <v>243.5</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
+        <v>0.0389169854792176</v>
+      </c>
+      <c r="H3" t="n">
         <v>0.506</v>
       </c>
-      <c r="G3" t="n">
+      <c r="I3" t="n">
         <v>0.322</v>
       </c>
-      <c r="H3" t="n">
+      <c r="J3" t="n">
         <v>0.270712906666334</v>
       </c>
-      <c r="I3" t="n">
+      <c r="K3" t="n">
         <v>0.880517357628651</v>
       </c>
-      <c r="J3" t="n">
+      <c r="L3" t="n">
         <v>0.309990520594351</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" t="s">
         <v>62</v>
-      </c>
-      <c r="C4" t="s">
-        <v>60</v>
       </c>
       <c r="D4" t="n">
         <v>218.4</v>
       </c>
       <c r="E4" t="n">
+        <v>0.362269389200314</v>
+      </c>
+      <c r="F4" t="n">
         <v>245.4</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
+        <v>0.0149326080218231</v>
+      </c>
+      <c r="H4" t="n">
         <v>0.542</v>
       </c>
-      <c r="G4" t="n">
+      <c r="I4" t="n">
         <v>0.307</v>
       </c>
-      <c r="H4" t="n">
+      <c r="J4" t="n">
         <v>0.339921366849096</v>
       </c>
-      <c r="I4" t="n">
+      <c r="K4" t="n">
         <v>0.824553438127845</v>
       </c>
-      <c r="J4" t="n">
+      <c r="L4" t="n">
         <v>0.29777176529434</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D5" t="n">
         <v>225.6</v>
       </c>
       <c r="E5" t="n">
+        <v>0.0101114805243965</v>
+      </c>
+      <c r="F5" t="n">
         <v>248.1</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
+        <v>0.00394846099478588</v>
+      </c>
+      <c r="H5" t="n">
         <v>0.442</v>
       </c>
-      <c r="G5" t="n">
+      <c r="I5" t="n">
         <v>0.253</v>
       </c>
-      <c r="H5" t="n">
+      <c r="J5" t="n">
         <v>0.252780623700835</v>
       </c>
-      <c r="I5" t="n">
+      <c r="K5" t="n">
         <v>0.931849378942401</v>
       </c>
-      <c r="J5" t="n">
+      <c r="L5" t="n">
         <v>0.323013483263546</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D6" t="n">
         <v>221.6</v>
       </c>
       <c r="E6" t="n">
+        <v>0.0730842900050484</v>
+      </c>
+      <c r="F6" t="n">
         <v>239.6</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
+        <v>0.270362348894944</v>
+      </c>
+      <c r="H6" t="n">
         <v>0.442</v>
       </c>
-      <c r="G6" t="n">
+      <c r="I6" t="n">
         <v>0.254</v>
       </c>
-      <c r="H6" t="n">
+      <c r="J6" t="n">
         <v>0.252287909332907</v>
       </c>
-      <c r="I6" t="n">
+      <c r="K6" t="n">
         <v>0.933847193844437</v>
       </c>
-      <c r="J6" t="n">
+      <c r="L6" t="n">
         <v>0.322867004307088</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D7" t="n">
         <v>220.1</v>
       </c>
       <c r="E7" t="n">
+        <v>0.156128467145257</v>
+      </c>
+      <c r="F7" t="n">
         <v>247.1</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
+        <v>0.00643555671671473</v>
+      </c>
+      <c r="H7" t="n">
         <v>0.511</v>
       </c>
-      <c r="G7" t="n">
+      <c r="I7" t="n">
         <v>0.329</v>
       </c>
-      <c r="H7" t="n">
+      <c r="J7" t="n">
         <v>0.272155096268899</v>
       </c>
-      <c r="I7" t="n">
+      <c r="K7" t="n">
         <v>0.874876231377499</v>
       </c>
-      <c r="J7" t="n">
+      <c r="L7" t="n">
         <v>0.307314521780736</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D8" t="n">
         <v>222.1</v>
       </c>
       <c r="E8" t="n">
+        <v>0.0584384593621647</v>
+      </c>
+      <c r="F8" t="n">
         <v>237.8</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
+        <v>0.665388781996849</v>
+      </c>
+      <c r="H8" t="n">
         <v>0.37</v>
       </c>
-      <c r="G8" t="n">
+      <c r="I8" t="n">
         <v>0.088</v>
       </c>
-      <c r="H8" t="n">
+      <c r="J8" t="n">
         <v>0.308813845572371</v>
       </c>
-      <c r="I8" t="n">
+      <c r="K8" t="n">
         <v>0.936882341333349</v>
       </c>
-      <c r="J8" t="n">
+      <c r="L8" t="n">
         <v>0.331059051431514</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D9" t="n">
         <v>110.7</v>
       </c>
       <c r="E9" t="n">
+        <v>0.0142713175128634</v>
+      </c>
+      <c r="F9" t="n">
         <v>128.3</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
+        <v>0.000223987725579265</v>
+      </c>
+      <c r="H9" t="n">
         <v>0.427</v>
       </c>
-      <c r="G9" t="n">
+      <c r="I9" t="n">
         <v>0.347</v>
       </c>
-      <c r="H9" t="n">
+      <c r="J9" t="n">
         <v>0.12264193082729</v>
       </c>
-      <c r="I9" t="n">
+      <c r="K9" t="n">
         <v>1.00977970615862</v>
       </c>
-      <c r="J9" t="n">
+      <c r="L9" t="n">
         <v>0.335976868226673</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D10" t="n">
         <v>106</v>
       </c>
       <c r="E10" t="n">
+        <v>0.147046341763083</v>
+      </c>
+      <c r="F10" t="n">
         <v>118.6</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
+        <v>0.0285747963670422</v>
+      </c>
+      <c r="H10" t="n">
         <v>0.341</v>
       </c>
-      <c r="G10" t="n">
+      <c r="I10" t="n">
         <v>0.292</v>
       </c>
-      <c r="H10" t="n">
+      <c r="J10" t="n">
         <v>0.069512358021633</v>
       </c>
-      <c r="I10" t="n">
+      <c r="K10" t="n">
         <v>1.12393872070358</v>
       </c>
-      <c r="J10" t="n">
+      <c r="L10" t="n">
         <v>0.353702412571083</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D11" t="n">
         <v>106.9</v>
       </c>
       <c r="E11" t="n">
+        <v>0.0960456146502793</v>
+      </c>
+      <c r="F11" t="n">
         <v>119.5</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
+        <v>0.0186640745201331</v>
+      </c>
+      <c r="H11" t="n">
         <v>0.313</v>
       </c>
-      <c r="G11" t="n">
+      <c r="I11" t="n">
         <v>0.271</v>
       </c>
-      <c r="H11" t="n">
+      <c r="J11" t="n">
         <v>0.0572627646077092</v>
       </c>
-      <c r="I11" t="n">
+      <c r="K11" t="n">
         <v>1.11383231952833</v>
       </c>
-      <c r="J11" t="n">
+      <c r="L11" t="n">
         <v>0.352824835342725</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D12" t="n">
         <v>102.8</v>
       </c>
       <c r="E12" t="n">
+        <v>0.742636726073774</v>
+      </c>
+      <c r="F12" t="n">
         <v>111.6</v>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
+        <v>0.952537141387246</v>
+      </c>
+      <c r="H12" t="n">
         <v>0.268</v>
       </c>
-      <c r="G12" t="n">
+      <c r="I12" t="n">
         <v>0.224</v>
       </c>
-      <c r="H12" t="n">
+      <c r="J12" t="n">
         <v>0.056048071109652</v>
       </c>
-      <c r="I12" t="n">
+      <c r="K12" t="n">
         <v>1.19677569320301</v>
       </c>
-      <c r="J12" t="n">
+      <c r="L12" t="n">
         <v>0.36408716814135</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D13" t="n">
         <v>153.1</v>
       </c>
       <c r="E13" t="n">
+        <v>0.000942088337633318</v>
+      </c>
+      <c r="F13" t="n">
         <v>182.9</v>
       </c>
-      <c r="F13" t="n">
+      <c r="G13" t="n">
+        <v>0.000000490675746961884</v>
+      </c>
+      <c r="H13" t="n">
         <v>0.527</v>
       </c>
-      <c r="G13" t="n">
+      <c r="I13" t="n">
         <v>0.199</v>
       </c>
-      <c r="H13" t="n">
+      <c r="J13" t="n">
         <v>0.409641426216089</v>
       </c>
-      <c r="I13" t="n">
+      <c r="K13" t="n">
         <v>0.70697164728988</v>
       </c>
-      <c r="J13" t="n">
+      <c r="L13" t="n">
         <v>0.229916347254973</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D14" t="n">
         <v>145.9</v>
       </c>
       <c r="E14" t="n">
+        <v>0.0336921939959352</v>
+      </c>
+      <c r="F14" t="n">
         <v>167.8</v>
       </c>
-      <c r="F14" t="n">
+      <c r="G14" t="n">
+        <v>0.000937220650941962</v>
+      </c>
+      <c r="H14" t="n">
         <v>0.521</v>
       </c>
-      <c r="G14" t="n">
+      <c r="I14" t="n">
         <v>0.195</v>
       </c>
-      <c r="H14" t="n">
+      <c r="J14" t="n">
         <v>0.405142466313655</v>
       </c>
-      <c r="I14" t="n">
+      <c r="K14" t="n">
         <v>0.710112914902594</v>
       </c>
-      <c r="J14" t="n">
+      <c r="L14" t="n">
         <v>0.231080474175141</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D15" t="n">
         <v>146.2</v>
       </c>
       <c r="E15" t="n">
+        <v>0.0289917494562144</v>
+      </c>
+      <c r="F15" t="n">
         <v>166.1</v>
       </c>
-      <c r="F15" t="n">
+      <c r="G15" t="n">
+        <v>0.00218016507203759</v>
+      </c>
+      <c r="H15" t="n">
         <v>0.5</v>
       </c>
-      <c r="G15" t="n">
+      <c r="I15" t="n">
         <v>0.174</v>
       </c>
-      <c r="H15" t="n">
+      <c r="J15" t="n">
         <v>0.394017895328747</v>
       </c>
-      <c r="I15" t="n">
+      <c r="K15" t="n">
         <v>0.734044282144376</v>
       </c>
-      <c r="J15" t="n">
+      <c r="L15" t="n">
         <v>0.23735001040535</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D16" t="n">
         <v>142.3</v>
       </c>
       <c r="E16" t="n">
+        <v>0.204393622665867</v>
+      </c>
+      <c r="F16" t="n">
         <v>158.2</v>
       </c>
-      <c r="F16" t="n">
+      <c r="G16" t="n">
+        <v>0.112327758313534</v>
+      </c>
+      <c r="H16" t="n">
         <v>0.499</v>
       </c>
-      <c r="G16" t="n">
+      <c r="I16" t="n">
         <v>0.174</v>
       </c>
-      <c r="H16" t="n">
+      <c r="J16" t="n">
         <v>0.393286214699538</v>
       </c>
-      <c r="I16" t="n">
+      <c r="K16" t="n">
         <v>0.73324439340205</v>
       </c>
-      <c r="J16" t="n">
+      <c r="L16" t="n">
         <v>0.237295448480225</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D17" t="n">
         <v>147.9</v>
       </c>
       <c r="E17" t="n">
+        <v>0.0125689310659239</v>
+      </c>
+      <c r="F17" t="n">
         <v>171.8</v>
       </c>
-      <c r="F17" t="n">
+      <c r="G17" t="n">
+        <v>0.00012933274732436</v>
+      </c>
+      <c r="H17" t="n">
         <v>0.522</v>
       </c>
-      <c r="G17" t="n">
+      <c r="I17" t="n">
         <v>0.195</v>
       </c>
-      <c r="H17" t="n">
+      <c r="J17" t="n">
         <v>0.405616901269354</v>
       </c>
-      <c r="I17" t="n">
+      <c r="K17" t="n">
         <v>0.709947971925215</v>
       </c>
-      <c r="J17" t="n">
+      <c r="L17" t="n">
         <v>0.230951400774421</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" t="s">
         <v>68</v>
       </c>
-      <c r="B18" t="s">
-        <v>66</v>
-      </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D18" t="n">
         <v>140.4</v>
       </c>
       <c r="E18" t="n">
+        <v>0.522443416391658</v>
+      </c>
+      <c r="F18" t="n">
         <v>154.4</v>
       </c>
-      <c r="F18" t="n">
+      <c r="G18" t="n">
+        <v>0.776178144031763</v>
+      </c>
+      <c r="H18" t="n">
         <v>0.485</v>
       </c>
-      <c r="G18" t="n">
+      <c r="I18" t="n">
         <v>0.147</v>
       </c>
-      <c r="H18" t="n">
+      <c r="J18" t="n">
         <v>0.396708536396551</v>
       </c>
-      <c r="I18" t="n">
+      <c r="K18" t="n">
         <v>0.732981216183524</v>
       </c>
-      <c r="J18" t="n">
+      <c r="L18" t="n">
         <v>0.238221370362628</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D19" t="n">
         <v>142.4</v>
       </c>
       <c r="E19" t="n">
+        <v>0.196967998086768</v>
+      </c>
+      <c r="F19" t="n">
         <v>158.3</v>
       </c>
-      <c r="F19" t="n">
+      <c r="G19" t="n">
+        <v>0.108246888508652</v>
+      </c>
+      <c r="H19" t="n">
         <v>0.493</v>
       </c>
-      <c r="G19" t="n">
+      <c r="I19" t="n">
         <v>0.145</v>
       </c>
-      <c r="H19" t="n">
+      <c r="J19" t="n">
         <v>0.40760856417087</v>
       </c>
-      <c r="I19" t="n">
+      <c r="K19" t="n">
         <v>0.727645208726944</v>
       </c>
-      <c r="J19" t="n">
+      <c r="L19" t="n">
         <v>0.236972613071863</v>
       </c>
     </row>
@@ -2342,27 +2462,27 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -2380,12 +2500,12 @@
         <v>0.00067</v>
       </c>
       <c r="G2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -2403,12 +2523,12 @@
         <v>0.05463</v>
       </c>
       <c r="G3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -2426,12 +2546,12 @@
         <v>0.00133</v>
       </c>
       <c r="G4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B5" t="n">
         <v>80</v>
@@ -2445,12 +2565,12 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B6" t="n">
         <v>85</v>
@@ -2464,12 +2584,12 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B7" t="n">
         <v>1</v>
@@ -2487,12 +2607,12 @@
         <v>0.00067</v>
       </c>
       <c r="G7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B8" t="n">
         <v>1</v>
@@ -2510,12 +2630,12 @@
         <v>0.00067</v>
       </c>
       <c r="G8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B9" t="n">
         <v>3</v>
@@ -2533,12 +2653,12 @@
         <v>0.22252</v>
       </c>
       <c r="G9" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B10" t="n">
         <v>71</v>
@@ -2552,12 +2672,12 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B11" t="n">
         <v>76</v>
@@ -2571,12 +2691,12 @@
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B12" t="n">
         <v>1</v>
@@ -2594,12 +2714,12 @@
         <v>0.48568</v>
       </c>
       <c r="G12" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B13" t="n">
         <v>1</v>
@@ -2617,12 +2737,12 @@
         <v>0.00133</v>
       </c>
       <c r="G13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B14" t="n">
         <v>3</v>
@@ -2640,12 +2760,12 @@
         <v>0.00067</v>
       </c>
       <c r="G14" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B15" t="n">
         <v>62</v>
@@ -2659,12 +2779,12 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B16" t="n">
         <v>67</v>
@@ -2678,7 +2798,7 @@
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2708,24 +2828,24 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B2" t="n">
         <v>1.05</v>
@@ -2740,12 +2860,12 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B3" t="n">
         <v>0.01</v>
@@ -2760,12 +2880,12 @@
         <v>0.085</v>
       </c>
       <c r="F3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B4" t="n">
         <v>0.378</v>
@@ -2780,12 +2900,12 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B5" t="n">
         <v>0.223</v>
@@ -2800,12 +2920,12 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B6" t="n">
         <v>0.444</v>
@@ -2820,12 +2940,12 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B7" t="n">
         <v>0.002</v>
@@ -2840,12 +2960,12 @@
         <v>0.753</v>
       </c>
       <c r="F7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B8" t="n">
         <v>-0.771</v>
@@ -2860,12 +2980,12 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B9" t="n">
         <v>-0.446</v>
@@ -2880,12 +3000,12 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B10" t="n">
         <v>-0.33</v>
@@ -2900,12 +3020,12 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B11" t="n">
         <v>0.542</v>
@@ -2914,12 +3034,12 @@
       <c r="D11"/>
       <c r="E11"/>
       <c r="F11" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B12" t="n">
         <v>0.307</v>
@@ -2928,12 +3048,12 @@
       <c r="D12"/>
       <c r="E12"/>
       <c r="F12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B13" t="n">
         <v>1.279</v>
@@ -2948,12 +3068,12 @@
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B14" t="n">
         <v>-0.338</v>
@@ -2968,12 +3088,12 @@
         <v>0.08</v>
       </c>
       <c r="F14" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B15" t="n">
         <v>-0.059</v>
@@ -2988,12 +3108,12 @@
         <v>0.753</v>
       </c>
       <c r="F15" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B16" t="n">
         <v>0.227</v>
@@ -3008,12 +3128,12 @@
         <v>0.19</v>
       </c>
       <c r="F16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B17" t="n">
         <v>0.232</v>
@@ -3022,12 +3142,12 @@
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B18" t="n">
         <v>0.188</v>
@@ -3036,12 +3156,12 @@
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B19" t="n">
         <v>1.033</v>
@@ -3056,12 +3176,12 @@
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B20" t="n">
         <v>-0.045</v>
@@ -3076,12 +3196,12 @@
         <v>0.694</v>
       </c>
       <c r="F20" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B21" t="n">
         <v>0.033</v>
@@ -3096,12 +3216,12 @@
         <v>0.676</v>
       </c>
       <c r="F21" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B22" t="n">
         <v>0.124</v>
@@ -3116,12 +3236,12 @@
         <v>0.131</v>
       </c>
       <c r="F22" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B23" t="n">
         <v>0.262</v>
@@ -3136,12 +3256,12 @@
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B24" t="n">
         <v>0.493</v>
@@ -3150,12 +3270,12 @@
       <c r="D24"/>
       <c r="E24"/>
       <c r="F24" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B25" t="n">
         <v>0.145</v>
@@ -3164,7 +3284,7 @@
       <c r="D25"/>
       <c r="E25"/>
       <c r="F25" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -3194,24 +3314,24 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -3231,7 +3351,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -3251,7 +3371,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -3271,7 +3391,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B5" t="n">
         <v>2</v>
@@ -3291,7 +3411,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B6" t="n">
         <v>2</v>
@@ -3311,7 +3431,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B7" t="n">
         <v>6</v>
@@ -3331,7 +3451,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B8" t="n">
         <v>2</v>
@@ -3351,7 +3471,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B9" t="n">
         <v>214</v>
@@ -3367,7 +3487,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B10" t="n">
         <v>231</v>
@@ -3414,42 +3534,42 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="I1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="K1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="L1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -3482,12 +3602,12 @@
         <v>0.00067</v>
       </c>
       <c r="L2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -3520,12 +3640,12 @@
         <v>0.09061</v>
       </c>
       <c r="L3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -3558,12 +3678,12 @@
         <v>0.00266</v>
       </c>
       <c r="L4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B5" t="n">
         <v>80</v>
@@ -3588,12 +3708,12 @@
       <c r="J5"/>
       <c r="K5"/>
       <c r="L5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B6" t="n">
         <v>85</v>
@@ -3618,12 +3738,12 @@
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B7" t="n">
         <v>3</v>
@@ -3656,12 +3776,12 @@
         <v>0.27848</v>
       </c>
       <c r="L7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B8" t="n">
         <v>1</v>
@@ -3694,12 +3814,12 @@
         <v>0.00067</v>
       </c>
       <c r="L8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B9" t="n">
         <v>1</v>
@@ -3732,12 +3852,12 @@
         <v>0.002</v>
       </c>
       <c r="L9" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B10" t="n">
         <v>71</v>
@@ -3762,12 +3882,12 @@
       <c r="J10"/>
       <c r="K10"/>
       <c r="L10" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B11" t="n">
         <v>76</v>
@@ -3792,12 +3912,12 @@
       <c r="J11"/>
       <c r="K11"/>
       <c r="L11" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B12" t="n">
         <v>3</v>
@@ -3830,12 +3950,12 @@
         <v>0.00067</v>
       </c>
       <c r="L12" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B13" t="n">
         <v>1</v>
@@ -3868,12 +3988,12 @@
         <v>0.00067</v>
       </c>
       <c r="L13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B14" t="n">
         <v>1</v>
@@ -3906,12 +4026,12 @@
         <v>0.48168</v>
       </c>
       <c r="L14" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B15" t="n">
         <v>62</v>
@@ -3936,12 +4056,12 @@
       <c r="J15"/>
       <c r="K15"/>
       <c r="L15" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B16" t="n">
         <v>67</v>
@@ -3966,7 +4086,7 @@
       <c r="J16"/>
       <c r="K16"/>
       <c r="L16" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -3986,10 +4106,10 @@
     <col min="1" max="1" width="71.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="8.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="5.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="6.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="14.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="11.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="6.71" hidden="0" customWidth="1"/>
     <col min="6" max="6" width="11.71" hidden="0" customWidth="1"/>
-    <col min="7" max="7" width="11.71" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="14.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4020,323 +4140,395 @@
       <c r="I1" t="s">
         <v>57</v>
       </c>
+      <c r="J1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C2" t="n">
         <v>923.1</v>
       </c>
       <c r="D2" t="n">
+        <v>0.000000000356173661287928</v>
+      </c>
+      <c r="E2" t="n">
         <v>1219.4</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
+        <v>0.00000000000000000000000000000000000000000000000000000000000000106026935087453</v>
+      </c>
+      <c r="G2" t="n">
         <v>0.43</v>
       </c>
-      <c r="F2" t="n">
+      <c r="H2" t="n">
         <v>0.318</v>
       </c>
-      <c r="G2" t="n">
+      <c r="I2" t="n">
         <v>0.163808918846475</v>
       </c>
-      <c r="H2" t="n">
+      <c r="J2" t="n">
         <v>0.884761957169536</v>
       </c>
-      <c r="I2" t="n">
+      <c r="K2" t="n">
         <v>0.445413568051623</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C3" t="n">
         <v>904.6</v>
       </c>
       <c r="D3" t="n">
+        <v>0.00000356476632034088</v>
+      </c>
+      <c r="E3" t="n">
         <v>1086.1</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
+        <v>0.0000000000000000000000000000000000907895747647671</v>
+      </c>
+      <c r="G3" t="n">
         <v>0.338</v>
       </c>
-      <c r="F3" t="n">
+      <c r="H3" t="n">
         <v>0.225</v>
       </c>
-      <c r="G3" t="n">
+      <c r="I3" t="n">
         <v>0.144860307744428</v>
       </c>
-      <c r="H3" t="n">
+      <c r="J3" t="n">
         <v>0.948916968928776</v>
       </c>
-      <c r="I3" t="n">
+      <c r="K3" t="n">
         <v>0.477395026003451</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C4" t="n">
         <v>890.2</v>
       </c>
       <c r="D4" t="n">
+        <v>0.0049751824323713</v>
+      </c>
+      <c r="E4" t="n">
         <v>964.2</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
+        <v>0.0000000267012839066756</v>
+      </c>
+      <c r="G4" t="n">
         <v>0.222</v>
       </c>
-      <c r="F4" t="n">
+      <c r="H4" t="n">
         <v>0.113</v>
       </c>
-      <c r="G4" t="n">
+      <c r="I4" t="n">
         <v>0.122648785796666</v>
       </c>
-      <c r="H4" t="n">
+      <c r="J4" t="n">
         <v>1.00853413602528</v>
       </c>
-      <c r="I4" t="n">
+      <c r="K4" t="n">
         <v>0.508488836608921</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C5" t="n">
         <v>881.2</v>
       </c>
       <c r="D5" t="n">
+        <v>0.436931983172524</v>
+      </c>
+      <c r="E5" t="n">
         <v>929.4</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
+        <v>0.999999973298655</v>
+      </c>
+      <c r="G5" t="n">
         <v>0.205</v>
       </c>
-      <c r="F5" t="n">
+      <c r="H5" t="n">
         <v>0.095</v>
       </c>
-      <c r="G5" t="n">
+      <c r="I5" t="n">
         <v>0.121607431312658</v>
       </c>
-      <c r="H5" t="n">
+      <c r="J5" t="n">
         <v>1.01492820585159</v>
       </c>
-      <c r="I5" t="n">
+      <c r="K5" t="n">
         <v>0.513921291826242</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C6" t="n">
         <v>902.1</v>
       </c>
       <c r="D6" t="n">
+        <v>0.000012830993710202</v>
+      </c>
+      <c r="E6" t="n">
         <v>1124.3</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
+        <v>0.000000000000000000000000000000000000000000464876516436139</v>
+      </c>
+      <c r="G6" t="n">
         <v>0.391</v>
       </c>
-      <c r="F6" t="n">
+      <c r="H6" t="n">
         <v>0.279</v>
       </c>
-      <c r="G6" t="n">
+      <c r="I6" t="n">
         <v>0.155601596236995</v>
       </c>
-      <c r="H6" t="n">
+      <c r="J6" t="n">
         <v>0.913117790532039</v>
       </c>
-      <c r="I6" t="n">
+      <c r="K6" t="n">
         <v>0.45931696402324</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C7" t="n">
         <v>890.2</v>
       </c>
       <c r="D7" t="n">
+        <v>0.00479961344622744</v>
+      </c>
+      <c r="E7" t="n">
         <v>990.2</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
+        <v>0.0000000000000604040943674256</v>
+      </c>
+      <c r="G7" t="n">
         <v>0.235</v>
       </c>
-      <c r="F7" t="n">
+      <c r="H7" t="n">
         <v>0.093</v>
       </c>
-      <c r="G7" t="n">
+      <c r="I7" t="n">
         <v>0.157143513626403</v>
       </c>
-      <c r="H7" t="n">
+      <c r="J7" t="n">
         <v>0.982507593585701</v>
       </c>
-      <c r="I7" t="n">
+      <c r="K7" t="n">
         <v>0.505803686093402</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C8" t="n">
         <v>902.1</v>
       </c>
       <c r="D8" t="n">
+        <v>0.0000128309937101984</v>
+      </c>
+      <c r="E8" t="n">
         <v>1124.3</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
+        <v>0.000000000000000000000000000000000000000000464876516436033</v>
+      </c>
+      <c r="G8" t="n">
         <v>0.391</v>
       </c>
-      <c r="F8" t="n">
+      <c r="H8" t="n">
         <v>0.279</v>
       </c>
-      <c r="G8" t="n">
+      <c r="I8" t="n">
         <v>0.155601596236034</v>
       </c>
-      <c r="H8" t="n">
+      <c r="J8" t="n">
         <v>0.913117790532143</v>
       </c>
-      <c r="I8" t="n">
+      <c r="K8" t="n">
         <v>0.459316964023365</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C9" t="n">
         <v>902.1</v>
       </c>
       <c r="D9" t="n">
+        <v>0.0000128309937101984</v>
+      </c>
+      <c r="E9" t="n">
         <v>1124.3</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
+        <v>0.000000000000000000000000000000000000000000464876516436033</v>
+      </c>
+      <c r="G9" t="n">
         <v>0.391</v>
       </c>
-      <c r="F9" t="n">
+      <c r="H9" t="n">
         <v>0.279</v>
       </c>
-      <c r="G9" t="n">
+      <c r="I9" t="n">
         <v>0.155601596236034</v>
       </c>
-      <c r="H9" t="n">
+      <c r="J9" t="n">
         <v>0.913117790532143</v>
       </c>
-      <c r="I9" t="n">
+      <c r="K9" t="n">
         <v>0.459316964023365</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C10" t="n">
         <v>882</v>
       </c>
       <c r="D10" t="n">
+        <v>0.302098653514401</v>
+      </c>
+      <c r="E10" t="n">
         <v>1000.5</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
+        <v>0.000000000000000361974667895156</v>
+      </c>
+      <c r="G10" t="n">
         <v>0.28</v>
       </c>
-      <c r="F10" t="n">
+      <c r="H10" t="n">
         <v>0.139</v>
       </c>
-      <c r="G10" t="n">
+      <c r="I10" t="n">
         <v>0.163720683028945</v>
       </c>
-      <c r="H10" t="n">
+      <c r="J10" t="n">
         <v>0.950425796937665</v>
       </c>
-      <c r="I10" t="n">
+      <c r="K10" t="n">
         <v>0.488694314791684</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C11" t="n">
         <v>883.5</v>
       </c>
       <c r="D11" t="n">
+        <v>0.138174298373614</v>
+      </c>
+      <c r="E11" t="n">
         <v>1005.7</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
+        <v>0.0000000000000000259830728679035</v>
+      </c>
+      <c r="G11" t="n">
         <v>0.282</v>
       </c>
-      <c r="F11" t="n">
+      <c r="H11" t="n">
         <v>0.144</v>
       </c>
-      <c r="G11" t="n">
+      <c r="I11" t="n">
         <v>0.161404588856711</v>
       </c>
-      <c r="H11" t="n">
+      <c r="J11" t="n">
         <v>0.950207028246836</v>
       </c>
-      <c r="I11" t="n">
+      <c r="K11" t="n">
         <v>0.488554386709045</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C12" t="n">
         <v>883.9</v>
       </c>
       <c r="D12" t="n">
+        <v>0.112978210957238</v>
+      </c>
+      <c r="E12" t="n">
         <v>1024.7</v>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
+        <v>0.00000000000000000000202268013528013</v>
+      </c>
+      <c r="G12" t="n">
         <v>0.323</v>
       </c>
-      <c r="F12" t="n">
+      <c r="H12" t="n">
         <v>0.212</v>
       </c>
-      <c r="G12" t="n">
+      <c r="I12" t="n">
         <v>0.140275722020262</v>
       </c>
-      <c r="H12" t="n">
+      <c r="J12" t="n">
         <v>0.935551604873005</v>
       </c>
-      <c r="I12" t="n">
+      <c r="K12" t="n">
         <v>0.476818047697685</v>
       </c>
     </row>
@@ -4367,21 +4559,21 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B2" t="n">
         <v>0.8</v>
@@ -4398,7 +4590,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B3" t="n">
         <v>0.199</v>
@@ -4415,7 +4607,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B4" t="n">
         <v>-0.357</v>
@@ -4432,7 +4624,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B5" t="n">
         <v>-0.515</v>
@@ -4449,7 +4641,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B6" t="n">
         <v>0.234</v>
@@ -4466,7 +4658,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B7" t="n">
         <v>0.005</v>
@@ -4483,7 +4675,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B8" t="n">
         <v>-0.021</v>
@@ -4500,7 +4692,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B9" t="n">
         <v>-0.252</v>
@@ -4517,7 +4709,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B10" t="n">
         <v>0.223</v>
@@ -4534,7 +4726,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B11" t="n">
         <v>0.685</v>
@@ -4551,7 +4743,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B12" t="n">
         <v>-0.088</v>
@@ -4568,7 +4760,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B13" t="n">
         <v>-0.568</v>
@@ -4585,7 +4777,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B14" t="n">
         <v>-0.45</v>
@@ -4602,7 +4794,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B15" t="n">
         <v>0.051</v>
@@ -4619,7 +4811,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B16" t="n">
         <v>-0.154</v>
@@ -4636,7 +4828,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B17" t="n">
         <v>0.236</v>
@@ -4653,7 +4845,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B18" t="n">
         <v>0.072</v>
@@ -4670,7 +4862,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B19" t="n">
         <v>0.608</v>
@@ -4687,7 +4879,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B20" t="n">
         <v>-0.299</v>
@@ -4704,7 +4896,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B21" t="n">
         <v>0.134</v>
@@ -4721,7 +4913,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B22" t="n">
         <v>0.564</v>
@@ -4738,7 +4930,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B23" t="n">
         <v>0.524</v>
@@ -4755,7 +4947,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B24" t="n">
         <v>0.362</v>
@@ -4772,7 +4964,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B25" t="n">
         <v>0.673</v>
@@ -4789,7 +4981,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B26" t="n">
         <v>-0.179</v>
@@ -4806,7 +4998,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B27" t="n">
         <v>-0.18</v>
@@ -4823,7 +5015,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B28" t="n">
         <v>-0.482</v>
@@ -4840,7 +5032,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B29" t="n">
         <v>-0.89</v>
@@ -4857,7 +5049,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B30" t="n">
         <v>0.189</v>
@@ -4874,7 +5066,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B31" t="n">
         <v>-0.607</v>
@@ -4891,7 +5083,7 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B32" t="n">
         <v>0.28</v>
@@ -4902,7 +5094,7 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B33" t="n">
         <v>0.139</v>

</xml_diff>

<commit_message>
reran all code, no major changes
</commit_message>
<xml_diff>
--- a/Data/Supplemental/Supplemental_Tables.xlsx
+++ b/Data/Supplemental/Supplemental_Tables.xlsx
@@ -3366,7 +3366,7 @@
         <v>2.87</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0966</v>
+        <v>0.09927</v>
       </c>
     </row>
     <row r="4">
@@ -3386,7 +3386,7 @@
         <v>9.61</v>
       </c>
       <c r="F4" t="n">
-        <v>0.00133</v>
+        <v>0.002</v>
       </c>
     </row>
     <row r="5">
@@ -3446,7 +3446,7 @@
         <v>2.51</v>
       </c>
       <c r="F7" t="n">
-        <v>0.02065</v>
+        <v>0.01932</v>
       </c>
     </row>
     <row r="8">
@@ -3466,7 +3466,7 @@
         <v>6.39</v>
       </c>
       <c r="F8" t="n">
-        <v>0.00266</v>
+        <v>0.002</v>
       </c>
     </row>
     <row r="9">
@@ -3584,7 +3584,7 @@
         <v>0.55</v>
       </c>
       <c r="F2" t="n">
-        <v>0.77615</v>
+        <v>0.77548</v>
       </c>
       <c r="G2" t="n">
         <v>3</v>
@@ -3758,7 +3758,7 @@
         <v>1.23</v>
       </c>
       <c r="F7" t="n">
-        <v>0.26382</v>
+        <v>0.26183</v>
       </c>
       <c r="G7" t="n">
         <v>3</v>
@@ -3773,7 +3773,7 @@
         <v>1.31</v>
       </c>
       <c r="K7" t="n">
-        <v>0.27848</v>
+        <v>0.27915</v>
       </c>
       <c r="L7" t="s">
         <v>84</v>
@@ -3834,7 +3834,7 @@
         <v>1.75</v>
       </c>
       <c r="F9" t="n">
-        <v>0.17255</v>
+        <v>0.17388</v>
       </c>
       <c r="G9" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
updated supplemental figure numbering
</commit_message>
<xml_diff>
--- a/Data/Supplemental/Supplemental_Tables.xlsx
+++ b/Data/Supplemental/Supplemental_Tables.xlsx
@@ -3366,7 +3366,7 @@
         <v>2.87</v>
       </c>
       <c r="F3" t="n">
-        <v>0.09927</v>
+        <v>0.0966</v>
       </c>
     </row>
     <row r="4">
@@ -3386,7 +3386,7 @@
         <v>9.61</v>
       </c>
       <c r="F4" t="n">
-        <v>0.002</v>
+        <v>0.00133</v>
       </c>
     </row>
     <row r="5">
@@ -3446,7 +3446,7 @@
         <v>2.51</v>
       </c>
       <c r="F7" t="n">
-        <v>0.01932</v>
+        <v>0.02065</v>
       </c>
     </row>
     <row r="8">
@@ -3466,7 +3466,7 @@
         <v>6.39</v>
       </c>
       <c r="F8" t="n">
-        <v>0.002</v>
+        <v>0.00266</v>
       </c>
     </row>
     <row r="9">
@@ -3584,7 +3584,7 @@
         <v>0.55</v>
       </c>
       <c r="F2" t="n">
-        <v>0.77548</v>
+        <v>0.77615</v>
       </c>
       <c r="G2" t="n">
         <v>3</v>
@@ -3758,7 +3758,7 @@
         <v>1.23</v>
       </c>
       <c r="F7" t="n">
-        <v>0.26183</v>
+        <v>0.26382</v>
       </c>
       <c r="G7" t="n">
         <v>3</v>
@@ -3773,7 +3773,7 @@
         <v>1.31</v>
       </c>
       <c r="K7" t="n">
-        <v>0.27915</v>
+        <v>0.27848</v>
       </c>
       <c r="L7" t="s">
         <v>84</v>
@@ -3834,7 +3834,7 @@
         <v>1.75</v>
       </c>
       <c r="F9" t="n">
-        <v>0.17388</v>
+        <v>0.17255</v>
       </c>
       <c r="G9" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
added SST figure to supps
</commit_message>
<xml_diff>
--- a/Data/Supplemental/Supplemental_Tables.xlsx
+++ b/Data/Supplemental/Supplemental_Tables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="137">
   <si>
     <t xml:space="preserve">group</t>
   </si>
@@ -178,13 +178,7 @@
     <t xml:space="preserve">AIC</t>
   </si>
   <si>
-    <t xml:space="preserve">AIC_wt</t>
-  </si>
-  <si>
     <t xml:space="preserve">BIC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BIC_wt</t>
   </si>
   <si>
     <t xml:space="preserve">Conditional R2</t>
@@ -1707,8 +1701,8 @@
     <col min="2" max="2" width="65.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="8.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="5.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="11.71" hidden="0" customWidth="1"/>
-    <col min="6" max="6" width="5.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="5.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="14.71" hidden="0" customWidth="1"/>
     <col min="7" max="7" width="11.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1743,694 +1737,580 @@
       <c r="J1" t="s">
         <v>57</v>
       </c>
-      <c r="K1" t="s">
-        <v>58</v>
-      </c>
-      <c r="L1" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s">
         <v>60</v>
-      </c>
-      <c r="B2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" t="s">
-        <v>62</v>
       </c>
       <c r="D2" t="n">
         <v>223.2</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0332206990579833</v>
+        <v>259.2</v>
       </c>
       <c r="F2" t="n">
-        <v>259.2</v>
+        <v>0.545</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0000152578956652519</v>
+        <v>0.366</v>
       </c>
       <c r="H2" t="n">
-        <v>0.545</v>
+        <v>0.282067343982829</v>
       </c>
       <c r="I2" t="n">
-        <v>0.366</v>
+        <v>0.855828398264632</v>
       </c>
       <c r="J2" t="n">
-        <v>0.282067343982829</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.855828398264632</v>
-      </c>
-      <c r="L2" t="n">
         <v>0.294010052236142</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" t="s">
         <v>60</v>
-      </c>
-      <c r="B3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" t="s">
-        <v>62</v>
       </c>
       <c r="D3" t="n">
         <v>218.8</v>
       </c>
       <c r="E3" t="n">
-        <v>0.306747214704836</v>
+        <v>243.5</v>
       </c>
       <c r="F3" t="n">
-        <v>243.5</v>
+        <v>0.506</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0389169854792176</v>
+        <v>0.322</v>
       </c>
       <c r="H3" t="n">
-        <v>0.506</v>
+        <v>0.270712906666334</v>
       </c>
       <c r="I3" t="n">
-        <v>0.322</v>
+        <v>0.880517357628651</v>
       </c>
       <c r="J3" t="n">
-        <v>0.270712906666334</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.880517357628651</v>
-      </c>
-      <c r="L3" t="n">
         <v>0.309990520594351</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
         <v>60</v>
-      </c>
-      <c r="B4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" t="s">
-        <v>62</v>
       </c>
       <c r="D4" t="n">
         <v>218.4</v>
       </c>
       <c r="E4" t="n">
-        <v>0.362269389200314</v>
+        <v>245.4</v>
       </c>
       <c r="F4" t="n">
-        <v>245.4</v>
+        <v>0.542</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0149326080218231</v>
+        <v>0.307</v>
       </c>
       <c r="H4" t="n">
-        <v>0.542</v>
+        <v>0.339921366849096</v>
       </c>
       <c r="I4" t="n">
-        <v>0.307</v>
+        <v>0.824553438127845</v>
       </c>
       <c r="J4" t="n">
-        <v>0.339921366849096</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.824553438127845</v>
-      </c>
-      <c r="L4" t="n">
         <v>0.29777176529434</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
         <v>60</v>
-      </c>
-      <c r="B5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" t="s">
-        <v>62</v>
       </c>
       <c r="D5" t="n">
         <v>225.6</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0101114805243965</v>
+        <v>248.1</v>
       </c>
       <c r="F5" t="n">
-        <v>248.1</v>
+        <v>0.442</v>
       </c>
       <c r="G5" t="n">
-        <v>0.00394846099478588</v>
+        <v>0.253</v>
       </c>
       <c r="H5" t="n">
-        <v>0.442</v>
+        <v>0.252780623700835</v>
       </c>
       <c r="I5" t="n">
-        <v>0.253</v>
+        <v>0.931849378942401</v>
       </c>
       <c r="J5" t="n">
-        <v>0.252780623700835</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0.931849378942401</v>
-      </c>
-      <c r="L5" t="n">
         <v>0.323013483263546</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" t="s">
         <v>60</v>
-      </c>
-      <c r="B6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" t="s">
-        <v>62</v>
       </c>
       <c r="D6" t="n">
         <v>221.6</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0730842900050484</v>
+        <v>239.6</v>
       </c>
       <c r="F6" t="n">
-        <v>239.6</v>
+        <v>0.442</v>
       </c>
       <c r="G6" t="n">
-        <v>0.270362348894944</v>
+        <v>0.254</v>
       </c>
       <c r="H6" t="n">
-        <v>0.442</v>
+        <v>0.252287909332907</v>
       </c>
       <c r="I6" t="n">
-        <v>0.254</v>
+        <v>0.933847193844437</v>
       </c>
       <c r="J6" t="n">
-        <v>0.252287909332907</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0.933847193844437</v>
-      </c>
-      <c r="L6" t="n">
         <v>0.322867004307088</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" t="s">
         <v>60</v>
-      </c>
-      <c r="B7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7" t="s">
-        <v>62</v>
       </c>
       <c r="D7" t="n">
         <v>220.1</v>
       </c>
       <c r="E7" t="n">
-        <v>0.156128467145257</v>
+        <v>247.1</v>
       </c>
       <c r="F7" t="n">
-        <v>247.1</v>
+        <v>0.511</v>
       </c>
       <c r="G7" t="n">
-        <v>0.00643555671671473</v>
+        <v>0.329</v>
       </c>
       <c r="H7" t="n">
-        <v>0.511</v>
+        <v>0.272155096268899</v>
       </c>
       <c r="I7" t="n">
-        <v>0.329</v>
+        <v>0.874876231377499</v>
       </c>
       <c r="J7" t="n">
-        <v>0.272155096268899</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.874876231377499</v>
-      </c>
-      <c r="L7" t="n">
         <v>0.307314521780736</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" t="s">
         <v>60</v>
-      </c>
-      <c r="B8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" t="s">
-        <v>62</v>
       </c>
       <c r="D8" t="n">
         <v>222.1</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0584384593621647</v>
+        <v>237.8</v>
       </c>
       <c r="F8" t="n">
-        <v>237.8</v>
+        <v>0.37</v>
       </c>
       <c r="G8" t="n">
-        <v>0.665388781996849</v>
+        <v>0.088</v>
       </c>
       <c r="H8" t="n">
-        <v>0.37</v>
+        <v>0.308813845572371</v>
       </c>
       <c r="I8" t="n">
-        <v>0.088</v>
+        <v>0.936882341333349</v>
       </c>
       <c r="J8" t="n">
-        <v>0.308813845572371</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.936882341333349</v>
-      </c>
-      <c r="L8" t="n">
         <v>0.331059051431514</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D9" t="n">
         <v>110.7</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0142713175128634</v>
+        <v>128.3</v>
       </c>
       <c r="F9" t="n">
-        <v>128.3</v>
+        <v>0.427</v>
       </c>
       <c r="G9" t="n">
-        <v>0.000223987725579265</v>
+        <v>0.347</v>
       </c>
       <c r="H9" t="n">
-        <v>0.427</v>
+        <v>0.12264193082729</v>
       </c>
       <c r="I9" t="n">
-        <v>0.347</v>
+        <v>1.00977970615862</v>
       </c>
       <c r="J9" t="n">
-        <v>0.12264193082729</v>
-      </c>
-      <c r="K9" t="n">
-        <v>1.00977970615862</v>
-      </c>
-      <c r="L9" t="n">
         <v>0.335976868226673</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D10" t="n">
         <v>106</v>
       </c>
       <c r="E10" t="n">
-        <v>0.147046341763083</v>
+        <v>118.6</v>
       </c>
       <c r="F10" t="n">
-        <v>118.6</v>
+        <v>0.341</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0285747963670422</v>
+        <v>0.292</v>
       </c>
       <c r="H10" t="n">
-        <v>0.341</v>
+        <v>0.069512358021633</v>
       </c>
       <c r="I10" t="n">
-        <v>0.292</v>
+        <v>1.12393872070358</v>
       </c>
       <c r="J10" t="n">
-        <v>0.069512358021633</v>
-      </c>
-      <c r="K10" t="n">
-        <v>1.12393872070358</v>
-      </c>
-      <c r="L10" t="n">
         <v>0.353702412571083</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D11" t="n">
         <v>106.9</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0960456146502793</v>
+        <v>119.5</v>
       </c>
       <c r="F11" t="n">
-        <v>119.5</v>
+        <v>0.313</v>
       </c>
       <c r="G11" t="n">
-        <v>0.0186640745201331</v>
+        <v>0.271</v>
       </c>
       <c r="H11" t="n">
-        <v>0.313</v>
+        <v>0.0572627646077092</v>
       </c>
       <c r="I11" t="n">
-        <v>0.271</v>
+        <v>1.11383231952833</v>
       </c>
       <c r="J11" t="n">
-        <v>0.0572627646077092</v>
-      </c>
-      <c r="K11" t="n">
-        <v>1.11383231952833</v>
-      </c>
-      <c r="L11" t="n">
         <v>0.352824835342725</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D12" t="n">
         <v>102.8</v>
       </c>
       <c r="E12" t="n">
-        <v>0.742636726073774</v>
+        <v>111.6</v>
       </c>
       <c r="F12" t="n">
-        <v>111.6</v>
+        <v>0.268</v>
       </c>
       <c r="G12" t="n">
-        <v>0.952537141387246</v>
+        <v>0.224</v>
       </c>
       <c r="H12" t="n">
-        <v>0.268</v>
+        <v>0.056048071109652</v>
       </c>
       <c r="I12" t="n">
-        <v>0.224</v>
+        <v>1.19677569320301</v>
       </c>
       <c r="J12" t="n">
-        <v>0.056048071109652</v>
-      </c>
-      <c r="K12" t="n">
-        <v>1.19677569320301</v>
-      </c>
-      <c r="L12" t="n">
         <v>0.36408716814135</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D13" t="n">
         <v>153.1</v>
       </c>
       <c r="E13" t="n">
-        <v>0.000942088337633318</v>
+        <v>182.9</v>
       </c>
       <c r="F13" t="n">
-        <v>182.9</v>
+        <v>0.527</v>
       </c>
       <c r="G13" t="n">
-        <v>0.000000490675746961884</v>
+        <v>0.199</v>
       </c>
       <c r="H13" t="n">
-        <v>0.527</v>
+        <v>0.409641426216089</v>
       </c>
       <c r="I13" t="n">
-        <v>0.199</v>
+        <v>0.70697164728988</v>
       </c>
       <c r="J13" t="n">
-        <v>0.409641426216089</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0.70697164728988</v>
-      </c>
-      <c r="L13" t="n">
         <v>0.229916347254973</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D14" t="n">
         <v>145.9</v>
       </c>
       <c r="E14" t="n">
-        <v>0.0336921939959352</v>
+        <v>167.8</v>
       </c>
       <c r="F14" t="n">
-        <v>167.8</v>
+        <v>0.521</v>
       </c>
       <c r="G14" t="n">
-        <v>0.000937220650941962</v>
+        <v>0.195</v>
       </c>
       <c r="H14" t="n">
-        <v>0.521</v>
+        <v>0.405142466313655</v>
       </c>
       <c r="I14" t="n">
-        <v>0.195</v>
+        <v>0.710112914902594</v>
       </c>
       <c r="J14" t="n">
-        <v>0.405142466313655</v>
-      </c>
-      <c r="K14" t="n">
-        <v>0.710112914902594</v>
-      </c>
-      <c r="L14" t="n">
         <v>0.231080474175141</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D15" t="n">
         <v>146.2</v>
       </c>
       <c r="E15" t="n">
-        <v>0.0289917494562144</v>
+        <v>166.1</v>
       </c>
       <c r="F15" t="n">
-        <v>166.1</v>
+        <v>0.5</v>
       </c>
       <c r="G15" t="n">
-        <v>0.00218016507203759</v>
+        <v>0.174</v>
       </c>
       <c r="H15" t="n">
-        <v>0.5</v>
+        <v>0.394017895328747</v>
       </c>
       <c r="I15" t="n">
-        <v>0.174</v>
+        <v>0.734044282144376</v>
       </c>
       <c r="J15" t="n">
-        <v>0.394017895328747</v>
-      </c>
-      <c r="K15" t="n">
-        <v>0.734044282144376</v>
-      </c>
-      <c r="L15" t="n">
         <v>0.23735001040535</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D16" t="n">
         <v>142.3</v>
       </c>
       <c r="E16" t="n">
-        <v>0.204393622665867</v>
+        <v>158.2</v>
       </c>
       <c r="F16" t="n">
-        <v>158.2</v>
+        <v>0.499</v>
       </c>
       <c r="G16" t="n">
-        <v>0.112327758313534</v>
+        <v>0.174</v>
       </c>
       <c r="H16" t="n">
-        <v>0.499</v>
+        <v>0.393286214699538</v>
       </c>
       <c r="I16" t="n">
-        <v>0.174</v>
+        <v>0.73324439340205</v>
       </c>
       <c r="J16" t="n">
-        <v>0.393286214699538</v>
-      </c>
-      <c r="K16" t="n">
-        <v>0.73324439340205</v>
-      </c>
-      <c r="L16" t="n">
         <v>0.237295448480225</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D17" t="n">
         <v>147.9</v>
       </c>
       <c r="E17" t="n">
-        <v>0.0125689310659239</v>
+        <v>171.8</v>
       </c>
       <c r="F17" t="n">
-        <v>171.8</v>
+        <v>0.522</v>
       </c>
       <c r="G17" t="n">
-        <v>0.00012933274732436</v>
+        <v>0.195</v>
       </c>
       <c r="H17" t="n">
-        <v>0.522</v>
+        <v>0.405616901269354</v>
       </c>
       <c r="I17" t="n">
-        <v>0.195</v>
+        <v>0.709947971925215</v>
       </c>
       <c r="J17" t="n">
-        <v>0.405616901269354</v>
-      </c>
-      <c r="K17" t="n">
-        <v>0.709947971925215</v>
-      </c>
-      <c r="L17" t="n">
         <v>0.230951400774421</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D18" t="n">
         <v>140.4</v>
       </c>
       <c r="E18" t="n">
-        <v>0.522443416391658</v>
+        <v>154.4</v>
       </c>
       <c r="F18" t="n">
-        <v>154.4</v>
+        <v>0.485</v>
       </c>
       <c r="G18" t="n">
-        <v>0.776178144031763</v>
+        <v>0.147</v>
       </c>
       <c r="H18" t="n">
-        <v>0.485</v>
+        <v>0.396708536396551</v>
       </c>
       <c r="I18" t="n">
-        <v>0.147</v>
+        <v>0.732981216183524</v>
       </c>
       <c r="J18" t="n">
-        <v>0.396708536396551</v>
-      </c>
-      <c r="K18" t="n">
-        <v>0.732981216183524</v>
-      </c>
-      <c r="L18" t="n">
         <v>0.238221370362628</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D19" t="n">
         <v>142.4</v>
       </c>
       <c r="E19" t="n">
-        <v>0.196967998086768</v>
+        <v>158.3</v>
       </c>
       <c r="F19" t="n">
-        <v>158.3</v>
+        <v>0.493</v>
       </c>
       <c r="G19" t="n">
-        <v>0.108246888508652</v>
+        <v>0.145</v>
       </c>
       <c r="H19" t="n">
-        <v>0.493</v>
+        <v>0.40760856417087</v>
       </c>
       <c r="I19" t="n">
-        <v>0.145</v>
+        <v>0.727645208726944</v>
       </c>
       <c r="J19" t="n">
-        <v>0.40760856417087</v>
-      </c>
-      <c r="K19" t="n">
-        <v>0.727645208726944</v>
-      </c>
-      <c r="L19" t="n">
         <v>0.236972613071863</v>
       </c>
     </row>
@@ -2462,27 +2342,27 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
         <v>72</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>73</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>74</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>75</v>
-      </c>
-      <c r="F1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -2500,12 +2380,12 @@
         <v>0.00067</v>
       </c>
       <c r="G2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -2523,12 +2403,12 @@
         <v>0.05463</v>
       </c>
       <c r="G3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -2546,12 +2426,12 @@
         <v>0.00133</v>
       </c>
       <c r="G4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B5" t="n">
         <v>80</v>
@@ -2565,12 +2445,12 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B6" t="n">
         <v>85</v>
@@ -2584,12 +2464,12 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B7" t="n">
         <v>1</v>
@@ -2607,12 +2487,12 @@
         <v>0.00067</v>
       </c>
       <c r="G7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B8" t="n">
         <v>1</v>
@@ -2630,12 +2510,12 @@
         <v>0.00067</v>
       </c>
       <c r="G8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B9" t="n">
         <v>3</v>
@@ -2653,12 +2533,12 @@
         <v>0.22252</v>
       </c>
       <c r="G9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B10" t="n">
         <v>71</v>
@@ -2672,12 +2552,12 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B11" t="n">
         <v>76</v>
@@ -2691,12 +2571,12 @@
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B12" t="n">
         <v>1</v>
@@ -2714,12 +2594,12 @@
         <v>0.48568</v>
       </c>
       <c r="G12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B13" t="n">
         <v>1</v>
@@ -2737,12 +2617,12 @@
         <v>0.00133</v>
       </c>
       <c r="G13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B14" t="n">
         <v>3</v>
@@ -2760,12 +2640,12 @@
         <v>0.00067</v>
       </c>
       <c r="G14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B15" t="n">
         <v>62</v>
@@ -2779,12 +2659,12 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B16" t="n">
         <v>67</v>
@@ -2798,7 +2678,7 @@
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2828,24 +2708,24 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" t="s">
         <v>86</v>
       </c>
-      <c r="C1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D1" t="s">
-        <v>88</v>
-      </c>
       <c r="E1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B2" t="n">
         <v>1.05</v>
@@ -2860,12 +2740,12 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B3" t="n">
         <v>0.01</v>
@@ -2880,12 +2760,12 @@
         <v>0.085</v>
       </c>
       <c r="F3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B4" t="n">
         <v>0.378</v>
@@ -2900,12 +2780,12 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B5" t="n">
         <v>0.223</v>
@@ -2920,12 +2800,12 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B6" t="n">
         <v>0.444</v>
@@ -2940,12 +2820,12 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B7" t="n">
         <v>0.002</v>
@@ -2960,12 +2840,12 @@
         <v>0.753</v>
       </c>
       <c r="F7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B8" t="n">
         <v>-0.771</v>
@@ -2980,12 +2860,12 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B9" t="n">
         <v>-0.446</v>
@@ -3000,12 +2880,12 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B10" t="n">
         <v>-0.33</v>
@@ -3020,12 +2900,12 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B11" t="n">
         <v>0.542</v>
@@ -3034,12 +2914,12 @@
       <c r="D11"/>
       <c r="E11"/>
       <c r="F11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B12" t="n">
         <v>0.307</v>
@@ -3048,12 +2928,12 @@
       <c r="D12"/>
       <c r="E12"/>
       <c r="F12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B13" t="n">
         <v>1.279</v>
@@ -3068,12 +2948,12 @@
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B14" t="n">
         <v>-0.338</v>
@@ -3088,12 +2968,12 @@
         <v>0.08</v>
       </c>
       <c r="F14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B15" t="n">
         <v>-0.059</v>
@@ -3108,12 +2988,12 @@
         <v>0.753</v>
       </c>
       <c r="F15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B16" t="n">
         <v>0.227</v>
@@ -3128,12 +3008,12 @@
         <v>0.19</v>
       </c>
       <c r="F16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B17" t="n">
         <v>0.232</v>
@@ -3142,12 +3022,12 @@
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B18" t="n">
         <v>0.188</v>
@@ -3156,12 +3036,12 @@
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B19" t="n">
         <v>1.033</v>
@@ -3176,12 +3056,12 @@
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B20" t="n">
         <v>-0.045</v>
@@ -3196,12 +3076,12 @@
         <v>0.694</v>
       </c>
       <c r="F20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B21" t="n">
         <v>0.033</v>
@@ -3216,12 +3096,12 @@
         <v>0.676</v>
       </c>
       <c r="F21" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B22" t="n">
         <v>0.124</v>
@@ -3236,12 +3116,12 @@
         <v>0.131</v>
       </c>
       <c r="F22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B23" t="n">
         <v>0.262</v>
@@ -3256,12 +3136,12 @@
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B24" t="n">
         <v>0.493</v>
@@ -3270,12 +3150,12 @@
       <c r="D24"/>
       <c r="E24"/>
       <c r="F24" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B25" t="n">
         <v>0.145</v>
@@ -3284,7 +3164,7 @@
       <c r="D25"/>
       <c r="E25"/>
       <c r="F25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -3314,24 +3194,24 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
         <v>72</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>73</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>74</v>
-      </c>
-      <c r="E1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -3351,7 +3231,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -3371,7 +3251,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -3391,7 +3271,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B5" t="n">
         <v>2</v>
@@ -3411,7 +3291,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B6" t="n">
         <v>2</v>
@@ -3431,7 +3311,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B7" t="n">
         <v>6</v>
@@ -3451,7 +3331,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B8" t="n">
         <v>2</v>
@@ -3471,7 +3351,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B9" t="n">
         <v>214</v>
@@ -3487,7 +3367,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B10" t="n">
         <v>231</v>
@@ -3534,42 +3414,42 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
         <v>72</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>73</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>74</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" t="s">
+        <v>102</v>
+      </c>
+      <c r="K1" t="s">
+        <v>103</v>
+      </c>
+      <c r="L1" t="s">
         <v>75</v>
-      </c>
-      <c r="F1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G1" t="s">
-        <v>101</v>
-      </c>
-      <c r="H1" t="s">
-        <v>102</v>
-      </c>
-      <c r="I1" t="s">
-        <v>103</v>
-      </c>
-      <c r="J1" t="s">
-        <v>104</v>
-      </c>
-      <c r="K1" t="s">
-        <v>105</v>
-      </c>
-      <c r="L1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -3602,12 +3482,12 @@
         <v>0.00067</v>
       </c>
       <c r="L2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -3640,12 +3520,12 @@
         <v>0.09061</v>
       </c>
       <c r="L3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -3678,12 +3558,12 @@
         <v>0.00266</v>
       </c>
       <c r="L4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B5" t="n">
         <v>80</v>
@@ -3708,12 +3588,12 @@
       <c r="J5"/>
       <c r="K5"/>
       <c r="L5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B6" t="n">
         <v>85</v>
@@ -3738,12 +3618,12 @@
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B7" t="n">
         <v>3</v>
@@ -3776,12 +3656,12 @@
         <v>0.27848</v>
       </c>
       <c r="L7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B8" t="n">
         <v>1</v>
@@ -3814,12 +3694,12 @@
         <v>0.00067</v>
       </c>
       <c r="L8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B9" t="n">
         <v>1</v>
@@ -3852,12 +3732,12 @@
         <v>0.002</v>
       </c>
       <c r="L9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B10" t="n">
         <v>71</v>
@@ -3882,12 +3762,12 @@
       <c r="J10"/>
       <c r="K10"/>
       <c r="L10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B11" t="n">
         <v>76</v>
@@ -3912,12 +3792,12 @@
       <c r="J11"/>
       <c r="K11"/>
       <c r="L11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B12" t="n">
         <v>3</v>
@@ -3950,12 +3830,12 @@
         <v>0.00067</v>
       </c>
       <c r="L12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B13" t="n">
         <v>1</v>
@@ -3988,12 +3868,12 @@
         <v>0.00067</v>
       </c>
       <c r="L13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B14" t="n">
         <v>1</v>
@@ -4026,12 +3906,12 @@
         <v>0.48168</v>
       </c>
       <c r="L14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B15" t="n">
         <v>62</v>
@@ -4056,12 +3936,12 @@
       <c r="J15"/>
       <c r="K15"/>
       <c r="L15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B16" t="n">
         <v>67</v>
@@ -4086,7 +3966,7 @@
       <c r="J16"/>
       <c r="K16"/>
       <c r="L16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -4106,10 +3986,10 @@
     <col min="1" max="1" width="71.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="8.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="5.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="11.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="6.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="6.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="14.71" hidden="0" customWidth="1"/>
     <col min="6" max="6" width="11.71" hidden="0" customWidth="1"/>
-    <col min="7" max="7" width="14.71" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="11.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4140,395 +4020,323 @@
       <c r="I1" t="s">
         <v>57</v>
       </c>
-      <c r="J1" t="s">
-        <v>58</v>
-      </c>
-      <c r="K1" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C2" t="n">
         <v>923.1</v>
       </c>
       <c r="D2" t="n">
-        <v>0.000000000356173661287928</v>
+        <v>1219.4</v>
       </c>
       <c r="E2" t="n">
-        <v>1219.4</v>
+        <v>0.43</v>
       </c>
       <c r="F2" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000106026935087453</v>
+        <v>0.318</v>
       </c>
       <c r="G2" t="n">
-        <v>0.43</v>
+        <v>0.163808918846475</v>
       </c>
       <c r="H2" t="n">
-        <v>0.318</v>
+        <v>0.884761957169536</v>
       </c>
       <c r="I2" t="n">
-        <v>0.163808918846475</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0.884761957169536</v>
-      </c>
-      <c r="K2" t="n">
         <v>0.445413568051623</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C3" t="n">
         <v>904.6</v>
       </c>
       <c r="D3" t="n">
-        <v>0.00000356476632034088</v>
+        <v>1086.1</v>
       </c>
       <c r="E3" t="n">
-        <v>1086.1</v>
+        <v>0.338</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0000000000000000000000000000000000907895747647671</v>
+        <v>0.225</v>
       </c>
       <c r="G3" t="n">
-        <v>0.338</v>
+        <v>0.144860307744428</v>
       </c>
       <c r="H3" t="n">
-        <v>0.225</v>
+        <v>0.948916968928776</v>
       </c>
       <c r="I3" t="n">
-        <v>0.144860307744428</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.948916968928776</v>
-      </c>
-      <c r="K3" t="n">
         <v>0.477395026003451</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C4" t="n">
         <v>890.2</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0049751824323713</v>
+        <v>964.2</v>
       </c>
       <c r="E4" t="n">
-        <v>964.2</v>
+        <v>0.222</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0000000267012839066756</v>
+        <v>0.113</v>
       </c>
       <c r="G4" t="n">
-        <v>0.222</v>
+        <v>0.122648785796666</v>
       </c>
       <c r="H4" t="n">
-        <v>0.113</v>
+        <v>1.00853413602528</v>
       </c>
       <c r="I4" t="n">
-        <v>0.122648785796666</v>
-      </c>
-      <c r="J4" t="n">
-        <v>1.00853413602528</v>
-      </c>
-      <c r="K4" t="n">
         <v>0.508488836608921</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C5" t="n">
         <v>881.2</v>
       </c>
       <c r="D5" t="n">
-        <v>0.436931983172524</v>
+        <v>929.4</v>
       </c>
       <c r="E5" t="n">
-        <v>929.4</v>
+        <v>0.205</v>
       </c>
       <c r="F5" t="n">
-        <v>0.999999973298655</v>
+        <v>0.095</v>
       </c>
       <c r="G5" t="n">
-        <v>0.205</v>
+        <v>0.121607431312658</v>
       </c>
       <c r="H5" t="n">
-        <v>0.095</v>
+        <v>1.01492820585159</v>
       </c>
       <c r="I5" t="n">
-        <v>0.121607431312658</v>
-      </c>
-      <c r="J5" t="n">
-        <v>1.01492820585159</v>
-      </c>
-      <c r="K5" t="n">
         <v>0.513921291826242</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C6" t="n">
         <v>902.1</v>
       </c>
       <c r="D6" t="n">
-        <v>0.000012830993710202</v>
+        <v>1124.3</v>
       </c>
       <c r="E6" t="n">
-        <v>1124.3</v>
+        <v>0.391</v>
       </c>
       <c r="F6" t="n">
-        <v>0.000000000000000000000000000000000000000000464876516436139</v>
+        <v>0.279</v>
       </c>
       <c r="G6" t="n">
-        <v>0.391</v>
+        <v>0.155601596236995</v>
       </c>
       <c r="H6" t="n">
-        <v>0.279</v>
+        <v>0.913117790532039</v>
       </c>
       <c r="I6" t="n">
-        <v>0.155601596236995</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.913117790532039</v>
-      </c>
-      <c r="K6" t="n">
         <v>0.45931696402324</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C7" t="n">
         <v>890.2</v>
       </c>
       <c r="D7" t="n">
-        <v>0.00479961344622744</v>
+        <v>990.2</v>
       </c>
       <c r="E7" t="n">
-        <v>990.2</v>
+        <v>0.235</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0000000000000604040943674256</v>
+        <v>0.093</v>
       </c>
       <c r="G7" t="n">
-        <v>0.235</v>
+        <v>0.157143513626403</v>
       </c>
       <c r="H7" t="n">
-        <v>0.093</v>
+        <v>0.982507593585701</v>
       </c>
       <c r="I7" t="n">
-        <v>0.157143513626403</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.982507593585701</v>
-      </c>
-      <c r="K7" t="n">
         <v>0.505803686093402</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C8" t="n">
         <v>902.1</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0000128309937101984</v>
+        <v>1124.3</v>
       </c>
       <c r="E8" t="n">
-        <v>1124.3</v>
+        <v>0.391</v>
       </c>
       <c r="F8" t="n">
-        <v>0.000000000000000000000000000000000000000000464876516436033</v>
+        <v>0.279</v>
       </c>
       <c r="G8" t="n">
-        <v>0.391</v>
+        <v>0.155601596236034</v>
       </c>
       <c r="H8" t="n">
-        <v>0.279</v>
+        <v>0.913117790532143</v>
       </c>
       <c r="I8" t="n">
-        <v>0.155601596236034</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.913117790532143</v>
-      </c>
-      <c r="K8" t="n">
         <v>0.459316964023365</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C9" t="n">
         <v>902.1</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0000128309937101984</v>
+        <v>1124.3</v>
       </c>
       <c r="E9" t="n">
-        <v>1124.3</v>
+        <v>0.391</v>
       </c>
       <c r="F9" t="n">
-        <v>0.000000000000000000000000000000000000000000464876516436033</v>
+        <v>0.279</v>
       </c>
       <c r="G9" t="n">
-        <v>0.391</v>
+        <v>0.155601596236034</v>
       </c>
       <c r="H9" t="n">
-        <v>0.279</v>
+        <v>0.913117790532143</v>
       </c>
       <c r="I9" t="n">
-        <v>0.155601596236034</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0.913117790532143</v>
-      </c>
-      <c r="K9" t="n">
         <v>0.459316964023365</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C10" t="n">
         <v>882</v>
       </c>
       <c r="D10" t="n">
-        <v>0.302098653514401</v>
+        <v>1000.5</v>
       </c>
       <c r="E10" t="n">
-        <v>1000.5</v>
+        <v>0.28</v>
       </c>
       <c r="F10" t="n">
-        <v>0.000000000000000361974667895156</v>
+        <v>0.139</v>
       </c>
       <c r="G10" t="n">
-        <v>0.28</v>
+        <v>0.163720683028945</v>
       </c>
       <c r="H10" t="n">
-        <v>0.139</v>
+        <v>0.950425796937665</v>
       </c>
       <c r="I10" t="n">
-        <v>0.163720683028945</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0.950425796937665</v>
-      </c>
-      <c r="K10" t="n">
         <v>0.488694314791684</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C11" t="n">
         <v>883.5</v>
       </c>
       <c r="D11" t="n">
-        <v>0.138174298373614</v>
+        <v>1005.7</v>
       </c>
       <c r="E11" t="n">
-        <v>1005.7</v>
+        <v>0.282</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0000000000000000259830728679035</v>
+        <v>0.144</v>
       </c>
       <c r="G11" t="n">
-        <v>0.282</v>
+        <v>0.161404588856711</v>
       </c>
       <c r="H11" t="n">
-        <v>0.144</v>
+        <v>0.950207028246836</v>
       </c>
       <c r="I11" t="n">
-        <v>0.161404588856711</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0.950207028246836</v>
-      </c>
-      <c r="K11" t="n">
         <v>0.488554386709045</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C12" t="n">
         <v>883.9</v>
       </c>
       <c r="D12" t="n">
-        <v>0.112978210957238</v>
+        <v>1024.7</v>
       </c>
       <c r="E12" t="n">
-        <v>1024.7</v>
+        <v>0.323</v>
       </c>
       <c r="F12" t="n">
-        <v>0.00000000000000000000202268013528013</v>
+        <v>0.212</v>
       </c>
       <c r="G12" t="n">
-        <v>0.323</v>
+        <v>0.140275722020262</v>
       </c>
       <c r="H12" t="n">
-        <v>0.212</v>
+        <v>0.935551604873005</v>
       </c>
       <c r="I12" t="n">
-        <v>0.140275722020262</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0.935551604873005</v>
-      </c>
-      <c r="K12" t="n">
         <v>0.476818047697685</v>
       </c>
     </row>
@@ -4559,21 +4367,21 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" t="s">
         <v>86</v>
       </c>
-      <c r="C1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D1" t="s">
-        <v>88</v>
-      </c>
       <c r="E1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B2" t="n">
         <v>0.8</v>
@@ -4590,7 +4398,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B3" t="n">
         <v>0.199</v>
@@ -4607,7 +4415,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B4" t="n">
         <v>-0.357</v>
@@ -4624,7 +4432,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B5" t="n">
         <v>-0.515</v>
@@ -4641,7 +4449,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B6" t="n">
         <v>0.234</v>
@@ -4658,7 +4466,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B7" t="n">
         <v>0.005</v>
@@ -4675,7 +4483,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B8" t="n">
         <v>-0.021</v>
@@ -4692,7 +4500,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B9" t="n">
         <v>-0.252</v>
@@ -4709,7 +4517,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B10" t="n">
         <v>0.223</v>
@@ -4726,7 +4534,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B11" t="n">
         <v>0.685</v>
@@ -4743,7 +4551,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B12" t="n">
         <v>-0.088</v>
@@ -4760,7 +4568,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B13" t="n">
         <v>-0.568</v>
@@ -4777,7 +4585,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B14" t="n">
         <v>-0.45</v>
@@ -4794,7 +4602,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B15" t="n">
         <v>0.051</v>
@@ -4811,7 +4619,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B16" t="n">
         <v>-0.154</v>
@@ -4828,7 +4636,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B17" t="n">
         <v>0.236</v>
@@ -4845,7 +4653,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B18" t="n">
         <v>0.072</v>
@@ -4862,7 +4670,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B19" t="n">
         <v>0.608</v>
@@ -4879,7 +4687,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B20" t="n">
         <v>-0.299</v>
@@ -4896,7 +4704,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B21" t="n">
         <v>0.134</v>
@@ -4913,7 +4721,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B22" t="n">
         <v>0.564</v>
@@ -4930,7 +4738,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B23" t="n">
         <v>0.524</v>
@@ -4947,7 +4755,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B24" t="n">
         <v>0.362</v>
@@ -4964,7 +4772,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B25" t="n">
         <v>0.673</v>
@@ -4981,7 +4789,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B26" t="n">
         <v>-0.179</v>
@@ -4998,7 +4806,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B27" t="n">
         <v>-0.18</v>
@@ -5015,7 +4823,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B28" t="n">
         <v>-0.482</v>
@@ -5032,7 +4840,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B29" t="n">
         <v>-0.89</v>
@@ -5049,7 +4857,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B30" t="n">
         <v>0.189</v>
@@ -5066,7 +4874,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B31" t="n">
         <v>-0.607</v>
@@ -5083,7 +4891,7 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B32" t="n">
         <v>0.28</v>
@@ -5094,7 +4902,7 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B33" t="n">
         <v>0.139</v>

</xml_diff>

<commit_message>
fix figure 1 caption text
</commit_message>
<xml_diff>
--- a/Data/Supplemental/Supplemental_Tables.xlsx
+++ b/Data/Supplemental/Supplemental_Tables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="139">
   <si>
     <t xml:space="preserve">group</t>
   </si>
@@ -178,7 +178,13 @@
     <t xml:space="preserve">AIC</t>
   </si>
   <si>
+    <t xml:space="preserve">AIC_wt</t>
+  </si>
+  <si>
     <t xml:space="preserve">BIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BIC_wt</t>
   </si>
   <si>
     <t xml:space="preserve">Conditional R2</t>
@@ -1701,8 +1707,8 @@
     <col min="2" max="2" width="65.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="8.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="5.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="5.71" hidden="0" customWidth="1"/>
-    <col min="6" max="6" width="14.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="11.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="5.71" hidden="0" customWidth="1"/>
     <col min="7" max="7" width="11.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1737,580 +1743,694 @@
       <c r="J1" t="s">
         <v>57</v>
       </c>
+      <c r="K1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D2" t="n">
         <v>223.2</v>
       </c>
       <c r="E2" t="n">
+        <v>0.0332206990579833</v>
+      </c>
+      <c r="F2" t="n">
         <v>259.2</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
+        <v>0.0000152578956652519</v>
+      </c>
+      <c r="H2" t="n">
         <v>0.545</v>
       </c>
-      <c r="G2" t="n">
+      <c r="I2" t="n">
         <v>0.366</v>
       </c>
-      <c r="H2" t="n">
+      <c r="J2" t="n">
         <v>0.282067343982829</v>
       </c>
-      <c r="I2" t="n">
+      <c r="K2" t="n">
         <v>0.855828398264632</v>
       </c>
-      <c r="J2" t="n">
+      <c r="L2" t="n">
         <v>0.294010052236142</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D3" t="n">
         <v>218.8</v>
       </c>
       <c r="E3" t="n">
+        <v>0.306747214704836</v>
+      </c>
+      <c r="F3" t="n">
         <v>243.5</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
+        <v>0.0389169854792176</v>
+      </c>
+      <c r="H3" t="n">
         <v>0.506</v>
       </c>
-      <c r="G3" t="n">
+      <c r="I3" t="n">
         <v>0.322</v>
       </c>
-      <c r="H3" t="n">
+      <c r="J3" t="n">
         <v>0.270712906666334</v>
       </c>
-      <c r="I3" t="n">
+      <c r="K3" t="n">
         <v>0.880517357628651</v>
       </c>
-      <c r="J3" t="n">
+      <c r="L3" t="n">
         <v>0.309990520594351</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" t="s">
         <v>62</v>
-      </c>
-      <c r="C4" t="s">
-        <v>60</v>
       </c>
       <c r="D4" t="n">
         <v>218.4</v>
       </c>
       <c r="E4" t="n">
+        <v>0.362269389200314</v>
+      </c>
+      <c r="F4" t="n">
         <v>245.4</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
+        <v>0.0149326080218231</v>
+      </c>
+      <c r="H4" t="n">
         <v>0.542</v>
       </c>
-      <c r="G4" t="n">
+      <c r="I4" t="n">
         <v>0.307</v>
       </c>
-      <c r="H4" t="n">
+      <c r="J4" t="n">
         <v>0.339921366849096</v>
       </c>
-      <c r="I4" t="n">
+      <c r="K4" t="n">
         <v>0.824553438127845</v>
       </c>
-      <c r="J4" t="n">
+      <c r="L4" t="n">
         <v>0.29777176529434</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D5" t="n">
         <v>225.6</v>
       </c>
       <c r="E5" t="n">
+        <v>0.0101114805243965</v>
+      </c>
+      <c r="F5" t="n">
         <v>248.1</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
+        <v>0.00394846099478588</v>
+      </c>
+      <c r="H5" t="n">
         <v>0.442</v>
       </c>
-      <c r="G5" t="n">
+      <c r="I5" t="n">
         <v>0.253</v>
       </c>
-      <c r="H5" t="n">
+      <c r="J5" t="n">
         <v>0.252780623700835</v>
       </c>
-      <c r="I5" t="n">
+      <c r="K5" t="n">
         <v>0.931849378942401</v>
       </c>
-      <c r="J5" t="n">
+      <c r="L5" t="n">
         <v>0.323013483263546</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D6" t="n">
         <v>221.6</v>
       </c>
       <c r="E6" t="n">
+        <v>0.0730842900050484</v>
+      </c>
+      <c r="F6" t="n">
         <v>239.6</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
+        <v>0.270362348894944</v>
+      </c>
+      <c r="H6" t="n">
         <v>0.442</v>
       </c>
-      <c r="G6" t="n">
+      <c r="I6" t="n">
         <v>0.254</v>
       </c>
-      <c r="H6" t="n">
+      <c r="J6" t="n">
         <v>0.252287909332907</v>
       </c>
-      <c r="I6" t="n">
+      <c r="K6" t="n">
         <v>0.933847193844437</v>
       </c>
-      <c r="J6" t="n">
+      <c r="L6" t="n">
         <v>0.322867004307088</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D7" t="n">
         <v>220.1</v>
       </c>
       <c r="E7" t="n">
+        <v>0.156128467145257</v>
+      </c>
+      <c r="F7" t="n">
         <v>247.1</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
+        <v>0.00643555671671473</v>
+      </c>
+      <c r="H7" t="n">
         <v>0.511</v>
       </c>
-      <c r="G7" t="n">
+      <c r="I7" t="n">
         <v>0.329</v>
       </c>
-      <c r="H7" t="n">
+      <c r="J7" t="n">
         <v>0.272155096268899</v>
       </c>
-      <c r="I7" t="n">
+      <c r="K7" t="n">
         <v>0.874876231377499</v>
       </c>
-      <c r="J7" t="n">
+      <c r="L7" t="n">
         <v>0.307314521780736</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D8" t="n">
         <v>222.1</v>
       </c>
       <c r="E8" t="n">
+        <v>0.0584384593621647</v>
+      </c>
+      <c r="F8" t="n">
         <v>237.8</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
+        <v>0.665388781996849</v>
+      </c>
+      <c r="H8" t="n">
         <v>0.37</v>
       </c>
-      <c r="G8" t="n">
+      <c r="I8" t="n">
         <v>0.088</v>
       </c>
-      <c r="H8" t="n">
+      <c r="J8" t="n">
         <v>0.308813845572371</v>
       </c>
-      <c r="I8" t="n">
+      <c r="K8" t="n">
         <v>0.936882341333349</v>
       </c>
-      <c r="J8" t="n">
+      <c r="L8" t="n">
         <v>0.331059051431514</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D9" t="n">
         <v>110.7</v>
       </c>
       <c r="E9" t="n">
+        <v>0.0142713175128634</v>
+      </c>
+      <c r="F9" t="n">
         <v>128.3</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
+        <v>0.000223987725579265</v>
+      </c>
+      <c r="H9" t="n">
         <v>0.427</v>
       </c>
-      <c r="G9" t="n">
+      <c r="I9" t="n">
         <v>0.347</v>
       </c>
-      <c r="H9" t="n">
+      <c r="J9" t="n">
         <v>0.12264193082729</v>
       </c>
-      <c r="I9" t="n">
+      <c r="K9" t="n">
         <v>1.00977970615862</v>
       </c>
-      <c r="J9" t="n">
+      <c r="L9" t="n">
         <v>0.335976868226673</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D10" t="n">
         <v>106</v>
       </c>
       <c r="E10" t="n">
+        <v>0.147046341763083</v>
+      </c>
+      <c r="F10" t="n">
         <v>118.6</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
+        <v>0.0285747963670422</v>
+      </c>
+      <c r="H10" t="n">
         <v>0.341</v>
       </c>
-      <c r="G10" t="n">
+      <c r="I10" t="n">
         <v>0.292</v>
       </c>
-      <c r="H10" t="n">
+      <c r="J10" t="n">
         <v>0.069512358021633</v>
       </c>
-      <c r="I10" t="n">
+      <c r="K10" t="n">
         <v>1.12393872070358</v>
       </c>
-      <c r="J10" t="n">
+      <c r="L10" t="n">
         <v>0.353702412571083</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D11" t="n">
         <v>106.9</v>
       </c>
       <c r="E11" t="n">
+        <v>0.0960456146502793</v>
+      </c>
+      <c r="F11" t="n">
         <v>119.5</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
+        <v>0.0186640745201331</v>
+      </c>
+      <c r="H11" t="n">
         <v>0.313</v>
       </c>
-      <c r="G11" t="n">
+      <c r="I11" t="n">
         <v>0.271</v>
       </c>
-      <c r="H11" t="n">
+      <c r="J11" t="n">
         <v>0.0572627646077092</v>
       </c>
-      <c r="I11" t="n">
+      <c r="K11" t="n">
         <v>1.11383231952833</v>
       </c>
-      <c r="J11" t="n">
+      <c r="L11" t="n">
         <v>0.352824835342725</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D12" t="n">
         <v>102.8</v>
       </c>
       <c r="E12" t="n">
+        <v>0.742636726073774</v>
+      </c>
+      <c r="F12" t="n">
         <v>111.6</v>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
+        <v>0.952537141387246</v>
+      </c>
+      <c r="H12" t="n">
         <v>0.268</v>
       </c>
-      <c r="G12" t="n">
+      <c r="I12" t="n">
         <v>0.224</v>
       </c>
-      <c r="H12" t="n">
+      <c r="J12" t="n">
         <v>0.056048071109652</v>
       </c>
-      <c r="I12" t="n">
+      <c r="K12" t="n">
         <v>1.19677569320301</v>
       </c>
-      <c r="J12" t="n">
+      <c r="L12" t="n">
         <v>0.36408716814135</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D13" t="n">
         <v>153.1</v>
       </c>
       <c r="E13" t="n">
+        <v>0.000942088337633318</v>
+      </c>
+      <c r="F13" t="n">
         <v>182.9</v>
       </c>
-      <c r="F13" t="n">
+      <c r="G13" t="n">
+        <v>0.000000490675746961884</v>
+      </c>
+      <c r="H13" t="n">
         <v>0.527</v>
       </c>
-      <c r="G13" t="n">
+      <c r="I13" t="n">
         <v>0.199</v>
       </c>
-      <c r="H13" t="n">
+      <c r="J13" t="n">
         <v>0.409641426216089</v>
       </c>
-      <c r="I13" t="n">
+      <c r="K13" t="n">
         <v>0.70697164728988</v>
       </c>
-      <c r="J13" t="n">
+      <c r="L13" t="n">
         <v>0.229916347254973</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D14" t="n">
         <v>145.9</v>
       </c>
       <c r="E14" t="n">
+        <v>0.0336921939959352</v>
+      </c>
+      <c r="F14" t="n">
         <v>167.8</v>
       </c>
-      <c r="F14" t="n">
+      <c r="G14" t="n">
+        <v>0.000937220650941962</v>
+      </c>
+      <c r="H14" t="n">
         <v>0.521</v>
       </c>
-      <c r="G14" t="n">
+      <c r="I14" t="n">
         <v>0.195</v>
       </c>
-      <c r="H14" t="n">
+      <c r="J14" t="n">
         <v>0.405142466313655</v>
       </c>
-      <c r="I14" t="n">
+      <c r="K14" t="n">
         <v>0.710112914902594</v>
       </c>
-      <c r="J14" t="n">
+      <c r="L14" t="n">
         <v>0.231080474175141</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D15" t="n">
         <v>146.2</v>
       </c>
       <c r="E15" t="n">
+        <v>0.0289917494562144</v>
+      </c>
+      <c r="F15" t="n">
         <v>166.1</v>
       </c>
-      <c r="F15" t="n">
+      <c r="G15" t="n">
+        <v>0.00218016507203759</v>
+      </c>
+      <c r="H15" t="n">
         <v>0.5</v>
       </c>
-      <c r="G15" t="n">
+      <c r="I15" t="n">
         <v>0.174</v>
       </c>
-      <c r="H15" t="n">
+      <c r="J15" t="n">
         <v>0.394017895328747</v>
       </c>
-      <c r="I15" t="n">
+      <c r="K15" t="n">
         <v>0.734044282144376</v>
       </c>
-      <c r="J15" t="n">
+      <c r="L15" t="n">
         <v>0.23735001040535</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D16" t="n">
         <v>142.3</v>
       </c>
       <c r="E16" t="n">
+        <v>0.204393622665867</v>
+      </c>
+      <c r="F16" t="n">
         <v>158.2</v>
       </c>
-      <c r="F16" t="n">
+      <c r="G16" t="n">
+        <v>0.112327758313534</v>
+      </c>
+      <c r="H16" t="n">
         <v>0.499</v>
       </c>
-      <c r="G16" t="n">
+      <c r="I16" t="n">
         <v>0.174</v>
       </c>
-      <c r="H16" t="n">
+      <c r="J16" t="n">
         <v>0.393286214699538</v>
       </c>
-      <c r="I16" t="n">
+      <c r="K16" t="n">
         <v>0.73324439340205</v>
       </c>
-      <c r="J16" t="n">
+      <c r="L16" t="n">
         <v>0.237295448480225</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D17" t="n">
         <v>147.9</v>
       </c>
       <c r="E17" t="n">
+        <v>0.0125689310659239</v>
+      </c>
+      <c r="F17" t="n">
         <v>171.8</v>
       </c>
-      <c r="F17" t="n">
+      <c r="G17" t="n">
+        <v>0.00012933274732436</v>
+      </c>
+      <c r="H17" t="n">
         <v>0.522</v>
       </c>
-      <c r="G17" t="n">
+      <c r="I17" t="n">
         <v>0.195</v>
       </c>
-      <c r="H17" t="n">
+      <c r="J17" t="n">
         <v>0.405616901269354</v>
       </c>
-      <c r="I17" t="n">
+      <c r="K17" t="n">
         <v>0.709947971925215</v>
       </c>
-      <c r="J17" t="n">
+      <c r="L17" t="n">
         <v>0.230951400774421</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" t="s">
         <v>68</v>
       </c>
-      <c r="B18" t="s">
-        <v>66</v>
-      </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D18" t="n">
         <v>140.4</v>
       </c>
       <c r="E18" t="n">
+        <v>0.522443416391658</v>
+      </c>
+      <c r="F18" t="n">
         <v>154.4</v>
       </c>
-      <c r="F18" t="n">
+      <c r="G18" t="n">
+        <v>0.776178144031763</v>
+      </c>
+      <c r="H18" t="n">
         <v>0.485</v>
       </c>
-      <c r="G18" t="n">
+      <c r="I18" t="n">
         <v>0.147</v>
       </c>
-      <c r="H18" t="n">
+      <c r="J18" t="n">
         <v>0.396708536396551</v>
       </c>
-      <c r="I18" t="n">
+      <c r="K18" t="n">
         <v>0.732981216183524</v>
       </c>
-      <c r="J18" t="n">
+      <c r="L18" t="n">
         <v>0.238221370362628</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D19" t="n">
         <v>142.4</v>
       </c>
       <c r="E19" t="n">
+        <v>0.196967998086768</v>
+      </c>
+      <c r="F19" t="n">
         <v>158.3</v>
       </c>
-      <c r="F19" t="n">
+      <c r="G19" t="n">
+        <v>0.108246888508652</v>
+      </c>
+      <c r="H19" t="n">
         <v>0.493</v>
       </c>
-      <c r="G19" t="n">
+      <c r="I19" t="n">
         <v>0.145</v>
       </c>
-      <c r="H19" t="n">
+      <c r="J19" t="n">
         <v>0.40760856417087</v>
       </c>
-      <c r="I19" t="n">
+      <c r="K19" t="n">
         <v>0.727645208726944</v>
       </c>
-      <c r="J19" t="n">
+      <c r="L19" t="n">
         <v>0.236972613071863</v>
       </c>
     </row>
@@ -2342,27 +2462,27 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -2380,12 +2500,12 @@
         <v>0.00067</v>
       </c>
       <c r="G2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -2403,12 +2523,12 @@
         <v>0.05463</v>
       </c>
       <c r="G3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -2426,12 +2546,12 @@
         <v>0.00133</v>
       </c>
       <c r="G4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B5" t="n">
         <v>80</v>
@@ -2445,12 +2565,12 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B6" t="n">
         <v>85</v>
@@ -2464,12 +2584,12 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B7" t="n">
         <v>1</v>
@@ -2487,12 +2607,12 @@
         <v>0.00067</v>
       </c>
       <c r="G7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B8" t="n">
         <v>1</v>
@@ -2510,12 +2630,12 @@
         <v>0.00067</v>
       </c>
       <c r="G8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B9" t="n">
         <v>3</v>
@@ -2533,12 +2653,12 @@
         <v>0.22252</v>
       </c>
       <c r="G9" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B10" t="n">
         <v>71</v>
@@ -2552,12 +2672,12 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B11" t="n">
         <v>76</v>
@@ -2571,12 +2691,12 @@
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B12" t="n">
         <v>1</v>
@@ -2594,12 +2714,12 @@
         <v>0.48568</v>
       </c>
       <c r="G12" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B13" t="n">
         <v>1</v>
@@ -2617,12 +2737,12 @@
         <v>0.00133</v>
       </c>
       <c r="G13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B14" t="n">
         <v>3</v>
@@ -2640,12 +2760,12 @@
         <v>0.00067</v>
       </c>
       <c r="G14" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B15" t="n">
         <v>62</v>
@@ -2659,12 +2779,12 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B16" t="n">
         <v>67</v>
@@ -2678,7 +2798,7 @@
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2708,24 +2828,24 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B2" t="n">
         <v>1.05</v>
@@ -2740,12 +2860,12 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B3" t="n">
         <v>0.01</v>
@@ -2760,12 +2880,12 @@
         <v>0.085</v>
       </c>
       <c r="F3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B4" t="n">
         <v>0.378</v>
@@ -2780,12 +2900,12 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B5" t="n">
         <v>0.223</v>
@@ -2800,12 +2920,12 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B6" t="n">
         <v>0.444</v>
@@ -2820,12 +2940,12 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B7" t="n">
         <v>0.002</v>
@@ -2840,12 +2960,12 @@
         <v>0.753</v>
       </c>
       <c r="F7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B8" t="n">
         <v>-0.771</v>
@@ -2860,12 +2980,12 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B9" t="n">
         <v>-0.446</v>
@@ -2880,12 +3000,12 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B10" t="n">
         <v>-0.33</v>
@@ -2900,12 +3020,12 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B11" t="n">
         <v>0.542</v>
@@ -2914,12 +3034,12 @@
       <c r="D11"/>
       <c r="E11"/>
       <c r="F11" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B12" t="n">
         <v>0.307</v>
@@ -2928,12 +3048,12 @@
       <c r="D12"/>
       <c r="E12"/>
       <c r="F12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B13" t="n">
         <v>1.279</v>
@@ -2948,12 +3068,12 @@
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B14" t="n">
         <v>-0.338</v>
@@ -2968,12 +3088,12 @@
         <v>0.08</v>
       </c>
       <c r="F14" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B15" t="n">
         <v>-0.059</v>
@@ -2988,12 +3108,12 @@
         <v>0.753</v>
       </c>
       <c r="F15" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B16" t="n">
         <v>0.227</v>
@@ -3008,12 +3128,12 @@
         <v>0.19</v>
       </c>
       <c r="F16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B17" t="n">
         <v>0.232</v>
@@ -3022,12 +3142,12 @@
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B18" t="n">
         <v>0.188</v>
@@ -3036,12 +3156,12 @@
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B19" t="n">
         <v>1.033</v>
@@ -3056,12 +3176,12 @@
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B20" t="n">
         <v>-0.045</v>
@@ -3076,12 +3196,12 @@
         <v>0.694</v>
       </c>
       <c r="F20" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B21" t="n">
         <v>0.033</v>
@@ -3096,12 +3216,12 @@
         <v>0.676</v>
       </c>
       <c r="F21" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B22" t="n">
         <v>0.124</v>
@@ -3116,12 +3236,12 @@
         <v>0.131</v>
       </c>
       <c r="F22" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B23" t="n">
         <v>0.262</v>
@@ -3136,12 +3256,12 @@
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B24" t="n">
         <v>0.493</v>
@@ -3150,12 +3270,12 @@
       <c r="D24"/>
       <c r="E24"/>
       <c r="F24" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B25" t="n">
         <v>0.145</v>
@@ -3164,7 +3284,7 @@
       <c r="D25"/>
       <c r="E25"/>
       <c r="F25" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -3194,24 +3314,24 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -3231,7 +3351,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -3251,7 +3371,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -3271,7 +3391,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B5" t="n">
         <v>2</v>
@@ -3291,7 +3411,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B6" t="n">
         <v>2</v>
@@ -3311,7 +3431,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B7" t="n">
         <v>6</v>
@@ -3331,7 +3451,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B8" t="n">
         <v>2</v>
@@ -3351,7 +3471,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B9" t="n">
         <v>214</v>
@@ -3367,7 +3487,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B10" t="n">
         <v>231</v>
@@ -3414,42 +3534,42 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="I1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="K1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="L1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -3482,12 +3602,12 @@
         <v>0.00067</v>
       </c>
       <c r="L2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -3520,12 +3640,12 @@
         <v>0.09061</v>
       </c>
       <c r="L3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -3558,12 +3678,12 @@
         <v>0.00266</v>
       </c>
       <c r="L4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B5" t="n">
         <v>80</v>
@@ -3588,12 +3708,12 @@
       <c r="J5"/>
       <c r="K5"/>
       <c r="L5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B6" t="n">
         <v>85</v>
@@ -3618,12 +3738,12 @@
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B7" t="n">
         <v>3</v>
@@ -3656,12 +3776,12 @@
         <v>0.27848</v>
       </c>
       <c r="L7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B8" t="n">
         <v>1</v>
@@ -3694,12 +3814,12 @@
         <v>0.00067</v>
       </c>
       <c r="L8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B9" t="n">
         <v>1</v>
@@ -3732,12 +3852,12 @@
         <v>0.002</v>
       </c>
       <c r="L9" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B10" t="n">
         <v>71</v>
@@ -3762,12 +3882,12 @@
       <c r="J10"/>
       <c r="K10"/>
       <c r="L10" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B11" t="n">
         <v>76</v>
@@ -3792,12 +3912,12 @@
       <c r="J11"/>
       <c r="K11"/>
       <c r="L11" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B12" t="n">
         <v>3</v>
@@ -3830,12 +3950,12 @@
         <v>0.00067</v>
       </c>
       <c r="L12" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B13" t="n">
         <v>1</v>
@@ -3868,12 +3988,12 @@
         <v>0.00067</v>
       </c>
       <c r="L13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B14" t="n">
         <v>1</v>
@@ -3906,12 +4026,12 @@
         <v>0.48168</v>
       </c>
       <c r="L14" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B15" t="n">
         <v>62</v>
@@ -3936,12 +4056,12 @@
       <c r="J15"/>
       <c r="K15"/>
       <c r="L15" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B16" t="n">
         <v>67</v>
@@ -3966,7 +4086,7 @@
       <c r="J16"/>
       <c r="K16"/>
       <c r="L16" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -3986,10 +4106,10 @@
     <col min="1" max="1" width="71.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="8.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="5.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="6.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="14.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="11.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="6.71" hidden="0" customWidth="1"/>
     <col min="6" max="6" width="11.71" hidden="0" customWidth="1"/>
-    <col min="7" max="7" width="11.71" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="14.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4020,323 +4140,395 @@
       <c r="I1" t="s">
         <v>57</v>
       </c>
+      <c r="J1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C2" t="n">
         <v>923.1</v>
       </c>
       <c r="D2" t="n">
+        <v>0.000000000356173661287928</v>
+      </c>
+      <c r="E2" t="n">
         <v>1219.4</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
+        <v>0.00000000000000000000000000000000000000000000000000000000000000106026935087453</v>
+      </c>
+      <c r="G2" t="n">
         <v>0.43</v>
       </c>
-      <c r="F2" t="n">
+      <c r="H2" t="n">
         <v>0.318</v>
       </c>
-      <c r="G2" t="n">
+      <c r="I2" t="n">
         <v>0.163808918846475</v>
       </c>
-      <c r="H2" t="n">
+      <c r="J2" t="n">
         <v>0.884761957169536</v>
       </c>
-      <c r="I2" t="n">
+      <c r="K2" t="n">
         <v>0.445413568051623</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C3" t="n">
         <v>904.6</v>
       </c>
       <c r="D3" t="n">
+        <v>0.00000356476632034088</v>
+      </c>
+      <c r="E3" t="n">
         <v>1086.1</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
+        <v>0.0000000000000000000000000000000000907895747647671</v>
+      </c>
+      <c r="G3" t="n">
         <v>0.338</v>
       </c>
-      <c r="F3" t="n">
+      <c r="H3" t="n">
         <v>0.225</v>
       </c>
-      <c r="G3" t="n">
+      <c r="I3" t="n">
         <v>0.144860307744428</v>
       </c>
-      <c r="H3" t="n">
+      <c r="J3" t="n">
         <v>0.948916968928776</v>
       </c>
-      <c r="I3" t="n">
+      <c r="K3" t="n">
         <v>0.477395026003451</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C4" t="n">
         <v>890.2</v>
       </c>
       <c r="D4" t="n">
+        <v>0.0049751824323713</v>
+      </c>
+      <c r="E4" t="n">
         <v>964.2</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
+        <v>0.0000000267012839066756</v>
+      </c>
+      <c r="G4" t="n">
         <v>0.222</v>
       </c>
-      <c r="F4" t="n">
+      <c r="H4" t="n">
         <v>0.113</v>
       </c>
-      <c r="G4" t="n">
+      <c r="I4" t="n">
         <v>0.122648785796666</v>
       </c>
-      <c r="H4" t="n">
+      <c r="J4" t="n">
         <v>1.00853413602528</v>
       </c>
-      <c r="I4" t="n">
+      <c r="K4" t="n">
         <v>0.508488836608921</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C5" t="n">
         <v>881.2</v>
       </c>
       <c r="D5" t="n">
+        <v>0.436931983172524</v>
+      </c>
+      <c r="E5" t="n">
         <v>929.4</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
+        <v>0.999999973298655</v>
+      </c>
+      <c r="G5" t="n">
         <v>0.205</v>
       </c>
-      <c r="F5" t="n">
+      <c r="H5" t="n">
         <v>0.095</v>
       </c>
-      <c r="G5" t="n">
+      <c r="I5" t="n">
         <v>0.121607431312658</v>
       </c>
-      <c r="H5" t="n">
+      <c r="J5" t="n">
         <v>1.01492820585159</v>
       </c>
-      <c r="I5" t="n">
+      <c r="K5" t="n">
         <v>0.513921291826242</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C6" t="n">
         <v>902.1</v>
       </c>
       <c r="D6" t="n">
+        <v>0.000012830993710202</v>
+      </c>
+      <c r="E6" t="n">
         <v>1124.3</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
+        <v>0.000000000000000000000000000000000000000000464876516436139</v>
+      </c>
+      <c r="G6" t="n">
         <v>0.391</v>
       </c>
-      <c r="F6" t="n">
+      <c r="H6" t="n">
         <v>0.279</v>
       </c>
-      <c r="G6" t="n">
+      <c r="I6" t="n">
         <v>0.155601596236995</v>
       </c>
-      <c r="H6" t="n">
+      <c r="J6" t="n">
         <v>0.913117790532039</v>
       </c>
-      <c r="I6" t="n">
+      <c r="K6" t="n">
         <v>0.45931696402324</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C7" t="n">
         <v>890.2</v>
       </c>
       <c r="D7" t="n">
+        <v>0.00479961344622744</v>
+      </c>
+      <c r="E7" t="n">
         <v>990.2</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
+        <v>0.0000000000000604040943674256</v>
+      </c>
+      <c r="G7" t="n">
         <v>0.235</v>
       </c>
-      <c r="F7" t="n">
+      <c r="H7" t="n">
         <v>0.093</v>
       </c>
-      <c r="G7" t="n">
+      <c r="I7" t="n">
         <v>0.157143513626403</v>
       </c>
-      <c r="H7" t="n">
+      <c r="J7" t="n">
         <v>0.982507593585701</v>
       </c>
-      <c r="I7" t="n">
+      <c r="K7" t="n">
         <v>0.505803686093402</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C8" t="n">
         <v>902.1</v>
       </c>
       <c r="D8" t="n">
+        <v>0.0000128309937101984</v>
+      </c>
+      <c r="E8" t="n">
         <v>1124.3</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
+        <v>0.000000000000000000000000000000000000000000464876516436033</v>
+      </c>
+      <c r="G8" t="n">
         <v>0.391</v>
       </c>
-      <c r="F8" t="n">
+      <c r="H8" t="n">
         <v>0.279</v>
       </c>
-      <c r="G8" t="n">
+      <c r="I8" t="n">
         <v>0.155601596236034</v>
       </c>
-      <c r="H8" t="n">
+      <c r="J8" t="n">
         <v>0.913117790532143</v>
       </c>
-      <c r="I8" t="n">
+      <c r="K8" t="n">
         <v>0.459316964023365</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C9" t="n">
         <v>902.1</v>
       </c>
       <c r="D9" t="n">
+        <v>0.0000128309937101984</v>
+      </c>
+      <c r="E9" t="n">
         <v>1124.3</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
+        <v>0.000000000000000000000000000000000000000000464876516436033</v>
+      </c>
+      <c r="G9" t="n">
         <v>0.391</v>
       </c>
-      <c r="F9" t="n">
+      <c r="H9" t="n">
         <v>0.279</v>
       </c>
-      <c r="G9" t="n">
+      <c r="I9" t="n">
         <v>0.155601596236034</v>
       </c>
-      <c r="H9" t="n">
+      <c r="J9" t="n">
         <v>0.913117790532143</v>
       </c>
-      <c r="I9" t="n">
+      <c r="K9" t="n">
         <v>0.459316964023365</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C10" t="n">
         <v>882</v>
       </c>
       <c r="D10" t="n">
+        <v>0.302098653514401</v>
+      </c>
+      <c r="E10" t="n">
         <v>1000.5</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
+        <v>0.000000000000000361974667895156</v>
+      </c>
+      <c r="G10" t="n">
         <v>0.28</v>
       </c>
-      <c r="F10" t="n">
+      <c r="H10" t="n">
         <v>0.139</v>
       </c>
-      <c r="G10" t="n">
+      <c r="I10" t="n">
         <v>0.163720683028945</v>
       </c>
-      <c r="H10" t="n">
+      <c r="J10" t="n">
         <v>0.950425796937665</v>
       </c>
-      <c r="I10" t="n">
+      <c r="K10" t="n">
         <v>0.488694314791684</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C11" t="n">
         <v>883.5</v>
       </c>
       <c r="D11" t="n">
+        <v>0.138174298373614</v>
+      </c>
+      <c r="E11" t="n">
         <v>1005.7</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
+        <v>0.0000000000000000259830728679035</v>
+      </c>
+      <c r="G11" t="n">
         <v>0.282</v>
       </c>
-      <c r="F11" t="n">
+      <c r="H11" t="n">
         <v>0.144</v>
       </c>
-      <c r="G11" t="n">
+      <c r="I11" t="n">
         <v>0.161404588856711</v>
       </c>
-      <c r="H11" t="n">
+      <c r="J11" t="n">
         <v>0.950207028246836</v>
       </c>
-      <c r="I11" t="n">
+      <c r="K11" t="n">
         <v>0.488554386709045</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C12" t="n">
         <v>883.9</v>
       </c>
       <c r="D12" t="n">
+        <v>0.112978210957238</v>
+      </c>
+      <c r="E12" t="n">
         <v>1024.7</v>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
+        <v>0.00000000000000000000202268013528013</v>
+      </c>
+      <c r="G12" t="n">
         <v>0.323</v>
       </c>
-      <c r="F12" t="n">
+      <c r="H12" t="n">
         <v>0.212</v>
       </c>
-      <c r="G12" t="n">
+      <c r="I12" t="n">
         <v>0.140275722020262</v>
       </c>
-      <c r="H12" t="n">
+      <c r="J12" t="n">
         <v>0.935551604873005</v>
       </c>
-      <c r="I12" t="n">
+      <c r="K12" t="n">
         <v>0.476818047697685</v>
       </c>
     </row>
@@ -4367,21 +4559,21 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B2" t="n">
         <v>0.8</v>
@@ -4398,7 +4590,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B3" t="n">
         <v>0.199</v>
@@ -4415,7 +4607,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B4" t="n">
         <v>-0.357</v>
@@ -4432,7 +4624,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B5" t="n">
         <v>-0.515</v>
@@ -4449,7 +4641,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B6" t="n">
         <v>0.234</v>
@@ -4466,7 +4658,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B7" t="n">
         <v>0.005</v>
@@ -4483,7 +4675,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B8" t="n">
         <v>-0.021</v>
@@ -4500,7 +4692,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B9" t="n">
         <v>-0.252</v>
@@ -4517,7 +4709,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B10" t="n">
         <v>0.223</v>
@@ -4534,7 +4726,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B11" t="n">
         <v>0.685</v>
@@ -4551,7 +4743,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B12" t="n">
         <v>-0.088</v>
@@ -4568,7 +4760,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B13" t="n">
         <v>-0.568</v>
@@ -4585,7 +4777,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B14" t="n">
         <v>-0.45</v>
@@ -4602,7 +4794,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B15" t="n">
         <v>0.051</v>
@@ -4619,7 +4811,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B16" t="n">
         <v>-0.154</v>
@@ -4636,7 +4828,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B17" t="n">
         <v>0.236</v>
@@ -4653,7 +4845,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B18" t="n">
         <v>0.072</v>
@@ -4670,7 +4862,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B19" t="n">
         <v>0.608</v>
@@ -4687,7 +4879,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B20" t="n">
         <v>-0.299</v>
@@ -4704,7 +4896,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B21" t="n">
         <v>0.134</v>
@@ -4721,7 +4913,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B22" t="n">
         <v>0.564</v>
@@ -4738,7 +4930,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B23" t="n">
         <v>0.524</v>
@@ -4755,7 +4947,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B24" t="n">
         <v>0.362</v>
@@ -4772,7 +4964,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B25" t="n">
         <v>0.673</v>
@@ -4789,7 +4981,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B26" t="n">
         <v>-0.179</v>
@@ -4806,7 +4998,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B27" t="n">
         <v>-0.18</v>
@@ -4823,7 +5015,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B28" t="n">
         <v>-0.482</v>
@@ -4840,7 +5032,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B29" t="n">
         <v>-0.89</v>
@@ -4857,7 +5049,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B30" t="n">
         <v>0.189</v>
@@ -4874,7 +5066,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B31" t="n">
         <v>-0.607</v>
@@ -4891,7 +5083,7 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B32" t="n">
         <v>0.28</v>
@@ -4902,7 +5094,7 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B33" t="n">
         <v>0.139</v>

</xml_diff>

<commit_message>
renaming figures and tables
</commit_message>
<xml_diff>
--- a/Data/Supplemental/Supplemental_Tables.xlsx
+++ b/Data/Supplemental/Supplemental_Tables.xlsx
@@ -6,15 +6,15 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Table S1 - Sample Size" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Table S2 - PERMANOVA AIC" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Table S3 - Plasticity AIC" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Table S4 - PERMANOVA" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Table S5 - Plasticity GLM" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Table S6 - Species PERMANOVA" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Table S7 - HostVsymb PERMANOVA" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Table S8 - HostVsymb Plast AIC" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="Table S9 - HostVsymb Plast GLM" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Table A - Sample Size" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Table B - PERMANOVA AIC" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Table C - Plasticity AIC" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Table D - PERMANOVA" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Table E - Plasticity GLM" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Table F - Species PERMANOVA" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Table G - HostVsymb PERMANOVA" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="HostVsymb Plast AIC" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="HostVsymb Plast GLM" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
 </workbook>
 </file>
@@ -3366,7 +3366,7 @@
         <v>2.87</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0966</v>
+        <v>0.09927</v>
       </c>
     </row>
     <row r="4">
@@ -3386,7 +3386,7 @@
         <v>9.61</v>
       </c>
       <c r="F4" t="n">
-        <v>0.00133</v>
+        <v>0.002</v>
       </c>
     </row>
     <row r="5">
@@ -3446,7 +3446,7 @@
         <v>2.51</v>
       </c>
       <c r="F7" t="n">
-        <v>0.02065</v>
+        <v>0.01932</v>
       </c>
     </row>
     <row r="8">
@@ -3466,7 +3466,7 @@
         <v>6.39</v>
       </c>
       <c r="F8" t="n">
-        <v>0.00266</v>
+        <v>0.002</v>
       </c>
     </row>
     <row r="9">
@@ -3584,7 +3584,7 @@
         <v>0.55</v>
       </c>
       <c r="F2" t="n">
-        <v>0.77615</v>
+        <v>0.77815</v>
       </c>
       <c r="G2" t="n">
         <v>3</v>
@@ -3660,7 +3660,7 @@
         <v>0.52</v>
       </c>
       <c r="F4" t="n">
-        <v>0.58894</v>
+        <v>0.59227</v>
       </c>
       <c r="G4" t="n">
         <v>1</v>
@@ -3758,7 +3758,7 @@
         <v>1.23</v>
       </c>
       <c r="F7" t="n">
-        <v>0.26382</v>
+        <v>0.26316</v>
       </c>
       <c r="G7" t="n">
         <v>3</v>
@@ -3834,7 +3834,7 @@
         <v>1.75</v>
       </c>
       <c r="F9" t="n">
-        <v>0.17255</v>
+        <v>0.17055</v>
       </c>
       <c r="G9" t="n">
         <v>1</v>
@@ -3932,7 +3932,7 @@
         <v>3.48</v>
       </c>
       <c r="F12" t="n">
-        <v>0.01666</v>
+        <v>0.01732</v>
       </c>
       <c r="G12" t="n">
         <v>3</v>
@@ -4008,7 +4008,7 @@
         <v>1.64</v>
       </c>
       <c r="F14" t="n">
-        <v>0.1992</v>
+        <v>0.1972</v>
       </c>
       <c r="G14" t="n">
         <v>1</v>

</xml_diff>